<commit_message>
Pushing the factors to run simulation with the fixed double entry
</commit_message>
<xml_diff>
--- a/heliostrome/jip_project/results/Factors to run simulation.xlsx
+++ b/heliostrome/jip_project/results/Factors to run simulation.xlsx
@@ -217,7 +217,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
   <numFmts count="0"/>
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -230,6 +230,12 @@
       <sz val="13"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
       <family val="2"/>
     </font>
     <font>
@@ -253,13 +259,13 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -362,7 +368,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="37">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
     <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -373,94 +379,103 @@
     <xf xfId="0" numFmtId="14" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf xfId="0" numFmtId="14" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="14" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="4" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="4" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf xfId="0" numFmtId="14" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="4" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="14" applyNumberFormat="1" borderId="3" applyBorder="1" fontId="4" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="14" applyNumberFormat="1" borderId="4" applyBorder="1" fontId="4" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="4" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="4" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="4" applyBorder="1" fontId="4" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="general"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="5" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="14" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="6" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="7" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="general"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="general"/>
+    </xf>
     <xf xfId="0" numFmtId="14" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="general"/>
     </xf>
     <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="general"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf xfId="0" numFmtId="14" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf xfId="0" numFmtId="14" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf xfId="0" numFmtId="14" applyNumberFormat="1" borderId="3" applyBorder="1" fontId="3" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf xfId="0" numFmtId="14" applyNumberFormat="1" borderId="4" applyBorder="1" fontId="3" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="4" applyBorder="1" fontId="3" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="4" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf xfId="0" numFmtId="14" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="5" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="6" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="4" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="4" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="4" applyBorder="1" fontId="4" applyFont="1" fillId="3" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="4" applyBorder="1" fontId="4" applyFont="1" fillId="4" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="4" applyBorder="1" fontId="4" applyFont="1" fillId="5" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="4" applyBorder="1" fontId="8" applyFont="1" fillId="3" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="4" applyBorder="1" fontId="4" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
-    </xf>
-    <xf xfId="0" numFmtId="14" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
-    </xf>
-    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="4" applyBorder="1" fontId="3" applyFont="1" fillId="3" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="4" applyBorder="1" fontId="3" applyFont="1" fillId="4" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="4" applyBorder="1" fontId="3" applyFont="1" fillId="5" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="4" applyBorder="1" fontId="7" applyFont="1" fillId="3" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="4" applyBorder="1" fontId="3" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -773,175 +788,175 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="23" width="14.719285714285713" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="36" width="14.719285714285713" customWidth="1" bestFit="1"/>
     <col min="2" max="2" style="23" width="19.433571428571426" customWidth="1" bestFit="1"/>
     <col min="3" max="3" style="23" width="21.433571428571426" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="23" width="17.005" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="36" width="17.005" customWidth="1" bestFit="1"/>
     <col min="5" max="5" style="23" width="13.576428571428572" customWidth="1" bestFit="1"/>
     <col min="6" max="6" style="23" width="13.576428571428572" customWidth="1" bestFit="1"/>
     <col min="7" max="7" style="23" width="13.576428571428572" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
-      <c r="A1" s="18"/>
-      <c r="B1" s="27" t="s">
+      <c r="A1" s="28"/>
+      <c r="B1" s="29" t="s">
         <v>47</v>
       </c>
-      <c r="C1" s="27" t="s">
+      <c r="C1" s="29" t="s">
         <v>48</v>
       </c>
-      <c r="D1" s="28" t="s">
+      <c r="D1" s="30" t="s">
         <v>0</v>
       </c>
-      <c r="E1" s="27" t="s">
+      <c r="E1" s="29" t="s">
         <v>49</v>
       </c>
-      <c r="F1" s="27" t="s">
+      <c r="F1" s="29" t="s">
         <v>50</v>
       </c>
-      <c r="G1" s="28" t="s">
+      <c r="G1" s="30" t="s">
         <v>51</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75">
-      <c r="A2" s="27" t="s">
+      <c r="A2" s="29" t="s">
         <v>52</v>
       </c>
-      <c r="B2" s="29"/>
-      <c r="C2" s="29"/>
-      <c r="D2" s="29"/>
-      <c r="E2" s="29"/>
-      <c r="F2" s="30"/>
-      <c r="G2" s="31"/>
+      <c r="B2" s="31"/>
+      <c r="C2" s="31"/>
+      <c r="D2" s="31"/>
+      <c r="E2" s="31"/>
+      <c r="F2" s="32"/>
+      <c r="G2" s="33"/>
     </row>
     <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18.75">
-      <c r="A3" s="27" t="s">
+      <c r="A3" s="29" t="s">
         <v>53</v>
       </c>
-      <c r="B3" s="29"/>
-      <c r="C3" s="30"/>
-      <c r="D3" s="29"/>
-      <c r="E3" s="30"/>
-      <c r="F3" s="29"/>
-      <c r="G3" s="29"/>
+      <c r="B3" s="31"/>
+      <c r="C3" s="32"/>
+      <c r="D3" s="31"/>
+      <c r="E3" s="32"/>
+      <c r="F3" s="31"/>
+      <c r="G3" s="31"/>
     </row>
     <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18.75">
-      <c r="A4" s="27" t="s">
+      <c r="A4" s="29" t="s">
         <v>54</v>
       </c>
-      <c r="B4" s="30"/>
-      <c r="C4" s="32"/>
-      <c r="D4" s="29"/>
-      <c r="E4" s="29"/>
-      <c r="F4" s="29"/>
-      <c r="G4" s="30"/>
+      <c r="B4" s="32"/>
+      <c r="C4" s="34"/>
+      <c r="D4" s="31"/>
+      <c r="E4" s="31"/>
+      <c r="F4" s="31"/>
+      <c r="G4" s="32"/>
     </row>
     <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18.75">
-      <c r="A5" s="27" t="s">
+      <c r="A5" s="29" t="s">
         <v>55</v>
       </c>
-      <c r="B5" s="30"/>
-      <c r="C5" s="31"/>
-      <c r="D5" s="29"/>
-      <c r="E5" s="29"/>
-      <c r="F5" s="31"/>
-      <c r="G5" s="29"/>
+      <c r="B5" s="32"/>
+      <c r="C5" s="33"/>
+      <c r="D5" s="31"/>
+      <c r="E5" s="31"/>
+      <c r="F5" s="33"/>
+      <c r="G5" s="31"/>
     </row>
     <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18.75">
-      <c r="A6" s="27" t="s">
+      <c r="A6" s="29" t="s">
         <v>56</v>
       </c>
-      <c r="B6" s="30"/>
-      <c r="C6" s="31"/>
-      <c r="D6" s="29"/>
-      <c r="E6" s="29"/>
-      <c r="F6" s="29"/>
-      <c r="G6" s="30"/>
+      <c r="B6" s="32"/>
+      <c r="C6" s="33"/>
+      <c r="D6" s="31"/>
+      <c r="E6" s="31"/>
+      <c r="F6" s="31"/>
+      <c r="G6" s="32"/>
     </row>
     <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="18.75">
-      <c r="A7" s="27" t="s">
+      <c r="A7" s="29" t="s">
         <v>57</v>
       </c>
-      <c r="B7" s="29"/>
-      <c r="C7" s="29"/>
-      <c r="D7" s="29"/>
-      <c r="E7" s="31"/>
-      <c r="F7" s="29"/>
-      <c r="G7" s="29"/>
+      <c r="B7" s="31"/>
+      <c r="C7" s="31"/>
+      <c r="D7" s="31"/>
+      <c r="E7" s="33"/>
+      <c r="F7" s="31"/>
+      <c r="G7" s="31"/>
     </row>
     <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="18.75">
-      <c r="A8" s="27" t="s">
+      <c r="A8" s="29" t="s">
         <v>58</v>
       </c>
-      <c r="B8" s="29"/>
-      <c r="C8" s="30"/>
-      <c r="D8" s="29"/>
-      <c r="E8" s="31"/>
-      <c r="F8" s="30"/>
-      <c r="G8" s="30"/>
+      <c r="B8" s="31"/>
+      <c r="C8" s="32"/>
+      <c r="D8" s="31"/>
+      <c r="E8" s="33"/>
+      <c r="F8" s="32"/>
+      <c r="G8" s="32"/>
     </row>
     <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="18.75">
-      <c r="A9" s="27" t="s">
+      <c r="A9" s="29" t="s">
         <v>59</v>
       </c>
-      <c r="B9" s="30"/>
-      <c r="C9" s="30"/>
-      <c r="D9" s="29"/>
-      <c r="E9" s="31"/>
-      <c r="F9" s="29"/>
-      <c r="G9" s="30"/>
+      <c r="B9" s="32"/>
+      <c r="C9" s="32"/>
+      <c r="D9" s="31"/>
+      <c r="E9" s="33"/>
+      <c r="F9" s="31"/>
+      <c r="G9" s="32"/>
     </row>
     <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="18.75">
-      <c r="A10" s="27" t="s">
+      <c r="A10" s="29" t="s">
         <v>60</v>
       </c>
-      <c r="B10" s="29"/>
-      <c r="C10" s="29"/>
-      <c r="D10" s="29"/>
-      <c r="E10" s="31"/>
-      <c r="F10" s="29"/>
-      <c r="G10" s="29"/>
+      <c r="B10" s="31"/>
+      <c r="C10" s="31"/>
+      <c r="D10" s="31"/>
+      <c r="E10" s="33"/>
+      <c r="F10" s="31"/>
+      <c r="G10" s="31"/>
     </row>
     <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="18.75">
-      <c r="A11" s="27" t="s">
+      <c r="A11" s="29" t="s">
         <v>61</v>
       </c>
-      <c r="B11" s="29"/>
-      <c r="C11" s="30"/>
-      <c r="D11" s="29"/>
-      <c r="E11" s="31"/>
-      <c r="F11" s="31"/>
-      <c r="G11" s="29"/>
+      <c r="B11" s="31"/>
+      <c r="C11" s="32"/>
+      <c r="D11" s="31"/>
+      <c r="E11" s="33"/>
+      <c r="F11" s="33"/>
+      <c r="G11" s="31"/>
     </row>
     <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="18.75">
-      <c r="A12" s="27" t="s">
+      <c r="A12" s="29" t="s">
         <v>62</v>
       </c>
       <c r="B12" s="18"/>
       <c r="C12" s="18"/>
-      <c r="D12" s="33"/>
+      <c r="D12" s="35"/>
       <c r="E12" s="18"/>
       <c r="F12" s="18"/>
       <c r="G12" s="18"/>
     </row>
     <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="18.75">
-      <c r="A13" s="27" t="s">
+      <c r="A13" s="29" t="s">
         <v>63</v>
       </c>
       <c r="B13" s="18"/>
       <c r="C13" s="18"/>
-      <c r="D13" s="33"/>
+      <c r="D13" s="35"/>
       <c r="E13" s="18"/>
       <c r="F13" s="18"/>
       <c r="G13" s="18"/>
     </row>
     <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="18.75">
-      <c r="A14" s="27" t="s">
+      <c r="A14" s="29" t="s">
         <v>64</v>
       </c>
       <c r="B14" s="18"/>
       <c r="C14" s="18"/>
-      <c r="D14" s="33"/>
+      <c r="D14" s="35"/>
       <c r="E14" s="18"/>
       <c r="F14" s="18"/>
       <c r="G14" s="18"/>
@@ -966,21 +981,21 @@
   <cols>
     <col min="1" max="1" style="23" width="44.005" customWidth="1" bestFit="1"/>
     <col min="2" max="2" style="24" width="30.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="24" width="30.433571428571426" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="24" width="30.005" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="24" width="28.719285714285714" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="24" width="31.005" customWidth="1" bestFit="1"/>
-    <col min="7" max="7" style="24" width="29.290714285714284" customWidth="1" bestFit="1"/>
-    <col min="8" max="8" style="24" width="31.433571428571426" customWidth="1" bestFit="1"/>
-    <col min="9" max="9" style="25" width="31.433571428571426" customWidth="1" bestFit="1"/>
-    <col min="10" max="10" style="25" width="32.86214285714286" customWidth="1" bestFit="1"/>
-    <col min="11" max="11" style="25" width="24.290714285714284" customWidth="1" bestFit="1"/>
-    <col min="12" max="12" style="25" width="24.290714285714284" customWidth="1" bestFit="1"/>
-    <col min="13" max="13" style="25" width="24.290714285714284" customWidth="1" bestFit="1"/>
-    <col min="14" max="14" style="25" width="24.290714285714284" customWidth="1" bestFit="1"/>
-    <col min="15" max="15" style="25" width="24.290714285714284" customWidth="1" bestFit="1"/>
-    <col min="16" max="16" style="26" width="24.005" customWidth="1" bestFit="1"/>
-    <col min="17" max="17" style="26" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="25" width="30.433571428571426" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="25" width="30.005" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="25" width="28.719285714285714" customWidth="1" bestFit="1"/>
+    <col min="6" max="6" style="25" width="31.005" customWidth="1" bestFit="1"/>
+    <col min="7" max="7" style="25" width="29.290714285714284" customWidth="1" bestFit="1"/>
+    <col min="8" max="8" style="25" width="31.433571428571426" customWidth="1" bestFit="1"/>
+    <col min="9" max="9" style="26" width="31.433571428571426" customWidth="1" bestFit="1"/>
+    <col min="10" max="10" style="26" width="32.86214285714286" customWidth="1" bestFit="1"/>
+    <col min="11" max="11" style="26" width="24.290714285714284" customWidth="1" bestFit="1"/>
+    <col min="12" max="12" style="26" width="24.290714285714284" customWidth="1" bestFit="1"/>
+    <col min="13" max="13" style="26" width="24.290714285714284" customWidth="1" bestFit="1"/>
+    <col min="14" max="14" style="26" width="24.290714285714284" customWidth="1" bestFit="1"/>
+    <col min="15" max="15" style="26" width="24.290714285714284" customWidth="1" bestFit="1"/>
+    <col min="16" max="16" style="27" width="24.005" customWidth="1" bestFit="1"/>
+    <col min="17" max="17" style="27" width="13.576428571428572" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="20.25">

</xml_diff>

<commit_message>
updated excel files. removed mistake of error in yield values for brinjal case study
</commit_message>
<xml_diff>
--- a/heliostrome/jip_project/results/Factors to run simulation.xlsx
+++ b/heliostrome/jip_project/results/Factors to run simulation.xlsx
@@ -1,21 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion rupBuild="9303" lowestEdited="5" lastEdited="5" appName="xl"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26731"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://tud365-my.sharepoint.com/personal/sparijs_tudelft_nl/Documents/Documents/helios/heliostrome/heliostrome/jip_project/results/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="6" documentId="11_2F5DD4142FB3D85116A7BFE12EBCB0C89471B905" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C11D5167-5E9E-4A62-AD56-196274C8819C}"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="1"/>
+    <workbookView xWindow="1905" yWindow="900" windowWidth="21390" windowHeight="14580" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet r:id="rId1" sheetId="1" name="Sheet1"/>
-    <sheet r:id="rId2" sheetId="2" name="Bangladesh Case Study"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Bangladesh Case Study" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr fullCalcOnLoad="1"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="63">
   <si>
     <t>Solar pump irrigation system for green agriculture</t>
   </si>
@@ -105,12 +111,6 @@
   </si>
   <si>
     <t>Yield (t/ha)</t>
-  </si>
-  <si>
-    <t>26.49-43.86</t>
-  </si>
-  <si>
-    <t>26.71-38.60</t>
   </si>
   <si>
     <t>Water used (mm)</t>
@@ -215,8 +215,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
-  <numFmts count="0"/>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -253,7 +252,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFffffff"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Courier New"/>
       <family val="2"/>
     </font>
@@ -271,7 +270,7 @@
     </font>
     <font>
       <sz val="10"/>
-      <color rgb="FF34a853"/>
+      <color rgb="FF34A853"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -285,22 +284,22 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFffffff"/>
+        <fgColor rgb="FFFFFFFF"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF34a853"/>
+        <fgColor rgb="FF34A853"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFff6d01"/>
+        <fgColor rgb="FFFF6D01"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFea4335"/>
+        <fgColor rgb="FFEA4335"/>
       </patternFill>
     </fill>
   </fills>
@@ -336,31 +335,31 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FFc6c6c6"/>
+        <color rgb="FFC6C6C6"/>
       </left>
       <right style="thin">
         <color rgb="FF000000"/>
       </right>
       <top style="thin">
-        <color rgb="FFc6c6c6"/>
+        <color rgb="FFC6C6C6"/>
       </top>
       <bottom style="thin">
-        <color rgb="FFc6c6c6"/>
+        <color rgb="FFC6C6C6"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color rgb="FFc6c6c6"/>
+        <color rgb="FFC6C6C6"/>
       </left>
       <right style="thin">
-        <color rgb="FFc6c6c6"/>
+        <color rgb="FFC6C6C6"/>
       </right>
       <top style="thin">
-        <color rgb="FFc6c6c6"/>
+        <color rgb="FFC6C6C6"/>
       </top>
       <bottom style="thin">
-        <color rgb="FFc6c6c6"/>
+        <color rgb="FFC6C6C6"/>
       </bottom>
       <diagonal/>
     </border>
@@ -368,125 +367,116 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+  <cellXfs count="35">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="14" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="14" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="4" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf xfId="0" numFmtId="14" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="4" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="4" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="3" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="4" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="4" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="4" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="14" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="4" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf xfId="0" numFmtId="14" applyNumberFormat="1" borderId="3" applyBorder="1" fontId="4" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf xfId="0" numFmtId="14" applyNumberFormat="1" borderId="4" applyBorder="1" fontId="4" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="4" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="4" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="14" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="14" fontId="4" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="14" fontId="4" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="3" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="3" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="4" applyBorder="1" fontId="4" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="4" fontId="4" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="3" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="5" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf xfId="0" numFmtId="14" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="6" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="7" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
-    </xf>
-    <xf xfId="0" numFmtId="14" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
-    </xf>
-    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="4" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="4" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="3" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="14" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="3" fontId="7" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="4" applyBorder="1" fontId="4" applyFont="1" fillId="3" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="4" applyBorder="1" fontId="4" applyFont="1" fillId="4" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="4" applyBorder="1" fontId="4" applyFont="1" fillId="5" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="4" applyBorder="1" fontId="8" applyFont="1" fillId="3" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="4" applyBorder="1" fontId="4" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" builtinId="0" name="Normal"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
-    <ext uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14ac:slicerStyles xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" defaultSlicerStyle="SlicerStyleLight1"/>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -497,10 +487,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr lastClr="000000" val="windowText"/>
+        <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr lastClr="FFFFFF" val="window"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="000000"/>
@@ -538,71 +528,71 @@
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
-        <a:font typeface="맑은 고딕" script="Hang"/>
-        <a:font typeface="宋体" script="Hans"/>
-        <a:font typeface="新細明體" script="Hant"/>
-        <a:font typeface="Times New Roman" script="Arab"/>
-        <a:font typeface="Times New Roman" script="Hebr"/>
-        <a:font typeface="Tahoma" script="Thai"/>
-        <a:font typeface="Nyala" script="Ethi"/>
-        <a:font typeface="Vrinda" script="Beng"/>
-        <a:font typeface="Shruti" script="Gujr"/>
-        <a:font typeface="MoolBoran" script="Khmr"/>
-        <a:font typeface="Tunga" script="Knda"/>
-        <a:font typeface="Raavi" script="Guru"/>
-        <a:font typeface="Euphemia" script="Cans"/>
-        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
-        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
-        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
-        <a:font typeface="MV Boli" script="Thaa"/>
-        <a:font typeface="Mangal" script="Deva"/>
-        <a:font typeface="Gautami" script="Telu"/>
-        <a:font typeface="Latha" script="Taml"/>
-        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
-        <a:font typeface="Kalinga" script="Orya"/>
-        <a:font typeface="Kartika" script="Mlym"/>
-        <a:font typeface="DokChampa" script="Laoo"/>
-        <a:font typeface="Iskoola Pota" script="Sinh"/>
-        <a:font typeface="Mongolian Baiti" script="Mong"/>
-        <a:font typeface="Times New Roman" script="Viet"/>
-        <a:font typeface="Microsoft Uighur" script="Uigh"/>
-        <a:font typeface="Sylfaen" script="Geor"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
-        <a:font typeface="맑은 고딕" script="Hang"/>
-        <a:font typeface="宋体" script="Hans"/>
-        <a:font typeface="新細明體" script="Hant"/>
-        <a:font typeface="Arial" script="Arab"/>
-        <a:font typeface="Arial" script="Hebr"/>
-        <a:font typeface="Tahoma" script="Thai"/>
-        <a:font typeface="Nyala" script="Ethi"/>
-        <a:font typeface="Vrinda" script="Beng"/>
-        <a:font typeface="Shruti" script="Gujr"/>
-        <a:font typeface="DaunPenh" script="Khmr"/>
-        <a:font typeface="Tunga" script="Knda"/>
-        <a:font typeface="Raavi" script="Guru"/>
-        <a:font typeface="Euphemia" script="Cans"/>
-        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
-        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
-        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
-        <a:font typeface="MV Boli" script="Thaa"/>
-        <a:font typeface="Mangal" script="Deva"/>
-        <a:font typeface="Gautami" script="Telu"/>
-        <a:font typeface="Latha" script="Taml"/>
-        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
-        <a:font typeface="Kalinga" script="Orya"/>
-        <a:font typeface="Kartika" script="Mlym"/>
-        <a:font typeface="DokChampa" script="Laoo"/>
-        <a:font typeface="Iskoola Pota" script="Sinh"/>
-        <a:font typeface="Mongolian Baiti" script="Mong"/>
-        <a:font typeface="Arial" script="Viet"/>
-        <a:font typeface="Microsoft Uighur" script="Uigh"/>
-        <a:font typeface="Sylfaen" script="Geor"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -630,7 +620,7 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin scaled="1" ang="16200000"/>
+          <a:lin ang="16200000" scaled="1"/>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
@@ -653,11 +643,11 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin scaled="1" ang="16200000"/>
+          <a:lin ang="16200000" scaled="1"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln algn="ctr" cmpd="sng" cap="flat" w="9525">
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr">
               <a:shade val="9500"/>
@@ -666,13 +656,13 @@
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln algn="ctr" cmpd="sng" cap="flat" w="25400">
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln algn="ctr" cmpd="sng" cap="flat" w="38100">
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -682,7 +672,7 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="38000"/>
               </a:srgbClr>
@@ -691,7 +681,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -700,7 +690,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -708,10 +698,10 @@
           </a:effectLst>
           <a:scene3d>
             <a:camera prst="orthographicFront">
-              <a:rot rev="0" lon="0" lat="0"/>
+              <a:rot lat="0" lon="0" rev="0"/>
             </a:camera>
-            <a:lightRig dir="t" rig="threePt">
-              <a:rot rev="1200000" lon="0" lat="0"/>
+            <a:lightRig rig="threePt" dir="t">
+              <a:rot lat="0" lon="0" rev="1200000"/>
             </a:lightRig>
           </a:scene3d>
           <a:sp3d>
@@ -776,190 +766,173 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
   <dimension ref="A1:G14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane state="frozen" activePane="topRight" topLeftCell="B1" ySplit="0" xSplit="1"/>
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="36" width="14.719285714285713" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="23" width="19.433571428571426" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="23" width="21.433571428571426" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="36" width="17.005" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="23" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="23" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="7" max="7" style="23" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" width="14.7109375" style="26" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17" style="26" bestFit="1" customWidth="1"/>
+    <col min="5" max="7" width="13.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
-      <c r="A1" s="28"/>
-      <c r="B1" s="29" t="s">
+    <row r="1" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B1" s="27" t="s">
+        <v>45</v>
+      </c>
+      <c r="C1" s="27" t="s">
+        <v>46</v>
+      </c>
+      <c r="D1" s="28" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" s="27" t="s">
         <v>47</v>
       </c>
-      <c r="C1" s="29" t="s">
+      <c r="F1" s="27" t="s">
         <v>48</v>
       </c>
-      <c r="D1" s="30" t="s">
-        <v>0</v>
-      </c>
-      <c r="E1" s="29" t="s">
+      <c r="G1" s="28" t="s">
         <v>49</v>
       </c>
-      <c r="F1" s="29" t="s">
+    </row>
+    <row r="2" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="27" t="s">
         <v>50</v>
       </c>
-      <c r="G1" s="30" t="s">
+      <c r="B2" s="29"/>
+      <c r="C2" s="29"/>
+      <c r="D2" s="29"/>
+      <c r="E2" s="29"/>
+      <c r="F2" s="30"/>
+      <c r="G2" s="31"/>
+    </row>
+    <row r="3" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="27" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75">
-      <c r="A2" s="29" t="s">
+      <c r="B3" s="29"/>
+      <c r="C3" s="30"/>
+      <c r="D3" s="29"/>
+      <c r="E3" s="30"/>
+      <c r="F3" s="29"/>
+      <c r="G3" s="29"/>
+    </row>
+    <row r="4" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="27" t="s">
         <v>52</v>
       </c>
-      <c r="B2" s="31"/>
-      <c r="C2" s="31"/>
-      <c r="D2" s="31"/>
-      <c r="E2" s="31"/>
-      <c r="F2" s="32"/>
-      <c r="G2" s="33"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18.75">
-      <c r="A3" s="29" t="s">
+      <c r="B4" s="30"/>
+      <c r="C4" s="32"/>
+      <c r="D4" s="29"/>
+      <c r="E4" s="29"/>
+      <c r="F4" s="29"/>
+      <c r="G4" s="30"/>
+    </row>
+    <row r="5" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="27" t="s">
         <v>53</v>
       </c>
-      <c r="B3" s="31"/>
-      <c r="C3" s="32"/>
-      <c r="D3" s="31"/>
-      <c r="E3" s="32"/>
-      <c r="F3" s="31"/>
-      <c r="G3" s="31"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18.75">
-      <c r="A4" s="29" t="s">
+      <c r="B5" s="30"/>
+      <c r="C5" s="31"/>
+      <c r="D5" s="29"/>
+      <c r="E5" s="29"/>
+      <c r="F5" s="31"/>
+      <c r="G5" s="29"/>
+    </row>
+    <row r="6" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="27" t="s">
         <v>54</v>
       </c>
-      <c r="B4" s="32"/>
-      <c r="C4" s="34"/>
-      <c r="D4" s="31"/>
-      <c r="E4" s="31"/>
-      <c r="F4" s="31"/>
-      <c r="G4" s="32"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18.75">
-      <c r="A5" s="29" t="s">
+      <c r="B6" s="30"/>
+      <c r="C6" s="31"/>
+      <c r="D6" s="29"/>
+      <c r="E6" s="29"/>
+      <c r="F6" s="29"/>
+      <c r="G6" s="30"/>
+    </row>
+    <row r="7" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="27" t="s">
         <v>55</v>
       </c>
-      <c r="B5" s="32"/>
-      <c r="C5" s="33"/>
-      <c r="D5" s="31"/>
-      <c r="E5" s="31"/>
-      <c r="F5" s="33"/>
-      <c r="G5" s="31"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18.75">
-      <c r="A6" s="29" t="s">
+      <c r="B7" s="29"/>
+      <c r="C7" s="29"/>
+      <c r="D7" s="29"/>
+      <c r="E7" s="31"/>
+      <c r="F7" s="29"/>
+      <c r="G7" s="29"/>
+    </row>
+    <row r="8" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="27" t="s">
         <v>56</v>
       </c>
-      <c r="B6" s="32"/>
-      <c r="C6" s="33"/>
-      <c r="D6" s="31"/>
-      <c r="E6" s="31"/>
-      <c r="F6" s="31"/>
-      <c r="G6" s="32"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="18.75">
-      <c r="A7" s="29" t="s">
+      <c r="B8" s="29"/>
+      <c r="C8" s="30"/>
+      <c r="D8" s="29"/>
+      <c r="E8" s="31"/>
+      <c r="F8" s="30"/>
+      <c r="G8" s="30"/>
+    </row>
+    <row r="9" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="27" t="s">
         <v>57</v>
       </c>
-      <c r="B7" s="31"/>
-      <c r="C7" s="31"/>
-      <c r="D7" s="31"/>
-      <c r="E7" s="33"/>
-      <c r="F7" s="31"/>
-      <c r="G7" s="31"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="18.75">
-      <c r="A8" s="29" t="s">
+      <c r="B9" s="30"/>
+      <c r="C9" s="30"/>
+      <c r="D9" s="29"/>
+      <c r="E9" s="31"/>
+      <c r="F9" s="29"/>
+      <c r="G9" s="30"/>
+    </row>
+    <row r="10" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="27" t="s">
         <v>58</v>
       </c>
-      <c r="B8" s="31"/>
-      <c r="C8" s="32"/>
-      <c r="D8" s="31"/>
-      <c r="E8" s="33"/>
-      <c r="F8" s="32"/>
-      <c r="G8" s="32"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="18.75">
-      <c r="A9" s="29" t="s">
+      <c r="B10" s="29"/>
+      <c r="C10" s="29"/>
+      <c r="D10" s="29"/>
+      <c r="E10" s="31"/>
+      <c r="F10" s="29"/>
+      <c r="G10" s="29"/>
+    </row>
+    <row r="11" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="27" t="s">
         <v>59</v>
       </c>
-      <c r="B9" s="32"/>
-      <c r="C9" s="32"/>
-      <c r="D9" s="31"/>
-      <c r="E9" s="33"/>
-      <c r="F9" s="31"/>
-      <c r="G9" s="32"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="18.75">
-      <c r="A10" s="29" t="s">
+      <c r="B11" s="29"/>
+      <c r="C11" s="30"/>
+      <c r="D11" s="29"/>
+      <c r="E11" s="31"/>
+      <c r="F11" s="31"/>
+      <c r="G11" s="29"/>
+    </row>
+    <row r="12" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="27" t="s">
         <v>60</v>
       </c>
-      <c r="B10" s="31"/>
-      <c r="C10" s="31"/>
-      <c r="D10" s="31"/>
-      <c r="E10" s="33"/>
-      <c r="F10" s="31"/>
-      <c r="G10" s="31"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="18.75">
-      <c r="A11" s="29" t="s">
+      <c r="D12" s="33"/>
+    </row>
+    <row r="13" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="27" t="s">
         <v>61</v>
       </c>
-      <c r="B11" s="31"/>
-      <c r="C11" s="32"/>
-      <c r="D11" s="31"/>
-      <c r="E11" s="33"/>
-      <c r="F11" s="33"/>
-      <c r="G11" s="31"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="18.75">
-      <c r="A12" s="29" t="s">
+      <c r="D13" s="33"/>
+    </row>
+    <row r="14" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="27" t="s">
         <v>62</v>
       </c>
-      <c r="B12" s="18"/>
-      <c r="C12" s="18"/>
-      <c r="D12" s="35"/>
-      <c r="E12" s="18"/>
-      <c r="F12" s="18"/>
-      <c r="G12" s="18"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="18.75">
-      <c r="A13" s="29" t="s">
-        <v>63</v>
-      </c>
-      <c r="B13" s="18"/>
-      <c r="C13" s="18"/>
-      <c r="D13" s="35"/>
-      <c r="E13" s="18"/>
-      <c r="F13" s="18"/>
-      <c r="G13" s="18"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="18.75">
-      <c r="A14" s="29" t="s">
-        <v>64</v>
-      </c>
-      <c r="B14" s="18"/>
-      <c r="C14" s="18"/>
-      <c r="D14" s="35"/>
-      <c r="E14" s="18"/>
-      <c r="F14" s="18"/>
-      <c r="G14" s="18"/>
+      <c r="D14" s="33"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -967,38 +940,35 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
   <dimension ref="A1:Q27"/>
   <sheetViews>
-    <sheetView workbookViewId="0" tabSelected="1">
-      <pane state="frozen" activePane="topRight" topLeftCell="B1" ySplit="0" xSplit="1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="K1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="N25" sqref="N25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="23" width="44.005" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="24" width="30.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="25" width="30.433571428571426" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="25" width="30.005" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="25" width="28.719285714285714" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="25" width="31.005" customWidth="1" bestFit="1"/>
-    <col min="7" max="7" style="25" width="29.290714285714284" customWidth="1" bestFit="1"/>
-    <col min="8" max="8" style="25" width="31.433571428571426" customWidth="1" bestFit="1"/>
-    <col min="9" max="9" style="26" width="31.433571428571426" customWidth="1" bestFit="1"/>
-    <col min="10" max="10" style="26" width="32.86214285714286" customWidth="1" bestFit="1"/>
-    <col min="11" max="11" style="26" width="24.290714285714284" customWidth="1" bestFit="1"/>
-    <col min="12" max="12" style="26" width="24.290714285714284" customWidth="1" bestFit="1"/>
-    <col min="13" max="13" style="26" width="24.290714285714284" customWidth="1" bestFit="1"/>
-    <col min="14" max="14" style="26" width="24.290714285714284" customWidth="1" bestFit="1"/>
-    <col min="15" max="15" style="26" width="24.290714285714284" customWidth="1" bestFit="1"/>
-    <col min="16" max="16" style="27" width="24.005" customWidth="1" bestFit="1"/>
-    <col min="17" max="17" style="27" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" width="44" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="30.5703125" style="22" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="30.42578125" style="23" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="30" style="23" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="28.7109375" style="23" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="31" style="23" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="29.28515625" style="23" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="31.42578125" style="23" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="31.42578125" style="24" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="32.85546875" style="24" bestFit="1" customWidth="1"/>
+    <col min="11" max="15" width="24.28515625" style="24" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="24" style="25" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="13.5703125" style="25" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="20.25">
+    <row r="1" spans="1:17" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
       <c r="B1" s="2" t="s">
         <v>0</v>
@@ -1019,7 +989,7 @@
       <c r="P1" s="5"/>
       <c r="Q1" s="5"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75">
+    <row r="2" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>1</v>
       </c>
@@ -1072,113 +1042,113 @@
         <v>14</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18.75">
+    <row r="3" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
         <v>15</v>
       </c>
       <c r="B3" s="10">
-        <v>90.4125</v>
+        <v>90.412499999999994</v>
       </c>
       <c r="C3" s="10">
-        <v>90.4125</v>
+        <v>90.412499999999994</v>
       </c>
       <c r="D3" s="10">
-        <v>90.4125</v>
+        <v>90.412499999999994</v>
       </c>
       <c r="E3" s="10">
-        <v>90.4125</v>
+        <v>90.412499999999994</v>
       </c>
       <c r="F3" s="10">
-        <v>90.4125</v>
+        <v>90.412499999999994</v>
       </c>
       <c r="G3" s="10">
-        <v>90.4125</v>
+        <v>90.412499999999994</v>
       </c>
       <c r="H3" s="10">
-        <v>90.4125</v>
+        <v>90.412499999999994</v>
       </c>
       <c r="I3" s="11">
-        <v>89.941109</v>
+        <v>89.941108999999997</v>
       </c>
       <c r="J3" s="11">
-        <v>89.941109</v>
+        <v>89.941108999999997</v>
       </c>
       <c r="K3" s="11">
-        <v>89.941109</v>
+        <v>89.941108999999997</v>
       </c>
       <c r="L3" s="11">
-        <v>89.941109</v>
+        <v>89.941108999999997</v>
       </c>
       <c r="M3" s="11">
-        <v>89.941109</v>
+        <v>89.941108999999997</v>
       </c>
       <c r="N3" s="11">
-        <v>89.941109</v>
+        <v>89.941108999999997</v>
       </c>
       <c r="O3" s="10">
-        <v>90.4125</v>
+        <v>90.412499999999994</v>
       </c>
       <c r="P3" s="11">
-        <v>89.421135</v>
+        <v>89.421135000000007</v>
       </c>
       <c r="Q3" s="11">
-        <v>90.3701305555555</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18.75">
+        <v>90.370130555555505</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
         <v>16</v>
       </c>
       <c r="B4" s="10">
-        <v>24.0958</v>
+        <v>24.095800000000001</v>
       </c>
       <c r="C4" s="10">
-        <v>24.0958</v>
+        <v>24.095800000000001</v>
       </c>
       <c r="D4" s="10">
-        <v>24.0958</v>
+        <v>24.095800000000001</v>
       </c>
       <c r="E4" s="10">
-        <v>24.0958</v>
+        <v>24.095800000000001</v>
       </c>
       <c r="F4" s="10">
-        <v>24.0958</v>
+        <v>24.095800000000001</v>
       </c>
       <c r="G4" s="10">
-        <v>24.0958</v>
+        <v>24.095800000000001</v>
       </c>
       <c r="H4" s="10">
-        <v>24.0958</v>
+        <v>24.095800000000001</v>
       </c>
       <c r="I4" s="11">
-        <v>24.91625</v>
+        <v>24.916250000000002</v>
       </c>
       <c r="J4" s="11">
-        <v>24.91625</v>
+        <v>24.916250000000002</v>
       </c>
       <c r="K4" s="11">
-        <v>24.91625</v>
+        <v>24.916250000000002</v>
       </c>
       <c r="L4" s="11">
-        <v>24.91625</v>
+        <v>24.916250000000002</v>
       </c>
       <c r="M4" s="11">
-        <v>24.91625</v>
+        <v>24.916250000000002</v>
       </c>
       <c r="N4" s="11">
-        <v>24.91625</v>
+        <v>24.916250000000002</v>
       </c>
       <c r="O4" s="10">
-        <v>24.0958</v>
+        <v>24.095800000000001</v>
       </c>
       <c r="P4" s="11">
         <v>23.490938</v>
       </c>
       <c r="Q4" s="11">
-        <v>22.7049694444444</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18.75">
+        <v>22.704969444444401</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
         <v>17</v>
       </c>
@@ -1231,7 +1201,7 @@
         <v>40179</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18.75">
+    <row r="6" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
         <v>18</v>
       </c>
@@ -1284,7 +1254,7 @@
         <v>41639</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="18.75">
+    <row r="7" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
         <v>19</v>
       </c>
@@ -1337,7 +1307,7 @@
         <v>38387</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="18.75">
+    <row r="8" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
         <v>20</v>
       </c>
@@ -1390,7 +1360,7 @@
         <v>22</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="18.75">
+    <row r="9" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
         <v>23</v>
       </c>
@@ -1443,7 +1413,7 @@
         <v>100</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="18.75">
+    <row r="10" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
         <v>24</v>
       </c>
@@ -1496,7 +1466,7 @@
         <v>41</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="18.75">
+    <row r="11" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
         <v>25</v>
       </c>
@@ -1549,7 +1519,7 @@
         <v>28</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="18.75">
+    <row r="12" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
         <v>29</v>
       </c>
@@ -1557,7 +1527,7 @@
         <v>31.86</v>
       </c>
       <c r="C12" s="10">
-        <v>33.73</v>
+        <v>33.729999999999997</v>
       </c>
       <c r="D12" s="10">
         <v>35.28</v>
@@ -1586,11 +1556,11 @@
       <c r="L12" s="11">
         <v>25.82</v>
       </c>
-      <c r="M12" s="12" t="s">
-        <v>30</v>
-      </c>
-      <c r="N12" s="12" t="s">
-        <v>31</v>
+      <c r="M12" s="34">
+        <v>35.174999999999997</v>
+      </c>
+      <c r="N12" s="34">
+        <v>32.655000000000001</v>
       </c>
       <c r="O12" s="16">
         <v>3</v>
@@ -1602,9 +1572,9 @@
         <v>3.4</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="18.75">
+    <row r="13" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B13" s="15">
         <v>429</v>
@@ -1640,10 +1610,10 @@
         <v>453</v>
       </c>
       <c r="M13" s="12" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="N13" s="12" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="O13" s="16">
         <v>430</v>
@@ -1655,15 +1625,14 @@
         <v>1252</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="18.75">
-      <c r="A14" s="18"/>
-      <c r="B14" s="19"/>
-      <c r="C14" s="19"/>
-      <c r="D14" s="19"/>
-      <c r="E14" s="19"/>
-      <c r="F14" s="19"/>
-      <c r="G14" s="19"/>
-      <c r="H14" s="19"/>
+    <row r="14" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B14" s="18"/>
+      <c r="C14" s="18"/>
+      <c r="D14" s="18"/>
+      <c r="E14" s="18"/>
+      <c r="F14" s="18"/>
+      <c r="G14" s="18"/>
+      <c r="H14" s="18"/>
       <c r="I14" s="4"/>
       <c r="J14" s="4"/>
       <c r="K14" s="4"/>
@@ -1674,7 +1643,7 @@
       <c r="P14" s="5"/>
       <c r="Q14" s="5"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="18.75">
+    <row r="15" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="6" t="s">
         <v>17</v>
       </c>
@@ -1727,7 +1696,7 @@
         <v>40544</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="18.75">
+    <row r="16" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="6" t="s">
         <v>18</v>
       </c>
@@ -1780,51 +1749,51 @@
         <v>41639</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="18.75">
+    <row r="17" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="6" t="s">
         <v>23</v>
       </c>
       <c r="B17" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="C17" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="D17" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="E17" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="F17" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="G17" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="H17" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="I17" s="12" t="s">
         <v>35</v>
       </c>
-      <c r="C17" s="15" t="s">
+      <c r="J17" s="12" t="s">
         <v>36</v>
       </c>
-      <c r="D17" s="15" t="s">
-        <v>36</v>
-      </c>
-      <c r="E17" s="15" t="s">
-        <v>36</v>
-      </c>
-      <c r="F17" s="15" t="s">
-        <v>35</v>
-      </c>
-      <c r="G17" s="15" t="s">
-        <v>36</v>
-      </c>
-      <c r="H17" s="15" t="s">
-        <v>35</v>
-      </c>
-      <c r="I17" s="12" t="s">
+      <c r="K17" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="J17" s="12" t="s">
+      <c r="L17" s="12" t="s">
         <v>38</v>
       </c>
-      <c r="K17" s="12" t="s">
+      <c r="M17" s="12" t="s">
         <v>39</v>
       </c>
-      <c r="L17" s="12" t="s">
+      <c r="N17" s="12" t="s">
         <v>40</v>
       </c>
-      <c r="M17" s="12" t="s">
+      <c r="O17" s="12" t="s">
         <v>41</v>
-      </c>
-      <c r="N17" s="12" t="s">
-        <v>42</v>
-      </c>
-      <c r="O17" s="12" t="s">
-        <v>43</v>
       </c>
       <c r="P17" s="17">
         <v>100</v>
@@ -1833,7 +1802,7 @@
         <v>100</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="18.75">
+    <row r="18" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="6" t="s">
         <v>24</v>
       </c>
@@ -1859,40 +1828,39 @@
         <v>26</v>
       </c>
       <c r="I18" s="12" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="J18" s="12" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="K18" s="12"/>
       <c r="L18" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="M18" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="N18" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="O18" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="P18" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="Q18" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="M18" s="12" t="s">
-        <v>44</v>
-      </c>
-      <c r="N18" s="12" t="s">
-        <v>44</v>
-      </c>
-      <c r="O18" s="12" t="s">
-        <v>44</v>
-      </c>
-      <c r="P18" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="Q18" s="10" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="18.75">
-      <c r="A19" s="18"/>
-      <c r="B19" s="19"/>
-      <c r="C19" s="19"/>
-      <c r="D19" s="19"/>
-      <c r="E19" s="19"/>
-      <c r="F19" s="19"/>
-      <c r="G19" s="19"/>
-      <c r="H19" s="19"/>
+    </row>
+    <row r="19" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B19" s="18"/>
+      <c r="C19" s="18"/>
+      <c r="D19" s="18"/>
+      <c r="E19" s="18"/>
+      <c r="F19" s="18"/>
+      <c r="G19" s="18"/>
+      <c r="H19" s="18"/>
       <c r="I19" s="4"/>
       <c r="J19" s="4"/>
       <c r="K19" s="4"/>
@@ -1903,15 +1871,14 @@
       <c r="P19" s="5"/>
       <c r="Q19" s="5"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="15.75">
-      <c r="A20" s="18"/>
-      <c r="B20" s="20"/>
-      <c r="C20" s="19"/>
-      <c r="D20" s="19"/>
-      <c r="E20" s="19"/>
-      <c r="F20" s="19"/>
-      <c r="G20" s="19"/>
-      <c r="H20" s="19"/>
+    <row r="20" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B20" s="19"/>
+      <c r="C20" s="18"/>
+      <c r="D20" s="18"/>
+      <c r="E20" s="18"/>
+      <c r="F20" s="18"/>
+      <c r="G20" s="18"/>
+      <c r="H20" s="18"/>
       <c r="I20" s="4"/>
       <c r="J20" s="4"/>
       <c r="K20" s="4"/>
@@ -1922,15 +1889,14 @@
       <c r="P20" s="5"/>
       <c r="Q20" s="5"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="18.75">
-      <c r="A21" s="18"/>
-      <c r="B21" s="19"/>
-      <c r="C21" s="19"/>
-      <c r="D21" s="19"/>
-      <c r="E21" s="19"/>
-      <c r="F21" s="19"/>
-      <c r="G21" s="19"/>
-      <c r="H21" s="19"/>
+    <row r="21" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B21" s="18"/>
+      <c r="C21" s="18"/>
+      <c r="D21" s="18"/>
+      <c r="E21" s="18"/>
+      <c r="F21" s="18"/>
+      <c r="G21" s="18"/>
+      <c r="H21" s="18"/>
       <c r="I21" s="4"/>
       <c r="J21" s="4"/>
       <c r="K21" s="4"/>
@@ -1941,15 +1907,14 @@
       <c r="P21" s="5"/>
       <c r="Q21" s="5"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="18.75">
-      <c r="A22" s="18"/>
-      <c r="B22" s="19"/>
-      <c r="C22" s="19"/>
-      <c r="D22" s="19"/>
-      <c r="E22" s="19"/>
-      <c r="F22" s="19"/>
-      <c r="G22" s="19"/>
-      <c r="H22" s="19"/>
+    <row r="22" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B22" s="18"/>
+      <c r="C22" s="18"/>
+      <c r="D22" s="18"/>
+      <c r="E22" s="18"/>
+      <c r="F22" s="18"/>
+      <c r="G22" s="18"/>
+      <c r="H22" s="18"/>
       <c r="I22" s="4"/>
       <c r="J22" s="4"/>
       <c r="K22" s="4"/>
@@ -1960,15 +1925,14 @@
       <c r="P22" s="5"/>
       <c r="Q22" s="5"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="18.75">
-      <c r="A23" s="18"/>
-      <c r="B23" s="19"/>
-      <c r="C23" s="19"/>
-      <c r="D23" s="19"/>
-      <c r="E23" s="19"/>
-      <c r="F23" s="19"/>
-      <c r="G23" s="19"/>
-      <c r="H23" s="19"/>
+    <row r="23" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B23" s="18"/>
+      <c r="C23" s="18"/>
+      <c r="D23" s="18"/>
+      <c r="E23" s="18"/>
+      <c r="F23" s="18"/>
+      <c r="G23" s="18"/>
+      <c r="H23" s="18"/>
       <c r="I23" s="4"/>
       <c r="J23" s="4"/>
       <c r="K23" s="4"/>
@@ -1979,15 +1943,14 @@
       <c r="P23" s="5"/>
       <c r="Q23" s="5"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="18.75">
-      <c r="A24" s="18"/>
-      <c r="B24" s="19"/>
-      <c r="C24" s="19"/>
-      <c r="D24" s="19"/>
-      <c r="E24" s="19"/>
-      <c r="F24" s="19"/>
-      <c r="G24" s="19"/>
-      <c r="H24" s="19"/>
+    <row r="24" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B24" s="18"/>
+      <c r="C24" s="18"/>
+      <c r="D24" s="18"/>
+      <c r="E24" s="18"/>
+      <c r="F24" s="18"/>
+      <c r="G24" s="18"/>
+      <c r="H24" s="18"/>
       <c r="I24" s="4"/>
       <c r="J24" s="4"/>
       <c r="K24" s="4"/>
@@ -1998,15 +1961,14 @@
       <c r="P24" s="5"/>
       <c r="Q24" s="5"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="18.75">
-      <c r="A25" s="18"/>
-      <c r="B25" s="19"/>
-      <c r="C25" s="19"/>
-      <c r="D25" s="19"/>
-      <c r="E25" s="19"/>
-      <c r="F25" s="19"/>
-      <c r="G25" s="19"/>
-      <c r="H25" s="19"/>
+    <row r="25" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B25" s="18"/>
+      <c r="C25" s="18"/>
+      <c r="D25" s="18"/>
+      <c r="E25" s="18"/>
+      <c r="F25" s="18"/>
+      <c r="G25" s="18"/>
+      <c r="H25" s="18"/>
       <c r="I25" s="4"/>
       <c r="J25" s="4"/>
       <c r="K25" s="4"/>
@@ -2017,15 +1979,14 @@
       <c r="P25" s="5"/>
       <c r="Q25" s="5"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="26" customHeight="1" ht="15.75">
-      <c r="A26" s="18"/>
-      <c r="B26" s="21"/>
-      <c r="C26" s="19"/>
-      <c r="D26" s="19"/>
-      <c r="E26" s="19"/>
-      <c r="F26" s="19"/>
-      <c r="G26" s="19"/>
-      <c r="H26" s="19"/>
+    <row r="26" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B26" s="20"/>
+      <c r="C26" s="18"/>
+      <c r="D26" s="18"/>
+      <c r="E26" s="18"/>
+      <c r="F26" s="18"/>
+      <c r="G26" s="18"/>
+      <c r="H26" s="18"/>
       <c r="I26" s="4"/>
       <c r="J26" s="4"/>
       <c r="K26" s="4"/>
@@ -2036,15 +1997,14 @@
       <c r="P26" s="5"/>
       <c r="Q26" s="5"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="27" customHeight="1" ht="15.75">
-      <c r="A27" s="18"/>
-      <c r="B27" s="22"/>
-      <c r="C27" s="19"/>
-      <c r="D27" s="19"/>
-      <c r="E27" s="19"/>
-      <c r="F27" s="19"/>
-      <c r="G27" s="19"/>
-      <c r="H27" s="19"/>
+    <row r="27" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B27" s="21"/>
+      <c r="C27" s="18"/>
+      <c r="D27" s="18"/>
+      <c r="E27" s="18"/>
+      <c r="F27" s="18"/>
+      <c r="G27" s="18"/>
+      <c r="H27" s="18"/>
       <c r="I27" s="4"/>
       <c r="J27" s="4"/>
       <c r="K27" s="4"/>

</xml_diff>

<commit_message>
problem with the excel dates formatted wrong. Has been force fixed. Correct format in excel = Short date!!. for future problem
</commit_message>
<xml_diff>
--- a/heliostrome/jip_project/results/Factors to run simulation.xlsx
+++ b/heliostrome/jip_project/results/Factors to run simulation.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://tud365-my.sharepoint.com/personal/sparijs_tudelft_nl/Documents/Documents/helios/heliostrome/heliostrome/jip_project/results/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="32" documentId="11_D32365DB1BF81EFE359F33EE7A0E21B336E84D7E" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{63B92688-6D63-4594-B657-6E3FFD31855C}"/>
+  <xr:revisionPtr revIDLastSave="51" documentId="11_D32365DB1BF81EFE359F33EE7A0E21B336E84D7E" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3F74CFFE-D5C9-4C08-899F-6715B9EF57AA}"/>
   <bookViews>
-    <workbookView xWindow="6030" yWindow="900" windowWidth="21390" windowHeight="14580" firstSheet="2" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="All Case Studies (compatability" sheetId="1" r:id="rId1"/>
@@ -1192,7 +1192,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="302" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="294" uniqueCount="135">
   <si>
     <t>Lowering the cost - MIT</t>
   </si>
@@ -1312,15 +1312,6 @@
   </si>
   <si>
     <t>26/06/2012</t>
-  </si>
-  <si>
-    <t>17/11/2012</t>
-  </si>
-  <si>
-    <t>23/11/2005</t>
-  </si>
-  <si>
-    <t>29/01/2005</t>
   </si>
   <si>
     <t>Soil Type</t>
@@ -1565,6 +1556,48 @@
   </si>
   <si>
     <t>Mulches</t>
+  </si>
+  <si>
+    <t>26/06/2013</t>
+  </si>
+  <si>
+    <t>26/06/2014</t>
+  </si>
+  <si>
+    <t>26/06/2015</t>
+  </si>
+  <si>
+    <t>26/06/2016</t>
+  </si>
+  <si>
+    <t>26/06/2017</t>
+  </si>
+  <si>
+    <t>26/06/2018</t>
+  </si>
+  <si>
+    <t>26/06/2019</t>
+  </si>
+  <si>
+    <t>26/06/2020</t>
+  </si>
+  <si>
+    <t>26/06/2021</t>
+  </si>
+  <si>
+    <t>26/06/2022</t>
+  </si>
+  <si>
+    <t>26/06/2023</t>
+  </si>
+  <si>
+    <t>26/06/2024</t>
+  </si>
+  <si>
+    <t>26/06/2025</t>
+  </si>
+  <si>
+    <t>26/06/2026</t>
   </si>
 </sst>
 </file>
@@ -1575,7 +1608,7 @@
     <numFmt numFmtId="164" formatCode="mm/dd/yyyy"/>
     <numFmt numFmtId="165" formatCode="m/d/yyyy"/>
   </numFmts>
-  <fonts count="14">
+  <fonts count="15">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -1655,6 +1688,11 @@
       <sz val="10"/>
       <name val="Arial"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <name val="Arial"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="8">
     <fill>
@@ -1700,7 +1738,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="11">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -1757,21 +1795,6 @@
       <top/>
       <bottom style="thin">
         <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFC6C6C6"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFC6C6C6"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFC6C6C6"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1838,7 +1861,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="55">
+  <cellXfs count="52">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1876,22 +1899,10 @@
     <xf numFmtId="164" fontId="6" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="6" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="6" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="165" fontId="6" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="4" fontId="6" fillId="6" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="4" fontId="6" fillId="6" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="4" fontId="6" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1907,7 +1918,7 @@
     <xf numFmtId="164" fontId="6" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1948,8 +1959,8 @@
     <xf numFmtId="4" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="6" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
@@ -1957,11 +1968,14 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="6" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2374,9 +2388,9 @@
   </sheetPr>
   <dimension ref="A1:Q27"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="C2" sqref="C2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="K1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B5" sqref="B5:Q7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1"/>
@@ -2566,56 +2580,56 @@
         <v>22.7</v>
       </c>
     </row>
-    <row r="5" spans="1:17" ht="12.75">
+    <row r="5" spans="1:17" ht="11.25" customHeight="1">
       <c r="A5" s="13" t="s">
         <v>35</v>
       </c>
-      <c r="B5" s="16">
+      <c r="B5" s="51">
         <v>40179</v>
       </c>
-      <c r="C5" s="16">
+      <c r="C5" s="51">
         <v>40179</v>
       </c>
-      <c r="D5" s="16">
+      <c r="D5" s="51">
         <v>40179</v>
       </c>
-      <c r="E5" s="16">
+      <c r="E5" s="51">
         <v>40179</v>
       </c>
-      <c r="F5" s="16">
+      <c r="F5" s="51">
         <v>40179</v>
       </c>
-      <c r="G5" s="16">
+      <c r="G5" s="51">
         <v>40179</v>
       </c>
-      <c r="H5" s="16">
+      <c r="H5" s="51">
         <v>40179</v>
       </c>
-      <c r="I5" s="16">
+      <c r="I5" s="51">
         <v>40179</v>
       </c>
-      <c r="J5" s="16">
+      <c r="J5" s="51">
         <v>40179</v>
       </c>
-      <c r="K5" s="16">
+      <c r="K5" s="51">
         <v>40179</v>
       </c>
-      <c r="L5" s="16">
+      <c r="L5" s="51">
         <v>40179</v>
       </c>
-      <c r="M5" s="16">
+      <c r="M5" s="51">
         <v>40179</v>
       </c>
-      <c r="N5" s="16">
+      <c r="N5" s="51">
         <v>40179</v>
       </c>
-      <c r="O5" s="16">
+      <c r="O5" s="51">
         <v>40179</v>
       </c>
-      <c r="P5" s="16">
+      <c r="P5" s="51">
         <v>40179</v>
       </c>
-      <c r="Q5" s="16">
+      <c r="Q5" s="51">
         <v>40179</v>
       </c>
     </row>
@@ -2623,164 +2637,164 @@
       <c r="A6" s="13" t="s">
         <v>36</v>
       </c>
-      <c r="B6" s="14" t="s">
-        <v>37</v>
-      </c>
-      <c r="C6" s="14" t="s">
-        <v>37</v>
-      </c>
-      <c r="D6" s="14" t="s">
-        <v>37</v>
-      </c>
-      <c r="E6" s="14" t="s">
-        <v>37</v>
-      </c>
-      <c r="F6" s="14" t="s">
-        <v>37</v>
-      </c>
-      <c r="G6" s="14" t="s">
-        <v>37</v>
-      </c>
-      <c r="H6" s="14" t="s">
-        <v>37</v>
-      </c>
-      <c r="I6" s="14" t="s">
-        <v>37</v>
-      </c>
-      <c r="J6" s="14" t="s">
-        <v>37</v>
-      </c>
-      <c r="K6" s="14" t="s">
-        <v>37</v>
-      </c>
-      <c r="L6" s="14" t="s">
-        <v>37</v>
-      </c>
-      <c r="M6" s="14" t="s">
-        <v>37</v>
-      </c>
-      <c r="N6" s="14" t="s">
-        <v>37</v>
-      </c>
-      <c r="O6" s="14" t="s">
-        <v>37</v>
-      </c>
-      <c r="P6" s="14" t="s">
-        <v>37</v>
-      </c>
-      <c r="Q6" s="14" t="s">
-        <v>37</v>
+      <c r="B6" s="51">
+        <v>41639</v>
+      </c>
+      <c r="C6" s="51">
+        <v>41639</v>
+      </c>
+      <c r="D6" s="51">
+        <v>41639</v>
+      </c>
+      <c r="E6" s="51">
+        <v>41639</v>
+      </c>
+      <c r="F6" s="51">
+        <v>41639</v>
+      </c>
+      <c r="G6" s="51">
+        <v>41639</v>
+      </c>
+      <c r="H6" s="51">
+        <v>41639</v>
+      </c>
+      <c r="I6" s="51">
+        <v>41639</v>
+      </c>
+      <c r="J6" s="51">
+        <v>41639</v>
+      </c>
+      <c r="K6" s="51">
+        <v>41639</v>
+      </c>
+      <c r="L6" s="51">
+        <v>41639</v>
+      </c>
+      <c r="M6" s="51">
+        <v>41639</v>
+      </c>
+      <c r="N6" s="51">
+        <v>41639</v>
+      </c>
+      <c r="O6" s="51">
+        <v>41639</v>
+      </c>
+      <c r="P6" s="51">
+        <v>41639</v>
+      </c>
+      <c r="Q6" s="51">
+        <v>41639</v>
       </c>
     </row>
     <row r="7" spans="1:17" ht="12.75">
       <c r="A7" s="13" t="s">
         <v>38</v>
       </c>
-      <c r="B7" s="14" t="s">
+      <c r="B7" s="51" t="s">
         <v>39</v>
       </c>
-      <c r="C7" s="14" t="s">
-        <v>39</v>
-      </c>
-      <c r="D7" s="14" t="s">
-        <v>39</v>
-      </c>
-      <c r="E7" s="16">
-        <v>40645</v>
-      </c>
-      <c r="F7" s="16">
-        <v>40645</v>
-      </c>
-      <c r="G7" s="16">
-        <v>40645</v>
-      </c>
-      <c r="H7" s="16">
-        <v>40645</v>
-      </c>
-      <c r="I7" s="17">
-        <v>40279</v>
-      </c>
-      <c r="J7" s="18">
-        <v>40279</v>
-      </c>
-      <c r="K7" s="19" t="s">
-        <v>40</v>
-      </c>
-      <c r="L7" s="14" t="s">
-        <v>40</v>
-      </c>
-      <c r="M7" s="20">
-        <v>40492</v>
-      </c>
-      <c r="N7" s="20">
-        <v>40492</v>
-      </c>
-      <c r="O7" s="14" t="s">
-        <v>41</v>
-      </c>
-      <c r="P7" s="14" t="s">
-        <v>42</v>
-      </c>
-      <c r="Q7" s="16">
+      <c r="C7" s="51" t="s">
+        <v>121</v>
+      </c>
+      <c r="D7" s="51" t="s">
+        <v>122</v>
+      </c>
+      <c r="E7" s="51" t="s">
+        <v>123</v>
+      </c>
+      <c r="F7" s="51" t="s">
+        <v>124</v>
+      </c>
+      <c r="G7" s="51" t="s">
+        <v>125</v>
+      </c>
+      <c r="H7" s="51" t="s">
+        <v>126</v>
+      </c>
+      <c r="I7" s="51" t="s">
+        <v>127</v>
+      </c>
+      <c r="J7" s="51" t="s">
+        <v>128</v>
+      </c>
+      <c r="K7" s="51" t="s">
+        <v>129</v>
+      </c>
+      <c r="L7" s="51" t="s">
+        <v>130</v>
+      </c>
+      <c r="M7" s="51" t="s">
+        <v>131</v>
+      </c>
+      <c r="N7" s="51" t="s">
+        <v>132</v>
+      </c>
+      <c r="O7" s="51" t="s">
+        <v>133</v>
+      </c>
+      <c r="P7" s="51" t="s">
+        <v>134</v>
+      </c>
+      <c r="Q7" s="51">
         <v>38444</v>
       </c>
     </row>
     <row r="8" spans="1:17" ht="12.75">
       <c r="A8" s="13" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="B8" s="14" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="C8" s="14" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="D8" s="14" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="E8" s="14" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="F8" s="14" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="G8" s="14" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="H8" s="14" t="s">
-        <v>44</v>
-      </c>
-      <c r="I8" s="21" t="s">
-        <v>45</v>
-      </c>
-      <c r="J8" s="21" t="s">
-        <v>45</v>
+        <v>41</v>
+      </c>
+      <c r="I8" s="17" t="s">
+        <v>42</v>
+      </c>
+      <c r="J8" s="17" t="s">
+        <v>42</v>
       </c>
       <c r="K8" s="14" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="L8" s="14" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="M8" s="14" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="N8" s="14" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="O8" s="14" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="P8" s="14" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="Q8" s="14" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
     </row>
     <row r="9" spans="1:17" ht="12.75">
       <c r="A9" s="13" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="B9" s="14">
         <v>35</v>
@@ -2824,16 +2838,16 @@
       <c r="O9" s="15">
         <v>100</v>
       </c>
-      <c r="P9" s="22">
+      <c r="P9" s="18">
         <v>100</v>
       </c>
-      <c r="Q9" s="23">
+      <c r="Q9" s="19">
         <v>100</v>
       </c>
     </row>
     <row r="10" spans="1:17" ht="12.75">
       <c r="A10" s="13" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="B10" s="14">
         <v>26</v>
@@ -2877,7 +2891,7 @@
       <c r="O10" s="15">
         <v>26</v>
       </c>
-      <c r="P10" s="24">
+      <c r="P10" s="20">
         <v>50</v>
       </c>
       <c r="Q10" s="15">
@@ -2886,60 +2900,60 @@
     </row>
     <row r="11" spans="1:17" ht="12.75">
       <c r="A11" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="B11" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="C11" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="D11" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="E11" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="F11" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="G11" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="H11" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="I11" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="J11" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="K11" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="L11" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="M11" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="N11" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="O11" s="14" t="s">
+        <v>47</v>
+      </c>
+      <c r="P11" s="14" t="s">
         <v>48</v>
       </c>
-      <c r="B11" s="14" t="s">
-        <v>49</v>
-      </c>
-      <c r="C11" s="14" t="s">
-        <v>49</v>
-      </c>
-      <c r="D11" s="14" t="s">
-        <v>49</v>
-      </c>
-      <c r="E11" s="14" t="s">
-        <v>49</v>
-      </c>
-      <c r="F11" s="14" t="s">
-        <v>49</v>
-      </c>
-      <c r="G11" s="14" t="s">
-        <v>49</v>
-      </c>
-      <c r="H11" s="14" t="s">
-        <v>49</v>
-      </c>
-      <c r="I11" s="14" t="s">
-        <v>49</v>
-      </c>
-      <c r="J11" s="14" t="s">
-        <v>49</v>
-      </c>
-      <c r="K11" s="14" t="s">
-        <v>49</v>
-      </c>
-      <c r="L11" s="14" t="s">
-        <v>49</v>
-      </c>
-      <c r="M11" s="14" t="s">
-        <v>49</v>
-      </c>
-      <c r="N11" s="14" t="s">
-        <v>49</v>
-      </c>
-      <c r="O11" s="14" t="s">
-        <v>50</v>
-      </c>
-      <c r="P11" s="14" t="s">
-        <v>51</v>
-      </c>
       <c r="Q11" s="14" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
     </row>
     <row r="12" spans="1:17" ht="12.75">
       <c r="A12" s="13" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="B12" s="14">
         <v>31.86</v>
@@ -2992,7 +3006,7 @@
     </row>
     <row r="13" spans="1:17" ht="12.75">
       <c r="A13" s="13" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="B13" s="14">
         <v>429</v>
@@ -3028,23 +3042,23 @@
         <v>453</v>
       </c>
       <c r="M13" s="14" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="N13" s="14" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="O13" s="15">
         <v>430</v>
       </c>
-      <c r="P13" s="25">
+      <c r="P13" s="21">
         <v>1324</v>
       </c>
-      <c r="Q13" s="25">
+      <c r="Q13" s="21">
         <v>1252</v>
       </c>
     </row>
     <row r="14" spans="1:17" ht="15.75" customHeight="1">
-      <c r="A14" s="26"/>
+      <c r="A14" s="22"/>
       <c r="B14" s="10"/>
       <c r="C14" s="10"/>
       <c r="D14" s="10"/>
@@ -3066,52 +3080,52 @@
       <c r="A15" s="11" t="s">
         <v>35</v>
       </c>
-      <c r="B15" s="27">
+      <c r="B15" s="23">
         <v>40548</v>
       </c>
-      <c r="C15" s="27">
+      <c r="C15" s="23">
         <v>40548</v>
       </c>
-      <c r="D15" s="21" t="s">
-        <v>56</v>
-      </c>
-      <c r="E15" s="27">
+      <c r="D15" s="17" t="s">
+        <v>53</v>
+      </c>
+      <c r="E15" s="23">
         <v>40553</v>
       </c>
-      <c r="F15" s="27">
+      <c r="F15" s="23">
         <v>40553</v>
       </c>
-      <c r="G15" s="27">
+      <c r="G15" s="23">
         <v>40918</v>
       </c>
-      <c r="H15" s="27">
+      <c r="H15" s="23">
         <v>40918</v>
       </c>
-      <c r="I15" s="21" t="s">
-        <v>57</v>
-      </c>
-      <c r="J15" s="21" t="s">
-        <v>57</v>
-      </c>
-      <c r="K15" s="27">
+      <c r="I15" s="17" t="s">
+        <v>54</v>
+      </c>
+      <c r="J15" s="17" t="s">
+        <v>54</v>
+      </c>
+      <c r="K15" s="23">
         <v>40544</v>
       </c>
-      <c r="L15" s="27">
+      <c r="L15" s="23">
         <v>40544</v>
       </c>
-      <c r="M15" s="27">
+      <c r="M15" s="23">
         <v>40179</v>
       </c>
-      <c r="N15" s="27">
+      <c r="N15" s="23">
         <v>40179</v>
       </c>
-      <c r="O15" s="27">
+      <c r="O15" s="23">
         <v>40544</v>
       </c>
-      <c r="P15" s="27">
+      <c r="P15" s="23">
         <v>40544</v>
       </c>
-      <c r="Q15" s="27">
+      <c r="Q15" s="23">
         <v>40544</v>
       </c>
     </row>
@@ -3126,31 +3140,31 @@
         <v>40913</v>
       </c>
       <c r="D16" s="14" t="s">
+        <v>55</v>
+      </c>
+      <c r="E16" s="14" t="s">
+        <v>56</v>
+      </c>
+      <c r="F16" s="14" t="s">
+        <v>56</v>
+      </c>
+      <c r="G16" s="14" t="s">
+        <v>57</v>
+      </c>
+      <c r="H16" s="14" t="s">
+        <v>57</v>
+      </c>
+      <c r="I16" s="14" t="s">
         <v>58</v>
       </c>
-      <c r="E16" s="14" t="s">
+      <c r="J16" s="14" t="s">
+        <v>58</v>
+      </c>
+      <c r="K16" s="14" t="s">
         <v>59</v>
       </c>
-      <c r="F16" s="14" t="s">
+      <c r="L16" s="14" t="s">
         <v>59</v>
-      </c>
-      <c r="G16" s="14" t="s">
-        <v>60</v>
-      </c>
-      <c r="H16" s="14" t="s">
-        <v>60</v>
-      </c>
-      <c r="I16" s="14" t="s">
-        <v>61</v>
-      </c>
-      <c r="J16" s="14" t="s">
-        <v>61</v>
-      </c>
-      <c r="K16" s="14" t="s">
-        <v>62</v>
-      </c>
-      <c r="L16" s="14" t="s">
-        <v>62</v>
       </c>
       <c r="M16" s="14" t="s">
         <v>37</v>
@@ -3170,60 +3184,60 @@
     </row>
     <row r="17" spans="1:17" ht="12.75">
       <c r="A17" s="13" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="B17" s="14" t="s">
+        <v>60</v>
+      </c>
+      <c r="C17" s="14" t="s">
+        <v>61</v>
+      </c>
+      <c r="D17" s="14" t="s">
+        <v>61</v>
+      </c>
+      <c r="E17" s="14" t="s">
+        <v>61</v>
+      </c>
+      <c r="F17" s="14" t="s">
+        <v>60</v>
+      </c>
+      <c r="G17" s="14" t="s">
+        <v>61</v>
+      </c>
+      <c r="H17" s="14" t="s">
+        <v>60</v>
+      </c>
+      <c r="I17" s="14" t="s">
+        <v>62</v>
+      </c>
+      <c r="J17" s="14" t="s">
         <v>63</v>
       </c>
-      <c r="C17" s="14" t="s">
+      <c r="K17" s="14" t="s">
         <v>64</v>
       </c>
-      <c r="D17" s="14" t="s">
-        <v>64</v>
-      </c>
-      <c r="E17" s="14" t="s">
-        <v>64</v>
-      </c>
-      <c r="F17" s="14" t="s">
-        <v>63</v>
-      </c>
-      <c r="G17" s="14" t="s">
-        <v>64</v>
-      </c>
-      <c r="H17" s="14" t="s">
-        <v>63</v>
-      </c>
-      <c r="I17" s="14" t="s">
+      <c r="L17" s="14" t="s">
         <v>65</v>
       </c>
-      <c r="J17" s="14" t="s">
+      <c r="M17" s="14" t="s">
         <v>66</v>
       </c>
-      <c r="K17" s="14" t="s">
+      <c r="N17" s="14" t="s">
         <v>67</v>
       </c>
-      <c r="L17" s="14" t="s">
+      <c r="O17" s="14" t="s">
         <v>68</v>
       </c>
-      <c r="M17" s="14" t="s">
-        <v>69</v>
-      </c>
-      <c r="N17" s="14" t="s">
-        <v>70</v>
-      </c>
-      <c r="O17" s="14" t="s">
-        <v>71</v>
-      </c>
-      <c r="P17" s="28">
+      <c r="P17" s="24">
         <v>100</v>
       </c>
-      <c r="Q17" s="29">
+      <c r="Q17" s="25">
         <v>100</v>
       </c>
     </row>
     <row r="18" spans="1:17" ht="12.75">
       <c r="A18" s="13" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="B18" s="14">
         <v>26</v>
@@ -3247,33 +3261,33 @@
         <v>26</v>
       </c>
       <c r="I18" s="14" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="J18" s="14" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="K18" s="14"/>
       <c r="L18" s="14" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="M18" s="14" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="N18" s="14" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="O18" s="14" t="s">
-        <v>72</v>
-      </c>
-      <c r="P18" s="21" t="s">
-        <v>73</v>
+        <v>69</v>
+      </c>
+      <c r="P18" s="17" t="s">
+        <v>70</v>
       </c>
       <c r="Q18" s="14" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
     </row>
     <row r="19" spans="1:17" ht="15.75" customHeight="1">
-      <c r="A19" s="26"/>
+      <c r="A19" s="22"/>
       <c r="B19" s="10"/>
       <c r="C19" s="10"/>
       <c r="D19" s="10"/>
@@ -3292,8 +3306,8 @@
       <c r="Q19" s="10"/>
     </row>
     <row r="20" spans="1:17" ht="15.75" customHeight="1">
-      <c r="A20" s="26"/>
-      <c r="B20" s="30"/>
+      <c r="A20" s="22"/>
+      <c r="B20" s="26"/>
       <c r="C20" s="10"/>
       <c r="D20" s="10"/>
       <c r="E20" s="10"/>
@@ -3311,7 +3325,7 @@
       <c r="Q20" s="10"/>
     </row>
     <row r="21" spans="1:17" ht="15.75" customHeight="1">
-      <c r="A21" s="26"/>
+      <c r="A21" s="22"/>
       <c r="B21" s="10"/>
       <c r="C21" s="10"/>
       <c r="D21" s="10"/>
@@ -3330,7 +3344,7 @@
       <c r="Q21" s="10"/>
     </row>
     <row r="22" spans="1:17" ht="15.75" customHeight="1">
-      <c r="A22" s="26"/>
+      <c r="A22" s="22"/>
       <c r="B22" s="10"/>
       <c r="C22" s="10"/>
       <c r="D22" s="10"/>
@@ -3349,7 +3363,7 @@
       <c r="Q22" s="10"/>
     </row>
     <row r="23" spans="1:17" ht="15.75" customHeight="1">
-      <c r="A23" s="26"/>
+      <c r="A23" s="22"/>
       <c r="B23" s="10"/>
       <c r="C23" s="10"/>
       <c r="D23" s="10"/>
@@ -3368,7 +3382,7 @@
       <c r="Q23" s="10"/>
     </row>
     <row r="24" spans="1:17" ht="15.75" customHeight="1">
-      <c r="A24" s="26"/>
+      <c r="A24" s="22"/>
       <c r="B24" s="10"/>
       <c r="C24" s="10"/>
       <c r="D24" s="10"/>
@@ -3387,7 +3401,7 @@
       <c r="Q24" s="10"/>
     </row>
     <row r="25" spans="1:17" ht="15.75" customHeight="1">
-      <c r="A25" s="26"/>
+      <c r="A25" s="22"/>
       <c r="B25" s="10"/>
       <c r="C25" s="10"/>
       <c r="D25" s="10"/>
@@ -3406,7 +3420,7 @@
       <c r="Q25" s="10"/>
     </row>
     <row r="26" spans="1:17" ht="15.75" customHeight="1">
-      <c r="A26" s="26"/>
+      <c r="A26" s="22"/>
       <c r="B26" s="9"/>
       <c r="C26" s="10"/>
       <c r="D26" s="10"/>
@@ -3425,8 +3439,8 @@
       <c r="Q26" s="10"/>
     </row>
     <row r="27" spans="1:17" ht="15.75" customHeight="1">
-      <c r="A27" s="26"/>
-      <c r="B27" s="31"/>
+      <c r="A27" s="22"/>
+      <c r="B27" s="27"/>
       <c r="C27" s="10"/>
       <c r="D27" s="10"/>
       <c r="E27" s="10"/>
@@ -3444,6 +3458,7 @@
       <c r="Q27" s="10"/>
     </row>
   </sheetData>
+  <phoneticPr fontId="14" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
 </worksheet>
@@ -3471,105 +3486,105 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" ht="15.75" customHeight="1">
-      <c r="A1" s="32"/>
-      <c r="B1" s="32" t="s">
+      <c r="A1" s="28"/>
+      <c r="B1" s="28" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="32"/>
-      <c r="D1" s="32"/>
-      <c r="E1" s="32"/>
-      <c r="F1" s="32"/>
-      <c r="G1" s="32"/>
-      <c r="H1" s="32"/>
-      <c r="I1" s="32"/>
-      <c r="J1" s="32"/>
+      <c r="C1" s="28"/>
+      <c r="D1" s="28"/>
+      <c r="E1" s="28"/>
+      <c r="F1" s="28"/>
+      <c r="G1" s="28"/>
+      <c r="H1" s="28"/>
+      <c r="I1" s="28"/>
+      <c r="J1" s="28"/>
     </row>
     <row r="2" spans="1:16" ht="12.75">
-      <c r="A2" s="33" t="s">
+      <c r="A2" s="29" t="s">
         <v>19</v>
       </c>
-      <c r="B2" s="33" t="s">
-        <v>75</v>
-      </c>
-      <c r="C2" s="33" t="s">
-        <v>76</v>
-      </c>
-      <c r="D2" s="34"/>
-      <c r="E2" s="34"/>
-      <c r="F2" s="34"/>
-      <c r="G2" s="34"/>
-      <c r="H2" s="34"/>
-      <c r="I2" s="34"/>
-      <c r="J2" s="34"/>
-      <c r="K2" s="34"/>
-      <c r="L2" s="34"/>
-      <c r="M2" s="34"/>
-      <c r="N2" s="34"/>
-      <c r="O2" s="34"/>
-      <c r="P2" s="34"/>
+      <c r="B2" s="29" t="s">
+        <v>72</v>
+      </c>
+      <c r="C2" s="29" t="s">
+        <v>73</v>
+      </c>
+      <c r="D2" s="30"/>
+      <c r="E2" s="30"/>
+      <c r="F2" s="30"/>
+      <c r="G2" s="30"/>
+      <c r="H2" s="30"/>
+      <c r="I2" s="30"/>
+      <c r="J2" s="30"/>
+      <c r="K2" s="30"/>
+      <c r="L2" s="30"/>
+      <c r="M2" s="30"/>
+      <c r="N2" s="30"/>
+      <c r="O2" s="30"/>
+      <c r="P2" s="30"/>
     </row>
     <row r="3" spans="1:16" ht="12.75">
-      <c r="A3" s="33" t="s">
+      <c r="A3" s="29" t="s">
         <v>33</v>
       </c>
-      <c r="B3" s="35">
+      <c r="B3" s="31">
         <v>-8.1051400000000005</v>
       </c>
-      <c r="C3" s="35">
+      <c r="C3" s="31">
         <v>36.008980000000001</v>
       </c>
-      <c r="D3" s="36"/>
-      <c r="E3" s="36"/>
-      <c r="F3" s="36"/>
-      <c r="G3" s="36"/>
+      <c r="D3" s="32"/>
+      <c r="E3" s="32"/>
+      <c r="F3" s="32"/>
+      <c r="G3" s="32"/>
       <c r="H3" s="1"/>
       <c r="I3" s="1"/>
       <c r="J3" s="1"/>
       <c r="K3" s="1"/>
       <c r="L3" s="1"/>
       <c r="M3" s="1"/>
-      <c r="N3" s="36"/>
+      <c r="N3" s="32"/>
       <c r="O3" s="1"/>
       <c r="P3" s="1"/>
     </row>
     <row r="4" spans="1:16" ht="12.75">
-      <c r="A4" s="33" t="s">
+      <c r="A4" s="29" t="s">
         <v>34</v>
       </c>
-      <c r="B4" s="35">
+      <c r="B4" s="31">
         <v>31.641110000000001</v>
       </c>
-      <c r="C4" s="35">
+      <c r="C4" s="31">
         <v>32.554589999999997</v>
       </c>
-      <c r="D4" s="36"/>
-      <c r="E4" s="36"/>
-      <c r="F4" s="36"/>
-      <c r="G4" s="36"/>
+      <c r="D4" s="32"/>
+      <c r="E4" s="32"/>
+      <c r="F4" s="32"/>
+      <c r="G4" s="32"/>
       <c r="H4" s="1"/>
       <c r="I4" s="1"/>
       <c r="J4" s="1"/>
       <c r="K4" s="1"/>
       <c r="L4" s="1"/>
       <c r="M4" s="1"/>
-      <c r="N4" s="36"/>
+      <c r="N4" s="32"/>
       <c r="O4" s="1"/>
       <c r="P4" s="1"/>
     </row>
     <row r="5" spans="1:16" ht="12.75">
-      <c r="A5" s="33" t="s">
+      <c r="A5" s="29" t="s">
         <v>35</v>
       </c>
-      <c r="B5" s="37">
+      <c r="B5" s="33">
         <v>42736</v>
       </c>
-      <c r="C5" s="37">
+      <c r="C5" s="33">
         <v>42736</v>
       </c>
-      <c r="D5" s="36"/>
-      <c r="E5" s="36"/>
-      <c r="F5" s="36"/>
-      <c r="G5" s="36"/>
+      <c r="D5" s="32"/>
+      <c r="E5" s="32"/>
+      <c r="F5" s="32"/>
+      <c r="G5" s="32"/>
       <c r="H5" s="1"/>
       <c r="I5" s="1"/>
       <c r="J5" s="1"/>
@@ -3581,19 +3596,19 @@
       <c r="P5" s="1"/>
     </row>
     <row r="6" spans="1:16" ht="12.75">
-      <c r="A6" s="33" t="s">
+      <c r="A6" s="29" t="s">
         <v>36</v>
       </c>
-      <c r="B6" s="37">
+      <c r="B6" s="33">
         <v>43101</v>
       </c>
-      <c r="C6" s="37">
+      <c r="C6" s="33">
         <v>43101</v>
       </c>
-      <c r="D6" s="36"/>
-      <c r="E6" s="36"/>
-      <c r="F6" s="36"/>
-      <c r="G6" s="36"/>
+      <c r="D6" s="32"/>
+      <c r="E6" s="32"/>
+      <c r="F6" s="32"/>
+      <c r="G6" s="32"/>
       <c r="H6" s="1"/>
       <c r="I6" s="1"/>
       <c r="J6" s="1"/>
@@ -3605,21 +3620,21 @@
       <c r="P6" s="1"/>
     </row>
     <row r="7" spans="1:16" ht="12.75">
-      <c r="A7" s="33" t="s">
+      <c r="A7" s="29" t="s">
         <v>38</v>
       </c>
-      <c r="B7" s="38" t="s">
-        <v>72</v>
-      </c>
-      <c r="C7" s="38" t="s">
-        <v>72</v>
-      </c>
-      <c r="D7" s="36"/>
-      <c r="E7" s="36"/>
-      <c r="F7" s="36"/>
-      <c r="G7" s="36"/>
-      <c r="H7" s="39"/>
-      <c r="I7" s="39"/>
+      <c r="B7" s="34" t="s">
+        <v>69</v>
+      </c>
+      <c r="C7" s="34" t="s">
+        <v>69</v>
+      </c>
+      <c r="D7" s="32"/>
+      <c r="E7" s="32"/>
+      <c r="F7" s="32"/>
+      <c r="G7" s="32"/>
+      <c r="H7" s="35"/>
+      <c r="I7" s="35"/>
       <c r="J7" s="1"/>
       <c r="K7" s="1"/>
       <c r="L7" s="1"/>
@@ -3629,19 +3644,19 @@
       <c r="P7" s="1"/>
     </row>
     <row r="8" spans="1:16" ht="12.75">
-      <c r="A8" s="33" t="s">
-        <v>43</v>
-      </c>
-      <c r="B8" s="40" t="s">
-        <v>77</v>
-      </c>
-      <c r="C8" s="38" t="s">
-        <v>72</v>
-      </c>
-      <c r="D8" s="36"/>
-      <c r="E8" s="36"/>
-      <c r="F8" s="36"/>
-      <c r="G8" s="36"/>
+      <c r="A8" s="29" t="s">
+        <v>40</v>
+      </c>
+      <c r="B8" s="36" t="s">
+        <v>74</v>
+      </c>
+      <c r="C8" s="34" t="s">
+        <v>69</v>
+      </c>
+      <c r="D8" s="32"/>
+      <c r="E8" s="32"/>
+      <c r="F8" s="32"/>
+      <c r="G8" s="32"/>
       <c r="H8" s="1"/>
       <c r="I8" s="1"/>
       <c r="J8" s="1"/>
@@ -3653,19 +3668,19 @@
       <c r="P8" s="1"/>
     </row>
     <row r="9" spans="1:16" ht="12.75">
-      <c r="A9" s="33" t="s">
-        <v>46</v>
-      </c>
-      <c r="B9" s="35" t="s">
-        <v>78</v>
-      </c>
-      <c r="C9" s="35" t="s">
-        <v>78</v>
-      </c>
-      <c r="D9" s="36"/>
-      <c r="E9" s="36"/>
-      <c r="F9" s="36"/>
-      <c r="G9" s="36"/>
+      <c r="A9" s="29" t="s">
+        <v>43</v>
+      </c>
+      <c r="B9" s="31" t="s">
+        <v>75</v>
+      </c>
+      <c r="C9" s="31" t="s">
+        <v>75</v>
+      </c>
+      <c r="D9" s="32"/>
+      <c r="E9" s="32"/>
+      <c r="F9" s="32"/>
+      <c r="G9" s="32"/>
       <c r="H9" s="1"/>
       <c r="I9" s="1"/>
       <c r="J9" s="1"/>
@@ -3673,19 +3688,19 @@
       <c r="L9" s="1"/>
       <c r="M9" s="1"/>
       <c r="N9" s="1"/>
-      <c r="O9" s="41"/>
-      <c r="P9" s="42"/>
+      <c r="O9" s="37"/>
+      <c r="P9" s="38"/>
     </row>
     <row r="10" spans="1:16" ht="12.75">
-      <c r="A10" s="33" t="s">
-        <v>47</v>
-      </c>
-      <c r="B10" s="35"/>
-      <c r="C10" s="35"/>
-      <c r="D10" s="36"/>
-      <c r="E10" s="36"/>
-      <c r="F10" s="36"/>
-      <c r="G10" s="36"/>
+      <c r="A10" s="29" t="s">
+        <v>44</v>
+      </c>
+      <c r="B10" s="31"/>
+      <c r="C10" s="31"/>
+      <c r="D10" s="32"/>
+      <c r="E10" s="32"/>
+      <c r="F10" s="32"/>
+      <c r="G10" s="32"/>
       <c r="H10" s="1"/>
       <c r="I10" s="1"/>
       <c r="J10" s="1"/>
@@ -3697,19 +3712,19 @@
       <c r="P10" s="1"/>
     </row>
     <row r="11" spans="1:16" ht="12.75">
-      <c r="A11" s="33" t="s">
-        <v>48</v>
-      </c>
-      <c r="B11" s="38" t="s">
-        <v>72</v>
-      </c>
-      <c r="C11" s="38" t="s">
-        <v>72</v>
-      </c>
-      <c r="D11" s="36"/>
-      <c r="E11" s="36"/>
-      <c r="F11" s="36"/>
-      <c r="G11" s="36"/>
+      <c r="A11" s="29" t="s">
+        <v>45</v>
+      </c>
+      <c r="B11" s="34" t="s">
+        <v>69</v>
+      </c>
+      <c r="C11" s="34" t="s">
+        <v>69</v>
+      </c>
+      <c r="D11" s="32"/>
+      <c r="E11" s="32"/>
+      <c r="F11" s="32"/>
+      <c r="G11" s="32"/>
       <c r="H11" s="1"/>
       <c r="I11" s="1"/>
       <c r="J11" s="1"/>
@@ -3721,15 +3736,15 @@
       <c r="P11" s="1"/>
     </row>
     <row r="12" spans="1:16" ht="12.75">
-      <c r="A12" s="33" t="s">
-        <v>52</v>
-      </c>
-      <c r="B12" s="35"/>
-      <c r="C12" s="35"/>
-      <c r="D12" s="36"/>
-      <c r="E12" s="36"/>
-      <c r="F12" s="36"/>
-      <c r="G12" s="36"/>
+      <c r="A12" s="29" t="s">
+        <v>49</v>
+      </c>
+      <c r="B12" s="31"/>
+      <c r="C12" s="31"/>
+      <c r="D12" s="32"/>
+      <c r="E12" s="32"/>
+      <c r="F12" s="32"/>
+      <c r="G12" s="32"/>
       <c r="H12" s="1"/>
       <c r="I12" s="1"/>
       <c r="J12" s="1"/>
@@ -3741,19 +3756,19 @@
       <c r="P12" s="1"/>
     </row>
     <row r="13" spans="1:16" ht="12.75">
-      <c r="A13" s="33" t="s">
-        <v>53</v>
-      </c>
-      <c r="B13" s="40" t="s">
-        <v>77</v>
-      </c>
-      <c r="C13" s="40" t="s">
-        <v>77</v>
-      </c>
-      <c r="D13" s="36"/>
-      <c r="E13" s="36"/>
-      <c r="F13" s="36"/>
-      <c r="G13" s="36"/>
+      <c r="A13" s="29" t="s">
+        <v>50</v>
+      </c>
+      <c r="B13" s="36" t="s">
+        <v>74</v>
+      </c>
+      <c r="C13" s="36" t="s">
+        <v>74</v>
+      </c>
+      <c r="D13" s="32"/>
+      <c r="E13" s="32"/>
+      <c r="F13" s="32"/>
+      <c r="G13" s="32"/>
       <c r="H13" s="1"/>
       <c r="I13" s="1"/>
       <c r="J13" s="1"/>
@@ -3792,213 +3807,213 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="15.75" customHeight="1">
-      <c r="A1" s="32"/>
-      <c r="B1" s="32" t="s">
+      <c r="A1" s="28"/>
+      <c r="B1" s="28" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="12.75">
-      <c r="A2" s="33" t="s">
+      <c r="A2" s="29" t="s">
         <v>19</v>
       </c>
-      <c r="B2" s="33" t="s">
+      <c r="B2" s="29" t="s">
+        <v>76</v>
+      </c>
+      <c r="C2" s="29" t="s">
+        <v>77</v>
+      </c>
+      <c r="D2" s="29" t="s">
+        <v>78</v>
+      </c>
+      <c r="E2" s="29" t="s">
         <v>79</v>
       </c>
-      <c r="C2" s="33" t="s">
+    </row>
+    <row r="3" spans="1:5" ht="12.75">
+      <c r="A3" s="29" t="s">
+        <v>33</v>
+      </c>
+      <c r="B3" s="31">
+        <v>48.717812000000002</v>
+      </c>
+      <c r="C3" s="31">
+        <v>48.717812000000002</v>
+      </c>
+      <c r="D3" s="31">
+        <v>48.717812000000002</v>
+      </c>
+      <c r="E3" s="31">
+        <v>48.717812000000002</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="12.75">
+      <c r="A4" s="29" t="s">
+        <v>34</v>
+      </c>
+      <c r="B4" s="31">
+        <v>31.323521</v>
+      </c>
+      <c r="C4" s="31">
+        <v>31.323521</v>
+      </c>
+      <c r="D4" s="31">
+        <v>31.323521</v>
+      </c>
+      <c r="E4" s="31">
+        <v>31.323521</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="12.75">
+      <c r="A5" s="29" t="s">
+        <v>35</v>
+      </c>
+      <c r="B5" s="33">
+        <v>36526</v>
+      </c>
+      <c r="C5" s="33">
+        <v>36526</v>
+      </c>
+      <c r="D5" s="33">
+        <v>37987</v>
+      </c>
+      <c r="E5" s="33">
+        <v>37987</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="12.75">
+      <c r="A6" s="29" t="s">
+        <v>36</v>
+      </c>
+      <c r="B6" s="31" t="s">
         <v>80</v>
       </c>
-      <c r="D2" s="33" t="s">
+      <c r="C6" s="31" t="s">
+        <v>80</v>
+      </c>
+      <c r="D6" s="31" t="s">
         <v>81</v>
       </c>
-      <c r="E2" s="33" t="s">
+      <c r="E6" s="31" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="12.75">
+      <c r="A7" s="29" t="s">
+        <v>38</v>
+      </c>
+      <c r="B7" s="31" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" ht="12.75">
-      <c r="A3" s="33" t="s">
-        <v>33</v>
-      </c>
-      <c r="B3" s="35">
-        <v>48.717812000000002</v>
-      </c>
-      <c r="C3" s="35">
-        <v>48.717812000000002</v>
-      </c>
-      <c r="D3" s="35">
-        <v>48.717812000000002</v>
-      </c>
-      <c r="E3" s="35">
-        <v>48.717812000000002</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" ht="12.75">
-      <c r="A4" s="33" t="s">
-        <v>34</v>
-      </c>
-      <c r="B4" s="35">
-        <v>31.323521</v>
-      </c>
-      <c r="C4" s="35">
-        <v>31.323521</v>
-      </c>
-      <c r="D4" s="35">
-        <v>31.323521</v>
-      </c>
-      <c r="E4" s="35">
-        <v>31.323521</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" ht="12.75">
-      <c r="A5" s="33" t="s">
-        <v>35</v>
-      </c>
-      <c r="B5" s="37">
-        <v>36526</v>
-      </c>
-      <c r="C5" s="37">
-        <v>36526</v>
-      </c>
-      <c r="D5" s="37">
-        <v>37987</v>
-      </c>
-      <c r="E5" s="37">
-        <v>37987</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" ht="12.75">
-      <c r="A6" s="33" t="s">
-        <v>36</v>
-      </c>
-      <c r="B6" s="35" t="s">
+      <c r="C7" s="31" t="s">
+        <v>82</v>
+      </c>
+      <c r="D7" s="31" t="s">
         <v>83</v>
       </c>
-      <c r="C6" s="35" t="s">
+      <c r="E7" s="31" t="s">
         <v>83</v>
       </c>
-      <c r="D6" s="35" t="s">
+    </row>
+    <row r="8" spans="1:5" ht="12.75">
+      <c r="A8" s="29" t="s">
+        <v>40</v>
+      </c>
+      <c r="B8" s="31" t="s">
         <v>84</v>
       </c>
-      <c r="E6" s="35" t="s">
+      <c r="C8" s="31" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" ht="12.75">
-      <c r="A7" s="33" t="s">
-        <v>38</v>
-      </c>
-      <c r="B7" s="35" t="s">
+      <c r="D8" s="31" t="s">
+        <v>84</v>
+      </c>
+      <c r="E8" s="31" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="12.75">
+      <c r="A9" s="29" t="s">
+        <v>43</v>
+      </c>
+      <c r="B9" s="31">
+        <v>50</v>
+      </c>
+      <c r="C9" s="31">
+        <v>50</v>
+      </c>
+      <c r="D9" s="31">
+        <v>50</v>
+      </c>
+      <c r="E9" s="31">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="12.75">
+      <c r="A10" s="29" t="s">
+        <v>44</v>
+      </c>
+      <c r="B10" s="31">
+        <v>44</v>
+      </c>
+      <c r="C10" s="31">
+        <v>44</v>
+      </c>
+      <c r="D10" s="31">
+        <v>44</v>
+      </c>
+      <c r="E10" s="31">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="12.75">
+      <c r="A11" s="29" t="s">
+        <v>45</v>
+      </c>
+      <c r="B11" s="31" t="s">
+        <v>47</v>
+      </c>
+      <c r="C11" s="31" t="s">
+        <v>47</v>
+      </c>
+      <c r="D11" s="31" t="s">
+        <v>47</v>
+      </c>
+      <c r="E11" s="31" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="12.75">
+      <c r="A12" s="29" t="s">
+        <v>49</v>
+      </c>
+      <c r="B12" s="31">
+        <v>15.8</v>
+      </c>
+      <c r="C12" s="31">
+        <v>14.7</v>
+      </c>
+      <c r="D12" s="31">
+        <v>6</v>
+      </c>
+      <c r="E12" s="31">
+        <v>5.8</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="12.75">
+      <c r="A13" s="29" t="s">
+        <v>50</v>
+      </c>
+      <c r="B13" s="31" t="s">
         <v>85</v>
       </c>
-      <c r="C7" s="35" t="s">
+      <c r="C13" s="31" t="s">
         <v>85</v>
       </c>
-      <c r="D7" s="35" t="s">
-        <v>86</v>
-      </c>
-      <c r="E7" s="35" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" ht="12.75">
-      <c r="A8" s="33" t="s">
-        <v>43</v>
-      </c>
-      <c r="B8" s="35" t="s">
-        <v>87</v>
-      </c>
-      <c r="C8" s="35" t="s">
-        <v>87</v>
-      </c>
-      <c r="D8" s="35" t="s">
-        <v>87</v>
-      </c>
-      <c r="E8" s="35" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" ht="12.75">
-      <c r="A9" s="33" t="s">
-        <v>46</v>
-      </c>
-      <c r="B9" s="35">
-        <v>50</v>
-      </c>
-      <c r="C9" s="35">
-        <v>50</v>
-      </c>
-      <c r="D9" s="35">
-        <v>50</v>
-      </c>
-      <c r="E9" s="35">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" ht="12.75">
-      <c r="A10" s="33" t="s">
-        <v>47</v>
-      </c>
-      <c r="B10" s="35">
-        <v>44</v>
-      </c>
-      <c r="C10" s="35">
-        <v>44</v>
-      </c>
-      <c r="D10" s="35">
-        <v>44</v>
-      </c>
-      <c r="E10" s="35">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" ht="12.75">
-      <c r="A11" s="33" t="s">
-        <v>48</v>
-      </c>
-      <c r="B11" s="35" t="s">
-        <v>50</v>
-      </c>
-      <c r="C11" s="35" t="s">
-        <v>50</v>
-      </c>
-      <c r="D11" s="35" t="s">
-        <v>50</v>
-      </c>
-      <c r="E11" s="35" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" ht="12.75">
-      <c r="A12" s="33" t="s">
-        <v>52</v>
-      </c>
-      <c r="B12" s="35">
-        <v>15.8</v>
-      </c>
-      <c r="C12" s="35">
-        <v>14.7</v>
-      </c>
-      <c r="D12" s="35">
-        <v>6</v>
-      </c>
-      <c r="E12" s="35">
-        <v>5.8</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" ht="12.75">
-      <c r="A13" s="33" t="s">
-        <v>53</v>
-      </c>
-      <c r="B13" s="35" t="s">
-        <v>88</v>
-      </c>
-      <c r="C13" s="35" t="s">
-        <v>88</v>
-      </c>
-      <c r="D13" s="35" t="s">
-        <v>88</v>
-      </c>
-      <c r="E13" s="35" t="s">
-        <v>88</v>
+      <c r="D13" s="31" t="s">
+        <v>85</v>
+      </c>
+      <c r="E13" s="31" t="s">
+        <v>85</v>
       </c>
     </row>
   </sheetData>
@@ -4014,8 +4029,8 @@
   </sheetPr>
   <dimension ref="A1:J21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J6" sqref="J6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1"/>
@@ -4025,561 +4040,561 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="15.75" customHeight="1">
-      <c r="A1" s="50" t="s">
+      <c r="A1" s="46" t="s">
+        <v>86</v>
+      </c>
+      <c r="B1" s="47"/>
+      <c r="C1" s="47"/>
+      <c r="D1" s="47"/>
+      <c r="E1" s="47"/>
+      <c r="F1" s="47"/>
+      <c r="G1" s="47"/>
+      <c r="H1" s="47"/>
+      <c r="I1" s="47"/>
+      <c r="J1" s="47"/>
+    </row>
+    <row r="2" spans="1:10" ht="12.75">
+      <c r="A2" s="29" t="s">
+        <v>19</v>
+      </c>
+      <c r="B2" s="39" t="s">
+        <v>87</v>
+      </c>
+      <c r="C2" s="39" t="s">
+        <v>88</v>
+      </c>
+      <c r="D2" s="39" t="s">
         <v>89</v>
       </c>
-      <c r="B1" s="51"/>
-      <c r="C1" s="51"/>
-      <c r="D1" s="51"/>
-      <c r="E1" s="51"/>
-      <c r="F1" s="51"/>
-      <c r="G1" s="51"/>
-      <c r="H1" s="51"/>
-      <c r="I1" s="51"/>
-      <c r="J1" s="51"/>
-    </row>
-    <row r="2" spans="1:10" ht="12.75">
-      <c r="A2" s="33" t="s">
-        <v>19</v>
-      </c>
-      <c r="B2" s="43" t="s">
+      <c r="E2" s="39" t="s">
         <v>90</v>
       </c>
-      <c r="C2" s="43" t="s">
+      <c r="F2" s="39" t="s">
         <v>91</v>
       </c>
-      <c r="D2" s="43" t="s">
+      <c r="G2" s="39" t="s">
         <v>92</v>
       </c>
-      <c r="E2" s="43" t="s">
+      <c r="H2" s="39" t="s">
         <v>93</v>
       </c>
-      <c r="F2" s="43" t="s">
+      <c r="I2" s="39" t="s">
         <v>94</v>
       </c>
-      <c r="G2" s="43" t="s">
+      <c r="J2" s="39" t="s">
         <v>95</v>
       </c>
-      <c r="H2" s="43" t="s">
+    </row>
+    <row r="3" spans="1:10" ht="12.75">
+      <c r="A3" s="29" t="s">
+        <v>33</v>
+      </c>
+      <c r="B3" s="40">
+        <v>-7.6097200000000003</v>
+      </c>
+      <c r="C3" s="40">
+        <v>-7.5916699999999997</v>
+      </c>
+      <c r="D3" s="40">
+        <v>-7.5944399999999996</v>
+      </c>
+      <c r="E3" s="40">
+        <v>-7.5916699999999997</v>
+      </c>
+      <c r="F3" s="40">
+        <v>-7.5888900000000001</v>
+      </c>
+      <c r="G3" s="40">
+        <v>-7.5986099999999999</v>
+      </c>
+      <c r="H3" s="40">
+        <v>-7.5958300000000003</v>
+      </c>
+      <c r="I3" s="40">
+        <v>-7.5916699999999997</v>
+      </c>
+      <c r="J3" s="40">
+        <v>-7.61111</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" ht="12.75">
+      <c r="A4" s="29" t="s">
+        <v>34</v>
+      </c>
+      <c r="B4" s="40">
+        <v>31.661110000000001</v>
+      </c>
+      <c r="C4" s="40">
+        <v>31.66667</v>
+      </c>
+      <c r="D4" s="40">
+        <v>31.668060000000001</v>
+      </c>
+      <c r="E4" s="40">
+        <v>31.677779999999998</v>
+      </c>
+      <c r="F4" s="40">
+        <v>31.68056</v>
+      </c>
+      <c r="G4" s="40">
+        <v>31.68056</v>
+      </c>
+      <c r="H4" s="40">
+        <v>31.68056</v>
+      </c>
+      <c r="I4" s="40">
+        <v>31.68056</v>
+      </c>
+      <c r="J4" s="40">
+        <v>31.66667</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" ht="12.75">
+      <c r="A5" s="29" t="s">
+        <v>35</v>
+      </c>
+      <c r="B5" s="45">
+        <v>38353</v>
+      </c>
+      <c r="C5" s="45">
+        <v>38353</v>
+      </c>
+      <c r="D5" s="45">
+        <v>38353</v>
+      </c>
+      <c r="E5" s="45">
+        <v>38353</v>
+      </c>
+      <c r="F5" s="45">
+        <v>38353</v>
+      </c>
+      <c r="G5" s="45">
+        <v>38353</v>
+      </c>
+      <c r="H5" s="45">
+        <v>38353</v>
+      </c>
+      <c r="I5" s="45">
+        <v>38353</v>
+      </c>
+      <c r="J5" s="45">
+        <v>38353</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" ht="12.75">
+      <c r="A6" s="29" t="s">
+        <v>36</v>
+      </c>
+      <c r="B6" s="45">
+        <v>39082</v>
+      </c>
+      <c r="C6" s="45">
+        <v>39082</v>
+      </c>
+      <c r="D6" s="45">
+        <v>39082</v>
+      </c>
+      <c r="E6" s="45">
+        <v>39082</v>
+      </c>
+      <c r="F6" s="45">
+        <v>39082</v>
+      </c>
+      <c r="G6" s="45">
+        <v>39082</v>
+      </c>
+      <c r="H6" s="45">
+        <v>39082</v>
+      </c>
+      <c r="I6" s="45">
+        <v>39082</v>
+      </c>
+      <c r="J6" s="45">
+        <v>39082</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" ht="12.75">
+      <c r="A7" s="29" t="s">
+        <v>38</v>
+      </c>
+      <c r="B7" s="45">
+        <v>38703</v>
+      </c>
+      <c r="C7" s="44">
+        <v>37632</v>
+      </c>
+      <c r="D7" s="44">
+        <v>37635</v>
+      </c>
+      <c r="E7" s="44">
+        <v>37946</v>
+      </c>
+      <c r="F7" s="44">
+        <v>37946</v>
+      </c>
+      <c r="G7" s="44">
+        <v>37970</v>
+      </c>
+      <c r="H7" s="44">
+        <v>37974</v>
+      </c>
+      <c r="I7" s="44">
+        <v>37975</v>
+      </c>
+      <c r="J7" s="44">
+        <v>37979</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" ht="12.75">
+      <c r="A8" s="29" t="s">
+        <v>40</v>
+      </c>
+      <c r="B8" s="39" t="s">
+        <v>41</v>
+      </c>
+      <c r="C8" s="39" t="s">
+        <v>41</v>
+      </c>
+      <c r="D8" s="39" t="s">
+        <v>41</v>
+      </c>
+      <c r="E8" s="39" t="s">
+        <v>41</v>
+      </c>
+      <c r="F8" s="39" t="s">
+        <v>41</v>
+      </c>
+      <c r="G8" s="39" t="s">
+        <v>41</v>
+      </c>
+      <c r="H8" s="39" t="s">
+        <v>41</v>
+      </c>
+      <c r="I8" s="39" t="s">
+        <v>41</v>
+      </c>
+      <c r="J8" s="39" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" ht="12.75">
+      <c r="A9" s="29" t="s">
+        <v>43</v>
+      </c>
+      <c r="B9" s="39">
+        <v>3</v>
+      </c>
+      <c r="C9" s="39">
+        <v>3</v>
+      </c>
+      <c r="D9" s="39">
+        <v>3</v>
+      </c>
+      <c r="E9" s="39">
+        <v>3</v>
+      </c>
+      <c r="F9" s="39">
+        <v>3</v>
+      </c>
+      <c r="G9" s="39">
+        <v>3</v>
+      </c>
+      <c r="H9" s="39">
+        <v>3</v>
+      </c>
+      <c r="I9" s="39">
+        <v>3</v>
+      </c>
+      <c r="J9" s="39">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" ht="12.75">
+      <c r="A10" s="29" t="s">
+        <v>44</v>
+      </c>
+      <c r="B10" s="48" t="s">
         <v>96</v>
       </c>
-      <c r="I2" s="43" t="s">
+      <c r="C10" s="49"/>
+      <c r="D10" s="49"/>
+      <c r="E10" s="49"/>
+      <c r="F10" s="49"/>
+      <c r="G10" s="49"/>
+      <c r="H10" s="49"/>
+      <c r="I10" s="49"/>
+      <c r="J10" s="50"/>
+    </row>
+    <row r="11" spans="1:10" ht="12.75">
+      <c r="A11" s="29" t="s">
+        <v>45</v>
+      </c>
+      <c r="B11" s="41" t="s">
+        <v>47</v>
+      </c>
+      <c r="C11" s="42" t="s">
+        <v>47</v>
+      </c>
+      <c r="D11" s="42" t="s">
+        <v>47</v>
+      </c>
+      <c r="E11" s="42" t="s">
+        <v>47</v>
+      </c>
+      <c r="F11" s="42" t="s">
+        <v>47</v>
+      </c>
+      <c r="G11" s="42" t="s">
+        <v>47</v>
+      </c>
+      <c r="H11" s="42" t="s">
+        <v>47</v>
+      </c>
+      <c r="I11" s="42" t="s">
+        <v>47</v>
+      </c>
+      <c r="J11" s="39" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" ht="12.75">
+      <c r="A12" s="29" t="s">
+        <v>49</v>
+      </c>
+      <c r="B12" s="39">
+        <v>2.75</v>
+      </c>
+      <c r="C12" s="39">
+        <v>2</v>
+      </c>
+      <c r="D12" s="39">
+        <v>0.85</v>
+      </c>
+      <c r="E12" s="39">
+        <v>2.75</v>
+      </c>
+      <c r="F12" s="39">
+        <v>2.25</v>
+      </c>
+      <c r="G12" s="39">
+        <v>2.25</v>
+      </c>
+      <c r="H12" s="39">
+        <v>3.25</v>
+      </c>
+      <c r="I12" s="39">
+        <v>1.25</v>
+      </c>
+      <c r="J12" s="39">
+        <v>2.25</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" ht="12.75">
+      <c r="A13" s="29" t="s">
+        <v>50</v>
+      </c>
+      <c r="B13" s="39">
+        <v>90</v>
+      </c>
+      <c r="C13" s="39">
+        <v>180</v>
+      </c>
+      <c r="D13" s="39">
+        <v>120</v>
+      </c>
+      <c r="E13" s="39">
+        <v>180</v>
+      </c>
+      <c r="F13" s="39">
+        <v>180</v>
+      </c>
+      <c r="G13" s="39">
+        <v>180</v>
+      </c>
+      <c r="H13" s="39">
+        <v>180</v>
+      </c>
+      <c r="I13" s="39">
+        <v>180</v>
+      </c>
+      <c r="J13" s="39">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" ht="12.75">
+      <c r="A14" s="29" t="s">
+        <v>103</v>
+      </c>
+      <c r="B14" s="39">
+        <v>337.3</v>
+      </c>
+      <c r="C14" s="39">
+        <v>225</v>
+      </c>
+      <c r="D14" s="39">
+        <v>337.3</v>
+      </c>
+      <c r="E14" s="39">
+        <v>337.3</v>
+      </c>
+      <c r="F14" s="39">
+        <v>225</v>
+      </c>
+      <c r="G14" s="39">
+        <v>337.3</v>
+      </c>
+      <c r="H14" s="39">
+        <v>225</v>
+      </c>
+      <c r="I14" s="39">
+        <v>225</v>
+      </c>
+      <c r="J14" s="39">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" ht="12.75">
+      <c r="A15" s="29" t="s">
+        <v>104</v>
+      </c>
+      <c r="B15" s="39">
+        <v>150</v>
+      </c>
+      <c r="C15" s="39">
+        <v>100</v>
+      </c>
+      <c r="D15" s="39">
+        <v>150</v>
+      </c>
+      <c r="E15" s="39">
+        <v>150</v>
+      </c>
+      <c r="F15" s="39">
+        <v>100</v>
+      </c>
+      <c r="G15" s="39">
+        <v>150</v>
+      </c>
+      <c r="H15" s="39">
+        <v>100</v>
+      </c>
+      <c r="I15" s="39">
+        <v>100</v>
+      </c>
+      <c r="J15" s="39">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" ht="12.75">
+      <c r="A16" s="29" t="s">
+        <v>105</v>
+      </c>
+      <c r="B16" s="39">
+        <v>20</v>
+      </c>
+      <c r="C16" s="39">
+        <v>65</v>
+      </c>
+      <c r="D16" s="39">
+        <v>20</v>
+      </c>
+      <c r="E16" s="39">
+        <v>45</v>
+      </c>
+      <c r="F16" s="39">
+        <v>20</v>
+      </c>
+      <c r="G16" s="39">
+        <v>20</v>
+      </c>
+      <c r="H16" s="39">
+        <v>65</v>
+      </c>
+      <c r="I16" s="39">
+        <v>20</v>
+      </c>
+      <c r="J16" s="39">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" ht="12.75">
+      <c r="A19" s="29" t="s">
+        <v>43</v>
+      </c>
+      <c r="B19" s="39">
+        <v>3</v>
+      </c>
+      <c r="C19" s="39">
+        <v>3</v>
+      </c>
+      <c r="D19" s="39">
+        <v>3</v>
+      </c>
+      <c r="E19" s="39">
+        <v>3</v>
+      </c>
+      <c r="F19" s="39">
+        <v>3</v>
+      </c>
+      <c r="G19" s="39">
+        <v>3</v>
+      </c>
+      <c r="H19" s="39">
+        <v>3</v>
+      </c>
+      <c r="I19" s="39">
+        <v>3</v>
+      </c>
+      <c r="J19" s="39">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" ht="12.75">
+      <c r="A20" s="29" t="s">
+        <v>44</v>
+      </c>
+      <c r="B20" s="48" t="s">
+        <v>96</v>
+      </c>
+      <c r="C20" s="49"/>
+      <c r="D20" s="49"/>
+      <c r="E20" s="49"/>
+      <c r="F20" s="49"/>
+      <c r="G20" s="49"/>
+      <c r="H20" s="49"/>
+      <c r="I20" s="49"/>
+      <c r="J20" s="50"/>
+    </row>
+    <row r="21" spans="1:10" ht="12.75">
+      <c r="A21" s="29" t="s">
+        <v>49</v>
+      </c>
+      <c r="B21" s="39" t="s">
         <v>97</v>
       </c>
-      <c r="J2" s="43" t="s">
+      <c r="C21" s="39" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="3" spans="1:10" ht="12.75">
-      <c r="A3" s="33" t="s">
-        <v>33</v>
-      </c>
-      <c r="B3" s="44">
-        <v>-7.6097200000000003</v>
-      </c>
-      <c r="C3" s="44">
-        <v>-7.5916699999999997</v>
-      </c>
-      <c r="D3" s="44">
-        <v>-7.5944399999999996</v>
-      </c>
-      <c r="E3" s="44">
-        <v>-7.5916699999999997</v>
-      </c>
-      <c r="F3" s="44">
-        <v>-7.5888900000000001</v>
-      </c>
-      <c r="G3" s="44">
-        <v>-7.5986099999999999</v>
-      </c>
-      <c r="H3" s="44">
-        <v>-7.5958300000000003</v>
-      </c>
-      <c r="I3" s="44">
-        <v>-7.5916699999999997</v>
-      </c>
-      <c r="J3" s="44">
-        <v>-7.61111</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" ht="12.75">
-      <c r="A4" s="33" t="s">
-        <v>34</v>
-      </c>
-      <c r="B4" s="44">
-        <v>31.661110000000001</v>
-      </c>
-      <c r="C4" s="44">
-        <v>31.66667</v>
-      </c>
-      <c r="D4" s="44">
-        <v>31.668060000000001</v>
-      </c>
-      <c r="E4" s="44">
-        <v>31.677779999999998</v>
-      </c>
-      <c r="F4" s="44">
-        <v>31.68056</v>
-      </c>
-      <c r="G4" s="44">
-        <v>31.68056</v>
-      </c>
-      <c r="H4" s="44">
-        <v>31.68056</v>
-      </c>
-      <c r="I4" s="44">
-        <v>31.68056</v>
-      </c>
-      <c r="J4" s="44">
-        <v>31.66667</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" ht="12.75">
-      <c r="A5" s="33" t="s">
-        <v>35</v>
-      </c>
-      <c r="B5" s="49">
-        <v>38353</v>
-      </c>
-      <c r="C5" s="49">
-        <v>38353</v>
-      </c>
-      <c r="D5" s="49">
-        <v>38353</v>
-      </c>
-      <c r="E5" s="49">
-        <v>38353</v>
-      </c>
-      <c r="F5" s="49">
-        <v>38353</v>
-      </c>
-      <c r="G5" s="49">
-        <v>38353</v>
-      </c>
-      <c r="H5" s="49">
-        <v>38353</v>
-      </c>
-      <c r="I5" s="49">
-        <v>38353</v>
-      </c>
-      <c r="J5" s="49">
-        <v>38353</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" ht="12.75">
-      <c r="A6" s="33" t="s">
-        <v>36</v>
-      </c>
-      <c r="B6" s="49">
-        <v>39082</v>
-      </c>
-      <c r="C6" s="49">
-        <v>39082</v>
-      </c>
-      <c r="D6" s="49">
-        <v>39082</v>
-      </c>
-      <c r="E6" s="49">
-        <v>39082</v>
-      </c>
-      <c r="F6" s="49">
-        <v>39082</v>
-      </c>
-      <c r="G6" s="49">
-        <v>39082</v>
-      </c>
-      <c r="H6" s="49">
-        <v>39082</v>
-      </c>
-      <c r="I6" s="49">
-        <v>39082</v>
-      </c>
-      <c r="J6" s="49">
-        <v>39082</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" ht="12.75">
-      <c r="A7" s="33" t="s">
-        <v>38</v>
-      </c>
-      <c r="B7" s="49">
-        <v>38703</v>
-      </c>
-      <c r="C7" s="48">
-        <v>37632</v>
-      </c>
-      <c r="D7" s="48">
-        <v>37635</v>
-      </c>
-      <c r="E7" s="48">
-        <v>37946</v>
-      </c>
-      <c r="F7" s="48">
-        <v>37946</v>
-      </c>
-      <c r="G7" s="48">
-        <v>37970</v>
-      </c>
-      <c r="H7" s="48">
-        <v>37974</v>
-      </c>
-      <c r="I7" s="48">
-        <v>37975</v>
-      </c>
-      <c r="J7" s="48">
-        <v>37979</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" ht="12.75">
-      <c r="A8" s="33" t="s">
-        <v>43</v>
-      </c>
-      <c r="B8" s="43" t="s">
-        <v>44</v>
-      </c>
-      <c r="C8" s="43" t="s">
-        <v>44</v>
-      </c>
-      <c r="D8" s="43" t="s">
-        <v>44</v>
-      </c>
-      <c r="E8" s="43" t="s">
-        <v>44</v>
-      </c>
-      <c r="F8" s="43" t="s">
-        <v>44</v>
-      </c>
-      <c r="G8" s="43" t="s">
-        <v>44</v>
-      </c>
-      <c r="H8" s="43" t="s">
-        <v>44</v>
-      </c>
-      <c r="I8" s="43" t="s">
-        <v>44</v>
-      </c>
-      <c r="J8" s="43" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" ht="12.75">
-      <c r="A9" s="33" t="s">
-        <v>46</v>
-      </c>
-      <c r="B9" s="43">
-        <v>3</v>
-      </c>
-      <c r="C9" s="43">
-        <v>3</v>
-      </c>
-      <c r="D9" s="43">
-        <v>3</v>
-      </c>
-      <c r="E9" s="43">
-        <v>3</v>
-      </c>
-      <c r="F9" s="43">
-        <v>3</v>
-      </c>
-      <c r="G9" s="43">
-        <v>3</v>
-      </c>
-      <c r="H9" s="43">
-        <v>3</v>
-      </c>
-      <c r="I9" s="43">
-        <v>3</v>
-      </c>
-      <c r="J9" s="43">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" ht="12.75">
-      <c r="A10" s="33" t="s">
-        <v>47</v>
-      </c>
-      <c r="B10" s="52" t="s">
+      <c r="D21" s="39" t="s">
         <v>99</v>
       </c>
-      <c r="C10" s="53"/>
-      <c r="D10" s="53"/>
-      <c r="E10" s="53"/>
-      <c r="F10" s="53"/>
-      <c r="G10" s="53"/>
-      <c r="H10" s="53"/>
-      <c r="I10" s="53"/>
-      <c r="J10" s="54"/>
-    </row>
-    <row r="11" spans="1:10" ht="12.75">
-      <c r="A11" s="33" t="s">
-        <v>48</v>
-      </c>
-      <c r="B11" s="45" t="s">
-        <v>50</v>
-      </c>
-      <c r="C11" s="46" t="s">
-        <v>50</v>
-      </c>
-      <c r="D11" s="46" t="s">
-        <v>50</v>
-      </c>
-      <c r="E11" s="46" t="s">
-        <v>50</v>
-      </c>
-      <c r="F11" s="46" t="s">
-        <v>50</v>
-      </c>
-      <c r="G11" s="46" t="s">
-        <v>50</v>
-      </c>
-      <c r="H11" s="46" t="s">
-        <v>50</v>
-      </c>
-      <c r="I11" s="46" t="s">
-        <v>50</v>
-      </c>
-      <c r="J11" s="43" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" ht="12.75">
-      <c r="A12" s="33" t="s">
-        <v>52</v>
-      </c>
-      <c r="B12" s="43">
-        <v>2.75</v>
-      </c>
-      <c r="C12" s="43">
-        <v>2</v>
-      </c>
-      <c r="D12" s="43">
-        <v>0.85</v>
-      </c>
-      <c r="E12" s="43">
-        <v>2.75</v>
-      </c>
-      <c r="F12" s="43">
-        <v>2.25</v>
-      </c>
-      <c r="G12" s="43">
-        <v>2.25</v>
-      </c>
-      <c r="H12" s="43">
-        <v>3.25</v>
-      </c>
-      <c r="I12" s="43">
-        <v>1.25</v>
-      </c>
-      <c r="J12" s="43">
-        <v>2.25</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" ht="12.75">
-      <c r="A13" s="33" t="s">
-        <v>53</v>
-      </c>
-      <c r="B13" s="43">
-        <v>90</v>
-      </c>
-      <c r="C13" s="43">
-        <v>180</v>
-      </c>
-      <c r="D13" s="43">
-        <v>120</v>
-      </c>
-      <c r="E13" s="43">
-        <v>180</v>
-      </c>
-      <c r="F13" s="43">
-        <v>180</v>
-      </c>
-      <c r="G13" s="43">
-        <v>180</v>
-      </c>
-      <c r="H13" s="43">
-        <v>180</v>
-      </c>
-      <c r="I13" s="43">
-        <v>180</v>
-      </c>
-      <c r="J13" s="43">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" ht="12.75">
-      <c r="A14" s="33" t="s">
-        <v>106</v>
-      </c>
-      <c r="B14" s="43">
-        <v>337.3</v>
-      </c>
-      <c r="C14" s="43">
-        <v>225</v>
-      </c>
-      <c r="D14" s="43">
-        <v>337.3</v>
-      </c>
-      <c r="E14" s="43">
-        <v>337.3</v>
-      </c>
-      <c r="F14" s="43">
-        <v>225</v>
-      </c>
-      <c r="G14" s="43">
-        <v>337.3</v>
-      </c>
-      <c r="H14" s="43">
-        <v>225</v>
-      </c>
-      <c r="I14" s="43">
-        <v>225</v>
-      </c>
-      <c r="J14" s="43">
-        <v>315</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" ht="12.75">
-      <c r="A15" s="33" t="s">
-        <v>107</v>
-      </c>
-      <c r="B15" s="43">
-        <v>150</v>
-      </c>
-      <c r="C15" s="43">
+      <c r="E21" s="39" t="s">
+        <v>97</v>
+      </c>
+      <c r="F21" s="39" t="s">
         <v>100</v>
       </c>
-      <c r="D15" s="43">
-        <v>150</v>
-      </c>
-      <c r="E15" s="43">
-        <v>150</v>
-      </c>
-      <c r="F15" s="43">
+      <c r="G21" s="39" t="s">
         <v>100</v>
       </c>
-      <c r="G15" s="43">
-        <v>150</v>
-      </c>
-      <c r="H15" s="43">
+      <c r="H21" s="39" t="s">
+        <v>101</v>
+      </c>
+      <c r="I21" s="39" t="s">
+        <v>102</v>
+      </c>
+      <c r="J21" s="39" t="s">
         <v>100</v>
-      </c>
-      <c r="I15" s="43">
-        <v>100</v>
-      </c>
-      <c r="J15" s="43">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" ht="12.75">
-      <c r="A16" s="33" t="s">
-        <v>108</v>
-      </c>
-      <c r="B16" s="43">
-        <v>20</v>
-      </c>
-      <c r="C16" s="43">
-        <v>65</v>
-      </c>
-      <c r="D16" s="43">
-        <v>20</v>
-      </c>
-      <c r="E16" s="43">
-        <v>45</v>
-      </c>
-      <c r="F16" s="43">
-        <v>20</v>
-      </c>
-      <c r="G16" s="43">
-        <v>20</v>
-      </c>
-      <c r="H16" s="43">
-        <v>65</v>
-      </c>
-      <c r="I16" s="43">
-        <v>20</v>
-      </c>
-      <c r="J16" s="43">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10" ht="12.75">
-      <c r="A19" s="33" t="s">
-        <v>46</v>
-      </c>
-      <c r="B19" s="43">
-        <v>3</v>
-      </c>
-      <c r="C19" s="43">
-        <v>3</v>
-      </c>
-      <c r="D19" s="43">
-        <v>3</v>
-      </c>
-      <c r="E19" s="43">
-        <v>3</v>
-      </c>
-      <c r="F19" s="43">
-        <v>3</v>
-      </c>
-      <c r="G19" s="43">
-        <v>3</v>
-      </c>
-      <c r="H19" s="43">
-        <v>3</v>
-      </c>
-      <c r="I19" s="43">
-        <v>3</v>
-      </c>
-      <c r="J19" s="43">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="20" spans="1:10" ht="12.75">
-      <c r="A20" s="33" t="s">
-        <v>47</v>
-      </c>
-      <c r="B20" s="52" t="s">
-        <v>99</v>
-      </c>
-      <c r="C20" s="53"/>
-      <c r="D20" s="53"/>
-      <c r="E20" s="53"/>
-      <c r="F20" s="53"/>
-      <c r="G20" s="53"/>
-      <c r="H20" s="53"/>
-      <c r="I20" s="53"/>
-      <c r="J20" s="54"/>
-    </row>
-    <row r="21" spans="1:10" ht="12.75">
-      <c r="A21" s="33" t="s">
-        <v>52</v>
-      </c>
-      <c r="B21" s="43" t="s">
-        <v>100</v>
-      </c>
-      <c r="C21" s="43" t="s">
-        <v>101</v>
-      </c>
-      <c r="D21" s="43" t="s">
-        <v>102</v>
-      </c>
-      <c r="E21" s="43" t="s">
-        <v>100</v>
-      </c>
-      <c r="F21" s="43" t="s">
-        <v>103</v>
-      </c>
-      <c r="G21" s="43" t="s">
-        <v>103</v>
-      </c>
-      <c r="H21" s="43" t="s">
-        <v>104</v>
-      </c>
-      <c r="I21" s="43" t="s">
-        <v>105</v>
-      </c>
-      <c r="J21" s="43" t="s">
-        <v>103</v>
       </c>
     </row>
   </sheetData>
@@ -4611,182 +4626,182 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="15.75" customHeight="1">
-      <c r="A1" s="32"/>
+      <c r="A1" s="28"/>
       <c r="B1" s="1" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="12.75">
+      <c r="A2" s="29" t="s">
+        <v>19</v>
+      </c>
+      <c r="B2" s="39" t="s">
+        <v>107</v>
+      </c>
+      <c r="C2" s="39" t="s">
+        <v>108</v>
+      </c>
+      <c r="D2" s="39" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" ht="12.75">
-      <c r="A2" s="33" t="s">
-        <v>19</v>
-      </c>
-      <c r="B2" s="43" t="s">
+      <c r="E2" s="39" t="s">
         <v>110</v>
       </c>
-      <c r="C2" s="43" t="s">
+      <c r="F2" s="39" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="12.75">
+      <c r="A3" s="29" t="s">
+        <v>33</v>
+      </c>
+      <c r="B3" s="39" t="s">
         <v>111</v>
       </c>
-      <c r="D2" s="43" t="s">
+      <c r="C3" s="39"/>
+      <c r="D3" s="39"/>
+      <c r="E3" s="39"/>
+      <c r="F3" s="39"/>
+    </row>
+    <row r="4" spans="1:6" ht="12.75">
+      <c r="A4" s="29" t="s">
+        <v>34</v>
+      </c>
+      <c r="B4" s="39"/>
+      <c r="C4" s="39"/>
+      <c r="D4" s="39"/>
+      <c r="E4" s="39"/>
+      <c r="F4" s="39"/>
+    </row>
+    <row r="5" spans="1:6" ht="12.75">
+      <c r="A5" s="29" t="s">
+        <v>35</v>
+      </c>
+      <c r="B5" s="39" t="s">
         <v>112</v>
       </c>
-      <c r="E2" s="43" t="s">
+      <c r="C5" s="39" t="s">
+        <v>112</v>
+      </c>
+      <c r="D5" s="39" t="s">
         <v>113</v>
       </c>
-      <c r="F2" s="43" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" ht="12.75">
-      <c r="A3" s="33" t="s">
-        <v>33</v>
-      </c>
-      <c r="B3" s="43" t="s">
+      <c r="E5" s="39" t="s">
+        <v>113</v>
+      </c>
+      <c r="F5" s="39" t="s">
         <v>114</v>
       </c>
-      <c r="C3" s="43"/>
-      <c r="D3" s="43"/>
-      <c r="E3" s="43"/>
-      <c r="F3" s="43"/>
-    </row>
-    <row r="4" spans="1:6" ht="12.75">
-      <c r="A4" s="33" t="s">
-        <v>34</v>
-      </c>
-      <c r="B4" s="43"/>
-      <c r="C4" s="43"/>
-      <c r="D4" s="43"/>
-      <c r="E4" s="43"/>
-      <c r="F4" s="43"/>
-    </row>
-    <row r="5" spans="1:6" ht="12.75">
-      <c r="A5" s="33" t="s">
-        <v>35</v>
-      </c>
-      <c r="B5" s="43" t="s">
+    </row>
+    <row r="6" spans="1:6" ht="12.75">
+      <c r="A6" s="29" t="s">
+        <v>36</v>
+      </c>
+      <c r="B6" s="39" t="s">
         <v>115</v>
       </c>
-      <c r="C5" s="43" t="s">
-        <v>115</v>
-      </c>
-      <c r="D5" s="43" t="s">
+      <c r="C6" s="39"/>
+      <c r="D6" s="39"/>
+      <c r="E6" s="39"/>
+      <c r="F6" s="39"/>
+    </row>
+    <row r="7" spans="1:6" ht="12.75">
+      <c r="A7" s="29" t="s">
+        <v>38</v>
+      </c>
+      <c r="B7" s="39"/>
+      <c r="C7" s="39"/>
+      <c r="D7" s="39"/>
+      <c r="E7" s="39"/>
+      <c r="F7" s="39"/>
+    </row>
+    <row r="8" spans="1:6" ht="12.75">
+      <c r="A8" s="29" t="s">
+        <v>40</v>
+      </c>
+      <c r="B8" s="43" t="s">
         <v>116</v>
       </c>
-      <c r="E5" s="43" t="s">
-        <v>116</v>
-      </c>
-      <c r="F5" s="43" t="s">
+      <c r="C8" s="39"/>
+      <c r="D8" s="39"/>
+      <c r="E8" s="39"/>
+      <c r="F8" s="39"/>
+    </row>
+    <row r="9" spans="1:6" ht="12.75">
+      <c r="A9" s="29" t="s">
+        <v>43</v>
+      </c>
+      <c r="B9" s="39" t="s">
         <v>117</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" ht="12.75">
-      <c r="A6" s="33" t="s">
-        <v>36</v>
-      </c>
-      <c r="B6" s="43" t="s">
+      <c r="C9" s="39"/>
+      <c r="D9" s="39" t="s">
+        <v>117</v>
+      </c>
+      <c r="E9" s="39"/>
+      <c r="F9" s="39" t="s">
         <v>118</v>
       </c>
-      <c r="C6" s="43"/>
-      <c r="D6" s="43"/>
-      <c r="E6" s="43"/>
-      <c r="F6" s="43"/>
-    </row>
-    <row r="7" spans="1:6" ht="12.75">
-      <c r="A7" s="33" t="s">
-        <v>38</v>
-      </c>
-      <c r="B7" s="43"/>
-      <c r="C7" s="43"/>
-      <c r="D7" s="43"/>
-      <c r="E7" s="43"/>
-      <c r="F7" s="43"/>
-    </row>
-    <row r="8" spans="1:6" ht="12.75">
-      <c r="A8" s="33" t="s">
-        <v>43</v>
-      </c>
-      <c r="B8" s="47" t="s">
+    </row>
+    <row r="10" spans="1:6" ht="12.75">
+      <c r="A10" s="29" t="s">
+        <v>44</v>
+      </c>
+      <c r="B10" s="39"/>
+      <c r="C10" s="39"/>
+      <c r="D10" s="39"/>
+      <c r="E10" s="39"/>
+      <c r="F10" s="39"/>
+    </row>
+    <row r="11" spans="1:6" ht="12.75">
+      <c r="A11" s="29" t="s">
+        <v>45</v>
+      </c>
+      <c r="B11" s="39" t="s">
         <v>119</v>
       </c>
-      <c r="C8" s="43"/>
-      <c r="D8" s="43"/>
-      <c r="E8" s="43"/>
-      <c r="F8" s="43"/>
-    </row>
-    <row r="9" spans="1:6" ht="12.75">
-      <c r="A9" s="33" t="s">
-        <v>46</v>
-      </c>
-      <c r="B9" s="43" t="s">
-        <v>120</v>
-      </c>
-      <c r="C9" s="43"/>
-      <c r="D9" s="43" t="s">
-        <v>120</v>
-      </c>
-      <c r="E9" s="43"/>
-      <c r="F9" s="43" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" ht="12.75">
-      <c r="A10" s="33" t="s">
-        <v>47</v>
-      </c>
-      <c r="B10" s="43"/>
-      <c r="C10" s="43"/>
-      <c r="D10" s="43"/>
-      <c r="E10" s="43"/>
-      <c r="F10" s="43"/>
-    </row>
-    <row r="11" spans="1:6" ht="12.75">
-      <c r="A11" s="33" t="s">
-        <v>48</v>
-      </c>
-      <c r="B11" s="43" t="s">
-        <v>122</v>
-      </c>
-      <c r="C11" s="43" t="s">
-        <v>122</v>
-      </c>
-      <c r="D11" s="43" t="s">
-        <v>122</v>
-      </c>
-      <c r="E11" s="43" t="s">
-        <v>122</v>
-      </c>
-      <c r="F11" s="43" t="s">
-        <v>122</v>
+      <c r="C11" s="39" t="s">
+        <v>119</v>
+      </c>
+      <c r="D11" s="39" t="s">
+        <v>119</v>
+      </c>
+      <c r="E11" s="39" t="s">
+        <v>119</v>
+      </c>
+      <c r="F11" s="39" t="s">
+        <v>119</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="12.75">
-      <c r="A12" s="33" t="s">
-        <v>52</v>
-      </c>
-      <c r="B12" s="43">
+      <c r="A12" s="29" t="s">
+        <v>49</v>
+      </c>
+      <c r="B12" s="39">
         <v>13.7</v>
       </c>
-      <c r="C12" s="43">
+      <c r="C12" s="39">
         <v>13</v>
       </c>
-      <c r="D12" s="43"/>
-      <c r="E12" s="43">
+      <c r="D12" s="39"/>
+      <c r="E12" s="39">
         <v>9.9</v>
       </c>
-      <c r="F12" s="43"/>
+      <c r="F12" s="39"/>
     </row>
     <row r="13" spans="1:6" ht="12.75">
-      <c r="A13" s="33" t="s">
-        <v>53</v>
-      </c>
-      <c r="B13" s="43"/>
-      <c r="C13" s="43"/>
-      <c r="D13" s="43"/>
-      <c r="E13" s="43"/>
-      <c r="F13" s="43"/>
+      <c r="A13" s="29" t="s">
+        <v>50</v>
+      </c>
+      <c r="B13" s="39"/>
+      <c r="C13" s="39"/>
+      <c r="D13" s="39"/>
+      <c r="E13" s="39"/>
+      <c r="F13" s="39"/>
     </row>
     <row r="14" spans="1:6" ht="12.75">
       <c r="A14" s="1" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="B14" s="1" t="b">
         <v>1</v>

</xml_diff>

<commit_message>
final excel file fix. Sowing dates are now the correct date and not duplicates
</commit_message>
<xml_diff>
--- a/heliostrome/jip_project/results/Factors to run simulation.xlsx
+++ b/heliostrome/jip_project/results/Factors to run simulation.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://tud365-my.sharepoint.com/personal/sparijs_tudelft_nl/Documents/Documents/helios/heliostrome/heliostrome/jip_project/results/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="51" documentId="11_D32365DB1BF81EFE359F33EE7A0E21B336E84D7E" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3F74CFFE-D5C9-4C08-899F-6715B9EF57AA}"/>
+  <xr:revisionPtr revIDLastSave="10" documentId="13_ncr:1_{4F584D95-94A6-41DE-B6E7-9DF03E400742}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4F380E3C-06E1-447B-8706-D566F853BC6C}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15360" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="All Case Studies (compatability" sheetId="1" r:id="rId1"/>
@@ -929,7 +929,21 @@
         </r>
       </text>
     </comment>
-    <comment ref="J7" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000003000000}">
+    <comment ref="J8" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000001000000}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Arial"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>says also clay but given i cant find an initial water content i think it's sandy
+	-Tabitha Minett</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="J19" authorId="0" shapeId="0" xr:uid="{B6F1F042-4155-43C6-81D0-51E2EE18DCC7}">
       <text>
         <r>
           <rPr>
@@ -939,20 +953,6 @@
             <scheme val="minor"/>
           </rPr>
           <t>2 sowing dates
-	-Tabitha Minett</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="J8" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000001000000}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Arial"/>
-            <scheme val="minor"/>
-          </rPr>
-          <t>says also clay but given i cant find an initial water content i think it's sandy
 	-Tabitha Minett</t>
         </r>
       </text>
@@ -1192,7 +1192,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="294" uniqueCount="135">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="294" uniqueCount="134">
   <si>
     <t>Lowering the cost - MIT</t>
   </si>
@@ -1309,9 +1309,6 @@
   </si>
   <si>
     <t>Sowing Date</t>
-  </si>
-  <si>
-    <t>26/06/2012</t>
   </si>
   <si>
     <t>Soil Type</t>
@@ -1608,7 +1605,7 @@
     <numFmt numFmtId="164" formatCode="mm/dd/yyyy"/>
     <numFmt numFmtId="165" formatCode="m/d/yyyy"/>
   </numFmts>
-  <fonts count="15">
+  <fonts count="16">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -1693,8 +1690,15 @@
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1737,8 +1741,14 @@
         <bgColor rgb="FFFF9900"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="10">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -1857,11 +1867,41 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="52">
+  <cellXfs count="53">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1872,64 +1912,6 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="4" fontId="6" fillId="6" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="4" fontId="6" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="3" fontId="6" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1973,9 +1955,28 @@
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="6" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
+    <xf numFmtId="14" fontId="15" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="14" fontId="15" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="14" fontId="15" fillId="8" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="14" fontId="6" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="4" fontId="6" fillId="6" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="4" fontId="6" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="3" fontId="6" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2000,10 +2001,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2389,1073 +2386,1108 @@
   <dimension ref="A1:Q27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="K1" activePane="topRight" state="frozen"/>
+      <pane xSplit="1" topLeftCell="P1" activePane="topRight" state="frozen"/>
       <selection pane="topRight" activeCell="B5" sqref="B5:Q7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="46.85546875" customWidth="1"/>
-    <col min="2" max="15" width="24.28515625" customWidth="1"/>
-    <col min="16" max="16" width="24" customWidth="1"/>
+    <col min="1" max="1" width="46.85546875" style="35" customWidth="1"/>
+    <col min="2" max="15" width="24.28515625" style="35" customWidth="1"/>
+    <col min="16" max="16" width="24" style="35" customWidth="1"/>
+    <col min="17" max="16384" width="12.5703125" style="35"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="15.75" customHeight="1">
-      <c r="A1" s="8"/>
-      <c r="B1" s="8" t="s">
+      <c r="A1" s="37"/>
+      <c r="B1" s="37" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="8"/>
-      <c r="D1" s="8"/>
-      <c r="E1" s="8"/>
-      <c r="F1" s="8"/>
-      <c r="G1" s="8"/>
-      <c r="H1" s="8"/>
-      <c r="I1" s="8"/>
-      <c r="J1" s="8"/>
-      <c r="K1" s="8"/>
-      <c r="L1" s="9"/>
-      <c r="M1" s="9"/>
-      <c r="N1" s="9"/>
-      <c r="O1" s="9"/>
-      <c r="P1" s="10"/>
-      <c r="Q1" s="10"/>
+      <c r="C1" s="37"/>
+      <c r="D1" s="37"/>
+      <c r="E1" s="37"/>
+      <c r="F1" s="37"/>
+      <c r="G1" s="37"/>
+      <c r="H1" s="37"/>
+      <c r="I1" s="37"/>
+      <c r="J1" s="37"/>
+      <c r="K1" s="37"/>
+      <c r="L1" s="36"/>
+      <c r="M1" s="36"/>
+      <c r="N1" s="36"/>
+      <c r="O1" s="36"/>
+      <c r="P1" s="36"/>
+      <c r="Q1" s="36"/>
     </row>
     <row r="2" spans="1:17" ht="12.75">
-      <c r="A2" s="11" t="s">
+      <c r="A2" s="38" t="s">
         <v>19</v>
       </c>
-      <c r="B2" s="12" t="s">
+      <c r="B2" s="39" t="s">
         <v>20</v>
       </c>
-      <c r="C2" s="12" t="s">
+      <c r="C2" s="39" t="s">
         <v>21</v>
       </c>
-      <c r="D2" s="12" t="s">
+      <c r="D2" s="39" t="s">
         <v>21</v>
       </c>
-      <c r="E2" s="12" t="s">
+      <c r="E2" s="39" t="s">
         <v>22</v>
       </c>
-      <c r="F2" s="12" t="s">
+      <c r="F2" s="39" t="s">
         <v>23</v>
       </c>
-      <c r="G2" s="12" t="s">
+      <c r="G2" s="39" t="s">
         <v>22</v>
       </c>
-      <c r="H2" s="12" t="s">
+      <c r="H2" s="39" t="s">
         <v>23</v>
       </c>
-      <c r="I2" s="12" t="s">
+      <c r="I2" s="39" t="s">
         <v>24</v>
       </c>
-      <c r="J2" s="12" t="s">
+      <c r="J2" s="39" t="s">
         <v>25</v>
       </c>
-      <c r="K2" s="12" t="s">
+      <c r="K2" s="39" t="s">
         <v>26</v>
       </c>
-      <c r="L2" s="12" t="s">
+      <c r="L2" s="39" t="s">
         <v>27</v>
       </c>
-      <c r="M2" s="12" t="s">
+      <c r="M2" s="39" t="s">
         <v>28</v>
       </c>
-      <c r="N2" s="12" t="s">
+      <c r="N2" s="39" t="s">
         <v>29</v>
       </c>
-      <c r="O2" s="12" t="s">
+      <c r="O2" s="39" t="s">
         <v>30</v>
       </c>
-      <c r="P2" s="12" t="s">
+      <c r="P2" s="39" t="s">
         <v>31</v>
       </c>
-      <c r="Q2" s="12" t="s">
+      <c r="Q2" s="39" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="3" spans="1:17" ht="12.75">
-      <c r="A3" s="13" t="s">
+      <c r="A3" s="40" t="s">
         <v>33</v>
       </c>
-      <c r="B3" s="14">
+      <c r="B3" s="41">
         <v>90.41</v>
       </c>
-      <c r="C3" s="14">
+      <c r="C3" s="41">
         <v>90.41</v>
       </c>
-      <c r="D3" s="14">
+      <c r="D3" s="41">
         <v>90.41</v>
       </c>
-      <c r="E3" s="14">
+      <c r="E3" s="41">
         <v>90.41</v>
       </c>
-      <c r="F3" s="14">
+      <c r="F3" s="41">
         <v>90.41</v>
       </c>
-      <c r="G3" s="14">
+      <c r="G3" s="41">
         <v>90.41</v>
       </c>
-      <c r="H3" s="14">
+      <c r="H3" s="41">
         <v>90.41</v>
       </c>
-      <c r="I3" s="15">
+      <c r="I3" s="41">
         <v>89.94</v>
       </c>
-      <c r="J3" s="15">
+      <c r="J3" s="41">
         <v>89.94</v>
       </c>
-      <c r="K3" s="15">
+      <c r="K3" s="41">
         <v>89.94</v>
       </c>
-      <c r="L3" s="15">
+      <c r="L3" s="41">
         <v>89.94</v>
       </c>
-      <c r="M3" s="15">
+      <c r="M3" s="41">
         <v>89.94</v>
       </c>
-      <c r="N3" s="15">
+      <c r="N3" s="41">
         <v>89.94</v>
       </c>
-      <c r="O3" s="14">
+      <c r="O3" s="41">
         <v>90.41</v>
       </c>
-      <c r="P3" s="15">
+      <c r="P3" s="41">
         <v>89.42</v>
       </c>
-      <c r="Q3" s="15">
+      <c r="Q3" s="41">
         <v>90.37</v>
       </c>
     </row>
     <row r="4" spans="1:17" ht="12.75">
-      <c r="A4" s="13" t="s">
+      <c r="A4" s="40" t="s">
         <v>34</v>
       </c>
-      <c r="B4" s="14">
+      <c r="B4" s="41">
         <v>24.1</v>
       </c>
-      <c r="C4" s="14">
+      <c r="C4" s="41">
         <v>24.1</v>
       </c>
-      <c r="D4" s="14">
+      <c r="D4" s="41">
         <v>24.1</v>
       </c>
-      <c r="E4" s="14">
+      <c r="E4" s="41">
         <v>24.1</v>
       </c>
-      <c r="F4" s="14">
+      <c r="F4" s="41">
         <v>24.1</v>
       </c>
-      <c r="G4" s="14">
+      <c r="G4" s="41">
         <v>24.1</v>
       </c>
-      <c r="H4" s="14">
+      <c r="H4" s="41">
         <v>24.1</v>
       </c>
-      <c r="I4" s="15">
+      <c r="I4" s="41">
         <v>24.92</v>
       </c>
-      <c r="J4" s="15">
+      <c r="J4" s="41">
         <v>24.92</v>
       </c>
-      <c r="K4" s="15">
+      <c r="K4" s="41">
         <v>24.92</v>
       </c>
-      <c r="L4" s="15">
+      <c r="L4" s="41">
         <v>24.92</v>
       </c>
-      <c r="M4" s="15">
+      <c r="M4" s="41">
         <v>24.92</v>
       </c>
-      <c r="N4" s="15">
+      <c r="N4" s="41">
         <v>24.92</v>
       </c>
-      <c r="O4" s="14">
+      <c r="O4" s="41">
         <v>24.1</v>
       </c>
-      <c r="P4" s="15">
+      <c r="P4" s="41">
         <v>23.49</v>
       </c>
-      <c r="Q4" s="15">
+      <c r="Q4" s="41">
         <v>22.7</v>
       </c>
     </row>
     <row r="5" spans="1:17" ht="11.25" customHeight="1">
-      <c r="A5" s="13" t="s">
+      <c r="A5" s="40" t="s">
         <v>35</v>
       </c>
-      <c r="B5" s="51">
+      <c r="B5" s="42">
         <v>40179</v>
       </c>
-      <c r="C5" s="51">
+      <c r="C5" s="42">
         <v>40179</v>
       </c>
-      <c r="D5" s="51">
+      <c r="D5" s="42">
         <v>40179</v>
       </c>
-      <c r="E5" s="51">
+      <c r="E5" s="42">
         <v>40179</v>
       </c>
-      <c r="F5" s="51">
+      <c r="F5" s="42">
         <v>40179</v>
       </c>
-      <c r="G5" s="51">
+      <c r="G5" s="42">
         <v>40179</v>
       </c>
-      <c r="H5" s="51">
+      <c r="H5" s="42">
         <v>40179</v>
       </c>
-      <c r="I5" s="51">
+      <c r="I5" s="42">
         <v>40179</v>
       </c>
-      <c r="J5" s="51">
+      <c r="J5" s="42">
         <v>40179</v>
       </c>
-      <c r="K5" s="51">
+      <c r="K5" s="42">
         <v>40179</v>
       </c>
-      <c r="L5" s="51">
+      <c r="L5" s="42">
         <v>40179</v>
       </c>
-      <c r="M5" s="51">
+      <c r="M5" s="42">
         <v>40179</v>
       </c>
-      <c r="N5" s="51">
+      <c r="N5" s="42">
         <v>40179</v>
       </c>
-      <c r="O5" s="51">
+      <c r="O5" s="42">
         <v>40179</v>
       </c>
-      <c r="P5" s="51">
+      <c r="P5" s="42">
         <v>40179</v>
       </c>
-      <c r="Q5" s="51">
+      <c r="Q5" s="42">
         <v>40179</v>
       </c>
     </row>
-    <row r="6" spans="1:17" ht="12.75">
-      <c r="A6" s="13" t="s">
+    <row r="6" spans="1:17" ht="13.5" thickBot="1">
+      <c r="A6" s="40" t="s">
         <v>36</v>
       </c>
-      <c r="B6" s="51">
+      <c r="B6" s="42">
         <v>41639</v>
       </c>
-      <c r="C6" s="51">
+      <c r="C6" s="42">
         <v>41639</v>
       </c>
-      <c r="D6" s="51">
+      <c r="D6" s="42">
         <v>41639</v>
       </c>
-      <c r="E6" s="51">
+      <c r="E6" s="42">
         <v>41639</v>
       </c>
-      <c r="F6" s="51">
+      <c r="F6" s="42">
         <v>41639</v>
       </c>
-      <c r="G6" s="51">
+      <c r="G6" s="42">
         <v>41639</v>
       </c>
-      <c r="H6" s="51">
+      <c r="H6" s="42">
         <v>41639</v>
       </c>
-      <c r="I6" s="51">
+      <c r="I6" s="42">
         <v>41639</v>
       </c>
-      <c r="J6" s="51">
+      <c r="J6" s="42">
         <v>41639</v>
       </c>
-      <c r="K6" s="51">
+      <c r="K6" s="42">
         <v>41639</v>
       </c>
-      <c r="L6" s="51">
+      <c r="L6" s="42">
         <v>41639</v>
       </c>
-      <c r="M6" s="51">
+      <c r="M6" s="42">
         <v>41639</v>
       </c>
-      <c r="N6" s="51">
+      <c r="N6" s="42">
         <v>41639</v>
       </c>
-      <c r="O6" s="51">
+      <c r="O6" s="42">
         <v>41639</v>
       </c>
-      <c r="P6" s="51">
+      <c r="P6" s="42">
         <v>41639</v>
       </c>
-      <c r="Q6" s="51">
+      <c r="Q6" s="42">
         <v>41639</v>
       </c>
     </row>
-    <row r="7" spans="1:17" ht="12.75">
-      <c r="A7" s="13" t="s">
+    <row r="7" spans="1:17" s="34" customFormat="1" ht="13.5" thickBot="1">
+      <c r="A7" s="40" t="s">
         <v>38</v>
       </c>
-      <c r="B7" s="51" t="s">
+      <c r="B7" s="31">
+        <v>41086</v>
+      </c>
+      <c r="C7" s="32">
+        <v>41086</v>
+      </c>
+      <c r="D7" s="32">
+        <v>41086</v>
+      </c>
+      <c r="E7" s="32">
+        <v>40881</v>
+      </c>
+      <c r="F7" s="32">
+        <v>40881</v>
+      </c>
+      <c r="G7" s="32">
+        <v>40881</v>
+      </c>
+      <c r="H7" s="32">
+        <v>40881</v>
+      </c>
+      <c r="I7" s="33">
+        <v>40486</v>
+      </c>
+      <c r="J7" s="33">
+        <v>40486</v>
+      </c>
+      <c r="K7" s="32">
+        <v>41230</v>
+      </c>
+      <c r="L7" s="32">
+        <v>41230</v>
+      </c>
+      <c r="M7" s="32">
+        <v>40462</v>
+      </c>
+      <c r="N7" s="32">
+        <v>40462</v>
+      </c>
+      <c r="O7" s="32">
+        <v>38679</v>
+      </c>
+      <c r="P7" s="32">
+        <v>38381</v>
+      </c>
+      <c r="Q7" s="32">
+        <v>38387</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" ht="12.75">
+      <c r="A8" s="40" t="s">
         <v>39</v>
       </c>
-      <c r="C7" s="51" t="s">
+      <c r="B8" s="41" t="s">
+        <v>40</v>
+      </c>
+      <c r="C8" s="41" t="s">
+        <v>40</v>
+      </c>
+      <c r="D8" s="41" t="s">
+        <v>40</v>
+      </c>
+      <c r="E8" s="41" t="s">
+        <v>40</v>
+      </c>
+      <c r="F8" s="41" t="s">
+        <v>40</v>
+      </c>
+      <c r="G8" s="41" t="s">
+        <v>40</v>
+      </c>
+      <c r="H8" s="41" t="s">
+        <v>40</v>
+      </c>
+      <c r="I8" s="43" t="s">
+        <v>41</v>
+      </c>
+      <c r="J8" s="43" t="s">
+        <v>41</v>
+      </c>
+      <c r="K8" s="41" t="s">
+        <v>41</v>
+      </c>
+      <c r="L8" s="41" t="s">
+        <v>41</v>
+      </c>
+      <c r="M8" s="41" t="s">
+        <v>41</v>
+      </c>
+      <c r="N8" s="41" t="s">
+        <v>41</v>
+      </c>
+      <c r="O8" s="41" t="s">
+        <v>40</v>
+      </c>
+      <c r="P8" s="41" t="s">
+        <v>40</v>
+      </c>
+      <c r="Q8" s="41" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" ht="12.75">
+      <c r="A9" s="40" t="s">
+        <v>42</v>
+      </c>
+      <c r="B9" s="41">
+        <v>35</v>
+      </c>
+      <c r="C9" s="41">
+        <v>35</v>
+      </c>
+      <c r="D9" s="41">
+        <v>35</v>
+      </c>
+      <c r="E9" s="41">
+        <v>35</v>
+      </c>
+      <c r="F9" s="41">
+        <v>35</v>
+      </c>
+      <c r="G9" s="41">
+        <v>35</v>
+      </c>
+      <c r="H9" s="41">
+        <v>35</v>
+      </c>
+      <c r="I9" s="41">
+        <v>33</v>
+      </c>
+      <c r="J9" s="41">
+        <v>33</v>
+      </c>
+      <c r="K9" s="41">
+        <v>30</v>
+      </c>
+      <c r="L9" s="41">
+        <v>30</v>
+      </c>
+      <c r="M9" s="41">
+        <v>32</v>
+      </c>
+      <c r="N9" s="41">
+        <v>32</v>
+      </c>
+      <c r="O9" s="41">
+        <v>100</v>
+      </c>
+      <c r="P9" s="44">
+        <v>100</v>
+      </c>
+      <c r="Q9" s="45">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" ht="12.75">
+      <c r="A10" s="40" t="s">
+        <v>43</v>
+      </c>
+      <c r="B10" s="41">
+        <v>26</v>
+      </c>
+      <c r="C10" s="41">
+        <v>26</v>
+      </c>
+      <c r="D10" s="41">
+        <v>26</v>
+      </c>
+      <c r="E10" s="41">
+        <v>26</v>
+      </c>
+      <c r="F10" s="41">
+        <v>26</v>
+      </c>
+      <c r="G10" s="41">
+        <v>26</v>
+      </c>
+      <c r="H10" s="41">
+        <v>26</v>
+      </c>
+      <c r="I10" s="41">
+        <v>22</v>
+      </c>
+      <c r="J10" s="41">
+        <v>22</v>
+      </c>
+      <c r="K10" s="41">
+        <v>22</v>
+      </c>
+      <c r="L10" s="41">
+        <v>22</v>
+      </c>
+      <c r="M10" s="41">
+        <v>22</v>
+      </c>
+      <c r="N10" s="41">
+        <v>22</v>
+      </c>
+      <c r="O10" s="41">
+        <v>26</v>
+      </c>
+      <c r="P10" s="43">
+        <v>50</v>
+      </c>
+      <c r="Q10" s="41">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" ht="12.75">
+      <c r="A11" s="40" t="s">
+        <v>44</v>
+      </c>
+      <c r="B11" s="41" t="s">
+        <v>45</v>
+      </c>
+      <c r="C11" s="41" t="s">
+        <v>45</v>
+      </c>
+      <c r="D11" s="41" t="s">
+        <v>45</v>
+      </c>
+      <c r="E11" s="41" t="s">
+        <v>45</v>
+      </c>
+      <c r="F11" s="41" t="s">
+        <v>45</v>
+      </c>
+      <c r="G11" s="41" t="s">
+        <v>45</v>
+      </c>
+      <c r="H11" s="41" t="s">
+        <v>45</v>
+      </c>
+      <c r="I11" s="41" t="s">
+        <v>45</v>
+      </c>
+      <c r="J11" s="41" t="s">
+        <v>45</v>
+      </c>
+      <c r="K11" s="41" t="s">
+        <v>45</v>
+      </c>
+      <c r="L11" s="41" t="s">
+        <v>45</v>
+      </c>
+      <c r="M11" s="41" t="s">
+        <v>45</v>
+      </c>
+      <c r="N11" s="41" t="s">
+        <v>45</v>
+      </c>
+      <c r="O11" s="41" t="s">
+        <v>46</v>
+      </c>
+      <c r="P11" s="41" t="s">
+        <v>47</v>
+      </c>
+      <c r="Q11" s="41" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" ht="12.75">
+      <c r="A12" s="40" t="s">
+        <v>48</v>
+      </c>
+      <c r="B12" s="41">
+        <v>31.86</v>
+      </c>
+      <c r="C12" s="41">
+        <v>33.729999999999997</v>
+      </c>
+      <c r="D12" s="41">
+        <v>35.28</v>
+      </c>
+      <c r="E12" s="41">
+        <v>62.95</v>
+      </c>
+      <c r="F12" s="41">
+        <v>53.52</v>
+      </c>
+      <c r="G12" s="41">
+        <v>39.92</v>
+      </c>
+      <c r="H12" s="41">
+        <v>30.53</v>
+      </c>
+      <c r="I12" s="41">
+        <v>35.64</v>
+      </c>
+      <c r="J12" s="41">
+        <v>33.83</v>
+      </c>
+      <c r="K12" s="41">
+        <v>27.29</v>
+      </c>
+      <c r="L12" s="41">
+        <v>25.82</v>
+      </c>
+      <c r="M12" s="41">
+        <v>35.18</v>
+      </c>
+      <c r="N12" s="41">
+        <v>32.659999999999997</v>
+      </c>
+      <c r="O12" s="41">
+        <v>3</v>
+      </c>
+      <c r="P12" s="41">
+        <v>2.5</v>
+      </c>
+      <c r="Q12" s="41">
+        <v>3.4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" ht="12.75">
+      <c r="A13" s="40" t="s">
+        <v>49</v>
+      </c>
+      <c r="B13" s="41">
+        <v>429</v>
+      </c>
+      <c r="C13" s="41">
+        <v>225</v>
+      </c>
+      <c r="D13" s="41">
+        <v>212</v>
+      </c>
+      <c r="E13" s="41">
+        <v>254</v>
+      </c>
+      <c r="F13" s="41">
+        <v>590</v>
+      </c>
+      <c r="G13" s="41">
+        <v>335</v>
+      </c>
+      <c r="H13" s="41">
+        <v>610</v>
+      </c>
+      <c r="I13" s="41">
+        <v>249</v>
+      </c>
+      <c r="J13" s="41">
+        <v>568</v>
+      </c>
+      <c r="K13" s="41">
+        <v>228</v>
+      </c>
+      <c r="L13" s="41">
+        <v>453</v>
+      </c>
+      <c r="M13" s="41" t="s">
+        <v>50</v>
+      </c>
+      <c r="N13" s="41" t="s">
+        <v>51</v>
+      </c>
+      <c r="O13" s="41">
+        <v>430</v>
+      </c>
+      <c r="P13" s="46">
+        <v>1324</v>
+      </c>
+      <c r="Q13" s="46">
+        <v>1252</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17" ht="15.75" customHeight="1">
+      <c r="A14" s="36"/>
+      <c r="B14" s="36"/>
+      <c r="C14" s="36"/>
+      <c r="D14" s="36"/>
+      <c r="E14" s="36"/>
+      <c r="F14" s="36"/>
+      <c r="G14" s="36"/>
+      <c r="H14" s="36"/>
+      <c r="I14" s="36"/>
+      <c r="J14" s="36"/>
+      <c r="K14" s="36"/>
+      <c r="L14" s="36"/>
+      <c r="M14" s="36"/>
+      <c r="N14" s="36"/>
+      <c r="O14" s="36"/>
+      <c r="P14" s="36"/>
+      <c r="Q14" s="36"/>
+    </row>
+    <row r="15" spans="1:17" ht="12.75">
+      <c r="A15" s="38" t="s">
+        <v>35</v>
+      </c>
+      <c r="B15" s="47">
+        <v>40548</v>
+      </c>
+      <c r="C15" s="47">
+        <v>40548</v>
+      </c>
+      <c r="D15" s="43" t="s">
+        <v>52</v>
+      </c>
+      <c r="E15" s="47">
+        <v>40553</v>
+      </c>
+      <c r="F15" s="47">
+        <v>40553</v>
+      </c>
+      <c r="G15" s="47">
+        <v>40918</v>
+      </c>
+      <c r="H15" s="47">
+        <v>40918</v>
+      </c>
+      <c r="I15" s="43" t="s">
+        <v>53</v>
+      </c>
+      <c r="J15" s="43" t="s">
+        <v>53</v>
+      </c>
+      <c r="K15" s="47">
+        <v>40544</v>
+      </c>
+      <c r="L15" s="47">
+        <v>40544</v>
+      </c>
+      <c r="M15" s="47">
+        <v>40179</v>
+      </c>
+      <c r="N15" s="47">
+        <v>40179</v>
+      </c>
+      <c r="O15" s="47">
+        <v>40544</v>
+      </c>
+      <c r="P15" s="47">
+        <v>40544</v>
+      </c>
+      <c r="Q15" s="47">
+        <v>40544</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17" ht="12.75">
+      <c r="A16" s="40" t="s">
+        <v>36</v>
+      </c>
+      <c r="B16" s="48">
+        <v>40913</v>
+      </c>
+      <c r="C16" s="48">
+        <v>40913</v>
+      </c>
+      <c r="D16" s="41" t="s">
+        <v>54</v>
+      </c>
+      <c r="E16" s="41" t="s">
+        <v>55</v>
+      </c>
+      <c r="F16" s="41" t="s">
+        <v>55</v>
+      </c>
+      <c r="G16" s="41" t="s">
+        <v>56</v>
+      </c>
+      <c r="H16" s="41" t="s">
+        <v>56</v>
+      </c>
+      <c r="I16" s="41" t="s">
+        <v>57</v>
+      </c>
+      <c r="J16" s="41" t="s">
+        <v>57</v>
+      </c>
+      <c r="K16" s="41" t="s">
+        <v>58</v>
+      </c>
+      <c r="L16" s="41" t="s">
+        <v>58</v>
+      </c>
+      <c r="M16" s="41" t="s">
+        <v>37</v>
+      </c>
+      <c r="N16" s="41" t="s">
+        <v>37</v>
+      </c>
+      <c r="O16" s="41" t="s">
+        <v>37</v>
+      </c>
+      <c r="P16" s="41" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q16" s="41" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="17" spans="1:17" ht="12.75">
+      <c r="A17" s="40" t="s">
+        <v>42</v>
+      </c>
+      <c r="B17" s="41" t="s">
+        <v>59</v>
+      </c>
+      <c r="C17" s="41" t="s">
+        <v>60</v>
+      </c>
+      <c r="D17" s="41" t="s">
+        <v>60</v>
+      </c>
+      <c r="E17" s="41" t="s">
+        <v>60</v>
+      </c>
+      <c r="F17" s="41" t="s">
+        <v>59</v>
+      </c>
+      <c r="G17" s="41" t="s">
+        <v>60</v>
+      </c>
+      <c r="H17" s="41" t="s">
+        <v>59</v>
+      </c>
+      <c r="I17" s="41" t="s">
+        <v>61</v>
+      </c>
+      <c r="J17" s="41" t="s">
+        <v>62</v>
+      </c>
+      <c r="K17" s="41" t="s">
+        <v>63</v>
+      </c>
+      <c r="L17" s="41" t="s">
+        <v>64</v>
+      </c>
+      <c r="M17" s="41" t="s">
+        <v>65</v>
+      </c>
+      <c r="N17" s="41" t="s">
+        <v>66</v>
+      </c>
+      <c r="O17" s="41" t="s">
+        <v>67</v>
+      </c>
+      <c r="P17" s="49">
+        <v>100</v>
+      </c>
+      <c r="Q17" s="50">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="18" spans="1:17" ht="12.75">
+      <c r="A18" s="40" t="s">
+        <v>43</v>
+      </c>
+      <c r="B18" s="41">
+        <v>26</v>
+      </c>
+      <c r="C18" s="41">
+        <v>26</v>
+      </c>
+      <c r="D18" s="41">
+        <v>26</v>
+      </c>
+      <c r="E18" s="41">
+        <v>26</v>
+      </c>
+      <c r="F18" s="41">
+        <v>26</v>
+      </c>
+      <c r="G18" s="41">
+        <v>26</v>
+      </c>
+      <c r="H18" s="41">
+        <v>26</v>
+      </c>
+      <c r="I18" s="41" t="s">
+        <v>68</v>
+      </c>
+      <c r="J18" s="41" t="s">
+        <v>68</v>
+      </c>
+      <c r="K18" s="41"/>
+      <c r="L18" s="41" t="s">
+        <v>68</v>
+      </c>
+      <c r="M18" s="41" t="s">
+        <v>68</v>
+      </c>
+      <c r="N18" s="41" t="s">
+        <v>68</v>
+      </c>
+      <c r="O18" s="41" t="s">
+        <v>68</v>
+      </c>
+      <c r="P18" s="43" t="s">
+        <v>69</v>
+      </c>
+      <c r="Q18" s="41" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="19" spans="1:17" s="34" customFormat="1" ht="12.75">
+      <c r="A19" s="40" t="s">
+        <v>38</v>
+      </c>
+      <c r="B19" s="42">
+        <v>41086</v>
+      </c>
+      <c r="C19" s="42" t="s">
+        <v>120</v>
+      </c>
+      <c r="D19" s="42" t="s">
         <v>121</v>
       </c>
-      <c r="D7" s="51" t="s">
+      <c r="E19" s="42" t="s">
         <v>122</v>
       </c>
-      <c r="E7" s="51" t="s">
+      <c r="F19" s="42" t="s">
         <v>123</v>
       </c>
-      <c r="F7" s="51" t="s">
+      <c r="G19" s="42" t="s">
         <v>124</v>
       </c>
-      <c r="G7" s="51" t="s">
+      <c r="H19" s="42" t="s">
         <v>125</v>
       </c>
-      <c r="H7" s="51" t="s">
+      <c r="I19" s="42" t="s">
         <v>126</v>
       </c>
-      <c r="I7" s="51" t="s">
+      <c r="J19" s="42" t="s">
         <v>127</v>
       </c>
-      <c r="J7" s="51" t="s">
+      <c r="K19" s="42" t="s">
         <v>128</v>
       </c>
-      <c r="K7" s="51" t="s">
+      <c r="L19" s="42" t="s">
         <v>129</v>
       </c>
-      <c r="L7" s="51" t="s">
+      <c r="M19" s="42" t="s">
         <v>130</v>
       </c>
-      <c r="M7" s="51" t="s">
+      <c r="N19" s="42" t="s">
         <v>131</v>
       </c>
-      <c r="N7" s="51" t="s">
+      <c r="O19" s="42" t="s">
         <v>132</v>
       </c>
-      <c r="O7" s="51" t="s">
+      <c r="P19" s="42" t="s">
         <v>133</v>
       </c>
-      <c r="P7" s="51" t="s">
-        <v>134</v>
-      </c>
-      <c r="Q7" s="51">
+      <c r="Q19" s="42">
         <v>38444</v>
       </c>
     </row>
-    <row r="8" spans="1:17" ht="12.75">
-      <c r="A8" s="13" t="s">
-        <v>40</v>
-      </c>
-      <c r="B8" s="14" t="s">
-        <v>41</v>
-      </c>
-      <c r="C8" s="14" t="s">
-        <v>41</v>
-      </c>
-      <c r="D8" s="14" t="s">
-        <v>41</v>
-      </c>
-      <c r="E8" s="14" t="s">
-        <v>41</v>
-      </c>
-      <c r="F8" s="14" t="s">
-        <v>41</v>
-      </c>
-      <c r="G8" s="14" t="s">
-        <v>41</v>
-      </c>
-      <c r="H8" s="14" t="s">
-        <v>41</v>
-      </c>
-      <c r="I8" s="17" t="s">
-        <v>42</v>
-      </c>
-      <c r="J8" s="17" t="s">
-        <v>42</v>
-      </c>
-      <c r="K8" s="14" t="s">
-        <v>42</v>
-      </c>
-      <c r="L8" s="14" t="s">
-        <v>42</v>
-      </c>
-      <c r="M8" s="14" t="s">
-        <v>42</v>
-      </c>
-      <c r="N8" s="14" t="s">
-        <v>42</v>
-      </c>
-      <c r="O8" s="14" t="s">
-        <v>41</v>
-      </c>
-      <c r="P8" s="14" t="s">
-        <v>41</v>
-      </c>
-      <c r="Q8" s="14" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="9" spans="1:17" ht="12.75">
-      <c r="A9" s="13" t="s">
-        <v>43</v>
-      </c>
-      <c r="B9" s="14">
-        <v>35</v>
-      </c>
-      <c r="C9" s="14">
-        <v>35</v>
-      </c>
-      <c r="D9" s="14">
-        <v>35</v>
-      </c>
-      <c r="E9" s="14">
-        <v>35</v>
-      </c>
-      <c r="F9" s="14">
-        <v>35</v>
-      </c>
-      <c r="G9" s="14">
-        <v>35</v>
-      </c>
-      <c r="H9" s="14">
-        <v>35</v>
-      </c>
-      <c r="I9" s="15">
-        <v>33</v>
-      </c>
-      <c r="J9" s="15">
-        <v>33</v>
-      </c>
-      <c r="K9" s="15">
-        <v>30</v>
-      </c>
-      <c r="L9" s="15">
-        <v>30</v>
-      </c>
-      <c r="M9" s="15">
-        <v>32</v>
-      </c>
-      <c r="N9" s="15">
-        <v>32</v>
-      </c>
-      <c r="O9" s="15">
-        <v>100</v>
-      </c>
-      <c r="P9" s="18">
-        <v>100</v>
-      </c>
-      <c r="Q9" s="19">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="10" spans="1:17" ht="12.75">
-      <c r="A10" s="13" t="s">
-        <v>44</v>
-      </c>
-      <c r="B10" s="14">
-        <v>26</v>
-      </c>
-      <c r="C10" s="14">
-        <v>26</v>
-      </c>
-      <c r="D10" s="14">
-        <v>26</v>
-      </c>
-      <c r="E10" s="14">
-        <v>26</v>
-      </c>
-      <c r="F10" s="14">
-        <v>26</v>
-      </c>
-      <c r="G10" s="14">
-        <v>26</v>
-      </c>
-      <c r="H10" s="14">
-        <v>26</v>
-      </c>
-      <c r="I10" s="15">
-        <v>22</v>
-      </c>
-      <c r="J10" s="15">
-        <v>22</v>
-      </c>
-      <c r="K10" s="15">
-        <v>22</v>
-      </c>
-      <c r="L10" s="15">
-        <v>22</v>
-      </c>
-      <c r="M10" s="15">
-        <v>22</v>
-      </c>
-      <c r="N10" s="15">
-        <v>22</v>
-      </c>
-      <c r="O10" s="15">
-        <v>26</v>
-      </c>
-      <c r="P10" s="20">
-        <v>50</v>
-      </c>
-      <c r="Q10" s="15">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="11" spans="1:17" ht="12.75">
-      <c r="A11" s="13" t="s">
-        <v>45</v>
-      </c>
-      <c r="B11" s="14" t="s">
-        <v>46</v>
-      </c>
-      <c r="C11" s="14" t="s">
-        <v>46</v>
-      </c>
-      <c r="D11" s="14" t="s">
-        <v>46</v>
-      </c>
-      <c r="E11" s="14" t="s">
-        <v>46</v>
-      </c>
-      <c r="F11" s="14" t="s">
-        <v>46</v>
-      </c>
-      <c r="G11" s="14" t="s">
-        <v>46</v>
-      </c>
-      <c r="H11" s="14" t="s">
-        <v>46</v>
-      </c>
-      <c r="I11" s="14" t="s">
-        <v>46</v>
-      </c>
-      <c r="J11" s="14" t="s">
-        <v>46</v>
-      </c>
-      <c r="K11" s="14" t="s">
-        <v>46</v>
-      </c>
-      <c r="L11" s="14" t="s">
-        <v>46</v>
-      </c>
-      <c r="M11" s="14" t="s">
-        <v>46</v>
-      </c>
-      <c r="N11" s="14" t="s">
-        <v>46</v>
-      </c>
-      <c r="O11" s="14" t="s">
-        <v>47</v>
-      </c>
-      <c r="P11" s="14" t="s">
-        <v>48</v>
-      </c>
-      <c r="Q11" s="14" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="12" spans="1:17" ht="12.75">
-      <c r="A12" s="13" t="s">
-        <v>49</v>
-      </c>
-      <c r="B12" s="14">
-        <v>31.86</v>
-      </c>
-      <c r="C12" s="14">
-        <v>33.729999999999997</v>
-      </c>
-      <c r="D12" s="14">
-        <v>35.28</v>
-      </c>
-      <c r="E12" s="14">
-        <v>62.95</v>
-      </c>
-      <c r="F12" s="14">
-        <v>53.52</v>
-      </c>
-      <c r="G12" s="14">
-        <v>39.92</v>
-      </c>
-      <c r="H12" s="14">
-        <v>30.53</v>
-      </c>
-      <c r="I12" s="15">
-        <v>35.64</v>
-      </c>
-      <c r="J12" s="15">
-        <v>33.83</v>
-      </c>
-      <c r="K12" s="15">
-        <v>27.29</v>
-      </c>
-      <c r="L12" s="15">
-        <v>25.82</v>
-      </c>
-      <c r="M12" s="14">
-        <v>35.18</v>
-      </c>
-      <c r="N12" s="14">
-        <v>32.659999999999997</v>
-      </c>
-      <c r="O12" s="15">
-        <v>3</v>
-      </c>
-      <c r="P12" s="15">
-        <v>2.5</v>
-      </c>
-      <c r="Q12" s="15">
-        <v>3.4</v>
-      </c>
-    </row>
-    <row r="13" spans="1:17" ht="12.75">
-      <c r="A13" s="13" t="s">
-        <v>50</v>
-      </c>
-      <c r="B13" s="14">
-        <v>429</v>
-      </c>
-      <c r="C13" s="14">
-        <v>225</v>
-      </c>
-      <c r="D13" s="14">
-        <v>212</v>
-      </c>
-      <c r="E13" s="14">
-        <v>254</v>
-      </c>
-      <c r="F13" s="14">
-        <v>590</v>
-      </c>
-      <c r="G13" s="14">
-        <v>335</v>
-      </c>
-      <c r="H13" s="14">
-        <v>610</v>
-      </c>
-      <c r="I13" s="15">
-        <v>249</v>
-      </c>
-      <c r="J13" s="15">
-        <v>568</v>
-      </c>
-      <c r="K13" s="15">
-        <v>228</v>
-      </c>
-      <c r="L13" s="15">
-        <v>453</v>
-      </c>
-      <c r="M13" s="14" t="s">
-        <v>51</v>
-      </c>
-      <c r="N13" s="14" t="s">
-        <v>52</v>
-      </c>
-      <c r="O13" s="15">
-        <v>430</v>
-      </c>
-      <c r="P13" s="21">
-        <v>1324</v>
-      </c>
-      <c r="Q13" s="21">
-        <v>1252</v>
-      </c>
-    </row>
-    <row r="14" spans="1:17" ht="15.75" customHeight="1">
-      <c r="A14" s="22"/>
-      <c r="B14" s="10"/>
-      <c r="C14" s="10"/>
-      <c r="D14" s="10"/>
-      <c r="E14" s="10"/>
-      <c r="F14" s="10"/>
-      <c r="G14" s="10"/>
-      <c r="H14" s="10"/>
-      <c r="I14" s="9"/>
-      <c r="J14" s="9"/>
-      <c r="K14" s="9"/>
-      <c r="L14" s="9"/>
-      <c r="M14" s="9"/>
-      <c r="N14" s="9"/>
-      <c r="O14" s="9"/>
-      <c r="P14" s="10"/>
-      <c r="Q14" s="10"/>
-    </row>
-    <row r="15" spans="1:17" ht="12.75">
-      <c r="A15" s="11" t="s">
-        <v>35</v>
-      </c>
-      <c r="B15" s="23">
-        <v>40548</v>
-      </c>
-      <c r="C15" s="23">
-        <v>40548</v>
-      </c>
-      <c r="D15" s="17" t="s">
-        <v>53</v>
-      </c>
-      <c r="E15" s="23">
-        <v>40553</v>
-      </c>
-      <c r="F15" s="23">
-        <v>40553</v>
-      </c>
-      <c r="G15" s="23">
-        <v>40918</v>
-      </c>
-      <c r="H15" s="23">
-        <v>40918</v>
-      </c>
-      <c r="I15" s="17" t="s">
-        <v>54</v>
-      </c>
-      <c r="J15" s="17" t="s">
-        <v>54</v>
-      </c>
-      <c r="K15" s="23">
-        <v>40544</v>
-      </c>
-      <c r="L15" s="23">
-        <v>40544</v>
-      </c>
-      <c r="M15" s="23">
-        <v>40179</v>
-      </c>
-      <c r="N15" s="23">
-        <v>40179</v>
-      </c>
-      <c r="O15" s="23">
-        <v>40544</v>
-      </c>
-      <c r="P15" s="23">
-        <v>40544</v>
-      </c>
-      <c r="Q15" s="23">
-        <v>40544</v>
-      </c>
-    </row>
-    <row r="16" spans="1:17" ht="12.75">
-      <c r="A16" s="13" t="s">
-        <v>36</v>
-      </c>
-      <c r="B16" s="16">
-        <v>40913</v>
-      </c>
-      <c r="C16" s="16">
-        <v>40913</v>
-      </c>
-      <c r="D16" s="14" t="s">
-        <v>55</v>
-      </c>
-      <c r="E16" s="14" t="s">
-        <v>56</v>
-      </c>
-      <c r="F16" s="14" t="s">
-        <v>56</v>
-      </c>
-      <c r="G16" s="14" t="s">
-        <v>57</v>
-      </c>
-      <c r="H16" s="14" t="s">
-        <v>57</v>
-      </c>
-      <c r="I16" s="14" t="s">
-        <v>58</v>
-      </c>
-      <c r="J16" s="14" t="s">
-        <v>58</v>
-      </c>
-      <c r="K16" s="14" t="s">
-        <v>59</v>
-      </c>
-      <c r="L16" s="14" t="s">
-        <v>59</v>
-      </c>
-      <c r="M16" s="14" t="s">
-        <v>37</v>
-      </c>
-      <c r="N16" s="14" t="s">
-        <v>37</v>
-      </c>
-      <c r="O16" s="14" t="s">
-        <v>37</v>
-      </c>
-      <c r="P16" s="14" t="s">
-        <v>37</v>
-      </c>
-      <c r="Q16" s="14" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="17" spans="1:17" ht="12.75">
-      <c r="A17" s="13" t="s">
-        <v>43</v>
-      </c>
-      <c r="B17" s="14" t="s">
-        <v>60</v>
-      </c>
-      <c r="C17" s="14" t="s">
-        <v>61</v>
-      </c>
-      <c r="D17" s="14" t="s">
-        <v>61</v>
-      </c>
-      <c r="E17" s="14" t="s">
-        <v>61</v>
-      </c>
-      <c r="F17" s="14" t="s">
-        <v>60</v>
-      </c>
-      <c r="G17" s="14" t="s">
-        <v>61</v>
-      </c>
-      <c r="H17" s="14" t="s">
-        <v>60</v>
-      </c>
-      <c r="I17" s="14" t="s">
-        <v>62</v>
-      </c>
-      <c r="J17" s="14" t="s">
-        <v>63</v>
-      </c>
-      <c r="K17" s="14" t="s">
-        <v>64</v>
-      </c>
-      <c r="L17" s="14" t="s">
-        <v>65</v>
-      </c>
-      <c r="M17" s="14" t="s">
-        <v>66</v>
-      </c>
-      <c r="N17" s="14" t="s">
-        <v>67</v>
-      </c>
-      <c r="O17" s="14" t="s">
-        <v>68</v>
-      </c>
-      <c r="P17" s="24">
-        <v>100</v>
-      </c>
-      <c r="Q17" s="25">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="18" spans="1:17" ht="12.75">
-      <c r="A18" s="13" t="s">
-        <v>44</v>
-      </c>
-      <c r="B18" s="14">
-        <v>26</v>
-      </c>
-      <c r="C18" s="14">
-        <v>26</v>
-      </c>
-      <c r="D18" s="14">
-        <v>26</v>
-      </c>
-      <c r="E18" s="14">
-        <v>26</v>
-      </c>
-      <c r="F18" s="14">
-        <v>26</v>
-      </c>
-      <c r="G18" s="14">
-        <v>26</v>
-      </c>
-      <c r="H18" s="14">
-        <v>26</v>
-      </c>
-      <c r="I18" s="14" t="s">
-        <v>69</v>
-      </c>
-      <c r="J18" s="14" t="s">
-        <v>69</v>
-      </c>
-      <c r="K18" s="14"/>
-      <c r="L18" s="14" t="s">
-        <v>69</v>
-      </c>
-      <c r="M18" s="14" t="s">
-        <v>69</v>
-      </c>
-      <c r="N18" s="14" t="s">
-        <v>69</v>
-      </c>
-      <c r="O18" s="14" t="s">
-        <v>69</v>
-      </c>
-      <c r="P18" s="17" t="s">
-        <v>70</v>
-      </c>
-      <c r="Q18" s="14" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="19" spans="1:17" ht="15.75" customHeight="1">
-      <c r="A19" s="22"/>
-      <c r="B19" s="10"/>
-      <c r="C19" s="10"/>
-      <c r="D19" s="10"/>
-      <c r="E19" s="10"/>
-      <c r="F19" s="10"/>
-      <c r="G19" s="10"/>
-      <c r="H19" s="10"/>
-      <c r="I19" s="9"/>
-      <c r="J19" s="9"/>
-      <c r="K19" s="9"/>
-      <c r="L19" s="9"/>
-      <c r="M19" s="9"/>
-      <c r="N19" s="9"/>
-      <c r="O19" s="9"/>
-      <c r="P19" s="10"/>
-      <c r="Q19" s="10"/>
-    </row>
     <row r="20" spans="1:17" ht="15.75" customHeight="1">
-      <c r="A20" s="22"/>
-      <c r="B20" s="26"/>
-      <c r="C20" s="10"/>
-      <c r="D20" s="10"/>
-      <c r="E20" s="10"/>
-      <c r="F20" s="10"/>
-      <c r="G20" s="10"/>
-      <c r="H20" s="10"/>
-      <c r="I20" s="9"/>
-      <c r="J20" s="9"/>
-      <c r="K20" s="9"/>
-      <c r="L20" s="9"/>
-      <c r="M20" s="9"/>
-      <c r="N20" s="9"/>
-      <c r="O20" s="9"/>
-      <c r="P20" s="10"/>
-      <c r="Q20" s="10"/>
+      <c r="A20" s="36"/>
+      <c r="B20" s="51"/>
+      <c r="C20" s="36"/>
+      <c r="D20" s="36"/>
+      <c r="E20" s="36"/>
+      <c r="F20" s="36"/>
+      <c r="G20" s="36"/>
+      <c r="H20" s="36"/>
+      <c r="I20" s="36"/>
+      <c r="J20" s="36"/>
+      <c r="K20" s="36"/>
+      <c r="L20" s="36"/>
+      <c r="M20" s="36"/>
+      <c r="N20" s="36"/>
+      <c r="O20" s="36"/>
+      <c r="P20" s="36"/>
+      <c r="Q20" s="36"/>
     </row>
     <row r="21" spans="1:17" ht="15.75" customHeight="1">
-      <c r="A21" s="22"/>
-      <c r="B21" s="10"/>
-      <c r="C21" s="10"/>
-      <c r="D21" s="10"/>
-      <c r="E21" s="10"/>
-      <c r="F21" s="10"/>
-      <c r="G21" s="10"/>
-      <c r="H21" s="10"/>
-      <c r="I21" s="9"/>
-      <c r="J21" s="9"/>
-      <c r="K21" s="9"/>
-      <c r="L21" s="9"/>
-      <c r="M21" s="9"/>
-      <c r="N21" s="9"/>
-      <c r="O21" s="9"/>
-      <c r="P21" s="10"/>
-      <c r="Q21" s="10"/>
+      <c r="A21" s="36"/>
+      <c r="B21" s="36"/>
+      <c r="C21" s="36"/>
+      <c r="D21" s="36"/>
+      <c r="E21" s="36"/>
+      <c r="F21" s="36"/>
+      <c r="G21" s="36"/>
+      <c r="H21" s="36"/>
+      <c r="I21" s="36"/>
+      <c r="J21" s="36"/>
+      <c r="K21" s="36"/>
+      <c r="L21" s="36"/>
+      <c r="M21" s="36"/>
+      <c r="N21" s="36"/>
+      <c r="O21" s="36"/>
+      <c r="P21" s="36"/>
+      <c r="Q21" s="36"/>
     </row>
     <row r="22" spans="1:17" ht="15.75" customHeight="1">
-      <c r="A22" s="22"/>
-      <c r="B22" s="10"/>
-      <c r="C22" s="10"/>
-      <c r="D22" s="10"/>
-      <c r="E22" s="10"/>
-      <c r="F22" s="10"/>
-      <c r="G22" s="10"/>
-      <c r="H22" s="10"/>
-      <c r="I22" s="9"/>
-      <c r="J22" s="9"/>
-      <c r="K22" s="9"/>
-      <c r="L22" s="9"/>
-      <c r="M22" s="9"/>
-      <c r="N22" s="9"/>
-      <c r="O22" s="9"/>
-      <c r="P22" s="10"/>
-      <c r="Q22" s="10"/>
+      <c r="A22" s="36"/>
+      <c r="B22" s="36"/>
+      <c r="C22" s="36"/>
+      <c r="D22" s="36"/>
+      <c r="E22" s="36"/>
+      <c r="F22" s="36"/>
+      <c r="G22" s="36"/>
+      <c r="H22" s="36"/>
+      <c r="I22" s="36"/>
+      <c r="J22" s="36"/>
+      <c r="K22" s="36"/>
+      <c r="L22" s="36"/>
+      <c r="M22" s="36"/>
+      <c r="N22" s="36"/>
+      <c r="O22" s="36"/>
+      <c r="P22" s="36"/>
+      <c r="Q22" s="36"/>
     </row>
     <row r="23" spans="1:17" ht="15.75" customHeight="1">
-      <c r="A23" s="22"/>
-      <c r="B23" s="10"/>
-      <c r="C23" s="10"/>
-      <c r="D23" s="10"/>
-      <c r="E23" s="10"/>
-      <c r="F23" s="10"/>
-      <c r="G23" s="10"/>
-      <c r="H23" s="10"/>
-      <c r="I23" s="9"/>
-      <c r="J23" s="9"/>
-      <c r="K23" s="9"/>
-      <c r="L23" s="9"/>
-      <c r="M23" s="9"/>
-      <c r="N23" s="9"/>
-      <c r="O23" s="9"/>
-      <c r="P23" s="10"/>
-      <c r="Q23" s="10"/>
+      <c r="A23" s="36"/>
+      <c r="B23" s="36"/>
+      <c r="C23" s="36"/>
+      <c r="D23" s="36"/>
+      <c r="E23" s="36"/>
+      <c r="F23" s="36"/>
+      <c r="G23" s="36"/>
+      <c r="H23" s="36"/>
+      <c r="I23" s="36"/>
+      <c r="J23" s="36"/>
+      <c r="K23" s="36"/>
+      <c r="L23" s="36"/>
+      <c r="M23" s="36"/>
+      <c r="N23" s="36"/>
+      <c r="O23" s="36"/>
+      <c r="P23" s="36"/>
+      <c r="Q23" s="36"/>
     </row>
     <row r="24" spans="1:17" ht="15.75" customHeight="1">
-      <c r="A24" s="22"/>
-      <c r="B24" s="10"/>
-      <c r="C24" s="10"/>
-      <c r="D24" s="10"/>
-      <c r="E24" s="10"/>
-      <c r="F24" s="10"/>
-      <c r="G24" s="10"/>
-      <c r="H24" s="10"/>
-      <c r="I24" s="9"/>
-      <c r="J24" s="9"/>
-      <c r="K24" s="9"/>
-      <c r="L24" s="9"/>
-      <c r="M24" s="9"/>
-      <c r="N24" s="9"/>
-      <c r="O24" s="9"/>
-      <c r="P24" s="10"/>
-      <c r="Q24" s="10"/>
+      <c r="A24" s="36"/>
+      <c r="B24" s="36"/>
+      <c r="C24" s="36"/>
+      <c r="D24" s="36"/>
+      <c r="E24" s="36"/>
+      <c r="F24" s="36"/>
+      <c r="G24" s="36"/>
+      <c r="H24" s="36"/>
+      <c r="I24" s="36"/>
+      <c r="J24" s="36"/>
+      <c r="K24" s="36"/>
+      <c r="L24" s="36"/>
+      <c r="M24" s="36"/>
+      <c r="N24" s="36"/>
+      <c r="O24" s="36"/>
+      <c r="P24" s="36"/>
+      <c r="Q24" s="36"/>
     </row>
     <row r="25" spans="1:17" ht="15.75" customHeight="1">
-      <c r="A25" s="22"/>
-      <c r="B25" s="10"/>
-      <c r="C25" s="10"/>
-      <c r="D25" s="10"/>
-      <c r="E25" s="10"/>
-      <c r="F25" s="10"/>
-      <c r="G25" s="10"/>
-      <c r="H25" s="10"/>
-      <c r="I25" s="9"/>
-      <c r="J25" s="9"/>
-      <c r="K25" s="9"/>
-      <c r="L25" s="9"/>
-      <c r="M25" s="9"/>
-      <c r="N25" s="9"/>
-      <c r="O25" s="9"/>
-      <c r="P25" s="10"/>
-      <c r="Q25" s="10"/>
+      <c r="A25" s="36"/>
+      <c r="B25" s="36"/>
+      <c r="C25" s="36"/>
+      <c r="D25" s="36"/>
+      <c r="E25" s="36"/>
+      <c r="F25" s="36"/>
+      <c r="G25" s="36"/>
+      <c r="H25" s="36"/>
+      <c r="I25" s="36"/>
+      <c r="J25" s="36"/>
+      <c r="K25" s="36"/>
+      <c r="L25" s="36"/>
+      <c r="M25" s="36"/>
+      <c r="N25" s="36"/>
+      <c r="O25" s="36"/>
+      <c r="P25" s="36"/>
+      <c r="Q25" s="36"/>
     </row>
     <row r="26" spans="1:17" ht="15.75" customHeight="1">
-      <c r="A26" s="22"/>
-      <c r="B26" s="9"/>
-      <c r="C26" s="10"/>
-      <c r="D26" s="10"/>
-      <c r="E26" s="10"/>
-      <c r="F26" s="10"/>
-      <c r="G26" s="10"/>
-      <c r="H26" s="10"/>
-      <c r="I26" s="9"/>
-      <c r="J26" s="9"/>
-      <c r="K26" s="9"/>
-      <c r="L26" s="9"/>
-      <c r="M26" s="9"/>
-      <c r="N26" s="9"/>
-      <c r="O26" s="9"/>
-      <c r="P26" s="10"/>
-      <c r="Q26" s="10"/>
+      <c r="A26" s="36"/>
+      <c r="B26" s="36"/>
+      <c r="C26" s="36"/>
+      <c r="D26" s="36"/>
+      <c r="E26" s="36"/>
+      <c r="F26" s="36"/>
+      <c r="G26" s="36"/>
+      <c r="H26" s="36"/>
+      <c r="I26" s="36"/>
+      <c r="J26" s="36"/>
+      <c r="K26" s="36"/>
+      <c r="L26" s="36"/>
+      <c r="M26" s="36"/>
+      <c r="N26" s="36"/>
+      <c r="O26" s="36"/>
+      <c r="P26" s="36"/>
+      <c r="Q26" s="36"/>
     </row>
     <row r="27" spans="1:17" ht="15.75" customHeight="1">
-      <c r="A27" s="22"/>
-      <c r="B27" s="27"/>
-      <c r="C27" s="10"/>
-      <c r="D27" s="10"/>
-      <c r="E27" s="10"/>
-      <c r="F27" s="10"/>
-      <c r="G27" s="10"/>
-      <c r="H27" s="10"/>
-      <c r="I27" s="9"/>
-      <c r="J27" s="9"/>
-      <c r="K27" s="9"/>
-      <c r="L27" s="9"/>
-      <c r="M27" s="9"/>
-      <c r="N27" s="9"/>
-      <c r="O27" s="9"/>
-      <c r="P27" s="10"/>
-      <c r="Q27" s="10"/>
+      <c r="A27" s="36"/>
+      <c r="B27" s="52"/>
+      <c r="C27" s="36"/>
+      <c r="D27" s="36"/>
+      <c r="E27" s="36"/>
+      <c r="F27" s="36"/>
+      <c r="G27" s="36"/>
+      <c r="H27" s="36"/>
+      <c r="I27" s="36"/>
+      <c r="J27" s="36"/>
+      <c r="K27" s="36"/>
+      <c r="L27" s="36"/>
+      <c r="M27" s="36"/>
+      <c r="N27" s="36"/>
+      <c r="O27" s="36"/>
+      <c r="P27" s="36"/>
+      <c r="Q27" s="36"/>
     </row>
   </sheetData>
   <phoneticPr fontId="14" type="noConversion"/>
@@ -3486,105 +3518,105 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" ht="15.75" customHeight="1">
-      <c r="A1" s="28"/>
-      <c r="B1" s="28" t="s">
+      <c r="A1" s="8"/>
+      <c r="B1" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="28"/>
-      <c r="D1" s="28"/>
-      <c r="E1" s="28"/>
-      <c r="F1" s="28"/>
-      <c r="G1" s="28"/>
-      <c r="H1" s="28"/>
-      <c r="I1" s="28"/>
-      <c r="J1" s="28"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
+      <c r="F1" s="8"/>
+      <c r="G1" s="8"/>
+      <c r="H1" s="8"/>
+      <c r="I1" s="8"/>
+      <c r="J1" s="8"/>
     </row>
     <row r="2" spans="1:16" ht="12.75">
-      <c r="A2" s="29" t="s">
+      <c r="A2" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="B2" s="29" t="s">
+      <c r="B2" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="C2" s="9" t="s">
         <v>72</v>
       </c>
-      <c r="C2" s="29" t="s">
-        <v>73</v>
-      </c>
-      <c r="D2" s="30"/>
-      <c r="E2" s="30"/>
-      <c r="F2" s="30"/>
-      <c r="G2" s="30"/>
-      <c r="H2" s="30"/>
-      <c r="I2" s="30"/>
-      <c r="J2" s="30"/>
-      <c r="K2" s="30"/>
-      <c r="L2" s="30"/>
-      <c r="M2" s="30"/>
-      <c r="N2" s="30"/>
-      <c r="O2" s="30"/>
-      <c r="P2" s="30"/>
+      <c r="D2" s="10"/>
+      <c r="E2" s="10"/>
+      <c r="F2" s="10"/>
+      <c r="G2" s="10"/>
+      <c r="H2" s="10"/>
+      <c r="I2" s="10"/>
+      <c r="J2" s="10"/>
+      <c r="K2" s="10"/>
+      <c r="L2" s="10"/>
+      <c r="M2" s="10"/>
+      <c r="N2" s="10"/>
+      <c r="O2" s="10"/>
+      <c r="P2" s="10"/>
     </row>
     <row r="3" spans="1:16" ht="12.75">
-      <c r="A3" s="29" t="s">
+      <c r="A3" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="B3" s="31">
+      <c r="B3" s="11">
         <v>-8.1051400000000005</v>
       </c>
-      <c r="C3" s="31">
+      <c r="C3" s="11">
         <v>36.008980000000001</v>
       </c>
-      <c r="D3" s="32"/>
-      <c r="E3" s="32"/>
-      <c r="F3" s="32"/>
-      <c r="G3" s="32"/>
+      <c r="D3" s="12"/>
+      <c r="E3" s="12"/>
+      <c r="F3" s="12"/>
+      <c r="G3" s="12"/>
       <c r="H3" s="1"/>
       <c r="I3" s="1"/>
       <c r="J3" s="1"/>
       <c r="K3" s="1"/>
       <c r="L3" s="1"/>
       <c r="M3" s="1"/>
-      <c r="N3" s="32"/>
+      <c r="N3" s="12"/>
       <c r="O3" s="1"/>
       <c r="P3" s="1"/>
     </row>
     <row r="4" spans="1:16" ht="12.75">
-      <c r="A4" s="29" t="s">
+      <c r="A4" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="B4" s="31">
+      <c r="B4" s="11">
         <v>31.641110000000001</v>
       </c>
-      <c r="C4" s="31">
+      <c r="C4" s="11">
         <v>32.554589999999997</v>
       </c>
-      <c r="D4" s="32"/>
-      <c r="E4" s="32"/>
-      <c r="F4" s="32"/>
-      <c r="G4" s="32"/>
+      <c r="D4" s="12"/>
+      <c r="E4" s="12"/>
+      <c r="F4" s="12"/>
+      <c r="G4" s="12"/>
       <c r="H4" s="1"/>
       <c r="I4" s="1"/>
       <c r="J4" s="1"/>
       <c r="K4" s="1"/>
       <c r="L4" s="1"/>
       <c r="M4" s="1"/>
-      <c r="N4" s="32"/>
+      <c r="N4" s="12"/>
       <c r="O4" s="1"/>
       <c r="P4" s="1"/>
     </row>
     <row r="5" spans="1:16" ht="12.75">
-      <c r="A5" s="29" t="s">
+      <c r="A5" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="B5" s="33">
+      <c r="B5" s="13">
         <v>42736</v>
       </c>
-      <c r="C5" s="33">
+      <c r="C5" s="13">
         <v>42736</v>
       </c>
-      <c r="D5" s="32"/>
-      <c r="E5" s="32"/>
-      <c r="F5" s="32"/>
-      <c r="G5" s="32"/>
+      <c r="D5" s="12"/>
+      <c r="E5" s="12"/>
+      <c r="F5" s="12"/>
+      <c r="G5" s="12"/>
       <c r="H5" s="1"/>
       <c r="I5" s="1"/>
       <c r="J5" s="1"/>
@@ -3596,19 +3628,19 @@
       <c r="P5" s="1"/>
     </row>
     <row r="6" spans="1:16" ht="12.75">
-      <c r="A6" s="29" t="s">
+      <c r="A6" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="B6" s="33">
+      <c r="B6" s="13">
         <v>43101</v>
       </c>
-      <c r="C6" s="33">
+      <c r="C6" s="13">
         <v>43101</v>
       </c>
-      <c r="D6" s="32"/>
-      <c r="E6" s="32"/>
-      <c r="F6" s="32"/>
-      <c r="G6" s="32"/>
+      <c r="D6" s="12"/>
+      <c r="E6" s="12"/>
+      <c r="F6" s="12"/>
+      <c r="G6" s="12"/>
       <c r="H6" s="1"/>
       <c r="I6" s="1"/>
       <c r="J6" s="1"/>
@@ -3620,21 +3652,21 @@
       <c r="P6" s="1"/>
     </row>
     <row r="7" spans="1:16" ht="12.75">
-      <c r="A7" s="29" t="s">
+      <c r="A7" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="B7" s="34" t="s">
-        <v>69</v>
-      </c>
-      <c r="C7" s="34" t="s">
-        <v>69</v>
-      </c>
-      <c r="D7" s="32"/>
-      <c r="E7" s="32"/>
-      <c r="F7" s="32"/>
-      <c r="G7" s="32"/>
-      <c r="H7" s="35"/>
-      <c r="I7" s="35"/>
+      <c r="B7" s="14" t="s">
+        <v>68</v>
+      </c>
+      <c r="C7" s="14" t="s">
+        <v>68</v>
+      </c>
+      <c r="D7" s="12"/>
+      <c r="E7" s="12"/>
+      <c r="F7" s="12"/>
+      <c r="G7" s="12"/>
+      <c r="H7" s="15"/>
+      <c r="I7" s="15"/>
       <c r="J7" s="1"/>
       <c r="K7" s="1"/>
       <c r="L7" s="1"/>
@@ -3644,19 +3676,19 @@
       <c r="P7" s="1"/>
     </row>
     <row r="8" spans="1:16" ht="12.75">
-      <c r="A8" s="29" t="s">
-        <v>40</v>
-      </c>
-      <c r="B8" s="36" t="s">
-        <v>74</v>
-      </c>
-      <c r="C8" s="34" t="s">
-        <v>69</v>
-      </c>
-      <c r="D8" s="32"/>
-      <c r="E8" s="32"/>
-      <c r="F8" s="32"/>
-      <c r="G8" s="32"/>
+      <c r="A8" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="B8" s="16" t="s">
+        <v>73</v>
+      </c>
+      <c r="C8" s="14" t="s">
+        <v>68</v>
+      </c>
+      <c r="D8" s="12"/>
+      <c r="E8" s="12"/>
+      <c r="F8" s="12"/>
+      <c r="G8" s="12"/>
       <c r="H8" s="1"/>
       <c r="I8" s="1"/>
       <c r="J8" s="1"/>
@@ -3668,19 +3700,19 @@
       <c r="P8" s="1"/>
     </row>
     <row r="9" spans="1:16" ht="12.75">
-      <c r="A9" s="29" t="s">
-        <v>43</v>
-      </c>
-      <c r="B9" s="31" t="s">
-        <v>75</v>
-      </c>
-      <c r="C9" s="31" t="s">
-        <v>75</v>
-      </c>
-      <c r="D9" s="32"/>
-      <c r="E9" s="32"/>
-      <c r="F9" s="32"/>
-      <c r="G9" s="32"/>
+      <c r="A9" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="B9" s="11" t="s">
+        <v>74</v>
+      </c>
+      <c r="C9" s="11" t="s">
+        <v>74</v>
+      </c>
+      <c r="D9" s="12"/>
+      <c r="E9" s="12"/>
+      <c r="F9" s="12"/>
+      <c r="G9" s="12"/>
       <c r="H9" s="1"/>
       <c r="I9" s="1"/>
       <c r="J9" s="1"/>
@@ -3688,19 +3720,19 @@
       <c r="L9" s="1"/>
       <c r="M9" s="1"/>
       <c r="N9" s="1"/>
-      <c r="O9" s="37"/>
-      <c r="P9" s="38"/>
+      <c r="O9" s="17"/>
+      <c r="P9" s="18"/>
     </row>
     <row r="10" spans="1:16" ht="12.75">
-      <c r="A10" s="29" t="s">
-        <v>44</v>
-      </c>
-      <c r="B10" s="31"/>
-      <c r="C10" s="31"/>
-      <c r="D10" s="32"/>
-      <c r="E10" s="32"/>
-      <c r="F10" s="32"/>
-      <c r="G10" s="32"/>
+      <c r="A10" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="B10" s="11"/>
+      <c r="C10" s="11"/>
+      <c r="D10" s="12"/>
+      <c r="E10" s="12"/>
+      <c r="F10" s="12"/>
+      <c r="G10" s="12"/>
       <c r="H10" s="1"/>
       <c r="I10" s="1"/>
       <c r="J10" s="1"/>
@@ -3712,19 +3744,19 @@
       <c r="P10" s="1"/>
     </row>
     <row r="11" spans="1:16" ht="12.75">
-      <c r="A11" s="29" t="s">
-        <v>45</v>
-      </c>
-      <c r="B11" s="34" t="s">
-        <v>69</v>
-      </c>
-      <c r="C11" s="34" t="s">
-        <v>69</v>
-      </c>
-      <c r="D11" s="32"/>
-      <c r="E11" s="32"/>
-      <c r="F11" s="32"/>
-      <c r="G11" s="32"/>
+      <c r="A11" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="B11" s="14" t="s">
+        <v>68</v>
+      </c>
+      <c r="C11" s="14" t="s">
+        <v>68</v>
+      </c>
+      <c r="D11" s="12"/>
+      <c r="E11" s="12"/>
+      <c r="F11" s="12"/>
+      <c r="G11" s="12"/>
       <c r="H11" s="1"/>
       <c r="I11" s="1"/>
       <c r="J11" s="1"/>
@@ -3736,15 +3768,15 @@
       <c r="P11" s="1"/>
     </row>
     <row r="12" spans="1:16" ht="12.75">
-      <c r="A12" s="29" t="s">
-        <v>49</v>
-      </c>
-      <c r="B12" s="31"/>
-      <c r="C12" s="31"/>
-      <c r="D12" s="32"/>
-      <c r="E12" s="32"/>
-      <c r="F12" s="32"/>
-      <c r="G12" s="32"/>
+      <c r="A12" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="B12" s="11"/>
+      <c r="C12" s="11"/>
+      <c r="D12" s="12"/>
+      <c r="E12" s="12"/>
+      <c r="F12" s="12"/>
+      <c r="G12" s="12"/>
       <c r="H12" s="1"/>
       <c r="I12" s="1"/>
       <c r="J12" s="1"/>
@@ -3756,19 +3788,19 @@
       <c r="P12" s="1"/>
     </row>
     <row r="13" spans="1:16" ht="12.75">
-      <c r="A13" s="29" t="s">
-        <v>50</v>
-      </c>
-      <c r="B13" s="36" t="s">
-        <v>74</v>
-      </c>
-      <c r="C13" s="36" t="s">
-        <v>74</v>
-      </c>
-      <c r="D13" s="32"/>
-      <c r="E13" s="32"/>
-      <c r="F13" s="32"/>
-      <c r="G13" s="32"/>
+      <c r="A13" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="B13" s="16" t="s">
+        <v>73</v>
+      </c>
+      <c r="C13" s="16" t="s">
+        <v>73</v>
+      </c>
+      <c r="D13" s="12"/>
+      <c r="E13" s="12"/>
+      <c r="F13" s="12"/>
+      <c r="G13" s="12"/>
       <c r="H13" s="1"/>
       <c r="I13" s="1"/>
       <c r="J13" s="1"/>
@@ -3807,213 +3839,213 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="15.75" customHeight="1">
-      <c r="A1" s="28"/>
-      <c r="B1" s="28" t="s">
+      <c r="A1" s="8"/>
+      <c r="B1" s="8" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="12.75">
-      <c r="A2" s="29" t="s">
+      <c r="A2" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="B2" s="29" t="s">
+      <c r="B2" s="9" t="s">
+        <v>75</v>
+      </c>
+      <c r="C2" s="9" t="s">
         <v>76</v>
       </c>
-      <c r="C2" s="29" t="s">
+      <c r="D2" s="9" t="s">
         <v>77</v>
       </c>
-      <c r="D2" s="29" t="s">
+      <c r="E2" s="9" t="s">
         <v>78</v>
       </c>
-      <c r="E2" s="29" t="s">
+    </row>
+    <row r="3" spans="1:5" ht="12.75">
+      <c r="A3" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="B3" s="11">
+        <v>48.717812000000002</v>
+      </c>
+      <c r="C3" s="11">
+        <v>48.717812000000002</v>
+      </c>
+      <c r="D3" s="11">
+        <v>48.717812000000002</v>
+      </c>
+      <c r="E3" s="11">
+        <v>48.717812000000002</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="12.75">
+      <c r="A4" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="B4" s="11">
+        <v>31.323521</v>
+      </c>
+      <c r="C4" s="11">
+        <v>31.323521</v>
+      </c>
+      <c r="D4" s="11">
+        <v>31.323521</v>
+      </c>
+      <c r="E4" s="11">
+        <v>31.323521</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="12.75">
+      <c r="A5" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="B5" s="13">
+        <v>36526</v>
+      </c>
+      <c r="C5" s="13">
+        <v>36526</v>
+      </c>
+      <c r="D5" s="13">
+        <v>37987</v>
+      </c>
+      <c r="E5" s="13">
+        <v>37987</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="12.75">
+      <c r="A6" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="B6" s="11" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" ht="12.75">
-      <c r="A3" s="29" t="s">
-        <v>33</v>
-      </c>
-      <c r="B3" s="31">
-        <v>48.717812000000002</v>
-      </c>
-      <c r="C3" s="31">
-        <v>48.717812000000002</v>
-      </c>
-      <c r="D3" s="31">
-        <v>48.717812000000002</v>
-      </c>
-      <c r="E3" s="31">
-        <v>48.717812000000002</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" ht="12.75">
-      <c r="A4" s="29" t="s">
-        <v>34</v>
-      </c>
-      <c r="B4" s="31">
-        <v>31.323521</v>
-      </c>
-      <c r="C4" s="31">
-        <v>31.323521</v>
-      </c>
-      <c r="D4" s="31">
-        <v>31.323521</v>
-      </c>
-      <c r="E4" s="31">
-        <v>31.323521</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" ht="12.75">
-      <c r="A5" s="29" t="s">
-        <v>35</v>
-      </c>
-      <c r="B5" s="33">
-        <v>36526</v>
-      </c>
-      <c r="C5" s="33">
-        <v>36526</v>
-      </c>
-      <c r="D5" s="33">
-        <v>37987</v>
-      </c>
-      <c r="E5" s="33">
-        <v>37987</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" ht="12.75">
-      <c r="A6" s="29" t="s">
-        <v>36</v>
-      </c>
-      <c r="B6" s="31" t="s">
+      <c r="C6" s="11" t="s">
+        <v>79</v>
+      </c>
+      <c r="D6" s="11" t="s">
         <v>80</v>
       </c>
-      <c r="C6" s="31" t="s">
+      <c r="E6" s="11" t="s">
         <v>80</v>
       </c>
-      <c r="D6" s="31" t="s">
+    </row>
+    <row r="7" spans="1:5" ht="12.75">
+      <c r="A7" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="B7" s="11" t="s">
         <v>81</v>
       </c>
-      <c r="E6" s="31" t="s">
+      <c r="C7" s="11" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" ht="12.75">
-      <c r="A7" s="29" t="s">
-        <v>38</v>
-      </c>
-      <c r="B7" s="31" t="s">
+      <c r="D7" s="11" t="s">
         <v>82</v>
       </c>
-      <c r="C7" s="31" t="s">
+      <c r="E7" s="11" t="s">
         <v>82</v>
       </c>
-      <c r="D7" s="31" t="s">
+    </row>
+    <row r="8" spans="1:5" ht="12.75">
+      <c r="A8" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="B8" s="11" t="s">
         <v>83</v>
       </c>
-      <c r="E7" s="31" t="s">
+      <c r="C8" s="11" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" ht="12.75">
-      <c r="A8" s="29" t="s">
-        <v>40</v>
-      </c>
-      <c r="B8" s="31" t="s">
+      <c r="D8" s="11" t="s">
+        <v>83</v>
+      </c>
+      <c r="E8" s="11" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="12.75">
+      <c r="A9" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="B9" s="11">
+        <v>50</v>
+      </c>
+      <c r="C9" s="11">
+        <v>50</v>
+      </c>
+      <c r="D9" s="11">
+        <v>50</v>
+      </c>
+      <c r="E9" s="11">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="12.75">
+      <c r="A10" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="B10" s="11">
+        <v>44</v>
+      </c>
+      <c r="C10" s="11">
+        <v>44</v>
+      </c>
+      <c r="D10" s="11">
+        <v>44</v>
+      </c>
+      <c r="E10" s="11">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="12.75">
+      <c r="A11" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="B11" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="C11" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="D11" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="E11" s="11" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="12.75">
+      <c r="A12" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="B12" s="11">
+        <v>15.8</v>
+      </c>
+      <c r="C12" s="11">
+        <v>14.7</v>
+      </c>
+      <c r="D12" s="11">
+        <v>6</v>
+      </c>
+      <c r="E12" s="11">
+        <v>5.8</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="12.75">
+      <c r="A13" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="B13" s="11" t="s">
         <v>84</v>
       </c>
-      <c r="C8" s="31" t="s">
+      <c r="C13" s="11" t="s">
         <v>84</v>
       </c>
-      <c r="D8" s="31" t="s">
+      <c r="D13" s="11" t="s">
         <v>84</v>
       </c>
-      <c r="E8" s="31" t="s">
+      <c r="E13" s="11" t="s">
         <v>84</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" ht="12.75">
-      <c r="A9" s="29" t="s">
-        <v>43</v>
-      </c>
-      <c r="B9" s="31">
-        <v>50</v>
-      </c>
-      <c r="C9" s="31">
-        <v>50</v>
-      </c>
-      <c r="D9" s="31">
-        <v>50</v>
-      </c>
-      <c r="E9" s="31">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" ht="12.75">
-      <c r="A10" s="29" t="s">
-        <v>44</v>
-      </c>
-      <c r="B10" s="31">
-        <v>44</v>
-      </c>
-      <c r="C10" s="31">
-        <v>44</v>
-      </c>
-      <c r="D10" s="31">
-        <v>44</v>
-      </c>
-      <c r="E10" s="31">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" ht="12.75">
-      <c r="A11" s="29" t="s">
-        <v>45</v>
-      </c>
-      <c r="B11" s="31" t="s">
-        <v>47</v>
-      </c>
-      <c r="C11" s="31" t="s">
-        <v>47</v>
-      </c>
-      <c r="D11" s="31" t="s">
-        <v>47</v>
-      </c>
-      <c r="E11" s="31" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" ht="12.75">
-      <c r="A12" s="29" t="s">
-        <v>49</v>
-      </c>
-      <c r="B12" s="31">
-        <v>15.8</v>
-      </c>
-      <c r="C12" s="31">
-        <v>14.7</v>
-      </c>
-      <c r="D12" s="31">
-        <v>6</v>
-      </c>
-      <c r="E12" s="31">
-        <v>5.8</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" ht="12.75">
-      <c r="A13" s="29" t="s">
-        <v>50</v>
-      </c>
-      <c r="B13" s="31" t="s">
-        <v>85</v>
-      </c>
-      <c r="C13" s="31" t="s">
-        <v>85</v>
-      </c>
-      <c r="D13" s="31" t="s">
-        <v>85</v>
-      </c>
-      <c r="E13" s="31" t="s">
-        <v>85</v>
       </c>
     </row>
   </sheetData>
@@ -4040,561 +4072,561 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="15.75" customHeight="1">
-      <c r="A1" s="46" t="s">
+      <c r="A1" s="26" t="s">
+        <v>85</v>
+      </c>
+      <c r="B1" s="27"/>
+      <c r="C1" s="27"/>
+      <c r="D1" s="27"/>
+      <c r="E1" s="27"/>
+      <c r="F1" s="27"/>
+      <c r="G1" s="27"/>
+      <c r="H1" s="27"/>
+      <c r="I1" s="27"/>
+      <c r="J1" s="27"/>
+    </row>
+    <row r="2" spans="1:10" ht="12.75">
+      <c r="A2" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="B2" s="19" t="s">
         <v>86</v>
       </c>
-      <c r="B1" s="47"/>
-      <c r="C1" s="47"/>
-      <c r="D1" s="47"/>
-      <c r="E1" s="47"/>
-      <c r="F1" s="47"/>
-      <c r="G1" s="47"/>
-      <c r="H1" s="47"/>
-      <c r="I1" s="47"/>
-      <c r="J1" s="47"/>
-    </row>
-    <row r="2" spans="1:10" ht="12.75">
-      <c r="A2" s="29" t="s">
-        <v>19</v>
-      </c>
-      <c r="B2" s="39" t="s">
+      <c r="C2" s="19" t="s">
         <v>87</v>
       </c>
-      <c r="C2" s="39" t="s">
+      <c r="D2" s="19" t="s">
         <v>88</v>
       </c>
-      <c r="D2" s="39" t="s">
+      <c r="E2" s="19" t="s">
         <v>89</v>
       </c>
-      <c r="E2" s="39" t="s">
+      <c r="F2" s="19" t="s">
         <v>90</v>
       </c>
-      <c r="F2" s="39" t="s">
+      <c r="G2" s="19" t="s">
         <v>91</v>
       </c>
-      <c r="G2" s="39" t="s">
+      <c r="H2" s="19" t="s">
         <v>92</v>
       </c>
-      <c r="H2" s="39" t="s">
+      <c r="I2" s="19" t="s">
         <v>93</v>
       </c>
-      <c r="I2" s="39" t="s">
+      <c r="J2" s="19" t="s">
         <v>94</v>
       </c>
-      <c r="J2" s="39" t="s">
+    </row>
+    <row r="3" spans="1:10" ht="12.75">
+      <c r="A3" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="B3" s="20">
+        <v>-7.6097200000000003</v>
+      </c>
+      <c r="C3" s="20">
+        <v>-7.5916699999999997</v>
+      </c>
+      <c r="D3" s="20">
+        <v>-7.5944399999999996</v>
+      </c>
+      <c r="E3" s="20">
+        <v>-7.5916699999999997</v>
+      </c>
+      <c r="F3" s="20">
+        <v>-7.5888900000000001</v>
+      </c>
+      <c r="G3" s="20">
+        <v>-7.5986099999999999</v>
+      </c>
+      <c r="H3" s="20">
+        <v>-7.5958300000000003</v>
+      </c>
+      <c r="I3" s="20">
+        <v>-7.5916699999999997</v>
+      </c>
+      <c r="J3" s="20">
+        <v>-7.61111</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" ht="12.75">
+      <c r="A4" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="B4" s="20">
+        <v>31.661110000000001</v>
+      </c>
+      <c r="C4" s="20">
+        <v>31.66667</v>
+      </c>
+      <c r="D4" s="20">
+        <v>31.668060000000001</v>
+      </c>
+      <c r="E4" s="20">
+        <v>31.677779999999998</v>
+      </c>
+      <c r="F4" s="20">
+        <v>31.68056</v>
+      </c>
+      <c r="G4" s="20">
+        <v>31.68056</v>
+      </c>
+      <c r="H4" s="20">
+        <v>31.68056</v>
+      </c>
+      <c r="I4" s="20">
+        <v>31.68056</v>
+      </c>
+      <c r="J4" s="20">
+        <v>31.66667</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" ht="12.75">
+      <c r="A5" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="B5" s="25">
+        <v>38353</v>
+      </c>
+      <c r="C5" s="25">
+        <v>38353</v>
+      </c>
+      <c r="D5" s="25">
+        <v>38353</v>
+      </c>
+      <c r="E5" s="25">
+        <v>38353</v>
+      </c>
+      <c r="F5" s="25">
+        <v>38353</v>
+      </c>
+      <c r="G5" s="25">
+        <v>38353</v>
+      </c>
+      <c r="H5" s="25">
+        <v>38353</v>
+      </c>
+      <c r="I5" s="25">
+        <v>38353</v>
+      </c>
+      <c r="J5" s="25">
+        <v>38353</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" ht="12.75">
+      <c r="A6" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="B6" s="25">
+        <v>39082</v>
+      </c>
+      <c r="C6" s="25">
+        <v>39082</v>
+      </c>
+      <c r="D6" s="25">
+        <v>39082</v>
+      </c>
+      <c r="E6" s="25">
+        <v>39082</v>
+      </c>
+      <c r="F6" s="25">
+        <v>39082</v>
+      </c>
+      <c r="G6" s="25">
+        <v>39082</v>
+      </c>
+      <c r="H6" s="25">
+        <v>39082</v>
+      </c>
+      <c r="I6" s="25">
+        <v>39082</v>
+      </c>
+      <c r="J6" s="25">
+        <v>39082</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" ht="12.75">
+      <c r="A7" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="B7" s="25">
+        <v>38703</v>
+      </c>
+      <c r="C7" s="24">
+        <v>37632</v>
+      </c>
+      <c r="D7" s="24">
+        <v>37635</v>
+      </c>
+      <c r="E7" s="24">
+        <v>37946</v>
+      </c>
+      <c r="F7" s="24">
+        <v>37946</v>
+      </c>
+      <c r="G7" s="24">
+        <v>37970</v>
+      </c>
+      <c r="H7" s="24">
+        <v>37974</v>
+      </c>
+      <c r="I7" s="24">
+        <v>37975</v>
+      </c>
+      <c r="J7" s="24">
+        <v>37979</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" ht="12.75">
+      <c r="A8" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="B8" s="19" t="s">
+        <v>40</v>
+      </c>
+      <c r="C8" s="19" t="s">
+        <v>40</v>
+      </c>
+      <c r="D8" s="19" t="s">
+        <v>40</v>
+      </c>
+      <c r="E8" s="19" t="s">
+        <v>40</v>
+      </c>
+      <c r="F8" s="19" t="s">
+        <v>40</v>
+      </c>
+      <c r="G8" s="19" t="s">
+        <v>40</v>
+      </c>
+      <c r="H8" s="19" t="s">
+        <v>40</v>
+      </c>
+      <c r="I8" s="19" t="s">
+        <v>40</v>
+      </c>
+      <c r="J8" s="19" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" ht="12.75">
+      <c r="A9" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="B9" s="19">
+        <v>3</v>
+      </c>
+      <c r="C9" s="19">
+        <v>3</v>
+      </c>
+      <c r="D9" s="19">
+        <v>3</v>
+      </c>
+      <c r="E9" s="19">
+        <v>3</v>
+      </c>
+      <c r="F9" s="19">
+        <v>3</v>
+      </c>
+      <c r="G9" s="19">
+        <v>3</v>
+      </c>
+      <c r="H9" s="19">
+        <v>3</v>
+      </c>
+      <c r="I9" s="19">
+        <v>3</v>
+      </c>
+      <c r="J9" s="19">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" ht="12.75">
+      <c r="A10" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="B10" s="28" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="3" spans="1:10" ht="12.75">
-      <c r="A3" s="29" t="s">
-        <v>33</v>
-      </c>
-      <c r="B3" s="40">
-        <v>-7.6097200000000003</v>
-      </c>
-      <c r="C3" s="40">
-        <v>-7.5916699999999997</v>
-      </c>
-      <c r="D3" s="40">
-        <v>-7.5944399999999996</v>
-      </c>
-      <c r="E3" s="40">
-        <v>-7.5916699999999997</v>
-      </c>
-      <c r="F3" s="40">
-        <v>-7.5888900000000001</v>
-      </c>
-      <c r="G3" s="40">
-        <v>-7.5986099999999999</v>
-      </c>
-      <c r="H3" s="40">
-        <v>-7.5958300000000003</v>
-      </c>
-      <c r="I3" s="40">
-        <v>-7.5916699999999997</v>
-      </c>
-      <c r="J3" s="40">
-        <v>-7.61111</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" ht="12.75">
-      <c r="A4" s="29" t="s">
-        <v>34</v>
-      </c>
-      <c r="B4" s="40">
-        <v>31.661110000000001</v>
-      </c>
-      <c r="C4" s="40">
-        <v>31.66667</v>
-      </c>
-      <c r="D4" s="40">
-        <v>31.668060000000001</v>
-      </c>
-      <c r="E4" s="40">
-        <v>31.677779999999998</v>
-      </c>
-      <c r="F4" s="40">
-        <v>31.68056</v>
-      </c>
-      <c r="G4" s="40">
-        <v>31.68056</v>
-      </c>
-      <c r="H4" s="40">
-        <v>31.68056</v>
-      </c>
-      <c r="I4" s="40">
-        <v>31.68056</v>
-      </c>
-      <c r="J4" s="40">
-        <v>31.66667</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" ht="12.75">
-      <c r="A5" s="29" t="s">
-        <v>35</v>
-      </c>
-      <c r="B5" s="45">
-        <v>38353</v>
-      </c>
-      <c r="C5" s="45">
-        <v>38353</v>
-      </c>
-      <c r="D5" s="45">
-        <v>38353</v>
-      </c>
-      <c r="E5" s="45">
-        <v>38353</v>
-      </c>
-      <c r="F5" s="45">
-        <v>38353</v>
-      </c>
-      <c r="G5" s="45">
-        <v>38353</v>
-      </c>
-      <c r="H5" s="45">
-        <v>38353</v>
-      </c>
-      <c r="I5" s="45">
-        <v>38353</v>
-      </c>
-      <c r="J5" s="45">
-        <v>38353</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" ht="12.75">
-      <c r="A6" s="29" t="s">
-        <v>36</v>
-      </c>
-      <c r="B6" s="45">
-        <v>39082</v>
-      </c>
-      <c r="C6" s="45">
-        <v>39082</v>
-      </c>
-      <c r="D6" s="45">
-        <v>39082</v>
-      </c>
-      <c r="E6" s="45">
-        <v>39082</v>
-      </c>
-      <c r="F6" s="45">
-        <v>39082</v>
-      </c>
-      <c r="G6" s="45">
-        <v>39082</v>
-      </c>
-      <c r="H6" s="45">
-        <v>39082</v>
-      </c>
-      <c r="I6" s="45">
-        <v>39082</v>
-      </c>
-      <c r="J6" s="45">
-        <v>39082</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" ht="12.75">
-      <c r="A7" s="29" t="s">
-        <v>38</v>
-      </c>
-      <c r="B7" s="45">
-        <v>38703</v>
-      </c>
-      <c r="C7" s="44">
-        <v>37632</v>
-      </c>
-      <c r="D7" s="44">
-        <v>37635</v>
-      </c>
-      <c r="E7" s="44">
-        <v>37946</v>
-      </c>
-      <c r="F7" s="44">
-        <v>37946</v>
-      </c>
-      <c r="G7" s="44">
-        <v>37970</v>
-      </c>
-      <c r="H7" s="44">
-        <v>37974</v>
-      </c>
-      <c r="I7" s="44">
-        <v>37975</v>
-      </c>
-      <c r="J7" s="44">
-        <v>37979</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" ht="12.75">
-      <c r="A8" s="29" t="s">
-        <v>40</v>
-      </c>
-      <c r="B8" s="39" t="s">
-        <v>41</v>
-      </c>
-      <c r="C8" s="39" t="s">
-        <v>41</v>
-      </c>
-      <c r="D8" s="39" t="s">
-        <v>41</v>
-      </c>
-      <c r="E8" s="39" t="s">
-        <v>41</v>
-      </c>
-      <c r="F8" s="39" t="s">
-        <v>41</v>
-      </c>
-      <c r="G8" s="39" t="s">
-        <v>41</v>
-      </c>
-      <c r="H8" s="39" t="s">
-        <v>41</v>
-      </c>
-      <c r="I8" s="39" t="s">
-        <v>41</v>
-      </c>
-      <c r="J8" s="39" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" ht="12.75">
-      <c r="A9" s="29" t="s">
+      <c r="C10" s="29"/>
+      <c r="D10" s="29"/>
+      <c r="E10" s="29"/>
+      <c r="F10" s="29"/>
+      <c r="G10" s="29"/>
+      <c r="H10" s="29"/>
+      <c r="I10" s="29"/>
+      <c r="J10" s="30"/>
+    </row>
+    <row r="11" spans="1:10" ht="12.75">
+      <c r="A11" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="B11" s="21" t="s">
+        <v>46</v>
+      </c>
+      <c r="C11" s="22" t="s">
+        <v>46</v>
+      </c>
+      <c r="D11" s="22" t="s">
+        <v>46</v>
+      </c>
+      <c r="E11" s="22" t="s">
+        <v>46</v>
+      </c>
+      <c r="F11" s="22" t="s">
+        <v>46</v>
+      </c>
+      <c r="G11" s="22" t="s">
+        <v>46</v>
+      </c>
+      <c r="H11" s="22" t="s">
+        <v>46</v>
+      </c>
+      <c r="I11" s="22" t="s">
+        <v>46</v>
+      </c>
+      <c r="J11" s="19" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" ht="12.75">
+      <c r="A12" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="B12" s="19">
+        <v>2.75</v>
+      </c>
+      <c r="C12" s="19">
+        <v>2</v>
+      </c>
+      <c r="D12" s="19">
+        <v>0.85</v>
+      </c>
+      <c r="E12" s="19">
+        <v>2.75</v>
+      </c>
+      <c r="F12" s="19">
+        <v>2.25</v>
+      </c>
+      <c r="G12" s="19">
+        <v>2.25</v>
+      </c>
+      <c r="H12" s="19">
+        <v>3.25</v>
+      </c>
+      <c r="I12" s="19">
+        <v>1.25</v>
+      </c>
+      <c r="J12" s="19">
+        <v>2.25</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" ht="12.75">
+      <c r="A13" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="B13" s="19">
+        <v>90</v>
+      </c>
+      <c r="C13" s="19">
+        <v>180</v>
+      </c>
+      <c r="D13" s="19">
+        <v>120</v>
+      </c>
+      <c r="E13" s="19">
+        <v>180</v>
+      </c>
+      <c r="F13" s="19">
+        <v>180</v>
+      </c>
+      <c r="G13" s="19">
+        <v>180</v>
+      </c>
+      <c r="H13" s="19">
+        <v>180</v>
+      </c>
+      <c r="I13" s="19">
+        <v>180</v>
+      </c>
+      <c r="J13" s="19">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" ht="12.75">
+      <c r="A14" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="B14" s="19">
+        <v>337.3</v>
+      </c>
+      <c r="C14" s="19">
+        <v>225</v>
+      </c>
+      <c r="D14" s="19">
+        <v>337.3</v>
+      </c>
+      <c r="E14" s="19">
+        <v>337.3</v>
+      </c>
+      <c r="F14" s="19">
+        <v>225</v>
+      </c>
+      <c r="G14" s="19">
+        <v>337.3</v>
+      </c>
+      <c r="H14" s="19">
+        <v>225</v>
+      </c>
+      <c r="I14" s="19">
+        <v>225</v>
+      </c>
+      <c r="J14" s="19">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" ht="12.75">
+      <c r="A15" s="9" t="s">
+        <v>103</v>
+      </c>
+      <c r="B15" s="19">
+        <v>150</v>
+      </c>
+      <c r="C15" s="19">
+        <v>100</v>
+      </c>
+      <c r="D15" s="19">
+        <v>150</v>
+      </c>
+      <c r="E15" s="19">
+        <v>150</v>
+      </c>
+      <c r="F15" s="19">
+        <v>100</v>
+      </c>
+      <c r="G15" s="19">
+        <v>150</v>
+      </c>
+      <c r="H15" s="19">
+        <v>100</v>
+      </c>
+      <c r="I15" s="19">
+        <v>100</v>
+      </c>
+      <c r="J15" s="19">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" ht="12.75">
+      <c r="A16" s="9" t="s">
+        <v>104</v>
+      </c>
+      <c r="B16" s="19">
+        <v>20</v>
+      </c>
+      <c r="C16" s="19">
+        <v>65</v>
+      </c>
+      <c r="D16" s="19">
+        <v>20</v>
+      </c>
+      <c r="E16" s="19">
+        <v>45</v>
+      </c>
+      <c r="F16" s="19">
+        <v>20</v>
+      </c>
+      <c r="G16" s="19">
+        <v>20</v>
+      </c>
+      <c r="H16" s="19">
+        <v>65</v>
+      </c>
+      <c r="I16" s="19">
+        <v>20</v>
+      </c>
+      <c r="J16" s="19">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" ht="12.75">
+      <c r="A19" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="B19" s="19">
+        <v>3</v>
+      </c>
+      <c r="C19" s="19">
+        <v>3</v>
+      </c>
+      <c r="D19" s="19">
+        <v>3</v>
+      </c>
+      <c r="E19" s="19">
+        <v>3</v>
+      </c>
+      <c r="F19" s="19">
+        <v>3</v>
+      </c>
+      <c r="G19" s="19">
+        <v>3</v>
+      </c>
+      <c r="H19" s="19">
+        <v>3</v>
+      </c>
+      <c r="I19" s="19">
+        <v>3</v>
+      </c>
+      <c r="J19" s="19">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" ht="12.75">
+      <c r="A20" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="B9" s="39">
-        <v>3</v>
-      </c>
-      <c r="C9" s="39">
-        <v>3</v>
-      </c>
-      <c r="D9" s="39">
-        <v>3</v>
-      </c>
-      <c r="E9" s="39">
-        <v>3</v>
-      </c>
-      <c r="F9" s="39">
-        <v>3</v>
-      </c>
-      <c r="G9" s="39">
-        <v>3</v>
-      </c>
-      <c r="H9" s="39">
-        <v>3</v>
-      </c>
-      <c r="I9" s="39">
-        <v>3</v>
-      </c>
-      <c r="J9" s="39">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" ht="12.75">
-      <c r="A10" s="29" t="s">
-        <v>44</v>
-      </c>
-      <c r="B10" s="48" t="s">
+      <c r="B20" s="28" t="s">
+        <v>95</v>
+      </c>
+      <c r="C20" s="29"/>
+      <c r="D20" s="29"/>
+      <c r="E20" s="29"/>
+      <c r="F20" s="29"/>
+      <c r="G20" s="29"/>
+      <c r="H20" s="29"/>
+      <c r="I20" s="29"/>
+      <c r="J20" s="30"/>
+    </row>
+    <row r="21" spans="1:10" ht="12.75">
+      <c r="A21" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="B21" s="19" t="s">
         <v>96</v>
       </c>
-      <c r="C10" s="49"/>
-      <c r="D10" s="49"/>
-      <c r="E10" s="49"/>
-      <c r="F10" s="49"/>
-      <c r="G10" s="49"/>
-      <c r="H10" s="49"/>
-      <c r="I10" s="49"/>
-      <c r="J10" s="50"/>
-    </row>
-    <row r="11" spans="1:10" ht="12.75">
-      <c r="A11" s="29" t="s">
-        <v>45</v>
-      </c>
-      <c r="B11" s="41" t="s">
-        <v>47</v>
-      </c>
-      <c r="C11" s="42" t="s">
-        <v>47</v>
-      </c>
-      <c r="D11" s="42" t="s">
-        <v>47</v>
-      </c>
-      <c r="E11" s="42" t="s">
-        <v>47</v>
-      </c>
-      <c r="F11" s="42" t="s">
-        <v>47</v>
-      </c>
-      <c r="G11" s="42" t="s">
-        <v>47</v>
-      </c>
-      <c r="H11" s="42" t="s">
-        <v>47</v>
-      </c>
-      <c r="I11" s="42" t="s">
-        <v>47</v>
-      </c>
-      <c r="J11" s="39" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" ht="12.75">
-      <c r="A12" s="29" t="s">
-        <v>49</v>
-      </c>
-      <c r="B12" s="39">
-        <v>2.75</v>
-      </c>
-      <c r="C12" s="39">
-        <v>2</v>
-      </c>
-      <c r="D12" s="39">
-        <v>0.85</v>
-      </c>
-      <c r="E12" s="39">
-        <v>2.75</v>
-      </c>
-      <c r="F12" s="39">
-        <v>2.25</v>
-      </c>
-      <c r="G12" s="39">
-        <v>2.25</v>
-      </c>
-      <c r="H12" s="39">
-        <v>3.25</v>
-      </c>
-      <c r="I12" s="39">
-        <v>1.25</v>
-      </c>
-      <c r="J12" s="39">
-        <v>2.25</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" ht="12.75">
-      <c r="A13" s="29" t="s">
-        <v>50</v>
-      </c>
-      <c r="B13" s="39">
-        <v>90</v>
-      </c>
-      <c r="C13" s="39">
-        <v>180</v>
-      </c>
-      <c r="D13" s="39">
-        <v>120</v>
-      </c>
-      <c r="E13" s="39">
-        <v>180</v>
-      </c>
-      <c r="F13" s="39">
-        <v>180</v>
-      </c>
-      <c r="G13" s="39">
-        <v>180</v>
-      </c>
-      <c r="H13" s="39">
-        <v>180</v>
-      </c>
-      <c r="I13" s="39">
-        <v>180</v>
-      </c>
-      <c r="J13" s="39">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" ht="12.75">
-      <c r="A14" s="29" t="s">
-        <v>103</v>
-      </c>
-      <c r="B14" s="39">
-        <v>337.3</v>
-      </c>
-      <c r="C14" s="39">
-        <v>225</v>
-      </c>
-      <c r="D14" s="39">
-        <v>337.3</v>
-      </c>
-      <c r="E14" s="39">
-        <v>337.3</v>
-      </c>
-      <c r="F14" s="39">
-        <v>225</v>
-      </c>
-      <c r="G14" s="39">
-        <v>337.3</v>
-      </c>
-      <c r="H14" s="39">
-        <v>225</v>
-      </c>
-      <c r="I14" s="39">
-        <v>225</v>
-      </c>
-      <c r="J14" s="39">
-        <v>315</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" ht="12.75">
-      <c r="A15" s="29" t="s">
-        <v>104</v>
-      </c>
-      <c r="B15" s="39">
-        <v>150</v>
-      </c>
-      <c r="C15" s="39">
+      <c r="C21" s="19" t="s">
+        <v>97</v>
+      </c>
+      <c r="D21" s="19" t="s">
+        <v>98</v>
+      </c>
+      <c r="E21" s="19" t="s">
+        <v>96</v>
+      </c>
+      <c r="F21" s="19" t="s">
+        <v>99</v>
+      </c>
+      <c r="G21" s="19" t="s">
+        <v>99</v>
+      </c>
+      <c r="H21" s="19" t="s">
         <v>100</v>
       </c>
-      <c r="D15" s="39">
-        <v>150</v>
-      </c>
-      <c r="E15" s="39">
-        <v>150</v>
-      </c>
-      <c r="F15" s="39">
-        <v>100</v>
-      </c>
-      <c r="G15" s="39">
-        <v>150</v>
-      </c>
-      <c r="H15" s="39">
-        <v>100</v>
-      </c>
-      <c r="I15" s="39">
-        <v>100</v>
-      </c>
-      <c r="J15" s="39">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" ht="12.75">
-      <c r="A16" s="29" t="s">
-        <v>105</v>
-      </c>
-      <c r="B16" s="39">
-        <v>20</v>
-      </c>
-      <c r="C16" s="39">
-        <v>65</v>
-      </c>
-      <c r="D16" s="39">
-        <v>20</v>
-      </c>
-      <c r="E16" s="39">
-        <v>45</v>
-      </c>
-      <c r="F16" s="39">
-        <v>20</v>
-      </c>
-      <c r="G16" s="39">
-        <v>20</v>
-      </c>
-      <c r="H16" s="39">
-        <v>65</v>
-      </c>
-      <c r="I16" s="39">
-        <v>20</v>
-      </c>
-      <c r="J16" s="39">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10" ht="12.75">
-      <c r="A19" s="29" t="s">
-        <v>43</v>
-      </c>
-      <c r="B19" s="39">
-        <v>3</v>
-      </c>
-      <c r="C19" s="39">
-        <v>3</v>
-      </c>
-      <c r="D19" s="39">
-        <v>3</v>
-      </c>
-      <c r="E19" s="39">
-        <v>3</v>
-      </c>
-      <c r="F19" s="39">
-        <v>3</v>
-      </c>
-      <c r="G19" s="39">
-        <v>3</v>
-      </c>
-      <c r="H19" s="39">
-        <v>3</v>
-      </c>
-      <c r="I19" s="39">
-        <v>3</v>
-      </c>
-      <c r="J19" s="39">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="20" spans="1:10" ht="12.75">
-      <c r="A20" s="29" t="s">
-        <v>44</v>
-      </c>
-      <c r="B20" s="48" t="s">
-        <v>96</v>
-      </c>
-      <c r="C20" s="49"/>
-      <c r="D20" s="49"/>
-      <c r="E20" s="49"/>
-      <c r="F20" s="49"/>
-      <c r="G20" s="49"/>
-      <c r="H20" s="49"/>
-      <c r="I20" s="49"/>
-      <c r="J20" s="50"/>
-    </row>
-    <row r="21" spans="1:10" ht="12.75">
-      <c r="A21" s="29" t="s">
-        <v>49</v>
-      </c>
-      <c r="B21" s="39" t="s">
-        <v>97</v>
-      </c>
-      <c r="C21" s="39" t="s">
-        <v>98</v>
-      </c>
-      <c r="D21" s="39" t="s">
+      <c r="I21" s="19" t="s">
+        <v>101</v>
+      </c>
+      <c r="J21" s="19" t="s">
         <v>99</v>
-      </c>
-      <c r="E21" s="39" t="s">
-        <v>97</v>
-      </c>
-      <c r="F21" s="39" t="s">
-        <v>100</v>
-      </c>
-      <c r="G21" s="39" t="s">
-        <v>100</v>
-      </c>
-      <c r="H21" s="39" t="s">
-        <v>101</v>
-      </c>
-      <c r="I21" s="39" t="s">
-        <v>102</v>
-      </c>
-      <c r="J21" s="39" t="s">
-        <v>100</v>
       </c>
     </row>
   </sheetData>
@@ -4626,182 +4658,182 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="15.75" customHeight="1">
-      <c r="A1" s="28"/>
+      <c r="A1" s="8"/>
       <c r="B1" s="1" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="12.75">
+      <c r="A2" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="B2" s="19" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" ht="12.75">
-      <c r="A2" s="29" t="s">
-        <v>19</v>
-      </c>
-      <c r="B2" s="39" t="s">
+      <c r="C2" s="19" t="s">
         <v>107</v>
       </c>
-      <c r="C2" s="39" t="s">
+      <c r="D2" s="19" t="s">
         <v>108</v>
       </c>
-      <c r="D2" s="39" t="s">
+      <c r="E2" s="19" t="s">
         <v>109</v>
       </c>
-      <c r="E2" s="39" t="s">
+      <c r="F2" s="19" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="12.75">
+      <c r="A3" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="B3" s="19" t="s">
         <v>110</v>
       </c>
-      <c r="F2" s="39" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" ht="12.75">
-      <c r="A3" s="29" t="s">
-        <v>33</v>
-      </c>
-      <c r="B3" s="39" t="s">
+      <c r="C3" s="19"/>
+      <c r="D3" s="19"/>
+      <c r="E3" s="19"/>
+      <c r="F3" s="19"/>
+    </row>
+    <row r="4" spans="1:6" ht="12.75">
+      <c r="A4" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="B4" s="19"/>
+      <c r="C4" s="19"/>
+      <c r="D4" s="19"/>
+      <c r="E4" s="19"/>
+      <c r="F4" s="19"/>
+    </row>
+    <row r="5" spans="1:6" ht="12.75">
+      <c r="A5" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="B5" s="19" t="s">
         <v>111</v>
       </c>
-      <c r="C3" s="39"/>
-      <c r="D3" s="39"/>
-      <c r="E3" s="39"/>
-      <c r="F3" s="39"/>
-    </row>
-    <row r="4" spans="1:6" ht="12.75">
-      <c r="A4" s="29" t="s">
-        <v>34</v>
-      </c>
-      <c r="B4" s="39"/>
-      <c r="C4" s="39"/>
-      <c r="D4" s="39"/>
-      <c r="E4" s="39"/>
-      <c r="F4" s="39"/>
-    </row>
-    <row r="5" spans="1:6" ht="12.75">
-      <c r="A5" s="29" t="s">
-        <v>35</v>
-      </c>
-      <c r="B5" s="39" t="s">
+      <c r="C5" s="19" t="s">
+        <v>111</v>
+      </c>
+      <c r="D5" s="19" t="s">
         <v>112</v>
       </c>
-      <c r="C5" s="39" t="s">
+      <c r="E5" s="19" t="s">
         <v>112</v>
       </c>
-      <c r="D5" s="39" t="s">
+      <c r="F5" s="19" t="s">
         <v>113</v>
       </c>
-      <c r="E5" s="39" t="s">
-        <v>113</v>
-      </c>
-      <c r="F5" s="39" t="s">
+    </row>
+    <row r="6" spans="1:6" ht="12.75">
+      <c r="A6" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="B6" s="19" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" ht="12.75">
-      <c r="A6" s="29" t="s">
-        <v>36</v>
-      </c>
-      <c r="B6" s="39" t="s">
+      <c r="C6" s="19"/>
+      <c r="D6" s="19"/>
+      <c r="E6" s="19"/>
+      <c r="F6" s="19"/>
+    </row>
+    <row r="7" spans="1:6" ht="12.75">
+      <c r="A7" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="B7" s="19"/>
+      <c r="C7" s="19"/>
+      <c r="D7" s="19"/>
+      <c r="E7" s="19"/>
+      <c r="F7" s="19"/>
+    </row>
+    <row r="8" spans="1:6" ht="12.75">
+      <c r="A8" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="B8" s="23" t="s">
         <v>115</v>
       </c>
-      <c r="C6" s="39"/>
-      <c r="D6" s="39"/>
-      <c r="E6" s="39"/>
-      <c r="F6" s="39"/>
-    </row>
-    <row r="7" spans="1:6" ht="12.75">
-      <c r="A7" s="29" t="s">
-        <v>38</v>
-      </c>
-      <c r="B7" s="39"/>
-      <c r="C7" s="39"/>
-      <c r="D7" s="39"/>
-      <c r="E7" s="39"/>
-      <c r="F7" s="39"/>
-    </row>
-    <row r="8" spans="1:6" ht="12.75">
-      <c r="A8" s="29" t="s">
-        <v>40</v>
-      </c>
-      <c r="B8" s="43" t="s">
+      <c r="C8" s="19"/>
+      <c r="D8" s="19"/>
+      <c r="E8" s="19"/>
+      <c r="F8" s="19"/>
+    </row>
+    <row r="9" spans="1:6" ht="12.75">
+      <c r="A9" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="B9" s="19" t="s">
         <v>116</v>
       </c>
-      <c r="C8" s="39"/>
-      <c r="D8" s="39"/>
-      <c r="E8" s="39"/>
-      <c r="F8" s="39"/>
-    </row>
-    <row r="9" spans="1:6" ht="12.75">
-      <c r="A9" s="29" t="s">
+      <c r="C9" s="19"/>
+      <c r="D9" s="19" t="s">
+        <v>116</v>
+      </c>
+      <c r="E9" s="19"/>
+      <c r="F9" s="19" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="12.75">
+      <c r="A10" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="B9" s="39" t="s">
-        <v>117</v>
-      </c>
-      <c r="C9" s="39"/>
-      <c r="D9" s="39" t="s">
-        <v>117</v>
-      </c>
-      <c r="E9" s="39"/>
-      <c r="F9" s="39" t="s">
+      <c r="B10" s="19"/>
+      <c r="C10" s="19"/>
+      <c r="D10" s="19"/>
+      <c r="E10" s="19"/>
+      <c r="F10" s="19"/>
+    </row>
+    <row r="11" spans="1:6" ht="12.75">
+      <c r="A11" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="B11" s="19" t="s">
         <v>118</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" ht="12.75">
-      <c r="A10" s="29" t="s">
-        <v>44</v>
-      </c>
-      <c r="B10" s="39"/>
-      <c r="C10" s="39"/>
-      <c r="D10" s="39"/>
-      <c r="E10" s="39"/>
-      <c r="F10" s="39"/>
-    </row>
-    <row r="11" spans="1:6" ht="12.75">
-      <c r="A11" s="29" t="s">
-        <v>45</v>
-      </c>
-      <c r="B11" s="39" t="s">
-        <v>119</v>
-      </c>
-      <c r="C11" s="39" t="s">
-        <v>119</v>
-      </c>
-      <c r="D11" s="39" t="s">
-        <v>119</v>
-      </c>
-      <c r="E11" s="39" t="s">
-        <v>119</v>
-      </c>
-      <c r="F11" s="39" t="s">
-        <v>119</v>
+      <c r="C11" s="19" t="s">
+        <v>118</v>
+      </c>
+      <c r="D11" s="19" t="s">
+        <v>118</v>
+      </c>
+      <c r="E11" s="19" t="s">
+        <v>118</v>
+      </c>
+      <c r="F11" s="19" t="s">
+        <v>118</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="12.75">
-      <c r="A12" s="29" t="s">
+      <c r="A12" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="B12" s="19">
+        <v>13.7</v>
+      </c>
+      <c r="C12" s="19">
+        <v>13</v>
+      </c>
+      <c r="D12" s="19"/>
+      <c r="E12" s="19">
+        <v>9.9</v>
+      </c>
+      <c r="F12" s="19"/>
+    </row>
+    <row r="13" spans="1:6" ht="12.75">
+      <c r="A13" s="9" t="s">
         <v>49</v>
       </c>
-      <c r="B12" s="39">
-        <v>13.7</v>
-      </c>
-      <c r="C12" s="39">
-        <v>13</v>
-      </c>
-      <c r="D12" s="39"/>
-      <c r="E12" s="39">
-        <v>9.9</v>
-      </c>
-      <c r="F12" s="39"/>
-    </row>
-    <row r="13" spans="1:6" ht="12.75">
-      <c r="A13" s="29" t="s">
-        <v>50</v>
-      </c>
-      <c r="B13" s="39"/>
-      <c r="C13" s="39"/>
-      <c r="D13" s="39"/>
-      <c r="E13" s="39"/>
-      <c r="F13" s="39"/>
+      <c r="B13" s="19"/>
+      <c r="C13" s="19"/>
+      <c r="D13" s="19"/>
+      <c r="E13" s="19"/>
+      <c r="F13" s="19"/>
     </row>
     <row r="14" spans="1:6" ht="12.75">
       <c r="A14" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B14" s="1" t="b">
         <v>1</v>

</xml_diff>

<commit_message>
completed case study for north east china case. Note: location is not accurate (42.57;119.19) but this is the closest that work. In addition the mulches have been let on default but can still be explored. 2016 is a gap year, so a longer simulation was done to fix that again. This commit adds a compile for NE china, results excel file, and a plot.py. In addition a name change for the bangladesh results_plot.py file and a change in the input factors file to make it compatible with the latest case study simulation
</commit_message>
<xml_diff>
--- a/heliostrome/jip_project/results/Factors to run simulation.xlsx
+++ b/heliostrome/jip_project/results/Factors to run simulation.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://tud365-my.sharepoint.com/personal/sparijs_tudelft_nl/Documents/Documents/helios/heliostrome/heliostrome/jip_project/results/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="14_{4DB74DB0-FE42-482F-A370-D6BB3F0DF436}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="5" documentId="11_CCED90458BCA10E459EEC6424CC4CFDBB62AFD01" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DB82C555-FB83-47B1-A5D5-EF28F956E0C7}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="298" uniqueCount="130">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="298" uniqueCount="129">
   <si>
     <t>Evaluation of AquaCrop model performance under mulched drip irrigation for maize in Northeast China</t>
   </si>
@@ -69,7 +69,7 @@
     <t>Soil Type</t>
   </si>
   <si>
-    <t>Sandy Loam</t>
+    <t>SandyLoam</t>
   </si>
   <si>
     <t>Irrigation Method (method with SMT if possible)</t>
@@ -248,9 +248,6 @@
   </si>
   <si>
     <t>Rice (Barisal)</t>
-  </si>
-  <si>
-    <t>SandyLoam</t>
   </si>
   <si>
     <t>Tomato</t>
@@ -460,14 +457,14 @@
       <family val="2"/>
     </font>
     <font>
-      <sz val="10"/>
-      <color rgb="FF333333"/>
-      <name val="Arial"/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
       <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
-      <color theme="1"/>
+      <color rgb="FF333333"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -749,7 +746,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="86">
+  <cellXfs count="84">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -811,14 +808,13 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="3" fontId="1" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="4" fontId="5" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="4" fontId="6" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="14" fontId="1" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -830,6 +826,9 @@
     <xf numFmtId="3" fontId="1" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="3" fontId="1" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -932,9 +931,6 @@
     <xf numFmtId="3" fontId="1" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="3" fontId="1" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -968,8 +964,9 @@
     <xf numFmtId="14" fontId="9" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
@@ -988,14 +985,16 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="3" fontId="5" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="3" fontId="1" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="3" fontId="6" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="3" fontId="6" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -1013,6 +1012,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1312,158 +1315,158 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.7109375" style="17" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="19.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="21.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17" style="17" bestFit="1" customWidth="1"/>
     <col min="5" max="7" width="13.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="18.75" customHeight="1">
       <c r="B1" s="38" t="s">
+        <v>111</v>
+      </c>
+      <c r="C1" s="38" t="s">
         <v>112</v>
       </c>
-      <c r="C1" s="38" t="s">
+      <c r="D1" s="74" t="s">
+        <v>45</v>
+      </c>
+      <c r="E1" s="38" t="s">
         <v>113</v>
       </c>
-      <c r="D1" s="76" t="s">
-        <v>45</v>
-      </c>
-      <c r="E1" s="38" t="s">
+      <c r="F1" s="38" t="s">
         <v>114</v>
       </c>
-      <c r="F1" s="38" t="s">
+      <c r="G1" s="74" t="s">
         <v>115</v>
-      </c>
-      <c r="G1" s="76" t="s">
-        <v>116</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="18.75" customHeight="1">
       <c r="A2" s="38" t="s">
-        <v>117</v>
-      </c>
-      <c r="B2" s="77"/>
-      <c r="C2" s="77"/>
-      <c r="D2" s="77"/>
-      <c r="E2" s="77"/>
-      <c r="F2" s="78"/>
-      <c r="G2" s="79"/>
+        <v>116</v>
+      </c>
+      <c r="B2" s="75"/>
+      <c r="C2" s="75"/>
+      <c r="D2" s="75"/>
+      <c r="E2" s="75"/>
+      <c r="F2" s="76"/>
+      <c r="G2" s="77"/>
     </row>
     <row r="3" spans="1:7" ht="18.75" customHeight="1">
       <c r="A3" s="38" t="s">
-        <v>118</v>
-      </c>
-      <c r="B3" s="77"/>
-      <c r="C3" s="78"/>
-      <c r="D3" s="77"/>
-      <c r="E3" s="78"/>
-      <c r="F3" s="77"/>
-      <c r="G3" s="77"/>
+        <v>117</v>
+      </c>
+      <c r="B3" s="75"/>
+      <c r="C3" s="76"/>
+      <c r="D3" s="75"/>
+      <c r="E3" s="76"/>
+      <c r="F3" s="75"/>
+      <c r="G3" s="75"/>
     </row>
     <row r="4" spans="1:7" ht="18.75" customHeight="1">
       <c r="A4" s="38" t="s">
-        <v>119</v>
-      </c>
-      <c r="B4" s="78"/>
-      <c r="C4" s="80"/>
-      <c r="D4" s="77"/>
-      <c r="E4" s="77"/>
-      <c r="F4" s="77"/>
-      <c r="G4" s="78"/>
+        <v>118</v>
+      </c>
+      <c r="B4" s="76"/>
+      <c r="C4" s="78"/>
+      <c r="D4" s="75"/>
+      <c r="E4" s="75"/>
+      <c r="F4" s="75"/>
+      <c r="G4" s="76"/>
     </row>
     <row r="5" spans="1:7" ht="18.75" customHeight="1">
       <c r="A5" s="38" t="s">
-        <v>120</v>
-      </c>
-      <c r="B5" s="78"/>
-      <c r="C5" s="79"/>
-      <c r="D5" s="77"/>
-      <c r="E5" s="77"/>
-      <c r="F5" s="79"/>
-      <c r="G5" s="77"/>
+        <v>119</v>
+      </c>
+      <c r="B5" s="76"/>
+      <c r="C5" s="77"/>
+      <c r="D5" s="75"/>
+      <c r="E5" s="75"/>
+      <c r="F5" s="77"/>
+      <c r="G5" s="75"/>
     </row>
     <row r="6" spans="1:7" ht="18.75" customHeight="1">
       <c r="A6" s="38" t="s">
-        <v>121</v>
-      </c>
-      <c r="B6" s="78"/>
-      <c r="C6" s="79"/>
-      <c r="D6" s="77"/>
-      <c r="E6" s="77"/>
-      <c r="F6" s="77"/>
-      <c r="G6" s="78"/>
+        <v>120</v>
+      </c>
+      <c r="B6" s="76"/>
+      <c r="C6" s="77"/>
+      <c r="D6" s="75"/>
+      <c r="E6" s="75"/>
+      <c r="F6" s="75"/>
+      <c r="G6" s="76"/>
     </row>
     <row r="7" spans="1:7" ht="18.75" customHeight="1">
       <c r="A7" s="38" t="s">
-        <v>122</v>
-      </c>
-      <c r="B7" s="77"/>
-      <c r="C7" s="77"/>
-      <c r="D7" s="77"/>
-      <c r="E7" s="79"/>
-      <c r="F7" s="77"/>
-      <c r="G7" s="77"/>
+        <v>121</v>
+      </c>
+      <c r="B7" s="75"/>
+      <c r="C7" s="75"/>
+      <c r="D7" s="75"/>
+      <c r="E7" s="77"/>
+      <c r="F7" s="75"/>
+      <c r="G7" s="75"/>
     </row>
     <row r="8" spans="1:7" ht="18.75" customHeight="1">
       <c r="A8" s="38" t="s">
-        <v>123</v>
-      </c>
-      <c r="B8" s="77"/>
-      <c r="C8" s="78"/>
-      <c r="D8" s="77"/>
-      <c r="E8" s="79"/>
-      <c r="F8" s="78"/>
-      <c r="G8" s="78"/>
+        <v>122</v>
+      </c>
+      <c r="B8" s="75"/>
+      <c r="C8" s="76"/>
+      <c r="D8" s="75"/>
+      <c r="E8" s="77"/>
+      <c r="F8" s="76"/>
+      <c r="G8" s="76"/>
     </row>
     <row r="9" spans="1:7" ht="18.75" customHeight="1">
       <c r="A9" s="38" t="s">
-        <v>124</v>
-      </c>
-      <c r="B9" s="78"/>
-      <c r="C9" s="78"/>
-      <c r="D9" s="77"/>
-      <c r="E9" s="79"/>
-      <c r="F9" s="77"/>
-      <c r="G9" s="78"/>
+        <v>123</v>
+      </c>
+      <c r="B9" s="76"/>
+      <c r="C9" s="76"/>
+      <c r="D9" s="75"/>
+      <c r="E9" s="77"/>
+      <c r="F9" s="75"/>
+      <c r="G9" s="76"/>
     </row>
     <row r="10" spans="1:7" ht="18.75" customHeight="1">
       <c r="A10" s="38" t="s">
-        <v>125</v>
-      </c>
-      <c r="B10" s="77"/>
-      <c r="C10" s="77"/>
-      <c r="D10" s="77"/>
-      <c r="E10" s="79"/>
-      <c r="F10" s="77"/>
-      <c r="G10" s="77"/>
+        <v>124</v>
+      </c>
+      <c r="B10" s="75"/>
+      <c r="C10" s="75"/>
+      <c r="D10" s="75"/>
+      <c r="E10" s="77"/>
+      <c r="F10" s="75"/>
+      <c r="G10" s="75"/>
     </row>
     <row r="11" spans="1:7" ht="18.75" customHeight="1">
       <c r="A11" s="38" t="s">
-        <v>126</v>
-      </c>
-      <c r="B11" s="77"/>
-      <c r="C11" s="78"/>
-      <c r="D11" s="77"/>
-      <c r="E11" s="79"/>
-      <c r="F11" s="79"/>
-      <c r="G11" s="77"/>
+        <v>125</v>
+      </c>
+      <c r="B11" s="75"/>
+      <c r="C11" s="76"/>
+      <c r="D11" s="75"/>
+      <c r="E11" s="77"/>
+      <c r="F11" s="77"/>
+      <c r="G11" s="75"/>
     </row>
     <row r="12" spans="1:7" ht="18.75" customHeight="1">
       <c r="A12" s="38" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D12" s="40"/>
     </row>
     <row r="13" spans="1:7" ht="18.75" customHeight="1">
       <c r="A13" s="38" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D13" s="40"/>
     </row>
     <row r="14" spans="1:7" ht="18.75" customHeight="1">
       <c r="A14" s="38" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D14" s="40"/>
     </row>
@@ -1486,12 +1489,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="46.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="24.28515625" style="74" bestFit="1" customWidth="1"/>
-    <col min="3" max="10" width="24.28515625" style="21" bestFit="1" customWidth="1"/>
-    <col min="11" max="15" width="24.28515625" style="75" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="24" style="21" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="13.5703125" style="74" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="46.85546875" style="17" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.28515625" style="44" bestFit="1" customWidth="1"/>
+    <col min="3" max="10" width="24.28515625" style="19" bestFit="1" customWidth="1"/>
+    <col min="11" max="15" width="24.28515625" style="73" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="24" style="19" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="13.5703125" style="44" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="15.75" customHeight="1">
@@ -1516,7 +1519,7 @@
       <c r="Q1" s="51"/>
     </row>
     <row r="2" spans="1:17" ht="18.75" customHeight="1">
-      <c r="A2" s="22" t="s">
+      <c r="A2" s="21" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="52" t="s">
@@ -1858,84 +1861,84 @@
       <c r="H8" s="61" t="s">
         <v>33</v>
       </c>
-      <c r="I8" s="62" t="s">
-        <v>74</v>
-      </c>
-      <c r="J8" s="62" t="s">
-        <v>74</v>
-      </c>
-      <c r="K8" s="63" t="s">
-        <v>74</v>
-      </c>
-      <c r="L8" s="63" t="s">
-        <v>74</v>
-      </c>
-      <c r="M8" s="63" t="s">
-        <v>74</v>
-      </c>
-      <c r="N8" s="63" t="s">
-        <v>74</v>
-      </c>
-      <c r="O8" s="63" t="s">
+      <c r="I8" s="27" t="s">
+        <v>14</v>
+      </c>
+      <c r="J8" s="27" t="s">
+        <v>14</v>
+      </c>
+      <c r="K8" s="62" t="s">
+        <v>14</v>
+      </c>
+      <c r="L8" s="62" t="s">
+        <v>14</v>
+      </c>
+      <c r="M8" s="62" t="s">
+        <v>14</v>
+      </c>
+      <c r="N8" s="62" t="s">
+        <v>14</v>
+      </c>
+      <c r="O8" s="62" t="s">
         <v>33</v>
       </c>
       <c r="P8" s="61" t="s">
         <v>33</v>
       </c>
       <c r="Q8" s="57" t="s">
-        <v>74</v>
+        <v>14</v>
       </c>
     </row>
     <row r="9" spans="1:17" ht="18.75" customHeight="1">
       <c r="A9" s="55" t="s">
         <v>15</v>
       </c>
-      <c r="B9" s="64">
+      <c r="B9" s="63">
         <v>35</v>
       </c>
-      <c r="C9" s="64">
+      <c r="C9" s="63">
         <v>35</v>
       </c>
-      <c r="D9" s="64">
+      <c r="D9" s="63">
         <v>35</v>
       </c>
-      <c r="E9" s="64">
+      <c r="E9" s="63">
         <v>35</v>
       </c>
-      <c r="F9" s="64">
+      <c r="F9" s="63">
         <v>35</v>
       </c>
-      <c r="G9" s="64">
+      <c r="G9" s="63">
         <v>35</v>
       </c>
-      <c r="H9" s="64">
+      <c r="H9" s="63">
         <v>35</v>
       </c>
-      <c r="I9" s="64">
+      <c r="I9" s="63">
         <v>33</v>
       </c>
-      <c r="J9" s="64">
+      <c r="J9" s="63">
         <v>33</v>
       </c>
-      <c r="K9" s="64">
+      <c r="K9" s="63">
         <v>30</v>
       </c>
-      <c r="L9" s="64">
+      <c r="L9" s="63">
         <v>30</v>
       </c>
-      <c r="M9" s="64">
+      <c r="M9" s="63">
         <v>32</v>
       </c>
-      <c r="N9" s="64">
+      <c r="N9" s="63">
         <v>32</v>
       </c>
-      <c r="O9" s="64">
+      <c r="O9" s="63">
         <v>100</v>
       </c>
-      <c r="P9" s="65">
+      <c r="P9" s="64">
         <v>100</v>
       </c>
-      <c r="Q9" s="66">
+      <c r="Q9" s="65">
         <v>100</v>
       </c>
     </row>
@@ -1943,52 +1946,52 @@
       <c r="A10" s="55" t="s">
         <v>16</v>
       </c>
-      <c r="B10" s="64">
+      <c r="B10" s="63">
         <v>26</v>
       </c>
-      <c r="C10" s="64">
+      <c r="C10" s="63">
         <v>26</v>
       </c>
-      <c r="D10" s="64">
+      <c r="D10" s="63">
         <v>26</v>
       </c>
-      <c r="E10" s="64">
+      <c r="E10" s="63">
         <v>26</v>
       </c>
-      <c r="F10" s="64">
+      <c r="F10" s="63">
         <v>26</v>
       </c>
-      <c r="G10" s="64">
+      <c r="G10" s="63">
         <v>26</v>
       </c>
-      <c r="H10" s="64">
+      <c r="H10" s="63">
         <v>26</v>
       </c>
-      <c r="I10" s="64">
+      <c r="I10" s="63">
         <v>22</v>
       </c>
-      <c r="J10" s="64">
+      <c r="J10" s="63">
         <v>22</v>
       </c>
-      <c r="K10" s="64">
+      <c r="K10" s="63">
         <v>22</v>
       </c>
-      <c r="L10" s="64">
+      <c r="L10" s="63">
         <v>22</v>
       </c>
-      <c r="M10" s="64">
+      <c r="M10" s="63">
         <v>22</v>
       </c>
-      <c r="N10" s="64">
+      <c r="N10" s="63">
         <v>22</v>
       </c>
-      <c r="O10" s="64">
+      <c r="O10" s="63">
         <v>26</v>
       </c>
-      <c r="P10" s="67">
+      <c r="P10" s="66">
         <v>50</v>
       </c>
-      <c r="Q10" s="64">
+      <c r="Q10" s="63">
         <v>41</v>
       </c>
     </row>
@@ -1997,52 +2000,52 @@
         <v>17</v>
       </c>
       <c r="B11" s="57" t="s">
+        <v>74</v>
+      </c>
+      <c r="C11" s="61" t="s">
+        <v>74</v>
+      </c>
+      <c r="D11" s="61" t="s">
+        <v>74</v>
+      </c>
+      <c r="E11" s="61" t="s">
+        <v>74</v>
+      </c>
+      <c r="F11" s="61" t="s">
+        <v>74</v>
+      </c>
+      <c r="G11" s="61" t="s">
+        <v>74</v>
+      </c>
+      <c r="H11" s="61" t="s">
+        <v>74</v>
+      </c>
+      <c r="I11" s="61" t="s">
+        <v>74</v>
+      </c>
+      <c r="J11" s="61" t="s">
+        <v>74</v>
+      </c>
+      <c r="K11" s="62" t="s">
+        <v>74</v>
+      </c>
+      <c r="L11" s="62" t="s">
+        <v>74</v>
+      </c>
+      <c r="M11" s="62" t="s">
+        <v>74</v>
+      </c>
+      <c r="N11" s="62" t="s">
+        <v>74</v>
+      </c>
+      <c r="O11" s="62" t="s">
+        <v>35</v>
+      </c>
+      <c r="P11" s="61" t="s">
         <v>75</v>
       </c>
-      <c r="C11" s="61" t="s">
+      <c r="Q11" s="57" t="s">
         <v>75</v>
-      </c>
-      <c r="D11" s="61" t="s">
-        <v>75</v>
-      </c>
-      <c r="E11" s="61" t="s">
-        <v>75</v>
-      </c>
-      <c r="F11" s="61" t="s">
-        <v>75</v>
-      </c>
-      <c r="G11" s="61" t="s">
-        <v>75</v>
-      </c>
-      <c r="H11" s="61" t="s">
-        <v>75</v>
-      </c>
-      <c r="I11" s="61" t="s">
-        <v>75</v>
-      </c>
-      <c r="J11" s="61" t="s">
-        <v>75</v>
-      </c>
-      <c r="K11" s="63" t="s">
-        <v>75</v>
-      </c>
-      <c r="L11" s="63" t="s">
-        <v>75</v>
-      </c>
-      <c r="M11" s="63" t="s">
-        <v>75</v>
-      </c>
-      <c r="N11" s="63" t="s">
-        <v>75</v>
-      </c>
-      <c r="O11" s="63" t="s">
-        <v>35</v>
-      </c>
-      <c r="P11" s="61" t="s">
-        <v>76</v>
-      </c>
-      <c r="Q11" s="57" t="s">
-        <v>76</v>
       </c>
     </row>
     <row r="12" spans="1:17" ht="18.75" customHeight="1">
@@ -2088,7 +2091,7 @@
       <c r="N12" s="56">
         <v>32.659999999999997</v>
       </c>
-      <c r="O12" s="64">
+      <c r="O12" s="63">
         <v>3</v>
       </c>
       <c r="P12" s="56">
@@ -2102,57 +2105,57 @@
       <c r="A13" s="55" t="s">
         <v>20</v>
       </c>
-      <c r="B13" s="64">
+      <c r="B13" s="63">
         <v>429</v>
       </c>
-      <c r="C13" s="64">
+      <c r="C13" s="63">
         <v>225</v>
       </c>
-      <c r="D13" s="64">
+      <c r="D13" s="63">
         <v>212</v>
       </c>
-      <c r="E13" s="64">
+      <c r="E13" s="63">
         <v>254</v>
       </c>
-      <c r="F13" s="64">
+      <c r="F13" s="63">
         <v>590</v>
       </c>
-      <c r="G13" s="64">
+      <c r="G13" s="63">
         <v>335</v>
       </c>
-      <c r="H13" s="64">
+      <c r="H13" s="63">
         <v>610</v>
       </c>
-      <c r="I13" s="64">
+      <c r="I13" s="63">
         <v>249</v>
       </c>
-      <c r="J13" s="64">
+      <c r="J13" s="63">
         <v>568</v>
       </c>
-      <c r="K13" s="64">
+      <c r="K13" s="63">
         <v>228</v>
       </c>
-      <c r="L13" s="64">
+      <c r="L13" s="63">
         <v>453</v>
       </c>
-      <c r="M13" s="63" t="s">
+      <c r="M13" s="62" t="s">
+        <v>76</v>
+      </c>
+      <c r="N13" s="62" t="s">
         <v>77</v>
       </c>
-      <c r="N13" s="63" t="s">
-        <v>78</v>
-      </c>
-      <c r="O13" s="64">
+      <c r="O13" s="63">
         <v>430</v>
       </c>
-      <c r="P13" s="64">
+      <c r="P13" s="63">
         <v>1324</v>
       </c>
-      <c r="Q13" s="64">
+      <c r="Q13" s="63">
         <v>1252</v>
       </c>
     </row>
     <row r="14" spans="1:17" ht="15.75" customHeight="1">
-      <c r="A14" s="68"/>
+      <c r="A14" s="67"/>
       <c r="B14" s="51"/>
       <c r="C14" s="50"/>
       <c r="D14" s="50"/>
@@ -2171,55 +2174,55 @@
       <c r="Q14" s="51"/>
     </row>
     <row r="15" spans="1:17" ht="18.75" customHeight="1">
-      <c r="A15" s="22" t="s">
+      <c r="A15" s="21" t="s">
         <v>10</v>
       </c>
-      <c r="B15" s="69">
+      <c r="B15" s="68">
         <v>40548</v>
       </c>
-      <c r="C15" s="69">
+      <c r="C15" s="68">
         <v>40548</v>
       </c>
-      <c r="D15" s="62" t="s">
+      <c r="D15" s="27" t="s">
+        <v>78</v>
+      </c>
+      <c r="E15" s="68">
+        <v>40553</v>
+      </c>
+      <c r="F15" s="68">
+        <v>40553</v>
+      </c>
+      <c r="G15" s="68">
+        <v>40918</v>
+      </c>
+      <c r="H15" s="68">
+        <v>40918</v>
+      </c>
+      <c r="I15" s="27" t="s">
         <v>79</v>
       </c>
-      <c r="E15" s="69">
-        <v>40553</v>
-      </c>
-      <c r="F15" s="69">
-        <v>40553</v>
-      </c>
-      <c r="G15" s="69">
-        <v>40918</v>
-      </c>
-      <c r="H15" s="69">
-        <v>40918</v>
-      </c>
-      <c r="I15" s="62" t="s">
-        <v>80</v>
-      </c>
-      <c r="J15" s="62" t="s">
-        <v>80</v>
-      </c>
-      <c r="K15" s="69">
+      <c r="J15" s="27" t="s">
+        <v>79</v>
+      </c>
+      <c r="K15" s="68">
         <v>40544</v>
       </c>
-      <c r="L15" s="69">
+      <c r="L15" s="68">
         <v>40544</v>
       </c>
-      <c r="M15" s="69">
+      <c r="M15" s="68">
         <v>40179</v>
       </c>
-      <c r="N15" s="69">
+      <c r="N15" s="68">
         <v>40179</v>
       </c>
-      <c r="O15" s="69">
+      <c r="O15" s="68">
         <v>40544</v>
       </c>
-      <c r="P15" s="69">
+      <c r="P15" s="68">
         <v>40544</v>
       </c>
-      <c r="Q15" s="69">
+      <c r="Q15" s="68">
         <v>40544</v>
       </c>
     </row>
@@ -2227,53 +2230,53 @@
       <c r="A16" s="55" t="s">
         <v>11</v>
       </c>
-      <c r="B16" s="63">
+      <c r="B16" s="62">
         <v>40913</v>
       </c>
-      <c r="C16" s="63">
+      <c r="C16" s="62">
         <v>40913</v>
       </c>
       <c r="D16" s="61" t="s">
+        <v>80</v>
+      </c>
+      <c r="E16" s="61" t="s">
         <v>81</v>
       </c>
-      <c r="E16" s="61" t="s">
+      <c r="F16" s="61" t="s">
+        <v>81</v>
+      </c>
+      <c r="G16" s="61" t="s">
         <v>82</v>
       </c>
-      <c r="F16" s="61" t="s">
+      <c r="H16" s="61" t="s">
         <v>82</v>
       </c>
-      <c r="G16" s="61" t="s">
+      <c r="I16" s="61" t="s">
         <v>83</v>
       </c>
-      <c r="H16" s="61" t="s">
+      <c r="J16" s="61" t="s">
         <v>83</v>
       </c>
-      <c r="I16" s="61" t="s">
+      <c r="K16" s="62" t="s">
         <v>84</v>
       </c>
-      <c r="J16" s="61" t="s">
+      <c r="L16" s="62" t="s">
         <v>84</v>
       </c>
-      <c r="K16" s="63" t="s">
+      <c r="M16" s="62" t="s">
         <v>85</v>
       </c>
-      <c r="L16" s="63" t="s">
+      <c r="N16" s="62" t="s">
         <v>85</v>
       </c>
-      <c r="M16" s="63" t="s">
-        <v>86</v>
-      </c>
-      <c r="N16" s="63" t="s">
-        <v>86</v>
-      </c>
-      <c r="O16" s="63" t="s">
-        <v>86</v>
+      <c r="O16" s="62" t="s">
+        <v>85</v>
       </c>
       <c r="P16" s="61" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="Q16" s="57" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="17" spans="1:17" ht="18.75" customHeight="1">
@@ -2281,51 +2284,51 @@
         <v>15</v>
       </c>
       <c r="B17" s="57" t="s">
+        <v>86</v>
+      </c>
+      <c r="C17" s="61" t="s">
         <v>87</v>
       </c>
-      <c r="C17" s="61" t="s">
+      <c r="D17" s="61" t="s">
+        <v>87</v>
+      </c>
+      <c r="E17" s="61" t="s">
+        <v>87</v>
+      </c>
+      <c r="F17" s="61" t="s">
+        <v>86</v>
+      </c>
+      <c r="G17" s="61" t="s">
+        <v>87</v>
+      </c>
+      <c r="H17" s="61" t="s">
+        <v>86</v>
+      </c>
+      <c r="I17" s="61" t="s">
         <v>88</v>
       </c>
-      <c r="D17" s="61" t="s">
-        <v>88</v>
-      </c>
-      <c r="E17" s="61" t="s">
-        <v>88</v>
-      </c>
-      <c r="F17" s="61" t="s">
-        <v>87</v>
-      </c>
-      <c r="G17" s="61" t="s">
-        <v>88</v>
-      </c>
-      <c r="H17" s="61" t="s">
-        <v>87</v>
-      </c>
-      <c r="I17" s="61" t="s">
+      <c r="J17" s="61" t="s">
         <v>89</v>
       </c>
-      <c r="J17" s="61" t="s">
+      <c r="K17" s="62" t="s">
         <v>90</v>
       </c>
-      <c r="K17" s="63" t="s">
+      <c r="L17" s="62" t="s">
         <v>91</v>
       </c>
-      <c r="L17" s="63" t="s">
+      <c r="M17" s="62" t="s">
         <v>92</v>
       </c>
-      <c r="M17" s="63" t="s">
+      <c r="N17" s="62" t="s">
         <v>93</v>
       </c>
-      <c r="N17" s="63" t="s">
+      <c r="O17" s="62" t="s">
         <v>94</v>
       </c>
-      <c r="O17" s="63" t="s">
-        <v>95</v>
-      </c>
-      <c r="P17" s="70">
+      <c r="P17" s="69">
         <v>100</v>
       </c>
-      <c r="Q17" s="71">
+      <c r="Q17" s="70">
         <v>100</v>
       </c>
     </row>
@@ -2333,25 +2336,25 @@
       <c r="A18" s="55" t="s">
         <v>16</v>
       </c>
-      <c r="B18" s="64">
+      <c r="B18" s="63">
         <v>26</v>
       </c>
-      <c r="C18" s="64">
+      <c r="C18" s="63">
         <v>26</v>
       </c>
-      <c r="D18" s="64">
+      <c r="D18" s="63">
         <v>26</v>
       </c>
-      <c r="E18" s="64">
+      <c r="E18" s="63">
         <v>26</v>
       </c>
-      <c r="F18" s="64">
+      <c r="F18" s="63">
         <v>26</v>
       </c>
-      <c r="G18" s="64">
+      <c r="G18" s="63">
         <v>26</v>
       </c>
-      <c r="H18" s="64">
+      <c r="H18" s="63">
         <v>26</v>
       </c>
       <c r="I18" s="61" t="s">
@@ -2360,24 +2363,24 @@
       <c r="J18" s="61" t="s">
         <v>58</v>
       </c>
-      <c r="K18" s="63"/>
-      <c r="L18" s="63" t="s">
+      <c r="K18" s="62"/>
+      <c r="L18" s="62" t="s">
         <v>58</v>
       </c>
-      <c r="M18" s="63" t="s">
+      <c r="M18" s="62" t="s">
         <v>58</v>
       </c>
-      <c r="N18" s="63" t="s">
+      <c r="N18" s="62" t="s">
         <v>58</v>
       </c>
-      <c r="O18" s="63" t="s">
+      <c r="O18" s="62" t="s">
         <v>58</v>
       </c>
-      <c r="P18" s="62" t="s">
+      <c r="P18" s="27" t="s">
+        <v>95</v>
+      </c>
+      <c r="Q18" s="57" t="s">
         <v>96</v>
-      </c>
-      <c r="Q18" s="57" t="s">
-        <v>97</v>
       </c>
     </row>
     <row r="19" spans="1:17" ht="18.75" customHeight="1">
@@ -2388,54 +2391,54 @@
         <v>41086</v>
       </c>
       <c r="C19" s="61" t="s">
+        <v>97</v>
+      </c>
+      <c r="D19" s="61" t="s">
         <v>98</v>
       </c>
-      <c r="D19" s="61" t="s">
+      <c r="E19" s="61" t="s">
         <v>99</v>
       </c>
-      <c r="E19" s="61" t="s">
+      <c r="F19" s="61" t="s">
         <v>100</v>
       </c>
-      <c r="F19" s="61" t="s">
+      <c r="G19" s="61" t="s">
         <v>101</v>
       </c>
-      <c r="G19" s="61" t="s">
+      <c r="H19" s="61" t="s">
         <v>102</v>
       </c>
-      <c r="H19" s="61" t="s">
+      <c r="I19" s="61" t="s">
         <v>103</v>
       </c>
-      <c r="I19" s="61" t="s">
+      <c r="J19" s="61" t="s">
         <v>104</v>
       </c>
-      <c r="J19" s="61" t="s">
+      <c r="K19" s="62" t="s">
         <v>105</v>
       </c>
-      <c r="K19" s="63" t="s">
+      <c r="L19" s="62" t="s">
         <v>106</v>
       </c>
-      <c r="L19" s="63" t="s">
+      <c r="M19" s="62" t="s">
         <v>107</v>
       </c>
-      <c r="M19" s="63" t="s">
+      <c r="N19" s="62" t="s">
         <v>108</v>
       </c>
-      <c r="N19" s="63" t="s">
+      <c r="O19" s="62" t="s">
         <v>109</v>
       </c>
-      <c r="O19" s="63" t="s">
+      <c r="P19" s="61" t="s">
         <v>110</v>
-      </c>
-      <c r="P19" s="61" t="s">
-        <v>111</v>
       </c>
       <c r="Q19" s="57">
         <v>38444</v>
       </c>
     </row>
     <row r="20" spans="1:17" ht="15.75" customHeight="1">
-      <c r="A20" s="68"/>
-      <c r="B20" s="72"/>
+      <c r="A20" s="67"/>
+      <c r="B20" s="71"/>
       <c r="C20" s="50"/>
       <c r="D20" s="50"/>
       <c r="E20" s="50"/>
@@ -2453,7 +2456,7 @@
       <c r="Q20" s="51"/>
     </row>
     <row r="21" spans="1:17" ht="15.75" customHeight="1">
-      <c r="A21" s="68"/>
+      <c r="A21" s="67"/>
       <c r="B21" s="51"/>
       <c r="C21" s="50"/>
       <c r="D21" s="50"/>
@@ -2472,7 +2475,7 @@
       <c r="Q21" s="51"/>
     </row>
     <row r="22" spans="1:17" ht="15.75" customHeight="1">
-      <c r="A22" s="68"/>
+      <c r="A22" s="67"/>
       <c r="B22" s="51"/>
       <c r="C22" s="50"/>
       <c r="D22" s="50"/>
@@ -2491,7 +2494,7 @@
       <c r="Q22" s="51"/>
     </row>
     <row r="23" spans="1:17" ht="15.75" customHeight="1">
-      <c r="A23" s="68"/>
+      <c r="A23" s="67"/>
       <c r="B23" s="51"/>
       <c r="C23" s="50"/>
       <c r="D23" s="50"/>
@@ -2510,7 +2513,7 @@
       <c r="Q23" s="51"/>
     </row>
     <row r="24" spans="1:17" ht="15.75" customHeight="1">
-      <c r="A24" s="68"/>
+      <c r="A24" s="67"/>
       <c r="B24" s="51"/>
       <c r="C24" s="50"/>
       <c r="D24" s="50"/>
@@ -2529,7 +2532,7 @@
       <c r="Q24" s="51"/>
     </row>
     <row r="25" spans="1:17" ht="15.75" customHeight="1">
-      <c r="A25" s="68"/>
+      <c r="A25" s="67"/>
       <c r="B25" s="51"/>
       <c r="C25" s="50"/>
       <c r="D25" s="50"/>
@@ -2548,7 +2551,7 @@
       <c r="Q25" s="51"/>
     </row>
     <row r="26" spans="1:17" ht="15.75" customHeight="1">
-      <c r="A26" s="68"/>
+      <c r="A26" s="67"/>
       <c r="B26" s="51"/>
       <c r="C26" s="50"/>
       <c r="D26" s="50"/>
@@ -2567,8 +2570,8 @@
       <c r="Q26" s="51"/>
     </row>
     <row r="27" spans="1:17" ht="15.75" customHeight="1">
-      <c r="A27" s="68"/>
-      <c r="B27" s="73"/>
+      <c r="A27" s="67"/>
+      <c r="B27" s="72"/>
       <c r="C27" s="50"/>
       <c r="D27" s="50"/>
       <c r="E27" s="50"/>
@@ -2604,13 +2607,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="46.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="46.85546875" style="17" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="30.140625" style="44" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="28.85546875" style="44" bestFit="1" customWidth="1"/>
-    <col min="4" max="7" width="24.28515625" style="17" bestFit="1" customWidth="1"/>
-    <col min="8" max="14" width="24.28515625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="24" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="14" width="24.28515625" style="17" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="24" style="17" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="13.5703125" style="17" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16" ht="15.75" customHeight="1">
@@ -2628,7 +2630,7 @@
       <c r="J1" s="20"/>
     </row>
     <row r="2" spans="1:16" ht="18.75" customHeight="1">
-      <c r="A2" s="22" t="s">
+      <c r="A2" s="21" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="36" t="s">
@@ -2652,7 +2654,7 @@
       <c r="P2" s="37"/>
     </row>
     <row r="3" spans="1:16" ht="18.75" customHeight="1">
-      <c r="A3" s="22" t="s">
+      <c r="A3" s="21" t="s">
         <v>8</v>
       </c>
       <c r="B3" s="34">
@@ -2676,7 +2678,7 @@
       <c r="P3" s="38"/>
     </row>
     <row r="4" spans="1:16" ht="18.75" customHeight="1">
-      <c r="A4" s="22" t="s">
+      <c r="A4" s="21" t="s">
         <v>32</v>
       </c>
       <c r="B4" s="34">
@@ -2700,13 +2702,13 @@
       <c r="P4" s="38"/>
     </row>
     <row r="5" spans="1:16" ht="18.75" customHeight="1">
-      <c r="A5" s="22" t="s">
+      <c r="A5" s="21" t="s">
         <v>10</v>
       </c>
-      <c r="B5" s="25">
+      <c r="B5" s="24">
         <v>42736</v>
       </c>
-      <c r="C5" s="25">
+      <c r="C5" s="24">
         <v>42736</v>
       </c>
       <c r="D5" s="38"/>
@@ -2724,13 +2726,13 @@
       <c r="P5" s="38"/>
     </row>
     <row r="6" spans="1:16" ht="18.75" customHeight="1">
-      <c r="A6" s="22" t="s">
+      <c r="A6" s="21" t="s">
         <v>11</v>
       </c>
-      <c r="B6" s="25">
+      <c r="B6" s="24">
         <v>43101</v>
       </c>
-      <c r="C6" s="25">
+      <c r="C6" s="24">
         <v>43101</v>
       </c>
       <c r="D6" s="38"/>
@@ -2748,7 +2750,7 @@
       <c r="P6" s="38"/>
     </row>
     <row r="7" spans="1:16" ht="18.75" customHeight="1">
-      <c r="A7" s="22" t="s">
+      <c r="A7" s="21" t="s">
         <v>12</v>
       </c>
       <c r="B7" s="39" t="s">
@@ -2772,7 +2774,7 @@
       <c r="P7" s="38"/>
     </row>
     <row r="8" spans="1:16" ht="18.75" customHeight="1">
-      <c r="A8" s="22" t="s">
+      <c r="A8" s="21" t="s">
         <v>13</v>
       </c>
       <c r="B8" s="41" t="s">
@@ -2796,13 +2798,13 @@
       <c r="P8" s="38"/>
     </row>
     <row r="9" spans="1:16" ht="18.75" customHeight="1">
-      <c r="A9" s="22" t="s">
+      <c r="A9" s="21" t="s">
         <v>15</v>
       </c>
-      <c r="B9" s="25" t="s">
+      <c r="B9" s="24" t="s">
         <v>60</v>
       </c>
-      <c r="C9" s="25" t="s">
+      <c r="C9" s="24" t="s">
         <v>60</v>
       </c>
       <c r="D9" s="38"/>
@@ -2820,11 +2822,11 @@
       <c r="P9" s="43"/>
     </row>
     <row r="10" spans="1:16" ht="18.75" customHeight="1">
-      <c r="A10" s="22" t="s">
+      <c r="A10" s="21" t="s">
         <v>16</v>
       </c>
-      <c r="B10" s="25"/>
-      <c r="C10" s="25"/>
+      <c r="B10" s="24"/>
+      <c r="C10" s="24"/>
       <c r="D10" s="38"/>
       <c r="E10" s="38"/>
       <c r="F10" s="38"/>
@@ -2840,7 +2842,7 @@
       <c r="P10" s="38"/>
     </row>
     <row r="11" spans="1:16" ht="18.75" customHeight="1">
-      <c r="A11" s="22" t="s">
+      <c r="A11" s="21" t="s">
         <v>17</v>
       </c>
       <c r="B11" s="39" t="s">
@@ -2864,11 +2866,11 @@
       <c r="P11" s="38"/>
     </row>
     <row r="12" spans="1:16" ht="18.75" customHeight="1">
-      <c r="A12" s="22" t="s">
+      <c r="A12" s="21" t="s">
         <v>19</v>
       </c>
-      <c r="B12" s="25"/>
-      <c r="C12" s="25"/>
+      <c r="B12" s="24"/>
+      <c r="C12" s="24"/>
       <c r="D12" s="38"/>
       <c r="E12" s="38"/>
       <c r="F12" s="38"/>
@@ -2884,7 +2886,7 @@
       <c r="P12" s="38"/>
     </row>
     <row r="13" spans="1:16" ht="18.75" customHeight="1">
-      <c r="A13" s="22" t="s">
+      <c r="A13" s="21" t="s">
         <v>20</v>
       </c>
       <c r="B13" s="41" t="s">
@@ -2926,7 +2928,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="46.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="46.85546875" style="17" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="24.28515625" style="18" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="24.42578125" style="18" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="25.140625" style="19" bestFit="1" customWidth="1"/>
@@ -2940,7 +2942,7 @@
       </c>
     </row>
     <row r="2" spans="1:5" ht="18.75" customHeight="1">
-      <c r="A2" s="22" t="s">
+      <c r="A2" s="21" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="32" t="s">
@@ -2957,7 +2959,7 @@
       </c>
     </row>
     <row r="3" spans="1:5" ht="18.75" customHeight="1">
-      <c r="A3" s="22" t="s">
+      <c r="A3" s="21" t="s">
         <v>8</v>
       </c>
       <c r="B3" s="34">
@@ -2974,7 +2976,7 @@
       </c>
     </row>
     <row r="4" spans="1:5" ht="18.75" customHeight="1">
-      <c r="A4" s="22" t="s">
+      <c r="A4" s="21" t="s">
         <v>32</v>
       </c>
       <c r="B4" s="34">
@@ -2991,24 +2993,24 @@
       </c>
     </row>
     <row r="5" spans="1:5" ht="18.75" customHeight="1">
-      <c r="A5" s="22" t="s">
+      <c r="A5" s="21" t="s">
         <v>10</v>
       </c>
-      <c r="B5" s="25">
+      <c r="B5" s="24">
         <v>36526</v>
       </c>
-      <c r="C5" s="25">
+      <c r="C5" s="24">
         <v>36526</v>
       </c>
-      <c r="D5" s="25">
+      <c r="D5" s="24">
         <v>37987</v>
       </c>
-      <c r="E5" s="25">
+      <c r="E5" s="24">
         <v>37987</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="18.75" customHeight="1">
-      <c r="A6" s="22" t="s">
+      <c r="A6" s="21" t="s">
         <v>11</v>
       </c>
       <c r="B6" s="34" t="s">
@@ -3017,7 +3019,7 @@
       <c r="C6" s="34" t="s">
         <v>50</v>
       </c>
-      <c r="D6" s="23" t="s">
+      <c r="D6" s="22" t="s">
         <v>51</v>
       </c>
       <c r="E6" s="34" t="s">
@@ -3025,7 +3027,7 @@
       </c>
     </row>
     <row r="7" spans="1:5" ht="18.75" customHeight="1">
-      <c r="A7" s="22" t="s">
+      <c r="A7" s="21" t="s">
         <v>12</v>
       </c>
       <c r="B7" s="34" t="s">
@@ -3034,7 +3036,7 @@
       <c r="C7" s="34" t="s">
         <v>52</v>
       </c>
-      <c r="D7" s="23" t="s">
+      <c r="D7" s="22" t="s">
         <v>53</v>
       </c>
       <c r="E7" s="34" t="s">
@@ -3042,7 +3044,7 @@
       </c>
     </row>
     <row r="8" spans="1:5" ht="18.75" customHeight="1">
-      <c r="A8" s="22" t="s">
+      <c r="A8" s="21" t="s">
         <v>13</v>
       </c>
       <c r="B8" s="34" t="s">
@@ -3051,7 +3053,7 @@
       <c r="C8" s="34" t="s">
         <v>54</v>
       </c>
-      <c r="D8" s="23" t="s">
+      <c r="D8" s="22" t="s">
         <v>54</v>
       </c>
       <c r="E8" s="34" t="s">
@@ -3059,41 +3061,41 @@
       </c>
     </row>
     <row r="9" spans="1:5" ht="18.75" customHeight="1">
-      <c r="A9" s="22" t="s">
+      <c r="A9" s="21" t="s">
         <v>15</v>
       </c>
-      <c r="B9" s="23">
+      <c r="B9" s="22">
         <v>50</v>
       </c>
-      <c r="C9" s="23">
+      <c r="C9" s="22">
         <v>50</v>
       </c>
-      <c r="D9" s="23">
+      <c r="D9" s="22">
         <v>50</v>
       </c>
-      <c r="E9" s="23">
+      <c r="E9" s="22">
         <v>50</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="18.75" customHeight="1">
-      <c r="A10" s="22" t="s">
+      <c r="A10" s="21" t="s">
         <v>16</v>
       </c>
-      <c r="B10" s="23">
+      <c r="B10" s="22">
         <v>44</v>
       </c>
-      <c r="C10" s="23">
+      <c r="C10" s="22">
         <v>44</v>
       </c>
-      <c r="D10" s="23">
+      <c r="D10" s="22">
         <v>44</v>
       </c>
-      <c r="E10" s="23">
+      <c r="E10" s="22">
         <v>44</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="18.75" customHeight="1">
-      <c r="A11" s="22" t="s">
+      <c r="A11" s="21" t="s">
         <v>17</v>
       </c>
       <c r="B11" s="34" t="s">
@@ -3102,7 +3104,7 @@
       <c r="C11" s="34" t="s">
         <v>35</v>
       </c>
-      <c r="D11" s="23" t="s">
+      <c r="D11" s="22" t="s">
         <v>35</v>
       </c>
       <c r="E11" s="34" t="s">
@@ -3110,7 +3112,7 @@
       </c>
     </row>
     <row r="12" spans="1:5" ht="18.75" customHeight="1">
-      <c r="A12" s="22" t="s">
+      <c r="A12" s="21" t="s">
         <v>19</v>
       </c>
       <c r="B12" s="34">
@@ -3119,7 +3121,7 @@
       <c r="C12" s="34">
         <v>14.7</v>
       </c>
-      <c r="D12" s="23">
+      <c r="D12" s="22">
         <v>6</v>
       </c>
       <c r="E12" s="34">
@@ -3127,7 +3129,7 @@
       </c>
     </row>
     <row r="13" spans="1:5" ht="18.75" customHeight="1">
-      <c r="A13" s="22" t="s">
+      <c r="A13" s="21" t="s">
         <v>20</v>
       </c>
       <c r="B13" s="34" t="s">
@@ -3136,7 +3138,7 @@
       <c r="C13" s="34" t="s">
         <v>55</v>
       </c>
-      <c r="D13" s="23" t="s">
+      <c r="D13" s="22" t="s">
         <v>55</v>
       </c>
       <c r="E13" s="34" t="s">
@@ -3159,299 +3161,299 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="49.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.140625" style="21" bestFit="1" customWidth="1"/>
-    <col min="3" max="10" width="13.5703125" style="21" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="49.5703125" style="17" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.140625" style="19" bestFit="1" customWidth="1"/>
+    <col min="3" max="10" width="13.5703125" style="19" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="15.75" customHeight="1">
-      <c r="A1" s="81" t="s">
+      <c r="A1" s="79" t="s">
         <v>24</v>
       </c>
-      <c r="B1" s="82"/>
-      <c r="C1" s="82"/>
-      <c r="D1" s="82"/>
-      <c r="E1" s="82"/>
-      <c r="F1" s="82"/>
-      <c r="G1" s="82"/>
-      <c r="H1" s="82"/>
-      <c r="I1" s="82"/>
-      <c r="J1" s="82"/>
+      <c r="B1" s="80"/>
+      <c r="C1" s="80"/>
+      <c r="D1" s="80"/>
+      <c r="E1" s="80"/>
+      <c r="F1" s="80"/>
+      <c r="G1" s="80"/>
+      <c r="H1" s="80"/>
+      <c r="I1" s="80"/>
+      <c r="J1" s="80"/>
     </row>
     <row r="2" spans="1:10" ht="18.75" customHeight="1">
-      <c r="A2" s="22" t="s">
+      <c r="A2" s="21" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="23" t="s">
+      <c r="B2" s="22" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="23" t="s">
+      <c r="C2" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="23" t="s">
+      <c r="D2" s="22" t="s">
         <v>25</v>
       </c>
-      <c r="E2" s="23" t="s">
+      <c r="E2" s="22" t="s">
         <v>26</v>
       </c>
-      <c r="F2" s="23" t="s">
+      <c r="F2" s="22" t="s">
         <v>27</v>
       </c>
-      <c r="G2" s="23" t="s">
+      <c r="G2" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="H2" s="23" t="s">
+      <c r="H2" s="22" t="s">
         <v>29</v>
       </c>
-      <c r="I2" s="23" t="s">
+      <c r="I2" s="22" t="s">
         <v>30</v>
       </c>
-      <c r="J2" s="23" t="s">
+      <c r="J2" s="22" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="3" spans="1:10" ht="18.75" customHeight="1">
-      <c r="A3" s="22" t="s">
+      <c r="A3" s="21" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="24">
+      <c r="B3" s="23">
         <v>-7.6097200000000003</v>
       </c>
-      <c r="C3" s="24">
+      <c r="C3" s="23">
         <v>-7.5916699999999997</v>
       </c>
-      <c r="D3" s="24">
+      <c r="D3" s="23">
         <v>-7.5944399999999996</v>
       </c>
-      <c r="E3" s="24">
+      <c r="E3" s="23">
         <v>-7.5916699999999997</v>
       </c>
-      <c r="F3" s="24">
+      <c r="F3" s="23">
         <v>-7.5888900000000001</v>
       </c>
-      <c r="G3" s="24">
+      <c r="G3" s="23">
         <v>-7.5986099999999999</v>
       </c>
-      <c r="H3" s="24">
+      <c r="H3" s="23">
         <v>-7.5958300000000003</v>
       </c>
-      <c r="I3" s="24">
+      <c r="I3" s="23">
         <v>-7.5916699999999997</v>
       </c>
-      <c r="J3" s="24">
+      <c r="J3" s="23">
         <v>-7.61111</v>
       </c>
     </row>
     <row r="4" spans="1:10" ht="18.75" customHeight="1">
-      <c r="A4" s="22" t="s">
+      <c r="A4" s="21" t="s">
         <v>32</v>
       </c>
-      <c r="B4" s="24">
+      <c r="B4" s="23">
         <v>31.661110000000001</v>
       </c>
-      <c r="C4" s="24">
+      <c r="C4" s="23">
         <v>31.66667</v>
       </c>
-      <c r="D4" s="24">
+      <c r="D4" s="23">
         <v>31.668060000000001</v>
       </c>
-      <c r="E4" s="24">
+      <c r="E4" s="23">
         <v>31.677779999999998</v>
       </c>
-      <c r="F4" s="24">
+      <c r="F4" s="23">
         <v>31.68056</v>
       </c>
-      <c r="G4" s="24">
+      <c r="G4" s="23">
         <v>31.68056</v>
       </c>
-      <c r="H4" s="24">
+      <c r="H4" s="23">
         <v>31.68056</v>
       </c>
-      <c r="I4" s="24">
+      <c r="I4" s="23">
         <v>31.68056</v>
       </c>
-      <c r="J4" s="24">
+      <c r="J4" s="23">
         <v>31.66667</v>
       </c>
     </row>
     <row r="5" spans="1:10" ht="18.75" customHeight="1">
-      <c r="A5" s="22" t="s">
+      <c r="A5" s="21" t="s">
         <v>10</v>
       </c>
-      <c r="B5" s="25">
+      <c r="B5" s="24">
         <v>38353</v>
       </c>
-      <c r="C5" s="25">
+      <c r="C5" s="24">
         <v>38353</v>
       </c>
-      <c r="D5" s="25">
+      <c r="D5" s="24">
         <v>38353</v>
       </c>
-      <c r="E5" s="25">
+      <c r="E5" s="24">
         <v>38353</v>
       </c>
-      <c r="F5" s="25">
+      <c r="F5" s="24">
         <v>38353</v>
       </c>
-      <c r="G5" s="25">
+      <c r="G5" s="24">
         <v>38353</v>
       </c>
-      <c r="H5" s="25">
+      <c r="H5" s="24">
         <v>38353</v>
       </c>
-      <c r="I5" s="25">
+      <c r="I5" s="24">
         <v>38353</v>
       </c>
-      <c r="J5" s="25">
+      <c r="J5" s="24">
         <v>38353</v>
       </c>
     </row>
     <row r="6" spans="1:10" ht="18.75" customHeight="1">
-      <c r="A6" s="22" t="s">
+      <c r="A6" s="21" t="s">
         <v>11</v>
       </c>
-      <c r="B6" s="25">
+      <c r="B6" s="24">
         <v>39082</v>
       </c>
-      <c r="C6" s="25">
+      <c r="C6" s="24">
         <v>39082</v>
       </c>
-      <c r="D6" s="25">
+      <c r="D6" s="24">
         <v>39082</v>
       </c>
-      <c r="E6" s="25">
+      <c r="E6" s="24">
         <v>39082</v>
       </c>
-      <c r="F6" s="25">
+      <c r="F6" s="24">
         <v>39082</v>
       </c>
-      <c r="G6" s="25">
+      <c r="G6" s="24">
         <v>39082</v>
       </c>
-      <c r="H6" s="25">
+      <c r="H6" s="24">
         <v>39082</v>
       </c>
-      <c r="I6" s="25">
+      <c r="I6" s="24">
         <v>39082</v>
       </c>
-      <c r="J6" s="25">
+      <c r="J6" s="24">
         <v>39082</v>
       </c>
     </row>
     <row r="7" spans="1:10" ht="18.75" customHeight="1">
-      <c r="A7" s="22" t="s">
+      <c r="A7" s="21" t="s">
         <v>12</v>
       </c>
-      <c r="B7" s="25">
+      <c r="B7" s="24">
         <v>38703</v>
       </c>
-      <c r="C7" s="26">
+      <c r="C7" s="25">
         <v>37632</v>
       </c>
-      <c r="D7" s="26">
+      <c r="D7" s="25">
         <v>37635</v>
       </c>
-      <c r="E7" s="26">
+      <c r="E7" s="25">
         <v>37946</v>
       </c>
-      <c r="F7" s="26">
+      <c r="F7" s="25">
         <v>37946</v>
       </c>
-      <c r="G7" s="26">
+      <c r="G7" s="25">
         <v>37970</v>
       </c>
-      <c r="H7" s="26">
+      <c r="H7" s="25">
         <v>37974</v>
       </c>
-      <c r="I7" s="26">
+      <c r="I7" s="25">
         <v>37975</v>
       </c>
-      <c r="J7" s="26">
+      <c r="J7" s="25">
         <v>37979</v>
       </c>
     </row>
     <row r="8" spans="1:10" ht="18.75" customHeight="1">
-      <c r="A8" s="22" t="s">
+      <c r="A8" s="21" t="s">
         <v>13</v>
       </c>
-      <c r="B8" s="23" t="s">
+      <c r="B8" s="22" t="s">
         <v>33</v>
       </c>
-      <c r="C8" s="23" t="s">
+      <c r="C8" s="22" t="s">
         <v>33</v>
       </c>
-      <c r="D8" s="23" t="s">
+      <c r="D8" s="22" t="s">
         <v>33</v>
       </c>
-      <c r="E8" s="23" t="s">
+      <c r="E8" s="22" t="s">
         <v>33</v>
       </c>
-      <c r="F8" s="23" t="s">
+      <c r="F8" s="22" t="s">
         <v>33</v>
       </c>
-      <c r="G8" s="23" t="s">
+      <c r="G8" s="22" t="s">
         <v>33</v>
       </c>
-      <c r="H8" s="23" t="s">
+      <c r="H8" s="22" t="s">
         <v>33</v>
       </c>
-      <c r="I8" s="23" t="s">
+      <c r="I8" s="22" t="s">
         <v>33</v>
       </c>
-      <c r="J8" s="23" t="s">
+      <c r="J8" s="22" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="9" spans="1:10" ht="18.75" customHeight="1">
-      <c r="A9" s="22" t="s">
+      <c r="A9" s="21" t="s">
         <v>15</v>
       </c>
-      <c r="B9" s="27">
+      <c r="B9" s="26">
         <v>3</v>
       </c>
-      <c r="C9" s="27">
+      <c r="C9" s="26">
         <v>3</v>
       </c>
-      <c r="D9" s="27">
+      <c r="D9" s="26">
         <v>3</v>
       </c>
-      <c r="E9" s="27">
+      <c r="E9" s="26">
         <v>3</v>
       </c>
-      <c r="F9" s="27">
+      <c r="F9" s="26">
         <v>3</v>
       </c>
-      <c r="G9" s="27">
+      <c r="G9" s="26">
         <v>3</v>
       </c>
-      <c r="H9" s="27">
+      <c r="H9" s="26">
         <v>3</v>
       </c>
-      <c r="I9" s="27">
+      <c r="I9" s="26">
         <v>3</v>
       </c>
-      <c r="J9" s="27">
+      <c r="J9" s="26">
         <v>3</v>
       </c>
     </row>
     <row r="10" spans="1:10" ht="18.75" customHeight="1">
-      <c r="A10" s="22" t="s">
+      <c r="A10" s="21" t="s">
         <v>16</v>
       </c>
-      <c r="B10" s="83" t="s">
+      <c r="B10" s="81" t="s">
         <v>34</v>
       </c>
-      <c r="C10" s="84"/>
-      <c r="D10" s="84"/>
-      <c r="E10" s="84"/>
-      <c r="F10" s="84"/>
-      <c r="G10" s="84"/>
-      <c r="H10" s="84"/>
-      <c r="I10" s="84"/>
-      <c r="J10" s="85"/>
+      <c r="C10" s="82"/>
+      <c r="D10" s="82"/>
+      <c r="E10" s="82"/>
+      <c r="F10" s="82"/>
+      <c r="G10" s="82"/>
+      <c r="H10" s="82"/>
+      <c r="I10" s="82"/>
+      <c r="J10" s="83"/>
     </row>
     <row r="11" spans="1:10" ht="18.75" customHeight="1">
-      <c r="A11" s="22" t="s">
+      <c r="A11" s="21" t="s">
         <v>17</v>
       </c>
       <c r="B11" s="28" t="s">
@@ -3478,18 +3480,18 @@
       <c r="I11" s="29" t="s">
         <v>35</v>
       </c>
-      <c r="J11" s="23" t="s">
+      <c r="J11" s="22" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="12" spans="1:10" ht="18.75" customHeight="1">
-      <c r="A12" s="22" t="s">
+      <c r="A12" s="21" t="s">
         <v>19</v>
       </c>
       <c r="B12" s="30">
         <v>2.75</v>
       </c>
-      <c r="C12" s="27">
+      <c r="C12" s="26">
         <v>2</v>
       </c>
       <c r="D12" s="30">
@@ -3515,45 +3517,45 @@
       </c>
     </row>
     <row r="13" spans="1:10" ht="18.75" customHeight="1">
-      <c r="A13" s="22" t="s">
+      <c r="A13" s="21" t="s">
         <v>20</v>
       </c>
-      <c r="B13" s="27">
+      <c r="B13" s="26">
         <v>90</v>
       </c>
-      <c r="C13" s="27">
+      <c r="C13" s="26">
         <v>180</v>
       </c>
-      <c r="D13" s="27">
+      <c r="D13" s="26">
         <v>120</v>
       </c>
-      <c r="E13" s="27">
+      <c r="E13" s="26">
         <v>180</v>
       </c>
-      <c r="F13" s="27">
+      <c r="F13" s="26">
         <v>180</v>
       </c>
-      <c r="G13" s="27">
+      <c r="G13" s="26">
         <v>180</v>
       </c>
-      <c r="H13" s="27">
+      <c r="H13" s="26">
         <v>180</v>
       </c>
-      <c r="I13" s="27">
+      <c r="I13" s="26">
         <v>180</v>
       </c>
-      <c r="J13" s="27">
+      <c r="J13" s="26">
         <v>180</v>
       </c>
     </row>
     <row r="14" spans="1:10" ht="18.75" customHeight="1">
-      <c r="A14" s="22" t="s">
+      <c r="A14" s="21" t="s">
         <v>36</v>
       </c>
       <c r="B14" s="30">
         <v>337.3</v>
       </c>
-      <c r="C14" s="27">
+      <c r="C14" s="26">
         <v>225</v>
       </c>
       <c r="D14" s="30">
@@ -3562,165 +3564,165 @@
       <c r="E14" s="30">
         <v>337.3</v>
       </c>
-      <c r="F14" s="27">
+      <c r="F14" s="26">
         <v>225</v>
       </c>
       <c r="G14" s="30">
         <v>337.3</v>
       </c>
-      <c r="H14" s="27">
+      <c r="H14" s="26">
         <v>225</v>
       </c>
-      <c r="I14" s="27">
+      <c r="I14" s="26">
         <v>225</v>
       </c>
-      <c r="J14" s="27">
+      <c r="J14" s="26">
         <v>315</v>
       </c>
     </row>
     <row r="15" spans="1:10" ht="18.75" customHeight="1">
-      <c r="A15" s="22" t="s">
+      <c r="A15" s="21" t="s">
         <v>37</v>
       </c>
-      <c r="B15" s="27">
+      <c r="B15" s="26">
         <v>150</v>
       </c>
-      <c r="C15" s="27">
+      <c r="C15" s="26">
         <v>100</v>
       </c>
-      <c r="D15" s="27">
+      <c r="D15" s="26">
         <v>150</v>
       </c>
-      <c r="E15" s="27">
+      <c r="E15" s="26">
         <v>150</v>
       </c>
-      <c r="F15" s="27">
+      <c r="F15" s="26">
         <v>100</v>
       </c>
-      <c r="G15" s="27">
+      <c r="G15" s="26">
         <v>150</v>
       </c>
-      <c r="H15" s="27">
+      <c r="H15" s="26">
         <v>100</v>
       </c>
-      <c r="I15" s="27">
+      <c r="I15" s="26">
         <v>100</v>
       </c>
-      <c r="J15" s="27">
+      <c r="J15" s="26">
         <v>140</v>
       </c>
     </row>
     <row r="16" spans="1:10" ht="18.75" customHeight="1">
-      <c r="A16" s="22" t="s">
+      <c r="A16" s="21" t="s">
         <v>38</v>
       </c>
-      <c r="B16" s="27">
+      <c r="B16" s="26">
         <v>20</v>
       </c>
-      <c r="C16" s="27">
+      <c r="C16" s="26">
         <v>65</v>
       </c>
-      <c r="D16" s="27">
+      <c r="D16" s="26">
         <v>20</v>
       </c>
-      <c r="E16" s="27">
+      <c r="E16" s="26">
         <v>45</v>
       </c>
-      <c r="F16" s="27">
+      <c r="F16" s="26">
         <v>20</v>
       </c>
-      <c r="G16" s="27">
+      <c r="G16" s="26">
         <v>20</v>
       </c>
-      <c r="H16" s="27">
+      <c r="H16" s="26">
         <v>65</v>
       </c>
-      <c r="I16" s="27">
+      <c r="I16" s="26">
         <v>20</v>
       </c>
-      <c r="J16" s="27">
+      <c r="J16" s="26">
         <v>45</v>
       </c>
     </row>
     <row r="17" spans="1:10" ht="18.75" customHeight="1"/>
     <row r="18" spans="1:10" ht="18.75" customHeight="1"/>
     <row r="19" spans="1:10" ht="18.75" customHeight="1">
-      <c r="A19" s="22" t="s">
+      <c r="A19" s="21" t="s">
         <v>15</v>
       </c>
-      <c r="B19" s="27">
+      <c r="B19" s="26">
         <v>3</v>
       </c>
-      <c r="C19" s="27">
+      <c r="C19" s="26">
         <v>3</v>
       </c>
-      <c r="D19" s="27">
+      <c r="D19" s="26">
         <v>3</v>
       </c>
-      <c r="E19" s="27">
+      <c r="E19" s="26">
         <v>3</v>
       </c>
-      <c r="F19" s="27">
+      <c r="F19" s="26">
         <v>3</v>
       </c>
-      <c r="G19" s="27">
+      <c r="G19" s="26">
         <v>3</v>
       </c>
-      <c r="H19" s="27">
+      <c r="H19" s="26">
         <v>3</v>
       </c>
-      <c r="I19" s="27">
+      <c r="I19" s="26">
         <v>3</v>
       </c>
-      <c r="J19" s="27">
+      <c r="J19" s="26">
         <v>3</v>
       </c>
     </row>
     <row r="20" spans="1:10" ht="18.75" customHeight="1">
-      <c r="A20" s="22" t="s">
+      <c r="A20" s="21" t="s">
         <v>16</v>
       </c>
-      <c r="B20" s="83" t="s">
+      <c r="B20" s="81" t="s">
         <v>34</v>
       </c>
-      <c r="C20" s="84"/>
-      <c r="D20" s="84"/>
-      <c r="E20" s="84"/>
-      <c r="F20" s="84"/>
-      <c r="G20" s="84"/>
-      <c r="H20" s="84"/>
-      <c r="I20" s="84"/>
-      <c r="J20" s="85"/>
+      <c r="C20" s="82"/>
+      <c r="D20" s="82"/>
+      <c r="E20" s="82"/>
+      <c r="F20" s="82"/>
+      <c r="G20" s="82"/>
+      <c r="H20" s="82"/>
+      <c r="I20" s="82"/>
+      <c r="J20" s="83"/>
     </row>
     <row r="21" spans="1:10" ht="18.75" customHeight="1">
-      <c r="A21" s="22" t="s">
+      <c r="A21" s="21" t="s">
         <v>19</v>
       </c>
-      <c r="B21" s="23" t="s">
+      <c r="B21" s="22" t="s">
         <v>39</v>
       </c>
-      <c r="C21" s="23" t="s">
+      <c r="C21" s="22" t="s">
         <v>40</v>
       </c>
-      <c r="D21" s="23" t="s">
+      <c r="D21" s="22" t="s">
         <v>41</v>
       </c>
-      <c r="E21" s="23" t="s">
+      <c r="E21" s="22" t="s">
         <v>39</v>
       </c>
-      <c r="F21" s="23" t="s">
+      <c r="F21" s="22" t="s">
         <v>42</v>
       </c>
-      <c r="G21" s="23" t="s">
+      <c r="G21" s="22" t="s">
         <v>42</v>
       </c>
-      <c r="H21" s="23" t="s">
+      <c r="H21" s="22" t="s">
         <v>43</v>
       </c>
-      <c r="I21" s="23" t="s">
+      <c r="I21" s="22" t="s">
         <v>44</v>
       </c>
-      <c r="J21" s="23" t="s">
+      <c r="J21" s="22" t="s">
         <v>42</v>
       </c>
     </row>
@@ -3742,7 +3744,7 @@
   <dimension ref="A1:G17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3852,10 +3854,10 @@
         <v>41744</v>
       </c>
       <c r="F5" s="9">
-        <v>42475</v>
+        <v>42109</v>
       </c>
       <c r="G5" s="9">
-        <v>42475</v>
+        <v>42109</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="18.75" customHeight="1">

</xml_diff>

<commit_message>
morocco wheat case study finalised. Added a flexible schedule. With some additional changes can be made to repeat yearly irrigation patterns. Increased simulation time for morroco to 10 with scheduled irrigation. also increased max irrigation to be compatible.
</commit_message>
<xml_diff>
--- a/heliostrome/jip_project/results/Factors to run simulation.xlsx
+++ b/heliostrome/jip_project/results/Factors to run simulation.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://tud365-my.sharepoint.com/personal/sparijs_tudelft_nl/Documents/Documents/helios/heliostrome/heliostrome/jip_project/results/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="29" documentId="11_13D963FD761544394477BF658C9F69163B1800BB" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FB729B84-B7CE-4AE6-BDBF-422035B4492D}"/>
+  <xr:revisionPtr revIDLastSave="60" documentId="11_13D963FD761544394477BF658C9F69163B1800BB" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EB68F0E4-4C1F-4A3C-9D31-62F7D3D27170}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="All Case Studies (compatability" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="343" uniqueCount="136">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="344" uniqueCount="136">
   <si>
     <t>Evaluation of AquaCrop for potato yield and biomass
 simulation under different water amounts in drip and
@@ -3279,10 +3279,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:J21"/>
+  <dimension ref="A1:J22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M7" sqref="M7"/>
+      <selection activeCell="O5" sqref="O5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3290,6 +3290,7 @@
     <col min="1" max="1" width="49.5703125" style="19" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12.140625" style="21" bestFit="1" customWidth="1"/>
     <col min="3" max="10" width="13.5703125" style="21" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="9.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="15.75" customHeight="1">
@@ -3439,31 +3440,31 @@
         <v>8</v>
       </c>
       <c r="B6" s="33">
-        <v>41639</v>
+        <v>42369</v>
       </c>
       <c r="C6" s="33">
-        <v>41639</v>
+        <v>42004</v>
       </c>
       <c r="D6" s="33">
-        <v>41639</v>
+        <v>42004</v>
       </c>
       <c r="E6" s="33">
-        <v>41639</v>
+        <v>42369</v>
       </c>
       <c r="F6" s="33">
-        <v>41639</v>
+        <v>42369</v>
       </c>
       <c r="G6" s="33">
-        <v>41639</v>
+        <v>42369</v>
       </c>
       <c r="H6" s="33">
-        <v>41639</v>
+        <v>42369</v>
       </c>
       <c r="I6" s="33">
-        <v>41639</v>
+        <v>42369</v>
       </c>
       <c r="J6" s="33">
-        <v>41639</v>
+        <v>42369</v>
       </c>
     </row>
     <row r="7" spans="1:10" ht="18.75" customHeight="1">
@@ -3850,6 +3851,38 @@
       </c>
       <c r="J21" s="31" t="s">
         <v>51</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" ht="18.75" customHeight="1">
+      <c r="A22" s="30" t="s">
+        <v>8</v>
+      </c>
+      <c r="B22" s="33">
+        <v>39082</v>
+      </c>
+      <c r="C22" s="33">
+        <v>38717</v>
+      </c>
+      <c r="D22" s="33">
+        <v>38717</v>
+      </c>
+      <c r="E22" s="33">
+        <v>39082</v>
+      </c>
+      <c r="F22" s="33">
+        <v>39082</v>
+      </c>
+      <c r="G22" s="33">
+        <v>39082</v>
+      </c>
+      <c r="H22" s="33">
+        <v>39082</v>
+      </c>
+      <c r="I22" s="33">
+        <v>39082</v>
+      </c>
+      <c r="J22" s="33">
+        <v>39082</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
A lot of updates. Added a module file and updated most scripts to be compatible with this. in addition the files related to irrigation amounts have been added to plot the irrigation intended to be matched with precipitation
</commit_message>
<xml_diff>
--- a/heliostrome/jip_project/results/Factors to run simulation.xlsx
+++ b/heliostrome/jip_project/results/Factors to run simulation.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://tud365-my.sharepoint.com/personal/sparijs_tudelft_nl/Documents/Documents/helios/heliostrome/heliostrome/jip_project/results/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="60" documentId="11_13D963FD761544394477BF658C9F69163B1800BB" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EB68F0E4-4C1F-4A3C-9D31-62F7D3D27170}"/>
+  <xr:revisionPtr revIDLastSave="88" documentId="11_13D963FD761544394477BF658C9F69163B1800BB" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DACCF725-E0F6-466F-9EF8-D57F62CA7DF0}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="All Case Studies (compatability" sheetId="1" r:id="rId1"/>
@@ -25,8 +25,37 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>tc={8A151525-7823-466D-A49A-B79F2B393CE3}</author>
+    <author>tc={10D2DA7D-571D-4FD1-A323-CFC7306F712D}</author>
+  </authors>
+  <commentList>
+    <comment ref="O9" authorId="0" shapeId="0" xr:uid="{8A151525-7823-466D-A49A-B79F2B393CE3}">
+      <text>
+        <t xml:space="preserve">[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Intervall maybe
+</t>
+      </text>
+    </comment>
+    <comment ref="O20" authorId="1" shapeId="0" xr:uid="{10D2DA7D-571D-4FD1-A323-CFC7306F712D}">
+      <text>
+        <t xml:space="preserve">[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Intervall maybe
+</t>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="344" uniqueCount="136">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="358" uniqueCount="137">
   <si>
     <t>Evaluation of AquaCrop for potato yield and biomass
 simulation under different water amounts in drip and
@@ -437,6 +466,9 @@
   </si>
   <si>
     <t>Irrigation Schedule</t>
+  </si>
+  <si>
+    <t>FC</t>
   </si>
 </sst>
 </file>
@@ -446,7 +478,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="mm/dd/yyyy"/>
   </numFmts>
-  <fonts count="10">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -490,12 +522,6 @@
       <sz val="10"/>
       <color rgb="FF333333"/>
       <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="&quot;Courier New&quot;"/>
       <family val="2"/>
     </font>
     <font>
@@ -834,7 +860,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="96">
+  <cellXfs count="95">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1076,9 +1102,6 @@
     <xf numFmtId="14" fontId="7" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="14" fontId="8" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1094,7 +1117,7 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1139,7 +1162,9 @@
 </file>
 
 <file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <person displayName="Sam Parijs" id="{4DDC1C4E-60F1-4420-AFA6-E392046EA936}" userId="S::sparijs@tudelft.nl::b925c39e-1c05-4535-b24c-f5b416736376" providerId="AD"/>
+</personList>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1425,6 +1450,19 @@
 </a:theme>
 </file>
 
+<file path=xl/threadedComments/threadedComment1.xml><?xml version="1.0" encoding="utf-8"?>
+<ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <threadedComment ref="O9" dT="2023-10-16T09:00:44.26" personId="{4DDC1C4E-60F1-4420-AFA6-E392046EA936}" id="{8A151525-7823-466D-A49A-B79F2B393CE3}">
+    <text xml:space="preserve">Intervall maybe
+</text>
+  </threadedComment>
+  <threadedComment ref="O20" dT="2023-10-16T09:00:44.26" personId="{4DDC1C4E-60F1-4420-AFA6-E392046EA936}" id="{10D2DA7D-571D-4FD1-A323-CFC7306F712D}">
+    <text xml:space="preserve">Intervall maybe
+</text>
+  </threadedComment>
+</ThreadedComments>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
@@ -1437,7 +1475,7 @@
       <selection pane="topRight"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14.7109375" style="19" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="19.42578125" bestFit="1" customWidth="1"/>
@@ -1446,14 +1484,14 @@
     <col min="5" max="7" width="13.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="18.75" customHeight="1">
+    <row r="1" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B1" s="47" t="s">
         <v>118</v>
       </c>
       <c r="C1" s="47" t="s">
         <v>119</v>
       </c>
-      <c r="D1" s="83" t="s">
+      <c r="D1" s="82" t="s">
         <v>54</v>
       </c>
       <c r="E1" s="47" t="s">
@@ -1462,133 +1500,133 @@
       <c r="F1" s="47" t="s">
         <v>121</v>
       </c>
-      <c r="G1" s="83" t="s">
+      <c r="G1" s="82" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="18.75" customHeight="1">
+    <row r="2" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="47" t="s">
         <v>123</v>
       </c>
-      <c r="B2" s="84"/>
-      <c r="C2" s="84"/>
-      <c r="D2" s="84"/>
-      <c r="E2" s="84"/>
-      <c r="F2" s="85"/>
-      <c r="G2" s="86"/>
-    </row>
-    <row r="3" spans="1:7" ht="18.75" customHeight="1">
+      <c r="B2" s="83"/>
+      <c r="C2" s="83"/>
+      <c r="D2" s="83"/>
+      <c r="E2" s="83"/>
+      <c r="F2" s="84"/>
+      <c r="G2" s="85"/>
+    </row>
+    <row r="3" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="47" t="s">
         <v>124</v>
       </c>
-      <c r="B3" s="84"/>
-      <c r="C3" s="85"/>
-      <c r="D3" s="84"/>
-      <c r="E3" s="85"/>
-      <c r="F3" s="84"/>
-      <c r="G3" s="84"/>
-    </row>
-    <row r="4" spans="1:7" ht="18.75" customHeight="1">
+      <c r="B3" s="83"/>
+      <c r="C3" s="84"/>
+      <c r="D3" s="83"/>
+      <c r="E3" s="84"/>
+      <c r="F3" s="83"/>
+      <c r="G3" s="83"/>
+    </row>
+    <row r="4" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="47" t="s">
         <v>125</v>
       </c>
-      <c r="B4" s="85"/>
-      <c r="C4" s="87"/>
-      <c r="D4" s="84"/>
-      <c r="E4" s="84"/>
-      <c r="F4" s="84"/>
-      <c r="G4" s="85"/>
-    </row>
-    <row r="5" spans="1:7" ht="18.75" customHeight="1">
+      <c r="B4" s="84"/>
+      <c r="C4" s="86"/>
+      <c r="D4" s="83"/>
+      <c r="E4" s="83"/>
+      <c r="F4" s="83"/>
+      <c r="G4" s="84"/>
+    </row>
+    <row r="5" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="47" t="s">
         <v>126</v>
       </c>
-      <c r="B5" s="85"/>
-      <c r="C5" s="86"/>
-      <c r="D5" s="84"/>
-      <c r="E5" s="84"/>
-      <c r="F5" s="86"/>
-      <c r="G5" s="84"/>
-    </row>
-    <row r="6" spans="1:7" ht="18.75" customHeight="1">
+      <c r="B5" s="84"/>
+      <c r="C5" s="85"/>
+      <c r="D5" s="83"/>
+      <c r="E5" s="83"/>
+      <c r="F5" s="85"/>
+      <c r="G5" s="83"/>
+    </row>
+    <row r="6" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="47" t="s">
         <v>127</v>
       </c>
-      <c r="B6" s="85"/>
-      <c r="C6" s="86"/>
-      <c r="D6" s="84"/>
-      <c r="E6" s="84"/>
-      <c r="F6" s="84"/>
-      <c r="G6" s="85"/>
-    </row>
-    <row r="7" spans="1:7" ht="18.75" customHeight="1">
+      <c r="B6" s="84"/>
+      <c r="C6" s="85"/>
+      <c r="D6" s="83"/>
+      <c r="E6" s="83"/>
+      <c r="F6" s="83"/>
+      <c r="G6" s="84"/>
+    </row>
+    <row r="7" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="47" t="s">
         <v>128</v>
       </c>
-      <c r="B7" s="84"/>
-      <c r="C7" s="84"/>
-      <c r="D7" s="84"/>
-      <c r="E7" s="86"/>
-      <c r="F7" s="84"/>
-      <c r="G7" s="84"/>
-    </row>
-    <row r="8" spans="1:7" ht="18.75" customHeight="1">
+      <c r="B7" s="83"/>
+      <c r="C7" s="83"/>
+      <c r="D7" s="83"/>
+      <c r="E7" s="85"/>
+      <c r="F7" s="83"/>
+      <c r="G7" s="83"/>
+    </row>
+    <row r="8" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="47" t="s">
         <v>129</v>
       </c>
-      <c r="B8" s="84"/>
-      <c r="C8" s="85"/>
-      <c r="D8" s="84"/>
-      <c r="E8" s="86"/>
-      <c r="F8" s="85"/>
-      <c r="G8" s="85"/>
-    </row>
-    <row r="9" spans="1:7" ht="18.75" customHeight="1">
+      <c r="B8" s="83"/>
+      <c r="C8" s="84"/>
+      <c r="D8" s="83"/>
+      <c r="E8" s="85"/>
+      <c r="F8" s="84"/>
+      <c r="G8" s="84"/>
+    </row>
+    <row r="9" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="47" t="s">
         <v>130</v>
       </c>
-      <c r="B9" s="85"/>
-      <c r="C9" s="85"/>
-      <c r="D9" s="84"/>
-      <c r="E9" s="86"/>
-      <c r="F9" s="84"/>
-      <c r="G9" s="85"/>
-    </row>
-    <row r="10" spans="1:7" ht="18.75" customHeight="1">
+      <c r="B9" s="84"/>
+      <c r="C9" s="84"/>
+      <c r="D9" s="83"/>
+      <c r="E9" s="85"/>
+      <c r="F9" s="83"/>
+      <c r="G9" s="84"/>
+    </row>
+    <row r="10" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="47" t="s">
         <v>131</v>
       </c>
-      <c r="B10" s="84"/>
-      <c r="C10" s="84"/>
-      <c r="D10" s="84"/>
-      <c r="E10" s="86"/>
-      <c r="F10" s="84"/>
-      <c r="G10" s="84"/>
-    </row>
-    <row r="11" spans="1:7" ht="18.75" customHeight="1">
+      <c r="B10" s="83"/>
+      <c r="C10" s="83"/>
+      <c r="D10" s="83"/>
+      <c r="E10" s="85"/>
+      <c r="F10" s="83"/>
+      <c r="G10" s="83"/>
+    </row>
+    <row r="11" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="47" t="s">
         <v>132</v>
       </c>
-      <c r="B11" s="84"/>
-      <c r="C11" s="85"/>
-      <c r="D11" s="84"/>
-      <c r="E11" s="86"/>
-      <c r="F11" s="86"/>
-      <c r="G11" s="84"/>
-    </row>
-    <row r="12" spans="1:7" ht="18.75" customHeight="1">
+      <c r="B11" s="83"/>
+      <c r="C11" s="84"/>
+      <c r="D11" s="83"/>
+      <c r="E11" s="85"/>
+      <c r="F11" s="85"/>
+      <c r="G11" s="83"/>
+    </row>
+    <row r="12" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="47" t="s">
         <v>133</v>
       </c>
       <c r="D12" s="49"/>
     </row>
-    <row r="13" spans="1:7" ht="18.75" customHeight="1">
+    <row r="13" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="47" t="s">
         <v>134</v>
       </c>
       <c r="D13" s="49"/>
     </row>
-    <row r="14" spans="1:7" ht="18.75" customHeight="1">
+    <row r="14" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="47" t="s">
         <v>135</v>
       </c>
@@ -1600,28 +1638,28 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
   <dimension ref="A1:Q27"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight"/>
+      <selection pane="topRight" activeCell="M29" sqref="M29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="46.85546875" style="19" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="24.28515625" style="53" bestFit="1" customWidth="1"/>
     <col min="3" max="10" width="24.28515625" style="21" bestFit="1" customWidth="1"/>
-    <col min="11" max="15" width="24.28515625" style="82" bestFit="1" customWidth="1"/>
+    <col min="11" max="15" width="24.28515625" style="81" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="24" style="21" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="13.5703125" style="53" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="15.75" customHeight="1">
+    <row r="1" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="54"/>
       <c r="B1" s="55" t="s">
         <v>54</v>
@@ -1642,7 +1680,7 @@
       <c r="P1" s="59"/>
       <c r="Q1" s="60"/>
     </row>
-    <row r="2" spans="1:17" ht="18.75" customHeight="1">
+    <row r="2" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="30" t="s">
         <v>1</v>
       </c>
@@ -1695,7 +1733,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="3" spans="1:17" ht="18.75" customHeight="1">
+    <row r="3" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="64" t="s">
         <v>5</v>
       </c>
@@ -1748,7 +1786,7 @@
         <v>90.37</v>
       </c>
     </row>
-    <row r="4" spans="1:17" ht="18.75" customHeight="1">
+    <row r="4" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="64" t="s">
         <v>41</v>
       </c>
@@ -1801,7 +1839,7 @@
         <v>22.7</v>
       </c>
     </row>
-    <row r="5" spans="1:17" ht="11.25" customHeight="1">
+    <row r="5" spans="1:17" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="64" t="s">
         <v>7</v>
       </c>
@@ -1854,7 +1892,7 @@
         <v>40179</v>
       </c>
     </row>
-    <row r="6" spans="1:17" ht="18.75" customHeight="1">
+    <row r="6" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="64" t="s">
         <v>8</v>
       </c>
@@ -1907,7 +1945,7 @@
         <v>41639</v>
       </c>
     </row>
-    <row r="7" spans="1:17" ht="18.75" customHeight="1">
+    <row r="7" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="64" t="s">
         <v>9</v>
       </c>
@@ -1960,7 +1998,7 @@
         <v>38387</v>
       </c>
     </row>
-    <row r="8" spans="1:17" ht="18.75" customHeight="1">
+    <row r="8" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="64" t="s">
         <v>10</v>
       </c>
@@ -2013,48 +2051,48 @@
         <v>28</v>
       </c>
     </row>
-    <row r="9" spans="1:17" ht="18.75" customHeight="1">
+    <row r="9" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="64" t="s">
         <v>12</v>
       </c>
       <c r="B9" s="72">
-        <v>35</v>
+        <v>60</v>
       </c>
       <c r="C9" s="72">
-        <v>35</v>
+        <v>60</v>
       </c>
       <c r="D9" s="72">
-        <v>35</v>
+        <v>60</v>
       </c>
       <c r="E9" s="72">
-        <v>35</v>
+        <v>60</v>
       </c>
       <c r="F9" s="72">
-        <v>35</v>
+        <v>60</v>
       </c>
       <c r="G9" s="72">
-        <v>35</v>
+        <v>60</v>
       </c>
       <c r="H9" s="72">
-        <v>35</v>
+        <v>60</v>
       </c>
       <c r="I9" s="72">
-        <v>33</v>
+        <v>60</v>
       </c>
       <c r="J9" s="72">
-        <v>33</v>
+        <v>60</v>
       </c>
       <c r="K9" s="72">
-        <v>30</v>
+        <v>60</v>
       </c>
       <c r="L9" s="72">
-        <v>30</v>
+        <v>60</v>
       </c>
       <c r="M9" s="72">
-        <v>32</v>
+        <v>60</v>
       </c>
       <c r="N9" s="72">
-        <v>32</v>
+        <v>60</v>
       </c>
       <c r="O9" s="72">
         <v>100</v>
@@ -2066,48 +2104,48 @@
         <v>100</v>
       </c>
     </row>
-    <row r="10" spans="1:17" ht="18.75" customHeight="1">
+    <row r="10" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="64" t="s">
         <v>13</v>
       </c>
-      <c r="B10" s="72">
-        <v>26</v>
-      </c>
-      <c r="C10" s="72">
-        <v>26</v>
-      </c>
-      <c r="D10" s="72">
-        <v>26</v>
-      </c>
-      <c r="E10" s="72">
-        <v>26</v>
-      </c>
-      <c r="F10" s="72">
-        <v>26</v>
-      </c>
-      <c r="G10" s="72">
-        <v>26</v>
-      </c>
-      <c r="H10" s="72">
-        <v>26</v>
-      </c>
-      <c r="I10" s="72">
-        <v>22</v>
-      </c>
-      <c r="J10" s="72">
-        <v>22</v>
-      </c>
-      <c r="K10" s="72">
-        <v>22</v>
-      </c>
-      <c r="L10" s="72">
-        <v>22</v>
-      </c>
-      <c r="M10" s="72">
-        <v>22</v>
-      </c>
-      <c r="N10" s="72">
-        <v>22</v>
+      <c r="B10" s="72" t="s">
+        <v>136</v>
+      </c>
+      <c r="C10" s="72" t="s">
+        <v>136</v>
+      </c>
+      <c r="D10" s="72" t="s">
+        <v>136</v>
+      </c>
+      <c r="E10" s="72" t="s">
+        <v>136</v>
+      </c>
+      <c r="F10" s="72" t="s">
+        <v>136</v>
+      </c>
+      <c r="G10" s="72" t="s">
+        <v>136</v>
+      </c>
+      <c r="H10" s="72" t="s">
+        <v>136</v>
+      </c>
+      <c r="I10" s="72" t="s">
+        <v>136</v>
+      </c>
+      <c r="J10" s="72" t="s">
+        <v>136</v>
+      </c>
+      <c r="K10" s="72" t="s">
+        <v>136</v>
+      </c>
+      <c r="L10" s="72" t="s">
+        <v>136</v>
+      </c>
+      <c r="M10" s="72" t="s">
+        <v>136</v>
+      </c>
+      <c r="N10" s="72" t="s">
+        <v>136</v>
       </c>
       <c r="O10" s="72">
         <v>26</v>
@@ -2119,7 +2157,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="11" spans="1:17" ht="18.75" customHeight="1">
+    <row r="11" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="64" t="s">
         <v>14</v>
       </c>
@@ -2172,7 +2210,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="12" spans="1:17" ht="18.75" customHeight="1">
+    <row r="12" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="64" t="s">
         <v>16</v>
       </c>
@@ -2225,7 +2263,7 @@
         <v>3.4</v>
       </c>
     </row>
-    <row r="13" spans="1:17" ht="18.75" customHeight="1">
+    <row r="13" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="64" t="s">
         <v>17</v>
       </c>
@@ -2278,7 +2316,7 @@
         <v>1252</v>
       </c>
     </row>
-    <row r="14" spans="1:17" ht="15.75" customHeight="1">
+    <row r="14" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="76"/>
       <c r="B14" s="60"/>
       <c r="C14" s="59"/>
@@ -2297,7 +2335,7 @@
       <c r="P14" s="59"/>
       <c r="Q14" s="60"/>
     </row>
-    <row r="15" spans="1:17" ht="18.75" customHeight="1">
+    <row r="15" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="30" t="s">
         <v>7</v>
       </c>
@@ -2350,7 +2388,7 @@
         <v>40544</v>
       </c>
     </row>
-    <row r="16" spans="1:17" ht="18.75" customHeight="1">
+    <row r="16" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="64" t="s">
         <v>8</v>
       </c>
@@ -2403,7 +2441,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="17" spans="1:17" ht="18.75" customHeight="1">
+    <row r="17" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="64" t="s">
         <v>12</v>
       </c>
@@ -2456,7 +2494,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="18" spans="1:17" ht="18.75" customHeight="1">
+    <row r="18" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="64" t="s">
         <v>13</v>
       </c>
@@ -2507,7 +2545,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="19" spans="1:17" ht="18.75" customHeight="1">
+    <row r="19" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="64" t="s">
         <v>9</v>
       </c>
@@ -2560,26 +2598,60 @@
         <v>38444</v>
       </c>
     </row>
-    <row r="20" spans="1:17" ht="15.75" customHeight="1">
-      <c r="A20" s="76"/>
-      <c r="B20" s="80"/>
-      <c r="C20" s="59"/>
-      <c r="D20" s="59"/>
-      <c r="E20" s="59"/>
-      <c r="F20" s="59"/>
-      <c r="G20" s="59"/>
-      <c r="H20" s="59"/>
-      <c r="I20" s="59"/>
-      <c r="J20" s="59"/>
-      <c r="K20" s="58"/>
-      <c r="L20" s="58"/>
-      <c r="M20" s="58"/>
-      <c r="N20" s="58"/>
-      <c r="O20" s="58"/>
-      <c r="P20" s="59"/>
-      <c r="Q20" s="60"/>
-    </row>
-    <row r="21" spans="1:17" ht="15.75" customHeight="1">
+    <row r="20" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="64" t="s">
+        <v>12</v>
+      </c>
+      <c r="B20" s="72">
+        <v>35</v>
+      </c>
+      <c r="C20" s="72">
+        <v>35</v>
+      </c>
+      <c r="D20" s="72">
+        <v>35</v>
+      </c>
+      <c r="E20" s="72">
+        <v>35</v>
+      </c>
+      <c r="F20" s="72">
+        <v>35</v>
+      </c>
+      <c r="G20" s="72">
+        <v>35</v>
+      </c>
+      <c r="H20" s="72">
+        <v>35</v>
+      </c>
+      <c r="I20" s="72">
+        <v>80</v>
+      </c>
+      <c r="J20" s="72">
+        <v>33</v>
+      </c>
+      <c r="K20" s="72">
+        <v>30</v>
+      </c>
+      <c r="L20" s="72">
+        <v>30</v>
+      </c>
+      <c r="M20" s="72">
+        <v>32</v>
+      </c>
+      <c r="N20" s="72">
+        <v>32</v>
+      </c>
+      <c r="O20" s="72">
+        <v>100</v>
+      </c>
+      <c r="P20" s="73">
+        <v>100</v>
+      </c>
+      <c r="Q20" s="74">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="21" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="76"/>
       <c r="B21" s="60"/>
       <c r="C21" s="59"/>
@@ -2598,7 +2670,7 @@
       <c r="P21" s="59"/>
       <c r="Q21" s="60"/>
     </row>
-    <row r="22" spans="1:17" ht="15.75" customHeight="1">
+    <row r="22" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="76"/>
       <c r="B22" s="60"/>
       <c r="C22" s="59"/>
@@ -2617,7 +2689,7 @@
       <c r="P22" s="59"/>
       <c r="Q22" s="60"/>
     </row>
-    <row r="23" spans="1:17" ht="15.75" customHeight="1">
+    <row r="23" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="76"/>
       <c r="B23" s="60"/>
       <c r="C23" s="59"/>
@@ -2636,7 +2708,7 @@
       <c r="P23" s="59"/>
       <c r="Q23" s="60"/>
     </row>
-    <row r="24" spans="1:17" ht="15.75" customHeight="1">
+    <row r="24" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="76"/>
       <c r="B24" s="60"/>
       <c r="C24" s="59"/>
@@ -2655,7 +2727,7 @@
       <c r="P24" s="59"/>
       <c r="Q24" s="60"/>
     </row>
-    <row r="25" spans="1:17" ht="15.75" customHeight="1">
+    <row r="25" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="76"/>
       <c r="B25" s="60"/>
       <c r="C25" s="59"/>
@@ -2674,7 +2746,7 @@
       <c r="P25" s="59"/>
       <c r="Q25" s="60"/>
     </row>
-    <row r="26" spans="1:17" ht="15.75" customHeight="1">
+    <row r="26" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="76"/>
       <c r="B26" s="60"/>
       <c r="C26" s="59"/>
@@ -2693,9 +2765,9 @@
       <c r="P26" s="59"/>
       <c r="Q26" s="60"/>
     </row>
-    <row r="27" spans="1:17" ht="15.75" customHeight="1">
+    <row r="27" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="76"/>
-      <c r="B27" s="81"/>
+      <c r="B27" s="80"/>
       <c r="C27" s="59"/>
       <c r="D27" s="59"/>
       <c r="E27" s="59"/>
@@ -2714,6 +2786,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -2729,7 +2802,7 @@
       <selection pane="topRight"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="46.85546875" style="19" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="30.140625" style="53" bestFit="1" customWidth="1"/>
@@ -2739,7 +2812,7 @@
     <col min="16" max="16" width="13.5703125" style="19" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="15.75" customHeight="1">
+    <row r="1" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="29"/>
       <c r="B1" s="44" t="s">
         <v>54</v>
@@ -2753,7 +2826,7 @@
       <c r="I1" s="29"/>
       <c r="J1" s="29"/>
     </row>
-    <row r="2" spans="1:16" ht="18.75" customHeight="1">
+    <row r="2" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="30" t="s">
         <v>1</v>
       </c>
@@ -2777,7 +2850,7 @@
       <c r="O2" s="46"/>
       <c r="P2" s="46"/>
     </row>
-    <row r="3" spans="1:16" ht="18.75" customHeight="1">
+    <row r="3" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="30" t="s">
         <v>5</v>
       </c>
@@ -2801,7 +2874,7 @@
       <c r="O3" s="47"/>
       <c r="P3" s="47"/>
     </row>
-    <row r="4" spans="1:16" ht="18.75" customHeight="1">
+    <row r="4" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="30" t="s">
         <v>41</v>
       </c>
@@ -2825,7 +2898,7 @@
       <c r="O4" s="47"/>
       <c r="P4" s="47"/>
     </row>
-    <row r="5" spans="1:16" ht="18.75" customHeight="1">
+    <row r="5" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="30" t="s">
         <v>7</v>
       </c>
@@ -2849,7 +2922,7 @@
       <c r="O5" s="47"/>
       <c r="P5" s="47"/>
     </row>
-    <row r="6" spans="1:16" ht="18.75" customHeight="1">
+    <row r="6" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="30" t="s">
         <v>8</v>
       </c>
@@ -2873,7 +2946,7 @@
       <c r="O6" s="47"/>
       <c r="P6" s="47"/>
     </row>
-    <row r="7" spans="1:16" ht="18.75" customHeight="1">
+    <row r="7" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="30" t="s">
         <v>9</v>
       </c>
@@ -2897,7 +2970,7 @@
       <c r="O7" s="47"/>
       <c r="P7" s="47"/>
     </row>
-    <row r="8" spans="1:16" ht="18.75" customHeight="1">
+    <row r="8" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="30" t="s">
         <v>10</v>
       </c>
@@ -2921,7 +2994,7 @@
       <c r="O8" s="47"/>
       <c r="P8" s="47"/>
     </row>
-    <row r="9" spans="1:16" ht="18.75" customHeight="1">
+    <row r="9" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="30" t="s">
         <v>12</v>
       </c>
@@ -2945,7 +3018,7 @@
       <c r="O9" s="51"/>
       <c r="P9" s="52"/>
     </row>
-    <row r="10" spans="1:16" ht="18.75" customHeight="1">
+    <row r="10" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="30" t="s">
         <v>13</v>
       </c>
@@ -2965,7 +3038,7 @@
       <c r="O10" s="47"/>
       <c r="P10" s="47"/>
     </row>
-    <row r="11" spans="1:16" ht="18.75" customHeight="1">
+    <row r="11" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="30" t="s">
         <v>14</v>
       </c>
@@ -2989,7 +3062,7 @@
       <c r="O11" s="47"/>
       <c r="P11" s="47"/>
     </row>
-    <row r="12" spans="1:16" ht="18.75" customHeight="1">
+    <row r="12" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="30" t="s">
         <v>16</v>
       </c>
@@ -3009,7 +3082,7 @@
       <c r="O12" s="47"/>
       <c r="P12" s="47"/>
     </row>
-    <row r="13" spans="1:16" ht="18.75" customHeight="1">
+    <row r="13" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="30" t="s">
         <v>17</v>
       </c>
@@ -3050,7 +3123,7 @@
       <selection pane="topRight"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="46.85546875" style="19" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="24.28515625" style="20" bestFit="1" customWidth="1"/>
@@ -3059,13 +3132,13 @@
     <col min="5" max="5" width="26.140625" style="20" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15.75" customHeight="1">
+    <row r="1" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="29"/>
       <c r="B1" s="40" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="18.75" customHeight="1">
+    <row r="2" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="30" t="s">
         <v>1</v>
       </c>
@@ -3082,7 +3155,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="18.75" customHeight="1">
+    <row r="3" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="30" t="s">
         <v>5</v>
       </c>
@@ -3099,7 +3172,7 @@
         <v>48.717812000000002</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="18.75" customHeight="1">
+    <row r="4" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="30" t="s">
         <v>41</v>
       </c>
@@ -3116,7 +3189,7 @@
         <v>31.323521</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="18.75" customHeight="1">
+    <row r="5" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="30" t="s">
         <v>7</v>
       </c>
@@ -3133,7 +3206,7 @@
         <v>37987</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="18.75" customHeight="1">
+    <row r="6" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="30" t="s">
         <v>8</v>
       </c>
@@ -3150,7 +3223,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="18.75" customHeight="1">
+    <row r="7" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="30" t="s">
         <v>9</v>
       </c>
@@ -3167,7 +3240,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="18.75" customHeight="1">
+    <row r="8" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="30" t="s">
         <v>10</v>
       </c>
@@ -3184,7 +3257,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="18.75" customHeight="1">
+    <row r="9" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="30" t="s">
         <v>12</v>
       </c>
@@ -3201,7 +3274,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="18.75" customHeight="1">
+    <row r="10" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="30" t="s">
         <v>13</v>
       </c>
@@ -3218,7 +3291,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="18.75" customHeight="1">
+    <row r="11" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="30" t="s">
         <v>14</v>
       </c>
@@ -3235,7 +3308,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="12" spans="1:5" ht="18.75" customHeight="1">
+    <row r="12" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="30" t="s">
         <v>16</v>
       </c>
@@ -3252,7 +3325,7 @@
         <v>5.8</v>
       </c>
     </row>
-    <row r="13" spans="1:5" ht="18.75" customHeight="1">
+    <row r="13" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="30" t="s">
         <v>17</v>
       </c>
@@ -3281,11 +3354,11 @@
   </sheetPr>
   <dimension ref="A1:J22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="O5" sqref="O5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="49.5703125" style="19" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12.140625" style="21" bestFit="1" customWidth="1"/>
@@ -3293,21 +3366,21 @@
     <col min="14" max="14" width="9.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="15.75" customHeight="1">
-      <c r="A1" s="88" t="s">
+    <row r="1" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="87" t="s">
         <v>33</v>
       </c>
-      <c r="B1" s="89"/>
-      <c r="C1" s="89"/>
-      <c r="D1" s="89"/>
-      <c r="E1" s="89"/>
-      <c r="F1" s="89"/>
-      <c r="G1" s="89"/>
-      <c r="H1" s="89"/>
-      <c r="I1" s="89"/>
-      <c r="J1" s="89"/>
-    </row>
-    <row r="2" spans="1:10" ht="18.75" customHeight="1">
+      <c r="B1" s="88"/>
+      <c r="C1" s="88"/>
+      <c r="D1" s="88"/>
+      <c r="E1" s="88"/>
+      <c r="F1" s="88"/>
+      <c r="G1" s="88"/>
+      <c r="H1" s="88"/>
+      <c r="I1" s="88"/>
+      <c r="J1" s="88"/>
+    </row>
+    <row r="2" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="30" t="s">
         <v>1</v>
       </c>
@@ -3339,7 +3412,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="18.75" customHeight="1">
+    <row r="3" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="30" t="s">
         <v>5</v>
       </c>
@@ -3371,7 +3444,7 @@
         <v>-7.61111</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="18.75" customHeight="1">
+    <row r="4" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="30" t="s">
         <v>41</v>
       </c>
@@ -3403,7 +3476,7 @@
         <v>31.66667</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="18.75" customHeight="1">
+    <row r="5" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="30" t="s">
         <v>7</v>
       </c>
@@ -3435,7 +3508,7 @@
         <v>38353</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="18.75" customHeight="1">
+    <row r="6" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="30" t="s">
         <v>8</v>
       </c>
@@ -3467,7 +3540,7 @@
         <v>42369</v>
       </c>
     </row>
-    <row r="7" spans="1:10" ht="18.75" customHeight="1">
+    <row r="7" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="30" t="s">
         <v>9</v>
       </c>
@@ -3499,7 +3572,7 @@
         <v>37979</v>
       </c>
     </row>
-    <row r="8" spans="1:10" ht="18.75" customHeight="1">
+    <row r="8" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="30" t="s">
         <v>10</v>
       </c>
@@ -3531,7 +3604,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="9" spans="1:10" ht="18.75" customHeight="1">
+    <row r="9" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="30" t="s">
         <v>12</v>
       </c>
@@ -3563,23 +3636,23 @@
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="18.75" customHeight="1">
+    <row r="10" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="30" t="s">
         <v>13</v>
       </c>
-      <c r="B10" s="90" t="s">
+      <c r="B10" s="89" t="s">
         <v>43</v>
       </c>
-      <c r="C10" s="91"/>
-      <c r="D10" s="91"/>
-      <c r="E10" s="91"/>
-      <c r="F10" s="91"/>
-      <c r="G10" s="91"/>
-      <c r="H10" s="91"/>
-      <c r="I10" s="91"/>
-      <c r="J10" s="92"/>
-    </row>
-    <row r="11" spans="1:10" ht="18.75" customHeight="1">
+      <c r="C10" s="90"/>
+      <c r="D10" s="90"/>
+      <c r="E10" s="90"/>
+      <c r="F10" s="90"/>
+      <c r="G10" s="90"/>
+      <c r="H10" s="90"/>
+      <c r="I10" s="90"/>
+      <c r="J10" s="91"/>
+    </row>
+    <row r="11" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="30" t="s">
         <v>14</v>
       </c>
@@ -3611,7 +3684,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="12" spans="1:10" ht="18.75" customHeight="1">
+    <row r="12" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="30" t="s">
         <v>16</v>
       </c>
@@ -3643,7 +3716,7 @@
         <v>2.25</v>
       </c>
     </row>
-    <row r="13" spans="1:10" ht="18.75" customHeight="1">
+    <row r="13" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="30" t="s">
         <v>17</v>
       </c>
@@ -3675,7 +3748,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="14" spans="1:10" ht="18.75" customHeight="1">
+    <row r="14" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="30" t="s">
         <v>45</v>
       </c>
@@ -3707,7 +3780,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="15" spans="1:10" ht="18.75" customHeight="1">
+    <row r="15" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="30" t="s">
         <v>46</v>
       </c>
@@ -3739,7 +3812,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="16" spans="1:10" ht="18.75" customHeight="1">
+    <row r="16" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="30" t="s">
         <v>47</v>
       </c>
@@ -3771,9 +3844,9 @@
         <v>45</v>
       </c>
     </row>
-    <row r="17" spans="1:10" ht="18.75" customHeight="1"/>
-    <row r="18" spans="1:10" ht="18.75" customHeight="1"/>
-    <row r="19" spans="1:10" ht="18.75" customHeight="1">
+    <row r="17" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="18" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="19" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="30" t="s">
         <v>12</v>
       </c>
@@ -3805,23 +3878,23 @@
         <v>3</v>
       </c>
     </row>
-    <row r="20" spans="1:10" ht="18.75" customHeight="1">
+    <row r="20" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="30" t="s">
         <v>13</v>
       </c>
-      <c r="B20" s="90" t="s">
+      <c r="B20" s="89" t="s">
         <v>43</v>
       </c>
-      <c r="C20" s="91"/>
-      <c r="D20" s="91"/>
-      <c r="E20" s="91"/>
-      <c r="F20" s="91"/>
-      <c r="G20" s="91"/>
-      <c r="H20" s="91"/>
-      <c r="I20" s="91"/>
-      <c r="J20" s="92"/>
-    </row>
-    <row r="21" spans="1:10" ht="18.75" customHeight="1">
+      <c r="C20" s="90"/>
+      <c r="D20" s="90"/>
+      <c r="E20" s="90"/>
+      <c r="F20" s="90"/>
+      <c r="G20" s="90"/>
+      <c r="H20" s="90"/>
+      <c r="I20" s="90"/>
+      <c r="J20" s="91"/>
+    </row>
+    <row r="21" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="30" t="s">
         <v>16</v>
       </c>
@@ -3853,7 +3926,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="22" spans="1:10" ht="18.75" customHeight="1">
+    <row r="22" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="30" t="s">
         <v>8</v>
       </c>
@@ -3904,7 +3977,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="47.140625" style="19" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="15.85546875" style="20" bestFit="1" customWidth="1"/>
@@ -3914,7 +3987,7 @@
     <col min="7" max="7" width="13.5703125" style="20" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="18.75" customHeight="1">
+    <row r="1" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
       <c r="B1" s="22" t="s">
         <v>21</v>
@@ -3925,7 +3998,7 @@
       <c r="F1" s="22"/>
       <c r="G1" s="24"/>
     </row>
-    <row r="2" spans="1:7" ht="18.75" customHeight="1">
+    <row r="2" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
@@ -3948,7 +4021,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="19.5" customHeight="1">
+    <row r="3" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>5</v>
       </c>
@@ -3971,7 +4044,7 @@
         <v>119.19</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="19.5" customHeight="1">
+    <row r="4" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>6</v>
       </c>
@@ -3994,7 +4067,7 @@
         <v>42.57</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="18.75" customHeight="1">
+    <row r="5" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>7</v>
       </c>
@@ -4017,7 +4090,7 @@
         <v>42109</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="18.75" customHeight="1">
+    <row r="6" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>8</v>
       </c>
@@ -4040,7 +4113,7 @@
         <v>42658</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="18.75" customHeight="1">
+    <row r="7" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>9</v>
       </c>
@@ -4063,7 +4136,7 @@
         <v>42491</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="18.75" customHeight="1">
+    <row r="8" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>10</v>
       </c>
@@ -4086,7 +4159,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="18.75" customHeight="1">
+    <row r="9" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>12</v>
       </c>
@@ -4109,7 +4182,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="18.75" customHeight="1">
+    <row r="10" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>13</v>
       </c>
@@ -4132,7 +4205,7 @@
         <v>30.01</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="18.75" customHeight="1">
+    <row r="11" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>14</v>
       </c>
@@ -4155,7 +4228,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="18.75" customHeight="1">
+    <row r="12" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>16</v>
       </c>
@@ -4178,7 +4251,7 @@
         <v>9.4</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="18.75" customHeight="1">
+    <row r="13" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>17</v>
       </c>
@@ -4189,7 +4262,7 @@
       <c r="F13" s="3"/>
       <c r="G13" s="3"/>
     </row>
-    <row r="14" spans="1:7" ht="18.75" customHeight="1">
+    <row r="14" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="25" t="s">
         <v>30</v>
       </c>
@@ -4212,7 +4285,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="18.75" customHeight="1">
+    <row r="15" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="26"/>
       <c r="B15" s="27"/>
       <c r="C15" s="28"/>
@@ -4221,7 +4294,7 @@
       <c r="F15" s="27"/>
       <c r="G15" s="27"/>
     </row>
-    <row r="16" spans="1:7" ht="18.75" customHeight="1">
+    <row r="16" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="1"/>
       <c r="B16" s="22"/>
       <c r="C16" s="23"/>
@@ -4230,7 +4303,7 @@
       <c r="F16" s="22"/>
       <c r="G16" s="22"/>
     </row>
-    <row r="17" spans="1:7" ht="18.75" customHeight="1">
+    <row r="17" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>12</v>
       </c>
@@ -4267,7 +4340,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="47.140625" style="19" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="15.85546875" style="20" bestFit="1" customWidth="1"/>
@@ -4278,18 +4351,18 @@
     <col min="7" max="7" width="13.5703125" style="20" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="39.75" customHeight="1">
+    <row r="1" spans="1:7" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
-      <c r="B1" s="93" t="s">
+      <c r="B1" s="92" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="94"/>
-      <c r="D1" s="94"/>
-      <c r="E1" s="94"/>
-      <c r="F1" s="94"/>
-      <c r="G1" s="95"/>
-    </row>
-    <row r="2" spans="1:7" ht="18.75" customHeight="1">
+      <c r="C1" s="93"/>
+      <c r="D1" s="93"/>
+      <c r="E1" s="93"/>
+      <c r="F1" s="93"/>
+      <c r="G1" s="94"/>
+    </row>
+    <row r="2" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
@@ -4312,7 +4385,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="19.5" customHeight="1">
+    <row r="3" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>5</v>
       </c>
@@ -4335,7 +4408,7 @@
         <v>50.55</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="19.5" customHeight="1">
+    <row r="4" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>6</v>
       </c>
@@ -4358,7 +4431,7 @@
         <v>32.18</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="18.75" customHeight="1">
+    <row r="5" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>7</v>
       </c>
@@ -4381,7 +4454,7 @@
         <v>41640</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="18.75" customHeight="1">
+    <row r="6" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>8</v>
       </c>
@@ -4404,7 +4477,7 @@
         <v>42004</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="18.75" customHeight="1">
+    <row r="7" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>9</v>
       </c>
@@ -4427,7 +4500,7 @@
         <v>41805</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="18.75" customHeight="1">
+    <row r="8" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>10</v>
       </c>
@@ -4450,7 +4523,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="18.75" customHeight="1">
+    <row r="9" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>12</v>
       </c>
@@ -4473,7 +4546,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="18.75" customHeight="1">
+    <row r="10" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>13</v>
       </c>
@@ -4496,7 +4569,7 @@
         <v>24.61</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="18.75" customHeight="1">
+    <row r="11" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>14</v>
       </c>
@@ -4519,7 +4592,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="18.75" customHeight="1">
+    <row r="12" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>16</v>
       </c>
@@ -4542,7 +4615,7 @@
         <v>6.84</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="18.75" customHeight="1">
+    <row r="13" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="10" t="s">
         <v>17</v>
       </c>
@@ -4565,7 +4638,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="18.75" customHeight="1">
+    <row r="14" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="13" t="s">
         <v>19</v>
       </c>
@@ -4588,7 +4661,7 @@
         <v>7.95</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="18.75" customHeight="1">
+    <row r="15" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="16"/>
       <c r="B15" s="17"/>
       <c r="C15" s="18"/>
@@ -4597,7 +4670,7 @@
       <c r="F15" s="17"/>
       <c r="G15" s="17"/>
     </row>
-    <row r="16" spans="1:7" ht="18.75" customHeight="1">
+    <row r="16" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>12</v>
       </c>

</xml_diff>

<commit_message>
Factors to run simulation has been updated with the pump factors as well as linking that in the compiler file
</commit_message>
<xml_diff>
--- a/heliostrome/jip_project/results/Factors to run simulation.xlsx
+++ b/heliostrome/jip_project/results/Factors to run simulation.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gaeta\Desktop\TU Delft\JIP\Github\heliostrome\heliostrome\jip_project\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B82A2919-1FA5-4174-8B5D-80196F1F0F92}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A98C91F8-B721-4382-941D-A6B13FD4C840}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11520" yWindow="0" windowWidth="11520" windowHeight="12360" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="All Case Studies (compatability" sheetId="1" r:id="rId1"/>
@@ -21,25 +21,12 @@
     <sheet name="Northeast China Case Study" sheetId="6" r:id="rId6"/>
     <sheet name="Iran Potato Case Study" sheetId="7" r:id="rId7"/>
   </sheets>
-  <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="421" uniqueCount="151">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="417" uniqueCount="151">
   <si>
     <t>Evaluation of AquaCrop for potato yield and biomass
 simulation under different water amounts in drip and
@@ -302,6 +289,48 @@
     <t>141-460</t>
   </si>
   <si>
+    <t>Mulch</t>
+  </si>
+  <si>
+    <t>Maximum Flow rate (L/min)</t>
+  </si>
+  <si>
+    <t>Average Flow Rate (L/min)</t>
+  </si>
+  <si>
+    <t>Modules Per String</t>
+  </si>
+  <si>
+    <t>String in Parralel</t>
+  </si>
+  <si>
+    <t>PV Module Name</t>
+  </si>
+  <si>
+    <t>Trina Solar TSM-260PA05A</t>
+  </si>
+  <si>
+    <t>Pump Name</t>
+  </si>
+  <si>
+    <t>Lorentz_ps1200</t>
+  </si>
+  <si>
+    <t>Static Head (m)</t>
+  </si>
+  <si>
+    <t>Total Length of Pipes (m)</t>
+  </si>
+  <si>
+    <t>Diameter of Pipes (m)</t>
+  </si>
+  <si>
+    <t>Material of Pipes</t>
+  </si>
+  <si>
+    <t>plastic</t>
+  </si>
+  <si>
     <t>31/08/2012</t>
   </si>
   <si>
@@ -401,12 +430,6 @@
     <t>26/06/2026</t>
   </si>
   <si>
-    <t>Average Flow Rate</t>
-  </si>
-  <si>
-    <t>61.24 L/min</t>
-  </si>
-  <si>
     <t>Lowering the cost - MIT</t>
   </si>
   <si>
@@ -459,42 +482,6 @@
   </si>
   <si>
     <t>Irrigation Schedule</t>
-  </si>
-  <si>
-    <t>Modules Per String</t>
-  </si>
-  <si>
-    <t>String in Parralel</t>
-  </si>
-  <si>
-    <t>PV Module Name</t>
-  </si>
-  <si>
-    <t>Pump Name</t>
-  </si>
-  <si>
-    <t>Trina Solar TSM-260PA05A</t>
-  </si>
-  <si>
-    <t>Lorentz_ps1200</t>
-  </si>
-  <si>
-    <t>plastic</t>
-  </si>
-  <si>
-    <t>Maximum Flow rate (L/min)</t>
-  </si>
-  <si>
-    <t>Static Head (m)</t>
-  </si>
-  <si>
-    <t>Total Length of Pipes (m)</t>
-  </si>
-  <si>
-    <t>Diameter of Pipes (m)</t>
-  </si>
-  <si>
-    <t>Material of Pipes</t>
   </si>
 </sst>
 </file>
@@ -504,9 +491,9 @@
   <numFmts count="3">
     <numFmt numFmtId="164" formatCode="mm/dd/yyyy"/>
     <numFmt numFmtId="165" formatCode="#,##0.0"/>
-    <numFmt numFmtId="166" formatCode="0.000"/>
+    <numFmt numFmtId="166" formatCode="#,##0.000"/>
   </numFmts>
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -553,24 +540,16 @@
       <family val="2"/>
     </font>
     <font>
-      <sz val="10"/>
-      <color rgb="FF34A853"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF34A853"/>
+      <name val="Arial"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -607,7 +586,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="25">
+  <borders count="23">
     <border>
       <left/>
       <right/>
@@ -893,34 +872,6 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFC6C6C6"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFC6C6C6"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFC6C6C6"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -1041,12 +992,24 @@
     <xf numFmtId="4" fontId="1" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="14" fontId="5" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="4" fontId="4" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="4" fontId="5" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="3" fontId="5" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="4" fontId="2" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1098,12 +1061,6 @@
     <xf numFmtId="164" fontId="5" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="3" fontId="5" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="14" fontId="5" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="3" fontId="2" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1146,7 +1103,22 @@
     <xf numFmtId="3" fontId="1" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="3" fontId="5" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="4" fontId="5" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="166" fontId="5" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1164,6 +1136,21 @@
     <xf numFmtId="4" fontId="1" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="4" fontId="1" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
@@ -1176,43 +1163,7 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="3" fontId="1" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="4" fontId="1" fillId="2" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="4" fontId="1" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="14" fontId="5" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="3" fontId="5" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="165" fontId="5" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1561,152 +1512,153 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B1" s="48" t="s">
-        <v>121</v>
-      </c>
-      <c r="C1" s="48" t="s">
-        <v>122</v>
-      </c>
-      <c r="D1" s="80" t="s">
+      <c r="A1" s="39"/>
+      <c r="B1" s="52" t="s">
+        <v>133</v>
+      </c>
+      <c r="C1" s="52" t="s">
+        <v>134</v>
+      </c>
+      <c r="D1" s="92" t="s">
         <v>54</v>
       </c>
-      <c r="E1" s="48" t="s">
-        <v>123</v>
-      </c>
-      <c r="F1" s="48" t="s">
-        <v>124</v>
-      </c>
-      <c r="G1" s="80" t="s">
-        <v>125</v>
+      <c r="E1" s="52" t="s">
+        <v>135</v>
+      </c>
+      <c r="F1" s="52" t="s">
+        <v>136</v>
+      </c>
+      <c r="G1" s="92" t="s">
+        <v>137</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="48" t="s">
-        <v>126</v>
-      </c>
-      <c r="B2" s="81"/>
-      <c r="C2" s="81"/>
-      <c r="D2" s="81"/>
-      <c r="E2" s="81"/>
-      <c r="F2" s="82"/>
-      <c r="G2" s="83"/>
+      <c r="A2" s="52" t="s">
+        <v>138</v>
+      </c>
+      <c r="B2" s="93"/>
+      <c r="C2" s="93"/>
+      <c r="D2" s="93"/>
+      <c r="E2" s="93"/>
+      <c r="F2" s="94"/>
+      <c r="G2" s="95"/>
     </row>
     <row r="3" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="48" t="s">
-        <v>127</v>
-      </c>
-      <c r="B3" s="81"/>
-      <c r="C3" s="82"/>
-      <c r="D3" s="81"/>
-      <c r="E3" s="82"/>
-      <c r="F3" s="81"/>
-      <c r="G3" s="81"/>
+      <c r="A3" s="52" t="s">
+        <v>139</v>
+      </c>
+      <c r="B3" s="93"/>
+      <c r="C3" s="94"/>
+      <c r="D3" s="93"/>
+      <c r="E3" s="94"/>
+      <c r="F3" s="93"/>
+      <c r="G3" s="93"/>
     </row>
     <row r="4" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="48" t="s">
-        <v>128</v>
-      </c>
-      <c r="B4" s="82"/>
-      <c r="C4" s="84"/>
-      <c r="D4" s="81"/>
-      <c r="E4" s="81"/>
-      <c r="F4" s="81"/>
-      <c r="G4" s="82"/>
+      <c r="A4" s="52" t="s">
+        <v>140</v>
+      </c>
+      <c r="B4" s="94"/>
+      <c r="C4" s="96"/>
+      <c r="D4" s="93"/>
+      <c r="E4" s="93"/>
+      <c r="F4" s="93"/>
+      <c r="G4" s="94"/>
     </row>
     <row r="5" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="48" t="s">
-        <v>129</v>
-      </c>
-      <c r="B5" s="82"/>
-      <c r="C5" s="83"/>
-      <c r="D5" s="81"/>
-      <c r="E5" s="81"/>
-      <c r="F5" s="83"/>
-      <c r="G5" s="81"/>
+      <c r="A5" s="52" t="s">
+        <v>141</v>
+      </c>
+      <c r="B5" s="94"/>
+      <c r="C5" s="95"/>
+      <c r="D5" s="93"/>
+      <c r="E5" s="93"/>
+      <c r="F5" s="95"/>
+      <c r="G5" s="93"/>
     </row>
     <row r="6" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="48" t="s">
-        <v>130</v>
-      </c>
-      <c r="B6" s="82"/>
-      <c r="C6" s="83"/>
-      <c r="D6" s="81"/>
-      <c r="E6" s="81"/>
-      <c r="F6" s="81"/>
-      <c r="G6" s="82"/>
+      <c r="A6" s="52" t="s">
+        <v>142</v>
+      </c>
+      <c r="B6" s="94"/>
+      <c r="C6" s="95"/>
+      <c r="D6" s="93"/>
+      <c r="E6" s="93"/>
+      <c r="F6" s="93"/>
+      <c r="G6" s="94"/>
     </row>
     <row r="7" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="48" t="s">
-        <v>131</v>
-      </c>
-      <c r="B7" s="81"/>
-      <c r="C7" s="81"/>
-      <c r="D7" s="81"/>
-      <c r="E7" s="83"/>
-      <c r="F7" s="81"/>
-      <c r="G7" s="81"/>
+      <c r="A7" s="52" t="s">
+        <v>143</v>
+      </c>
+      <c r="B7" s="93"/>
+      <c r="C7" s="93"/>
+      <c r="D7" s="93"/>
+      <c r="E7" s="95"/>
+      <c r="F7" s="93"/>
+      <c r="G7" s="93"/>
     </row>
     <row r="8" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="48" t="s">
-        <v>132</v>
-      </c>
-      <c r="B8" s="81"/>
-      <c r="C8" s="82"/>
-      <c r="D8" s="81"/>
-      <c r="E8" s="83"/>
-      <c r="F8" s="82"/>
-      <c r="G8" s="82"/>
+      <c r="A8" s="52" t="s">
+        <v>144</v>
+      </c>
+      <c r="B8" s="93"/>
+      <c r="C8" s="94"/>
+      <c r="D8" s="93"/>
+      <c r="E8" s="95"/>
+      <c r="F8" s="94"/>
+      <c r="G8" s="94"/>
     </row>
     <row r="9" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="48" t="s">
-        <v>133</v>
-      </c>
-      <c r="B9" s="82"/>
-      <c r="C9" s="82"/>
-      <c r="D9" s="81"/>
-      <c r="E9" s="83"/>
-      <c r="F9" s="81"/>
-      <c r="G9" s="82"/>
+      <c r="A9" s="52" t="s">
+        <v>145</v>
+      </c>
+      <c r="B9" s="94"/>
+      <c r="C9" s="94"/>
+      <c r="D9" s="93"/>
+      <c r="E9" s="95"/>
+      <c r="F9" s="93"/>
+      <c r="G9" s="94"/>
     </row>
     <row r="10" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="48" t="s">
-        <v>134</v>
-      </c>
-      <c r="B10" s="81"/>
-      <c r="C10" s="81"/>
-      <c r="D10" s="81"/>
-      <c r="E10" s="83"/>
-      <c r="F10" s="81"/>
-      <c r="G10" s="81"/>
+      <c r="A10" s="52" t="s">
+        <v>146</v>
+      </c>
+      <c r="B10" s="93"/>
+      <c r="C10" s="93"/>
+      <c r="D10" s="93"/>
+      <c r="E10" s="95"/>
+      <c r="F10" s="93"/>
+      <c r="G10" s="93"/>
     </row>
     <row r="11" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="48" t="s">
-        <v>135</v>
-      </c>
-      <c r="B11" s="81"/>
-      <c r="C11" s="82"/>
-      <c r="D11" s="81"/>
-      <c r="E11" s="83"/>
-      <c r="F11" s="83"/>
-      <c r="G11" s="81"/>
+      <c r="A11" s="52" t="s">
+        <v>147</v>
+      </c>
+      <c r="B11" s="93"/>
+      <c r="C11" s="94"/>
+      <c r="D11" s="93"/>
+      <c r="E11" s="95"/>
+      <c r="F11" s="95"/>
+      <c r="G11" s="93"/>
     </row>
     <row r="12" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="48" t="s">
-        <v>136</v>
-      </c>
-      <c r="D12" s="50"/>
+      <c r="A12" s="52" t="s">
+        <v>148</v>
+      </c>
+      <c r="D12" s="54"/>
     </row>
     <row r="13" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="48" t="s">
-        <v>137</v>
-      </c>
-      <c r="D13" s="50"/>
+      <c r="A13" s="52" t="s">
+        <v>149</v>
+      </c>
+      <c r="D13" s="54"/>
     </row>
     <row r="14" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="48" t="s">
-        <v>138</v>
-      </c>
-      <c r="D14" s="50"/>
+      <c r="A14" s="52" t="s">
+        <v>150</v>
+      </c>
+      <c r="D14" s="54"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1718,383 +1670,383 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:Q30"/>
+  <dimension ref="A1:Q31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="H1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="A17" sqref="A17"/>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="46.88671875" style="19" bestFit="1" customWidth="1"/>
-    <col min="2" max="15" width="24.33203125" style="21" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="24" style="20" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="22.33203125" style="20" customWidth="1"/>
+    <col min="2" max="15" width="24.33203125" style="90" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="24" style="91" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="22.33203125" style="91" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="54"/>
-      <c r="B1" s="55" t="s">
+      <c r="A1" s="58"/>
+      <c r="B1" s="59" t="s">
         <v>54</v>
       </c>
-      <c r="C1" s="55"/>
-      <c r="D1" s="55"/>
-      <c r="E1" s="55"/>
-      <c r="F1" s="55"/>
-      <c r="G1" s="55"/>
-      <c r="H1" s="55"/>
-      <c r="I1" s="55"/>
-      <c r="J1" s="55"/>
-      <c r="K1" s="56"/>
-      <c r="L1" s="57"/>
-      <c r="M1" s="57"/>
-      <c r="N1" s="57"/>
-      <c r="O1" s="57"/>
-      <c r="P1" s="58"/>
-      <c r="Q1" s="59"/>
+      <c r="C1" s="59"/>
+      <c r="D1" s="59"/>
+      <c r="E1" s="59"/>
+      <c r="F1" s="59"/>
+      <c r="G1" s="59"/>
+      <c r="H1" s="59"/>
+      <c r="I1" s="59"/>
+      <c r="J1" s="59"/>
+      <c r="K1" s="60"/>
+      <c r="L1" s="61"/>
+      <c r="M1" s="61"/>
+      <c r="N1" s="61"/>
+      <c r="O1" s="61"/>
+      <c r="P1" s="44"/>
+      <c r="Q1" s="40"/>
     </row>
     <row r="2" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="30" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="60" t="s">
+      <c r="B2" s="62" t="s">
         <v>68</v>
       </c>
-      <c r="C2" s="60" t="s">
+      <c r="C2" s="62" t="s">
         <v>69</v>
       </c>
-      <c r="D2" s="60" t="s">
+      <c r="D2" s="62" t="s">
         <v>69</v>
       </c>
-      <c r="E2" s="60" t="s">
+      <c r="E2" s="62" t="s">
         <v>70</v>
       </c>
-      <c r="F2" s="60" t="s">
+      <c r="F2" s="62" t="s">
         <v>71</v>
       </c>
-      <c r="G2" s="60" t="s">
+      <c r="G2" s="62" t="s">
         <v>70</v>
       </c>
-      <c r="H2" s="60" t="s">
+      <c r="H2" s="62" t="s">
         <v>71</v>
       </c>
-      <c r="I2" s="60" t="s">
+      <c r="I2" s="62" t="s">
         <v>72</v>
       </c>
-      <c r="J2" s="60" t="s">
+      <c r="J2" s="62" t="s">
         <v>73</v>
       </c>
-      <c r="K2" s="60" t="s">
+      <c r="K2" s="62" t="s">
         <v>74</v>
       </c>
-      <c r="L2" s="60" t="s">
+      <c r="L2" s="62" t="s">
         <v>75</v>
       </c>
-      <c r="M2" s="60" t="s">
+      <c r="M2" s="62" t="s">
         <v>76</v>
       </c>
-      <c r="N2" s="60" t="s">
+      <c r="N2" s="62" t="s">
         <v>77</v>
       </c>
-      <c r="O2" s="60" t="s">
+      <c r="O2" s="62" t="s">
         <v>78</v>
       </c>
-      <c r="P2" s="61" t="s">
+      <c r="P2" s="63" t="s">
         <v>79</v>
       </c>
-      <c r="Q2" s="61" t="s">
+      <c r="Q2" s="63" t="s">
         <v>80</v>
       </c>
     </row>
     <row r="3" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="62" t="s">
+      <c r="A3" s="64" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="63">
+      <c r="B3" s="65">
         <v>90.41</v>
       </c>
-      <c r="C3" s="63">
+      <c r="C3" s="65">
         <v>90.41</v>
       </c>
-      <c r="D3" s="63">
+      <c r="D3" s="65">
         <v>90.41</v>
       </c>
-      <c r="E3" s="63">
+      <c r="E3" s="65">
         <v>90.41</v>
       </c>
-      <c r="F3" s="63">
+      <c r="F3" s="65">
         <v>90.41</v>
       </c>
-      <c r="G3" s="63">
+      <c r="G3" s="65">
         <v>90.41</v>
       </c>
-      <c r="H3" s="63">
+      <c r="H3" s="65">
         <v>90.41</v>
       </c>
-      <c r="I3" s="63">
+      <c r="I3" s="65">
         <v>89.94</v>
       </c>
-      <c r="J3" s="63">
+      <c r="J3" s="65">
         <v>89.94</v>
       </c>
-      <c r="K3" s="63">
+      <c r="K3" s="65">
         <v>89.94</v>
       </c>
-      <c r="L3" s="63">
+      <c r="L3" s="65">
         <v>89.94</v>
       </c>
-      <c r="M3" s="63">
+      <c r="M3" s="65">
         <v>89.94</v>
       </c>
-      <c r="N3" s="63">
+      <c r="N3" s="65">
         <v>89.94</v>
       </c>
-      <c r="O3" s="63">
+      <c r="O3" s="65">
         <v>90.41</v>
       </c>
-      <c r="P3" s="63">
+      <c r="P3" s="65">
         <v>89.42</v>
       </c>
-      <c r="Q3" s="63">
+      <c r="Q3" s="65">
         <v>90.37</v>
       </c>
     </row>
     <row r="4" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="62" t="s">
+      <c r="A4" s="64" t="s">
         <v>41</v>
       </c>
-      <c r="B4" s="63">
+      <c r="B4" s="65">
         <v>24.1</v>
       </c>
-      <c r="C4" s="63">
+      <c r="C4" s="65">
         <v>24.1</v>
       </c>
-      <c r="D4" s="63">
+      <c r="D4" s="65">
         <v>24.1</v>
       </c>
-      <c r="E4" s="63">
+      <c r="E4" s="65">
         <v>24.1</v>
       </c>
-      <c r="F4" s="63">
+      <c r="F4" s="65">
         <v>24.1</v>
       </c>
-      <c r="G4" s="63">
+      <c r="G4" s="65">
         <v>24.1</v>
       </c>
-      <c r="H4" s="63">
+      <c r="H4" s="65">
         <v>24.1</v>
       </c>
-      <c r="I4" s="63">
+      <c r="I4" s="65">
         <v>24.92</v>
       </c>
-      <c r="J4" s="63">
+      <c r="J4" s="65">
         <v>24.92</v>
       </c>
-      <c r="K4" s="63">
+      <c r="K4" s="65">
         <v>24.92</v>
       </c>
-      <c r="L4" s="63">
+      <c r="L4" s="65">
         <v>24.92</v>
       </c>
-      <c r="M4" s="63">
+      <c r="M4" s="65">
         <v>24.92</v>
       </c>
-      <c r="N4" s="63">
+      <c r="N4" s="65">
         <v>24.92</v>
       </c>
-      <c r="O4" s="63">
+      <c r="O4" s="65">
         <v>24.1</v>
       </c>
-      <c r="P4" s="63">
+      <c r="P4" s="65">
         <v>23.49</v>
       </c>
-      <c r="Q4" s="63">
+      <c r="Q4" s="65">
         <v>22.7</v>
       </c>
     </row>
     <row r="5" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="62" t="s">
+      <c r="A5" s="64" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="64">
+      <c r="B5" s="66">
         <v>40179</v>
       </c>
-      <c r="C5" s="64">
+      <c r="C5" s="66">
         <v>40179</v>
       </c>
-      <c r="D5" s="64">
+      <c r="D5" s="66">
         <v>40179</v>
       </c>
-      <c r="E5" s="64">
+      <c r="E5" s="66">
         <v>40179</v>
       </c>
-      <c r="F5" s="64">
+      <c r="F5" s="66">
         <v>40179</v>
       </c>
-      <c r="G5" s="64">
+      <c r="G5" s="66">
         <v>40179</v>
       </c>
-      <c r="H5" s="64">
+      <c r="H5" s="66">
         <v>40179</v>
       </c>
-      <c r="I5" s="64">
+      <c r="I5" s="66">
         <v>40179</v>
       </c>
-      <c r="J5" s="64">
+      <c r="J5" s="66">
         <v>40179</v>
       </c>
-      <c r="K5" s="64">
+      <c r="K5" s="66">
         <v>40179</v>
       </c>
-      <c r="L5" s="64">
+      <c r="L5" s="66">
         <v>40179</v>
       </c>
-      <c r="M5" s="64">
+      <c r="M5" s="66">
         <v>40179</v>
       </c>
-      <c r="N5" s="64">
+      <c r="N5" s="66">
         <v>40179</v>
       </c>
-      <c r="O5" s="64">
+      <c r="O5" s="66">
         <v>40179</v>
       </c>
-      <c r="P5" s="64">
+      <c r="P5" s="66">
         <v>40179</v>
       </c>
-      <c r="Q5" s="64">
+      <c r="Q5" s="66">
         <v>40179</v>
       </c>
     </row>
     <row r="6" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="62" t="s">
+      <c r="A6" s="64" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="64">
+      <c r="B6" s="66">
         <v>41639</v>
       </c>
-      <c r="C6" s="64">
+      <c r="C6" s="66">
         <v>41639</v>
       </c>
-      <c r="D6" s="64">
+      <c r="D6" s="66">
         <v>41639</v>
       </c>
-      <c r="E6" s="64">
+      <c r="E6" s="66">
         <v>41639</v>
       </c>
-      <c r="F6" s="64">
+      <c r="F6" s="66">
         <v>41639</v>
       </c>
-      <c r="G6" s="64">
+      <c r="G6" s="66">
         <v>41639</v>
       </c>
-      <c r="H6" s="64">
+      <c r="H6" s="66">
         <v>41639</v>
       </c>
-      <c r="I6" s="64">
+      <c r="I6" s="66">
         <v>41639</v>
       </c>
-      <c r="J6" s="64">
+      <c r="J6" s="66">
         <v>41639</v>
       </c>
-      <c r="K6" s="64">
+      <c r="K6" s="66">
         <v>41639</v>
       </c>
-      <c r="L6" s="64">
+      <c r="L6" s="66">
         <v>41639</v>
       </c>
-      <c r="M6" s="64">
+      <c r="M6" s="66">
         <v>41639</v>
       </c>
-      <c r="N6" s="64">
+      <c r="N6" s="66">
         <v>41639</v>
       </c>
-      <c r="O6" s="64">
+      <c r="O6" s="66">
         <v>41639</v>
       </c>
-      <c r="P6" s="64">
+      <c r="P6" s="66">
         <v>41639</v>
       </c>
-      <c r="Q6" s="64">
+      <c r="Q6" s="66">
         <v>41639</v>
       </c>
     </row>
     <row r="7" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="62" t="s">
+      <c r="A7" s="64" t="s">
         <v>9</v>
       </c>
-      <c r="B7" s="65">
+      <c r="B7" s="67">
         <v>41086</v>
       </c>
-      <c r="C7" s="66">
+      <c r="C7" s="68">
         <v>41086</v>
       </c>
-      <c r="D7" s="66">
+      <c r="D7" s="68">
         <v>41086</v>
       </c>
-      <c r="E7" s="66">
+      <c r="E7" s="68">
         <v>40881</v>
       </c>
-      <c r="F7" s="66">
+      <c r="F7" s="68">
         <v>40881</v>
       </c>
-      <c r="G7" s="66">
+      <c r="G7" s="68">
         <v>40881</v>
       </c>
-      <c r="H7" s="66">
+      <c r="H7" s="68">
         <v>40881</v>
       </c>
-      <c r="I7" s="67">
+      <c r="I7" s="69">
         <v>40486</v>
       </c>
-      <c r="J7" s="67">
+      <c r="J7" s="69">
         <v>40486</v>
       </c>
-      <c r="K7" s="66">
+      <c r="K7" s="68">
         <v>41230</v>
       </c>
-      <c r="L7" s="66">
+      <c r="L7" s="68">
         <v>41230</v>
       </c>
-      <c r="M7" s="66">
+      <c r="M7" s="68">
         <v>40462</v>
       </c>
-      <c r="N7" s="66">
+      <c r="N7" s="68">
         <v>40462</v>
       </c>
-      <c r="O7" s="66">
+      <c r="O7" s="68">
         <v>38679</v>
       </c>
-      <c r="P7" s="66">
+      <c r="P7" s="68">
         <v>38381</v>
       </c>
-      <c r="Q7" s="66">
+      <c r="Q7" s="68">
         <v>38387</v>
       </c>
     </row>
     <row r="8" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="62" t="s">
+      <c r="A8" s="64" t="s">
         <v>10</v>
       </c>
-      <c r="B8" s="68" t="s">
+      <c r="B8" s="70" t="s">
         <v>42</v>
       </c>
-      <c r="C8" s="68" t="s">
+      <c r="C8" s="70" t="s">
         <v>42</v>
       </c>
-      <c r="D8" s="68" t="s">
+      <c r="D8" s="70" t="s">
         <v>42</v>
       </c>
-      <c r="E8" s="68" t="s">
+      <c r="E8" s="70" t="s">
         <v>42</v>
       </c>
-      <c r="F8" s="68" t="s">
+      <c r="F8" s="70" t="s">
         <v>42</v>
       </c>
-      <c r="G8" s="68" t="s">
+      <c r="G8" s="70" t="s">
         <v>42</v>
       </c>
-      <c r="H8" s="68" t="s">
+      <c r="H8" s="70" t="s">
         <v>42</v>
       </c>
       <c r="I8" s="35" t="s">
@@ -2103,1155 +2055,1208 @@
       <c r="J8" s="35" t="s">
         <v>28</v>
       </c>
-      <c r="K8" s="68" t="s">
+      <c r="K8" s="70" t="s">
         <v>28</v>
       </c>
-      <c r="L8" s="68" t="s">
+      <c r="L8" s="70" t="s">
         <v>28</v>
       </c>
-      <c r="M8" s="68" t="s">
+      <c r="M8" s="70" t="s">
         <v>28</v>
       </c>
-      <c r="N8" s="68" t="s">
+      <c r="N8" s="70" t="s">
         <v>28</v>
       </c>
-      <c r="O8" s="68" t="s">
+      <c r="O8" s="70" t="s">
         <v>42</v>
       </c>
-      <c r="P8" s="69" t="s">
+      <c r="P8" s="71" t="s">
         <v>42</v>
       </c>
-      <c r="Q8" s="69" t="s">
+      <c r="Q8" s="71" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="9" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="62" t="s">
+      <c r="A9" s="64" t="s">
         <v>12</v>
       </c>
-      <c r="B9" s="70">
+      <c r="B9" s="72">
         <v>60</v>
       </c>
-      <c r="C9" s="70">
+      <c r="C9" s="72">
         <v>60</v>
       </c>
-      <c r="D9" s="70">
+      <c r="D9" s="72">
         <v>60</v>
       </c>
-      <c r="E9" s="70">
+      <c r="E9" s="72">
         <v>60</v>
       </c>
-      <c r="F9" s="70">
+      <c r="F9" s="72">
         <v>60</v>
       </c>
-      <c r="G9" s="70">
+      <c r="G9" s="72">
         <v>60</v>
       </c>
-      <c r="H9" s="70">
+      <c r="H9" s="72">
         <v>60</v>
       </c>
-      <c r="I9" s="70">
+      <c r="I9" s="72">
         <v>60</v>
       </c>
-      <c r="J9" s="70">
+      <c r="J9" s="72">
         <v>60</v>
       </c>
-      <c r="K9" s="70">
+      <c r="K9" s="72">
         <v>60</v>
       </c>
-      <c r="L9" s="70">
+      <c r="L9" s="72">
         <v>60</v>
       </c>
-      <c r="M9" s="70">
+      <c r="M9" s="72">
         <v>60</v>
       </c>
-      <c r="N9" s="70">
+      <c r="N9" s="72">
         <v>60</v>
       </c>
-      <c r="O9" s="70">
+      <c r="O9" s="72">
         <v>100</v>
       </c>
-      <c r="P9" s="71">
+      <c r="P9" s="73">
         <v>100</v>
       </c>
-      <c r="Q9" s="72">
+      <c r="Q9" s="74">
         <v>100</v>
       </c>
     </row>
     <row r="10" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="62" t="s">
+      <c r="A10" s="64" t="s">
         <v>13</v>
       </c>
-      <c r="B10" s="70" t="s">
+      <c r="B10" s="72" t="s">
         <v>81</v>
       </c>
-      <c r="C10" s="70" t="s">
+      <c r="C10" s="72" t="s">
         <v>81</v>
       </c>
-      <c r="D10" s="70" t="s">
+      <c r="D10" s="72" t="s">
         <v>81</v>
       </c>
-      <c r="E10" s="70" t="s">
+      <c r="E10" s="72" t="s">
         <v>81</v>
       </c>
-      <c r="F10" s="70" t="s">
+      <c r="F10" s="72" t="s">
         <v>81</v>
       </c>
-      <c r="G10" s="70" t="s">
+      <c r="G10" s="72" t="s">
         <v>81</v>
       </c>
-      <c r="H10" s="70" t="s">
+      <c r="H10" s="72" t="s">
         <v>81</v>
       </c>
-      <c r="I10" s="70" t="s">
+      <c r="I10" s="72" t="s">
         <v>81</v>
       </c>
-      <c r="J10" s="70" t="s">
+      <c r="J10" s="72" t="s">
         <v>81</v>
       </c>
-      <c r="K10" s="70" t="s">
+      <c r="K10" s="72" t="s">
         <v>81</v>
       </c>
-      <c r="L10" s="70" t="s">
+      <c r="L10" s="72" t="s">
         <v>81</v>
       </c>
-      <c r="M10" s="70" t="s">
+      <c r="M10" s="72" t="s">
         <v>81</v>
       </c>
-      <c r="N10" s="70" t="s">
+      <c r="N10" s="72" t="s">
         <v>81</v>
       </c>
-      <c r="O10" s="70">
+      <c r="O10" s="72">
         <v>26</v>
       </c>
-      <c r="P10" s="73">
+      <c r="P10" s="75">
         <v>50</v>
       </c>
-      <c r="Q10" s="70">
+      <c r="Q10" s="72">
         <v>41</v>
       </c>
     </row>
     <row r="11" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="62" t="s">
+      <c r="A11" s="64" t="s">
         <v>14</v>
       </c>
-      <c r="B11" s="68" t="s">
+      <c r="B11" s="70" t="s">
         <v>82</v>
       </c>
-      <c r="C11" s="68" t="s">
+      <c r="C11" s="70" t="s">
         <v>82</v>
       </c>
-      <c r="D11" s="68" t="s">
+      <c r="D11" s="70" t="s">
         <v>82</v>
       </c>
-      <c r="E11" s="68" t="s">
+      <c r="E11" s="70" t="s">
         <v>82</v>
       </c>
-      <c r="F11" s="68" t="s">
+      <c r="F11" s="70" t="s">
         <v>82</v>
       </c>
-      <c r="G11" s="68" t="s">
+      <c r="G11" s="70" t="s">
         <v>82</v>
       </c>
-      <c r="H11" s="68" t="s">
+      <c r="H11" s="70" t="s">
         <v>82</v>
       </c>
-      <c r="I11" s="68" t="s">
+      <c r="I11" s="70" t="s">
         <v>82</v>
       </c>
-      <c r="J11" s="68" t="s">
+      <c r="J11" s="70" t="s">
         <v>82</v>
       </c>
-      <c r="K11" s="68" t="s">
+      <c r="K11" s="70" t="s">
         <v>82</v>
       </c>
-      <c r="L11" s="68" t="s">
+      <c r="L11" s="70" t="s">
         <v>82</v>
       </c>
-      <c r="M11" s="68" t="s">
+      <c r="M11" s="70" t="s">
         <v>82</v>
       </c>
-      <c r="N11" s="68" t="s">
+      <c r="N11" s="70" t="s">
         <v>82</v>
       </c>
-      <c r="O11" s="68" t="s">
+      <c r="O11" s="70" t="s">
         <v>44</v>
       </c>
-      <c r="P11" s="69" t="s">
+      <c r="P11" s="71" t="s">
         <v>83</v>
       </c>
-      <c r="Q11" s="69" t="s">
+      <c r="Q11" s="71" t="s">
         <v>83</v>
       </c>
     </row>
     <row r="12" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="62" t="s">
+      <c r="A12" s="64" t="s">
         <v>16</v>
       </c>
-      <c r="B12" s="63">
+      <c r="B12" s="65">
         <v>31.86</v>
       </c>
-      <c r="C12" s="63">
+      <c r="C12" s="65">
         <v>33.729999999999997</v>
       </c>
-      <c r="D12" s="63">
+      <c r="D12" s="65">
         <v>35.28</v>
       </c>
-      <c r="E12" s="63">
+      <c r="E12" s="65">
         <v>62.95</v>
       </c>
-      <c r="F12" s="63">
+      <c r="F12" s="65">
         <v>53.52</v>
       </c>
-      <c r="G12" s="63">
+      <c r="G12" s="65">
         <v>39.92</v>
       </c>
-      <c r="H12" s="63">
+      <c r="H12" s="65">
         <v>30.53</v>
       </c>
-      <c r="I12" s="63">
+      <c r="I12" s="65">
         <v>35.64</v>
       </c>
-      <c r="J12" s="63">
+      <c r="J12" s="65">
         <v>33.83</v>
       </c>
-      <c r="K12" s="63">
+      <c r="K12" s="65">
         <v>27.29</v>
       </c>
-      <c r="L12" s="63">
+      <c r="L12" s="65">
         <v>25.82</v>
       </c>
-      <c r="M12" s="63">
+      <c r="M12" s="65">
         <v>35.18</v>
       </c>
-      <c r="N12" s="63">
+      <c r="N12" s="65">
         <v>32.659999999999997</v>
       </c>
-      <c r="O12" s="70">
+      <c r="O12" s="72">
         <v>3</v>
       </c>
-      <c r="P12" s="63">
+      <c r="P12" s="65">
         <v>2.5</v>
       </c>
-      <c r="Q12" s="63">
+      <c r="Q12" s="65">
         <v>3.4</v>
       </c>
     </row>
     <row r="13" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="62" t="s">
+      <c r="A13" s="64" t="s">
         <v>17</v>
       </c>
-      <c r="B13" s="70">
+      <c r="B13" s="72">
         <v>429</v>
       </c>
-      <c r="C13" s="70">
+      <c r="C13" s="72">
         <v>225</v>
       </c>
-      <c r="D13" s="70">
+      <c r="D13" s="72">
         <v>212</v>
       </c>
-      <c r="E13" s="70">
+      <c r="E13" s="72">
         <v>254</v>
       </c>
-      <c r="F13" s="70">
+      <c r="F13" s="72">
         <v>590</v>
       </c>
-      <c r="G13" s="70">
+      <c r="G13" s="72">
         <v>335</v>
       </c>
-      <c r="H13" s="70">
+      <c r="H13" s="72">
         <v>610</v>
       </c>
-      <c r="I13" s="70">
+      <c r="I13" s="72">
         <v>249</v>
       </c>
-      <c r="J13" s="70">
+      <c r="J13" s="72">
         <v>568</v>
       </c>
-      <c r="K13" s="70">
+      <c r="K13" s="72">
         <v>228</v>
       </c>
-      <c r="L13" s="70">
+      <c r="L13" s="72">
         <v>453</v>
       </c>
-      <c r="M13" s="68" t="s">
+      <c r="M13" s="70" t="s">
         <v>84</v>
       </c>
-      <c r="N13" s="68" t="s">
+      <c r="N13" s="70" t="s">
         <v>85</v>
       </c>
-      <c r="O13" s="70">
+      <c r="O13" s="72">
         <v>430</v>
       </c>
-      <c r="P13" s="70">
+      <c r="P13" s="72">
         <v>1324</v>
       </c>
-      <c r="Q13" s="70">
+      <c r="Q13" s="72">
         <v>1252</v>
       </c>
     </row>
     <row r="14" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="95" t="s">
-        <v>146</v>
-      </c>
-      <c r="B14" s="92">
+      <c r="A14" s="51" t="s">
+        <v>86</v>
+      </c>
+      <c r="B14" s="76" t="b">
+        <v>0</v>
+      </c>
+      <c r="C14" s="76" t="b">
+        <v>0</v>
+      </c>
+      <c r="D14" s="76" t="b">
+        <v>0</v>
+      </c>
+      <c r="E14" s="76" t="b">
+        <v>0</v>
+      </c>
+      <c r="F14" s="76" t="b">
+        <v>0</v>
+      </c>
+      <c r="G14" s="76" t="b">
+        <v>0</v>
+      </c>
+      <c r="H14" s="76" t="b">
+        <v>0</v>
+      </c>
+      <c r="I14" s="76" t="b">
+        <v>0</v>
+      </c>
+      <c r="J14" s="76" t="b">
+        <v>0</v>
+      </c>
+      <c r="K14" s="76" t="b">
+        <v>0</v>
+      </c>
+      <c r="L14" s="76" t="b">
+        <v>0</v>
+      </c>
+      <c r="M14" s="76" t="b">
+        <v>0</v>
+      </c>
+      <c r="N14" s="76" t="b">
+        <v>0</v>
+      </c>
+      <c r="O14" s="76" t="b">
+        <v>0</v>
+      </c>
+      <c r="P14" s="76" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q14" s="76" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="77" t="s">
+        <v>87</v>
+      </c>
+      <c r="B15" s="78">
         <v>111</v>
       </c>
-      <c r="C14" s="92">
+      <c r="C15" s="78">
         <v>111</v>
       </c>
-      <c r="D14" s="92">
+      <c r="D15" s="78">
         <v>111</v>
       </c>
-      <c r="E14" s="92">
+      <c r="E15" s="78">
         <v>111</v>
       </c>
-      <c r="F14" s="92">
+      <c r="F15" s="78">
         <v>111</v>
       </c>
-      <c r="G14" s="92">
+      <c r="G15" s="78">
         <v>111</v>
       </c>
-      <c r="H14" s="92">
+      <c r="H15" s="78">
         <v>111</v>
       </c>
-      <c r="I14" s="92">
+      <c r="I15" s="78">
         <v>112</v>
       </c>
-      <c r="J14" s="92">
+      <c r="J15" s="78">
         <v>112</v>
       </c>
-      <c r="K14" s="92">
+      <c r="K15" s="78">
         <v>112</v>
       </c>
-      <c r="L14" s="92">
+      <c r="L15" s="78">
         <v>112</v>
       </c>
-      <c r="M14" s="92">
+      <c r="M15" s="78">
         <v>111</v>
       </c>
-      <c r="N14" s="92">
+      <c r="N15" s="78">
         <v>111</v>
       </c>
-      <c r="O14" s="92">
+      <c r="O15" s="78">
         <v>111</v>
       </c>
-      <c r="P14" s="92">
+      <c r="P15" s="78">
         <v>169</v>
       </c>
-      <c r="Q14" s="92">
+      <c r="Q15" s="78">
         <v>240</v>
       </c>
     </row>
-    <row r="15" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="95" t="s">
+    <row r="16" spans="1:17" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="77" t="s">
+        <v>88</v>
+      </c>
+      <c r="B16" s="78">
+        <v>61.24</v>
+      </c>
+      <c r="C16" s="78">
+        <v>61.24</v>
+      </c>
+      <c r="D16" s="78">
+        <v>61.24</v>
+      </c>
+      <c r="E16" s="78">
+        <v>61.24</v>
+      </c>
+      <c r="F16" s="78">
+        <v>61.24</v>
+      </c>
+      <c r="G16" s="79">
+        <v>61.24</v>
+      </c>
+      <c r="H16" s="79">
+        <v>61.24</v>
+      </c>
+      <c r="I16" s="78">
+        <v>74</v>
+      </c>
+      <c r="J16" s="78">
+        <v>74</v>
+      </c>
+      <c r="K16" s="78">
+        <v>74</v>
+      </c>
+      <c r="L16" s="78">
+        <v>74</v>
+      </c>
+      <c r="M16" s="79">
+        <v>61.24</v>
+      </c>
+      <c r="N16" s="79">
+        <v>61.24</v>
+      </c>
+      <c r="O16" s="79">
+        <v>61.24</v>
+      </c>
+      <c r="P16" s="78">
+        <v>110</v>
+      </c>
+      <c r="Q16" s="78">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="17" spans="1:17" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="77" t="s">
+        <v>89</v>
+      </c>
+      <c r="B17" s="78">
+        <v>4</v>
+      </c>
+      <c r="C17" s="78">
+        <v>4</v>
+      </c>
+      <c r="D17" s="78">
+        <v>4</v>
+      </c>
+      <c r="E17" s="78">
+        <v>4</v>
+      </c>
+      <c r="F17" s="78">
+        <v>4</v>
+      </c>
+      <c r="G17" s="78">
+        <v>4</v>
+      </c>
+      <c r="H17" s="78">
+        <v>4</v>
+      </c>
+      <c r="I17" s="78">
+        <v>4</v>
+      </c>
+      <c r="J17" s="78">
+        <v>4</v>
+      </c>
+      <c r="K17" s="78">
+        <v>4</v>
+      </c>
+      <c r="L17" s="78">
+        <v>4</v>
+      </c>
+      <c r="M17" s="78">
+        <v>4</v>
+      </c>
+      <c r="N17" s="78">
+        <v>4</v>
+      </c>
+      <c r="O17" s="78">
+        <v>4</v>
+      </c>
+      <c r="P17" s="78">
+        <v>4</v>
+      </c>
+      <c r="Q17" s="78">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="18" spans="1:17" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="77" t="s">
+        <v>90</v>
+      </c>
+      <c r="B18" s="78">
+        <v>1</v>
+      </c>
+      <c r="C18" s="78">
+        <v>1</v>
+      </c>
+      <c r="D18" s="78">
+        <v>1</v>
+      </c>
+      <c r="E18" s="78">
+        <v>1</v>
+      </c>
+      <c r="F18" s="78">
+        <v>1</v>
+      </c>
+      <c r="G18" s="78">
+        <v>1</v>
+      </c>
+      <c r="H18" s="78">
+        <v>1</v>
+      </c>
+      <c r="I18" s="78">
+        <v>1</v>
+      </c>
+      <c r="J18" s="78">
+        <v>1</v>
+      </c>
+      <c r="K18" s="78">
+        <v>1</v>
+      </c>
+      <c r="L18" s="78">
+        <v>1</v>
+      </c>
+      <c r="M18" s="78">
+        <v>1</v>
+      </c>
+      <c r="N18" s="78">
+        <v>1</v>
+      </c>
+      <c r="O18" s="78">
+        <v>1</v>
+      </c>
+      <c r="P18" s="78">
+        <v>1</v>
+      </c>
+      <c r="Q18" s="78">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:17" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="77" t="s">
+        <v>91</v>
+      </c>
+      <c r="B19" s="78" t="s">
+        <v>92</v>
+      </c>
+      <c r="C19" s="78" t="s">
+        <v>92</v>
+      </c>
+      <c r="D19" s="78" t="s">
+        <v>92</v>
+      </c>
+      <c r="E19" s="78" t="s">
+        <v>92</v>
+      </c>
+      <c r="F19" s="78" t="s">
+        <v>92</v>
+      </c>
+      <c r="G19" s="78" t="s">
+        <v>92</v>
+      </c>
+      <c r="H19" s="78" t="s">
+        <v>92</v>
+      </c>
+      <c r="I19" s="78" t="s">
+        <v>92</v>
+      </c>
+      <c r="J19" s="78" t="s">
+        <v>92</v>
+      </c>
+      <c r="K19" s="78" t="s">
+        <v>92</v>
+      </c>
+      <c r="L19" s="78" t="s">
+        <v>92</v>
+      </c>
+      <c r="M19" s="78" t="s">
+        <v>92</v>
+      </c>
+      <c r="N19" s="78" t="s">
+        <v>92</v>
+      </c>
+      <c r="O19" s="78" t="s">
+        <v>92</v>
+      </c>
+      <c r="P19" s="79" t="s">
+        <v>92</v>
+      </c>
+      <c r="Q19" s="79" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="20" spans="1:17" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="77" t="s">
+        <v>93</v>
+      </c>
+      <c r="B20" s="78" t="s">
+        <v>94</v>
+      </c>
+      <c r="C20" s="78" t="s">
+        <v>94</v>
+      </c>
+      <c r="D20" s="78" t="s">
+        <v>94</v>
+      </c>
+      <c r="E20" s="78" t="s">
+        <v>94</v>
+      </c>
+      <c r="F20" s="78" t="s">
+        <v>94</v>
+      </c>
+      <c r="G20" s="78" t="s">
+        <v>94</v>
+      </c>
+      <c r="H20" s="78" t="s">
+        <v>94</v>
+      </c>
+      <c r="I20" s="78" t="s">
+        <v>94</v>
+      </c>
+      <c r="J20" s="78" t="s">
+        <v>94</v>
+      </c>
+      <c r="K20" s="78" t="s">
+        <v>94</v>
+      </c>
+      <c r="L20" s="78" t="s">
+        <v>94</v>
+      </c>
+      <c r="M20" s="78" t="s">
+        <v>94</v>
+      </c>
+      <c r="N20" s="78" t="s">
+        <v>94</v>
+      </c>
+      <c r="O20" s="78" t="s">
+        <v>94</v>
+      </c>
+      <c r="P20" s="79" t="s">
+        <v>94</v>
+      </c>
+      <c r="Q20" s="79" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="21" spans="1:17" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="77" t="s">
+        <v>95</v>
+      </c>
+      <c r="B21" s="80">
+        <v>33.5</v>
+      </c>
+      <c r="C21" s="80">
+        <v>33.5</v>
+      </c>
+      <c r="D21" s="80">
+        <v>33.5</v>
+      </c>
+      <c r="E21" s="80">
+        <v>33.5</v>
+      </c>
+      <c r="F21" s="80">
+        <v>33.5</v>
+      </c>
+      <c r="G21" s="80">
+        <v>33.5</v>
+      </c>
+      <c r="H21" s="80">
+        <v>33.5</v>
+      </c>
+      <c r="I21" s="78">
+        <v>24</v>
+      </c>
+      <c r="J21" s="78">
+        <v>24</v>
+      </c>
+      <c r="K21" s="78">
+        <v>24</v>
+      </c>
+      <c r="L21" s="78">
+        <v>24</v>
+      </c>
+      <c r="M21" s="79">
+        <v>33.5</v>
+      </c>
+      <c r="N21" s="79">
+        <v>33.5</v>
+      </c>
+      <c r="O21" s="79">
+        <v>33.5</v>
+      </c>
+      <c r="P21" s="78">
+        <v>24</v>
+      </c>
+      <c r="Q21" s="78">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="22" spans="1:17" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="77" t="s">
+        <v>96</v>
+      </c>
+      <c r="B22" s="78">
+        <v>66</v>
+      </c>
+      <c r="C22" s="78">
+        <v>66</v>
+      </c>
+      <c r="D22" s="78">
+        <v>66</v>
+      </c>
+      <c r="E22" s="78">
+        <v>253</v>
+      </c>
+      <c r="F22" s="78">
+        <v>253</v>
+      </c>
+      <c r="G22" s="78">
+        <v>253</v>
+      </c>
+      <c r="H22" s="78">
+        <v>253</v>
+      </c>
+      <c r="I22" s="78">
+        <v>130</v>
+      </c>
+      <c r="J22" s="78">
+        <v>130</v>
+      </c>
+      <c r="K22" s="78">
+        <v>130</v>
+      </c>
+      <c r="L22" s="78">
+        <v>130</v>
+      </c>
+      <c r="M22" s="78">
+        <v>93</v>
+      </c>
+      <c r="N22" s="78">
+        <v>93</v>
+      </c>
+      <c r="O22" s="78">
+        <v>1250</v>
+      </c>
+      <c r="P22" s="78">
+        <v>426.5</v>
+      </c>
+      <c r="Q22" s="78">
+        <v>537.5</v>
+      </c>
+    </row>
+    <row r="23" spans="1:17" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="77" t="s">
+        <v>97</v>
+      </c>
+      <c r="B23" s="81">
+        <v>3.7999999999999999E-2</v>
+      </c>
+      <c r="C23" s="81">
+        <v>3.7999999999999999E-2</v>
+      </c>
+      <c r="D23" s="81">
+        <v>3.7999999999999999E-2</v>
+      </c>
+      <c r="E23" s="81">
+        <v>3.7999999999999999E-2</v>
+      </c>
+      <c r="F23" s="81">
+        <v>3.7999999999999999E-2</v>
+      </c>
+      <c r="G23" s="81">
+        <v>3.7999999999999999E-2</v>
+      </c>
+      <c r="H23" s="81">
+        <v>3.7999999999999999E-2</v>
+      </c>
+      <c r="I23" s="81">
+        <v>3.7999999999999999E-2</v>
+      </c>
+      <c r="J23" s="81">
+        <v>3.7999999999999999E-2</v>
+      </c>
+      <c r="K23" s="81">
+        <v>3.7999999999999999E-2</v>
+      </c>
+      <c r="L23" s="81">
+        <v>3.7999999999999999E-2</v>
+      </c>
+      <c r="M23" s="81">
+        <v>3.7999999999999999E-2</v>
+      </c>
+      <c r="N23" s="81">
+        <v>3.7999999999999999E-2</v>
+      </c>
+      <c r="O23" s="81">
+        <v>3.7999999999999999E-2</v>
+      </c>
+      <c r="P23" s="81">
+        <v>3.7999999999999999E-2</v>
+      </c>
+      <c r="Q23" s="81">
+        <v>3.7999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:17" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="77" t="s">
+        <v>98</v>
+      </c>
+      <c r="B24" s="78" t="s">
+        <v>99</v>
+      </c>
+      <c r="C24" s="78" t="s">
+        <v>99</v>
+      </c>
+      <c r="D24" s="78" t="s">
+        <v>99</v>
+      </c>
+      <c r="E24" s="78" t="s">
+        <v>99</v>
+      </c>
+      <c r="F24" s="78" t="s">
+        <v>99</v>
+      </c>
+      <c r="G24" s="78" t="s">
+        <v>99</v>
+      </c>
+      <c r="H24" s="78" t="s">
+        <v>99</v>
+      </c>
+      <c r="I24" s="78" t="s">
+        <v>99</v>
+      </c>
+      <c r="J24" s="78" t="s">
+        <v>99</v>
+      </c>
+      <c r="K24" s="78" t="s">
+        <v>99</v>
+      </c>
+      <c r="L24" s="78" t="s">
+        <v>99</v>
+      </c>
+      <c r="M24" s="78" t="s">
+        <v>99</v>
+      </c>
+      <c r="N24" s="78" t="s">
+        <v>99</v>
+      </c>
+      <c r="O24" s="78" t="s">
+        <v>99</v>
+      </c>
+      <c r="P24" s="79" t="s">
+        <v>99</v>
+      </c>
+      <c r="Q24" s="79" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="25" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="39"/>
+      <c r="B25" s="40"/>
+      <c r="C25" s="44"/>
+      <c r="D25" s="44"/>
+      <c r="E25" s="44"/>
+      <c r="F25" s="44"/>
+      <c r="G25" s="44"/>
+      <c r="H25" s="44"/>
+      <c r="I25" s="44"/>
+      <c r="J25" s="44"/>
+      <c r="K25" s="61"/>
+      <c r="L25" s="61"/>
+      <c r="M25" s="61"/>
+      <c r="N25" s="61"/>
+      <c r="O25" s="61"/>
+      <c r="P25" s="44"/>
+      <c r="Q25" s="40"/>
+    </row>
+    <row r="26" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="30" t="s">
+        <v>7</v>
+      </c>
+      <c r="B26" s="82">
+        <v>40548</v>
+      </c>
+      <c r="C26" s="82">
+        <v>40548</v>
+      </c>
+      <c r="D26" s="35" t="s">
+        <v>100</v>
+      </c>
+      <c r="E26" s="82">
+        <v>40553</v>
+      </c>
+      <c r="F26" s="82">
+        <v>40553</v>
+      </c>
+      <c r="G26" s="82">
+        <v>40918</v>
+      </c>
+      <c r="H26" s="82">
+        <v>40918</v>
+      </c>
+      <c r="I26" s="35" t="s">
+        <v>101</v>
+      </c>
+      <c r="J26" s="35" t="s">
+        <v>101</v>
+      </c>
+      <c r="K26" s="82">
+        <v>40544</v>
+      </c>
+      <c r="L26" s="82">
+        <v>40544</v>
+      </c>
+      <c r="M26" s="82">
+        <v>40179</v>
+      </c>
+      <c r="N26" s="82">
+        <v>40179</v>
+      </c>
+      <c r="O26" s="82">
+        <v>40544</v>
+      </c>
+      <c r="P26" s="82">
+        <v>40544</v>
+      </c>
+      <c r="Q26" s="82">
+        <v>40544</v>
+      </c>
+    </row>
+    <row r="27" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="64" t="s">
+        <v>8</v>
+      </c>
+      <c r="B27" s="83">
+        <v>40913</v>
+      </c>
+      <c r="C27" s="83">
+        <v>40913</v>
+      </c>
+      <c r="D27" s="70" t="s">
+        <v>102</v>
+      </c>
+      <c r="E27" s="70" t="s">
+        <v>103</v>
+      </c>
+      <c r="F27" s="70" t="s">
+        <v>103</v>
+      </c>
+      <c r="G27" s="70" t="s">
+        <v>104</v>
+      </c>
+      <c r="H27" s="70" t="s">
+        <v>104</v>
+      </c>
+      <c r="I27" s="70" t="s">
+        <v>105</v>
+      </c>
+      <c r="J27" s="70" t="s">
+        <v>105</v>
+      </c>
+      <c r="K27" s="70" t="s">
+        <v>106</v>
+      </c>
+      <c r="L27" s="70" t="s">
+        <v>106</v>
+      </c>
+      <c r="M27" s="70" t="s">
+        <v>107</v>
+      </c>
+      <c r="N27" s="70" t="s">
+        <v>107</v>
+      </c>
+      <c r="O27" s="70" t="s">
+        <v>107</v>
+      </c>
+      <c r="P27" s="71" t="s">
+        <v>107</v>
+      </c>
+      <c r="Q27" s="71" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="28" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="64" t="s">
+        <v>12</v>
+      </c>
+      <c r="B28" s="70" t="s">
+        <v>108</v>
+      </c>
+      <c r="C28" s="70" t="s">
+        <v>109</v>
+      </c>
+      <c r="D28" s="70" t="s">
+        <v>109</v>
+      </c>
+      <c r="E28" s="70" t="s">
+        <v>109</v>
+      </c>
+      <c r="F28" s="70" t="s">
+        <v>108</v>
+      </c>
+      <c r="G28" s="70" t="s">
+        <v>109</v>
+      </c>
+      <c r="H28" s="70" t="s">
+        <v>108</v>
+      </c>
+      <c r="I28" s="70" t="s">
+        <v>110</v>
+      </c>
+      <c r="J28" s="70" t="s">
+        <v>111</v>
+      </c>
+      <c r="K28" s="70" t="s">
+        <v>112</v>
+      </c>
+      <c r="L28" s="70" t="s">
+        <v>113</v>
+      </c>
+      <c r="M28" s="70" t="s">
+        <v>114</v>
+      </c>
+      <c r="N28" s="70" t="s">
+        <v>115</v>
+      </c>
+      <c r="O28" s="70" t="s">
+        <v>116</v>
+      </c>
+      <c r="P28" s="84">
+        <v>100</v>
+      </c>
+      <c r="Q28" s="85">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="29" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="64" t="s">
+        <v>13</v>
+      </c>
+      <c r="B29" s="72">
+        <v>26</v>
+      </c>
+      <c r="C29" s="72">
+        <v>26</v>
+      </c>
+      <c r="D29" s="72">
+        <v>26</v>
+      </c>
+      <c r="E29" s="72">
+        <v>26</v>
+      </c>
+      <c r="F29" s="72">
+        <v>26</v>
+      </c>
+      <c r="G29" s="72">
+        <v>26</v>
+      </c>
+      <c r="H29" s="72">
+        <v>26</v>
+      </c>
+      <c r="I29" s="70" t="s">
+        <v>18</v>
+      </c>
+      <c r="J29" s="70" t="s">
+        <v>18</v>
+      </c>
+      <c r="K29" s="83"/>
+      <c r="L29" s="70" t="s">
+        <v>18</v>
+      </c>
+      <c r="M29" s="70" t="s">
+        <v>18</v>
+      </c>
+      <c r="N29" s="70" t="s">
+        <v>18</v>
+      </c>
+      <c r="O29" s="70" t="s">
+        <v>18</v>
+      </c>
+      <c r="P29" s="86" t="s">
+        <v>117</v>
+      </c>
+      <c r="Q29" s="71" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="30" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="64" t="s">
+        <v>9</v>
+      </c>
+      <c r="B30" s="66">
+        <v>41086</v>
+      </c>
+      <c r="C30" s="70" t="s">
         <v>119</v>
       </c>
-      <c r="B15" s="92" t="s">
+      <c r="D30" s="70" t="s">
         <v>120</v>
       </c>
-      <c r="C15" s="92" t="s">
-        <v>120</v>
-      </c>
-      <c r="D15" s="92" t="s">
-        <v>120</v>
-      </c>
-      <c r="E15" s="92" t="s">
-        <v>120</v>
-      </c>
-      <c r="F15" s="92" t="s">
-        <v>120</v>
-      </c>
-      <c r="G15" s="92">
-        <v>61.24</v>
-      </c>
-      <c r="H15" s="92">
-        <v>61.24</v>
-      </c>
-      <c r="I15" s="92">
-        <v>74</v>
-      </c>
-      <c r="J15" s="92">
-        <v>74</v>
-      </c>
-      <c r="K15" s="92">
-        <v>74</v>
-      </c>
-      <c r="L15" s="92">
-        <v>74</v>
-      </c>
-      <c r="M15" s="92">
-        <v>61.24</v>
-      </c>
-      <c r="N15" s="92">
-        <v>61.24</v>
-      </c>
-      <c r="O15" s="92">
-        <v>61.24</v>
-      </c>
-      <c r="P15" s="92">
-        <v>110</v>
-      </c>
-      <c r="Q15" s="92">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="16" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="95" t="s">
-        <v>139</v>
-      </c>
-      <c r="B16" s="92">
-        <v>4</v>
-      </c>
-      <c r="C16" s="92">
-        <v>4</v>
-      </c>
-      <c r="D16" s="92">
-        <v>4</v>
-      </c>
-      <c r="E16" s="92">
-        <v>4</v>
-      </c>
-      <c r="F16" s="92">
-        <v>4</v>
-      </c>
-      <c r="G16" s="92">
-        <v>4</v>
-      </c>
-      <c r="H16" s="92">
-        <v>4</v>
-      </c>
-      <c r="I16" s="92">
-        <v>4</v>
-      </c>
-      <c r="J16" s="92">
-        <v>4</v>
-      </c>
-      <c r="K16" s="92">
-        <v>4</v>
-      </c>
-      <c r="L16" s="92">
-        <v>4</v>
-      </c>
-      <c r="M16" s="92">
-        <v>4</v>
-      </c>
-      <c r="N16" s="92">
-        <v>4</v>
-      </c>
-      <c r="O16" s="92">
-        <v>4</v>
-      </c>
-      <c r="P16" s="92">
-        <v>4</v>
-      </c>
-      <c r="Q16" s="92">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="17" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="95" t="s">
-        <v>140</v>
-      </c>
-      <c r="B17" s="92">
-        <v>1</v>
-      </c>
-      <c r="C17" s="92">
-        <v>1</v>
-      </c>
-      <c r="D17" s="92">
-        <v>1</v>
-      </c>
-      <c r="E17" s="92">
-        <v>1</v>
-      </c>
-      <c r="F17" s="92">
-        <v>1</v>
-      </c>
-      <c r="G17" s="92">
-        <v>1</v>
-      </c>
-      <c r="H17" s="92">
-        <v>1</v>
-      </c>
-      <c r="I17" s="92">
-        <v>1</v>
-      </c>
-      <c r="J17" s="92">
-        <v>1</v>
-      </c>
-      <c r="K17" s="92">
-        <v>1</v>
-      </c>
-      <c r="L17" s="92">
-        <v>1</v>
-      </c>
-      <c r="M17" s="92">
-        <v>1</v>
-      </c>
-      <c r="N17" s="92">
-        <v>1</v>
-      </c>
-      <c r="O17" s="92">
-        <v>1</v>
-      </c>
-      <c r="P17" s="92">
-        <v>1</v>
-      </c>
-      <c r="Q17" s="92">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="18" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="95" t="s">
-        <v>141</v>
-      </c>
-      <c r="B18" s="89" t="s">
-        <v>143</v>
-      </c>
-      <c r="C18" s="89" t="s">
-        <v>143</v>
-      </c>
-      <c r="D18" s="89" t="s">
-        <v>143</v>
-      </c>
-      <c r="E18" s="89" t="s">
-        <v>143</v>
-      </c>
-      <c r="F18" s="89" t="s">
-        <v>143</v>
-      </c>
-      <c r="G18" s="89" t="s">
-        <v>143</v>
-      </c>
-      <c r="H18" s="89" t="s">
-        <v>143</v>
-      </c>
-      <c r="I18" s="89" t="s">
-        <v>143</v>
-      </c>
-      <c r="J18" s="89" t="s">
-        <v>143</v>
-      </c>
-      <c r="K18" s="89" t="s">
-        <v>143</v>
-      </c>
-      <c r="L18" s="89" t="s">
-        <v>143</v>
-      </c>
-      <c r="M18" s="89" t="s">
-        <v>143</v>
-      </c>
-      <c r="N18" s="89" t="s">
-        <v>143</v>
-      </c>
-      <c r="O18" s="89" t="s">
-        <v>143</v>
-      </c>
-      <c r="P18" s="89" t="s">
-        <v>143</v>
-      </c>
-      <c r="Q18" s="89" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="19" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="95" t="s">
-        <v>142</v>
-      </c>
-      <c r="B19" s="89" t="s">
-        <v>144</v>
-      </c>
-      <c r="C19" s="89" t="s">
-        <v>144</v>
-      </c>
-      <c r="D19" s="89" t="s">
-        <v>144</v>
-      </c>
-      <c r="E19" s="89" t="s">
-        <v>144</v>
-      </c>
-      <c r="F19" s="89" t="s">
-        <v>144</v>
-      </c>
-      <c r="G19" s="89" t="s">
-        <v>144</v>
-      </c>
-      <c r="H19" s="89" t="s">
-        <v>144</v>
-      </c>
-      <c r="I19" s="89" t="s">
-        <v>144</v>
-      </c>
-      <c r="J19" s="89" t="s">
-        <v>144</v>
-      </c>
-      <c r="K19" s="89" t="s">
-        <v>144</v>
-      </c>
-      <c r="L19" s="89" t="s">
-        <v>144</v>
-      </c>
-      <c r="M19" s="89" t="s">
-        <v>144</v>
-      </c>
-      <c r="N19" s="89" t="s">
-        <v>144</v>
-      </c>
-      <c r="O19" s="89" t="s">
-        <v>144</v>
-      </c>
-      <c r="P19" s="89" t="s">
-        <v>144</v>
-      </c>
-      <c r="Q19" s="89" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="20" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="95" t="s">
-        <v>147</v>
-      </c>
-      <c r="B20" s="93">
-        <v>33.5</v>
-      </c>
-      <c r="C20" s="93">
-        <v>33.5</v>
-      </c>
-      <c r="D20" s="93">
-        <v>33.5</v>
-      </c>
-      <c r="E20" s="93">
-        <v>33.5</v>
-      </c>
-      <c r="F20" s="93">
-        <v>33.5</v>
-      </c>
-      <c r="G20" s="93">
-        <v>33.5</v>
-      </c>
-      <c r="H20" s="93">
-        <v>33.5</v>
-      </c>
-      <c r="I20" s="90">
-        <v>24</v>
-      </c>
-      <c r="J20" s="90">
-        <v>24</v>
-      </c>
-      <c r="K20" s="90">
-        <v>24</v>
-      </c>
-      <c r="L20" s="90">
-        <v>24</v>
-      </c>
-      <c r="M20" s="92">
-        <v>33.5</v>
-      </c>
-      <c r="N20" s="92">
-        <v>33.5</v>
-      </c>
-      <c r="O20" s="92">
-        <v>33.5</v>
-      </c>
-      <c r="P20" s="92">
-        <v>24</v>
-      </c>
-      <c r="Q20" s="92">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="21" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="96" t="s">
-        <v>148</v>
-      </c>
-      <c r="B21" s="91">
-        <v>66</v>
-      </c>
-      <c r="C21" s="91">
-        <v>66</v>
-      </c>
-      <c r="D21" s="91">
-        <v>66</v>
-      </c>
-      <c r="E21" s="91">
-        <v>253</v>
-      </c>
-      <c r="F21" s="91">
-        <v>253</v>
-      </c>
-      <c r="G21" s="91">
-        <v>253</v>
-      </c>
-      <c r="H21" s="91">
-        <v>253</v>
-      </c>
-      <c r="I21" s="91">
+      <c r="E30" s="70" t="s">
+        <v>121</v>
+      </c>
+      <c r="F30" s="70" t="s">
+        <v>122</v>
+      </c>
+      <c r="G30" s="70" t="s">
+        <v>123</v>
+      </c>
+      <c r="H30" s="70" t="s">
+        <v>124</v>
+      </c>
+      <c r="I30" s="70" t="s">
+        <v>125</v>
+      </c>
+      <c r="J30" s="70" t="s">
+        <v>126</v>
+      </c>
+      <c r="K30" s="70" t="s">
+        <v>127</v>
+      </c>
+      <c r="L30" s="70" t="s">
+        <v>128</v>
+      </c>
+      <c r="M30" s="70" t="s">
+        <v>129</v>
+      </c>
+      <c r="N30" s="70" t="s">
         <v>130</v>
       </c>
-      <c r="J21" s="91">
-        <v>130</v>
-      </c>
-      <c r="K21" s="91">
-        <v>130</v>
-      </c>
-      <c r="L21" s="91">
-        <v>130</v>
-      </c>
-      <c r="M21" s="91">
-        <v>93</v>
-      </c>
-      <c r="N21" s="91">
-        <v>93</v>
-      </c>
-      <c r="O21" s="91">
-        <v>1250</v>
-      </c>
-      <c r="P21" s="91">
-        <v>426.5</v>
-      </c>
-      <c r="Q21" s="91">
-        <v>537.5</v>
-      </c>
-    </row>
-    <row r="22" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="96" t="s">
-        <v>149</v>
-      </c>
-      <c r="B22" s="94">
-        <v>3.7999999999999999E-2</v>
-      </c>
-      <c r="C22" s="94">
-        <v>3.7999999999999999E-2</v>
-      </c>
-      <c r="D22" s="94">
-        <v>3.7999999999999999E-2</v>
-      </c>
-      <c r="E22" s="94">
-        <v>3.7999999999999999E-2</v>
-      </c>
-      <c r="F22" s="94">
-        <v>3.7999999999999999E-2</v>
-      </c>
-      <c r="G22" s="94">
-        <v>3.7999999999999999E-2</v>
-      </c>
-      <c r="H22" s="94">
-        <v>3.7999999999999999E-2</v>
-      </c>
-      <c r="I22" s="94">
-        <v>3.7999999999999999E-2</v>
-      </c>
-      <c r="J22" s="94">
-        <v>3.7999999999999999E-2</v>
-      </c>
-      <c r="K22" s="94">
-        <v>3.7999999999999999E-2</v>
-      </c>
-      <c r="L22" s="94">
-        <v>3.7999999999999999E-2</v>
-      </c>
-      <c r="M22" s="94">
-        <v>3.7999999999999999E-2</v>
-      </c>
-      <c r="N22" s="94">
-        <v>3.7999999999999999E-2</v>
-      </c>
-      <c r="O22" s="94">
-        <v>3.7999999999999999E-2</v>
-      </c>
-      <c r="P22" s="94">
-        <v>3.7999999999999999E-2</v>
-      </c>
-      <c r="Q22" s="94">
-        <v>3.7999999999999999E-2</v>
-      </c>
-    </row>
-    <row r="23" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="96" t="s">
-        <v>150</v>
-      </c>
-      <c r="B23" s="91" t="s">
-        <v>145</v>
-      </c>
-      <c r="C23" s="91" t="s">
-        <v>145</v>
-      </c>
-      <c r="D23" s="91" t="s">
-        <v>145</v>
-      </c>
-      <c r="E23" s="91" t="s">
-        <v>145</v>
-      </c>
-      <c r="F23" s="91" t="s">
-        <v>145</v>
-      </c>
-      <c r="G23" s="91" t="s">
-        <v>145</v>
-      </c>
-      <c r="H23" s="91" t="s">
-        <v>145</v>
-      </c>
-      <c r="I23" s="91" t="s">
-        <v>145</v>
-      </c>
-      <c r="J23" s="91" t="s">
-        <v>145</v>
-      </c>
-      <c r="K23" s="91" t="s">
-        <v>145</v>
-      </c>
-      <c r="L23" s="91" t="s">
-        <v>145</v>
-      </c>
-      <c r="M23" s="91" t="s">
-        <v>145</v>
-      </c>
-      <c r="N23" s="91" t="s">
-        <v>145</v>
-      </c>
-      <c r="O23" s="91" t="s">
-        <v>145</v>
-      </c>
-      <c r="P23" s="91" t="s">
-        <v>145</v>
-      </c>
-      <c r="Q23" s="91" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="24" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="74"/>
-      <c r="B24" s="59"/>
-      <c r="C24" s="58"/>
-      <c r="D24" s="58"/>
-      <c r="E24" s="58"/>
-      <c r="F24" s="58"/>
-      <c r="G24" s="58"/>
-      <c r="H24" s="58"/>
-      <c r="I24" s="58"/>
-      <c r="J24" s="58"/>
-      <c r="K24" s="57"/>
-      <c r="L24" s="57"/>
-      <c r="M24" s="57"/>
-      <c r="N24" s="57"/>
-      <c r="O24" s="57"/>
-      <c r="P24" s="58"/>
-      <c r="Q24" s="59"/>
-    </row>
-    <row r="25" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="30" t="s">
-        <v>7</v>
-      </c>
-      <c r="B25" s="75">
-        <v>40548</v>
-      </c>
-      <c r="C25" s="75">
-        <v>40548</v>
-      </c>
-      <c r="D25" s="35" t="s">
-        <v>86</v>
-      </c>
-      <c r="E25" s="75">
-        <v>40553</v>
-      </c>
-      <c r="F25" s="75">
-        <v>40553</v>
-      </c>
-      <c r="G25" s="75">
-        <v>40918</v>
-      </c>
-      <c r="H25" s="75">
-        <v>40918</v>
-      </c>
-      <c r="I25" s="35" t="s">
-        <v>87</v>
-      </c>
-      <c r="J25" s="35" t="s">
-        <v>87</v>
-      </c>
-      <c r="K25" s="75">
-        <v>40544</v>
-      </c>
-      <c r="L25" s="75">
-        <v>40544</v>
-      </c>
-      <c r="M25" s="75">
-        <v>40179</v>
-      </c>
-      <c r="N25" s="75">
-        <v>40179</v>
-      </c>
-      <c r="O25" s="75">
-        <v>40544</v>
-      </c>
-      <c r="P25" s="75">
-        <v>40544</v>
-      </c>
-      <c r="Q25" s="75">
-        <v>40544</v>
-      </c>
-    </row>
-    <row r="26" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="62" t="s">
-        <v>8</v>
-      </c>
-      <c r="B26" s="76">
-        <v>40913</v>
-      </c>
-      <c r="C26" s="76">
-        <v>40913</v>
-      </c>
-      <c r="D26" s="68" t="s">
-        <v>88</v>
-      </c>
-      <c r="E26" s="68" t="s">
-        <v>89</v>
-      </c>
-      <c r="F26" s="68" t="s">
-        <v>89</v>
-      </c>
-      <c r="G26" s="68" t="s">
-        <v>90</v>
-      </c>
-      <c r="H26" s="68" t="s">
-        <v>90</v>
-      </c>
-      <c r="I26" s="68" t="s">
-        <v>91</v>
-      </c>
-      <c r="J26" s="68" t="s">
-        <v>91</v>
-      </c>
-      <c r="K26" s="68" t="s">
-        <v>92</v>
-      </c>
-      <c r="L26" s="68" t="s">
-        <v>92</v>
-      </c>
-      <c r="M26" s="68" t="s">
-        <v>93</v>
-      </c>
-      <c r="N26" s="68" t="s">
-        <v>93</v>
-      </c>
-      <c r="O26" s="68" t="s">
-        <v>93</v>
-      </c>
-      <c r="P26" s="69" t="s">
-        <v>93</v>
-      </c>
-      <c r="Q26" s="69" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="27" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="62" t="s">
+      <c r="O30" s="70" t="s">
+        <v>131</v>
+      </c>
+      <c r="P30" s="71" t="s">
+        <v>132</v>
+      </c>
+      <c r="Q30" s="66">
+        <v>38444</v>
+      </c>
+    </row>
+    <row r="31" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="87" t="s">
         <v>12</v>
       </c>
-      <c r="B27" s="68" t="s">
-        <v>94</v>
-      </c>
-      <c r="C27" s="68" t="s">
-        <v>95</v>
-      </c>
-      <c r="D27" s="68" t="s">
-        <v>95</v>
-      </c>
-      <c r="E27" s="68" t="s">
-        <v>95</v>
-      </c>
-      <c r="F27" s="68" t="s">
-        <v>94</v>
-      </c>
-      <c r="G27" s="68" t="s">
-        <v>95</v>
-      </c>
-      <c r="H27" s="68" t="s">
-        <v>94</v>
-      </c>
-      <c r="I27" s="68" t="s">
-        <v>96</v>
-      </c>
-      <c r="J27" s="68" t="s">
-        <v>97</v>
-      </c>
-      <c r="K27" s="68" t="s">
-        <v>98</v>
-      </c>
-      <c r="L27" s="68" t="s">
-        <v>99</v>
-      </c>
-      <c r="M27" s="68" t="s">
+      <c r="B31" s="88">
+        <v>35</v>
+      </c>
+      <c r="C31" s="88">
+        <v>35</v>
+      </c>
+      <c r="D31" s="88">
+        <v>35</v>
+      </c>
+      <c r="E31" s="88">
+        <v>35</v>
+      </c>
+      <c r="F31" s="88">
+        <v>35</v>
+      </c>
+      <c r="G31" s="88">
+        <v>35</v>
+      </c>
+      <c r="H31" s="88">
+        <v>35</v>
+      </c>
+      <c r="I31" s="88">
+        <v>80</v>
+      </c>
+      <c r="J31" s="88">
+        <v>33</v>
+      </c>
+      <c r="K31" s="88">
+        <v>30</v>
+      </c>
+      <c r="L31" s="88">
+        <v>30</v>
+      </c>
+      <c r="M31" s="88">
+        <v>32</v>
+      </c>
+      <c r="N31" s="88">
+        <v>32</v>
+      </c>
+      <c r="O31" s="88">
         <v>100</v>
       </c>
-      <c r="N27" s="68" t="s">
-        <v>101</v>
-      </c>
-      <c r="O27" s="68" t="s">
-        <v>102</v>
-      </c>
-      <c r="P27" s="77">
+      <c r="P31" s="73">
         <v>100</v>
       </c>
-      <c r="Q27" s="78">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="28" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="62" t="s">
-        <v>13</v>
-      </c>
-      <c r="B28" s="70">
-        <v>26</v>
-      </c>
-      <c r="C28" s="70">
-        <v>26</v>
-      </c>
-      <c r="D28" s="70">
-        <v>26</v>
-      </c>
-      <c r="E28" s="70">
-        <v>26</v>
-      </c>
-      <c r="F28" s="70">
-        <v>26</v>
-      </c>
-      <c r="G28" s="70">
-        <v>26</v>
-      </c>
-      <c r="H28" s="70">
-        <v>26</v>
-      </c>
-      <c r="I28" s="68" t="s">
-        <v>18</v>
-      </c>
-      <c r="J28" s="68" t="s">
-        <v>18</v>
-      </c>
-      <c r="K28" s="76"/>
-      <c r="L28" s="68" t="s">
-        <v>18</v>
-      </c>
-      <c r="M28" s="68" t="s">
-        <v>18</v>
-      </c>
-      <c r="N28" s="68" t="s">
-        <v>18</v>
-      </c>
-      <c r="O28" s="68" t="s">
-        <v>18</v>
-      </c>
-      <c r="P28" s="79" t="s">
-        <v>103</v>
-      </c>
-      <c r="Q28" s="69" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="29" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="62" t="s">
-        <v>9</v>
-      </c>
-      <c r="B29" s="64">
-        <v>41086</v>
-      </c>
-      <c r="C29" s="68" t="s">
-        <v>105</v>
-      </c>
-      <c r="D29" s="68" t="s">
-        <v>106</v>
-      </c>
-      <c r="E29" s="68" t="s">
-        <v>107</v>
-      </c>
-      <c r="F29" s="68" t="s">
-        <v>108</v>
-      </c>
-      <c r="G29" s="68" t="s">
-        <v>109</v>
-      </c>
-      <c r="H29" s="68" t="s">
-        <v>110</v>
-      </c>
-      <c r="I29" s="68" t="s">
-        <v>111</v>
-      </c>
-      <c r="J29" s="68" t="s">
-        <v>112</v>
-      </c>
-      <c r="K29" s="68" t="s">
-        <v>113</v>
-      </c>
-      <c r="L29" s="68" t="s">
-        <v>114</v>
-      </c>
-      <c r="M29" s="68" t="s">
-        <v>115</v>
-      </c>
-      <c r="N29" s="68" t="s">
-        <v>116</v>
-      </c>
-      <c r="O29" s="68" t="s">
-        <v>117</v>
-      </c>
-      <c r="P29" s="69" t="s">
-        <v>118</v>
-      </c>
-      <c r="Q29" s="64">
-        <v>38444</v>
-      </c>
-    </row>
-    <row r="30" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="85" t="s">
-        <v>12</v>
-      </c>
-      <c r="B30" s="86">
-        <v>35</v>
-      </c>
-      <c r="C30" s="86">
-        <v>35</v>
-      </c>
-      <c r="D30" s="86">
-        <v>35</v>
-      </c>
-      <c r="E30" s="86">
-        <v>35</v>
-      </c>
-      <c r="F30" s="86">
-        <v>35</v>
-      </c>
-      <c r="G30" s="86">
-        <v>35</v>
-      </c>
-      <c r="H30" s="86">
-        <v>35</v>
-      </c>
-      <c r="I30" s="86">
-        <v>80</v>
-      </c>
-      <c r="J30" s="86">
-        <v>33</v>
-      </c>
-      <c r="K30" s="86">
-        <v>30</v>
-      </c>
-      <c r="L30" s="86">
-        <v>30</v>
-      </c>
-      <c r="M30" s="86">
-        <v>32</v>
-      </c>
-      <c r="N30" s="86">
-        <v>32</v>
-      </c>
-      <c r="O30" s="86">
-        <v>100</v>
-      </c>
-      <c r="P30" s="87">
-        <v>100</v>
-      </c>
-      <c r="Q30" s="88">
+      <c r="Q31" s="89">
         <v>100</v>
       </c>
     </row>
@@ -3275,8 +3280,8 @@
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="46.88671875" style="19" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="30.109375" style="39" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="28.88671875" style="39" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="30.109375" style="41" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="28.88671875" style="41" bestFit="1" customWidth="1"/>
     <col min="4" max="14" width="24.33203125" style="19" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="24" style="19" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="13.5546875" style="19" bestFit="1" customWidth="1"/>
@@ -3284,10 +3289,10 @@
   <sheetData>
     <row r="1" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="29"/>
-      <c r="B1" s="45" t="s">
+      <c r="B1" s="49" t="s">
         <v>54</v>
       </c>
-      <c r="C1" s="45"/>
+      <c r="C1" s="49"/>
       <c r="D1" s="29"/>
       <c r="E1" s="29"/>
       <c r="F1" s="29"/>
@@ -3295,78 +3300,84 @@
       <c r="H1" s="29"/>
       <c r="I1" s="29"/>
       <c r="J1" s="29"/>
+      <c r="K1" s="39"/>
+      <c r="L1" s="39"/>
+      <c r="M1" s="39"/>
+      <c r="N1" s="39"/>
+      <c r="O1" s="39"/>
+      <c r="P1" s="39"/>
     </row>
     <row r="2" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="30" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="46" t="s">
+      <c r="B2" s="50" t="s">
         <v>65</v>
       </c>
-      <c r="C2" s="46" t="s">
+      <c r="C2" s="50" t="s">
         <v>66</v>
       </c>
-      <c r="D2" s="47"/>
-      <c r="E2" s="47"/>
-      <c r="F2" s="47"/>
-      <c r="G2" s="47"/>
-      <c r="H2" s="47"/>
-      <c r="I2" s="47"/>
-      <c r="J2" s="47"/>
-      <c r="K2" s="47"/>
-      <c r="L2" s="47"/>
-      <c r="M2" s="47"/>
-      <c r="N2" s="47"/>
-      <c r="O2" s="47"/>
-      <c r="P2" s="47"/>
+      <c r="D2" s="51"/>
+      <c r="E2" s="51"/>
+      <c r="F2" s="51"/>
+      <c r="G2" s="51"/>
+      <c r="H2" s="51"/>
+      <c r="I2" s="51"/>
+      <c r="J2" s="51"/>
+      <c r="K2" s="51"/>
+      <c r="L2" s="51"/>
+      <c r="M2" s="51"/>
+      <c r="N2" s="51"/>
+      <c r="O2" s="51"/>
+      <c r="P2" s="51"/>
     </row>
     <row r="3" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="30" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="43">
+      <c r="B3" s="47">
         <v>-8.1051400000000005</v>
       </c>
-      <c r="C3" s="43">
+      <c r="C3" s="47">
         <v>36.008980000000001</v>
       </c>
-      <c r="D3" s="48"/>
-      <c r="E3" s="48"/>
-      <c r="F3" s="48"/>
-      <c r="G3" s="48"/>
-      <c r="H3" s="48"/>
-      <c r="I3" s="48"/>
-      <c r="J3" s="48"/>
-      <c r="K3" s="48"/>
-      <c r="L3" s="48"/>
-      <c r="M3" s="48"/>
-      <c r="N3" s="48"/>
-      <c r="O3" s="48"/>
-      <c r="P3" s="48"/>
+      <c r="D3" s="52"/>
+      <c r="E3" s="52"/>
+      <c r="F3" s="52"/>
+      <c r="G3" s="52"/>
+      <c r="H3" s="52"/>
+      <c r="I3" s="52"/>
+      <c r="J3" s="52"/>
+      <c r="K3" s="52"/>
+      <c r="L3" s="52"/>
+      <c r="M3" s="52"/>
+      <c r="N3" s="52"/>
+      <c r="O3" s="52"/>
+      <c r="P3" s="52"/>
     </row>
     <row r="4" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="30" t="s">
         <v>41</v>
       </c>
-      <c r="B4" s="43">
+      <c r="B4" s="47">
         <v>31.641110000000001</v>
       </c>
-      <c r="C4" s="43">
+      <c r="C4" s="47">
         <v>32.554589999999997</v>
       </c>
-      <c r="D4" s="48"/>
-      <c r="E4" s="48"/>
-      <c r="F4" s="48"/>
-      <c r="G4" s="48"/>
-      <c r="H4" s="48"/>
-      <c r="I4" s="48"/>
-      <c r="J4" s="48"/>
-      <c r="K4" s="48"/>
-      <c r="L4" s="48"/>
-      <c r="M4" s="48"/>
-      <c r="N4" s="48"/>
-      <c r="O4" s="48"/>
-      <c r="P4" s="48"/>
+      <c r="D4" s="52"/>
+      <c r="E4" s="52"/>
+      <c r="F4" s="52"/>
+      <c r="G4" s="52"/>
+      <c r="H4" s="52"/>
+      <c r="I4" s="52"/>
+      <c r="J4" s="52"/>
+      <c r="K4" s="52"/>
+      <c r="L4" s="52"/>
+      <c r="M4" s="52"/>
+      <c r="N4" s="52"/>
+      <c r="O4" s="52"/>
+      <c r="P4" s="52"/>
     </row>
     <row r="5" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="30" t="s">
@@ -3378,19 +3389,19 @@
       <c r="C5" s="31">
         <v>42736</v>
       </c>
-      <c r="D5" s="48"/>
-      <c r="E5" s="48"/>
-      <c r="F5" s="48"/>
-      <c r="G5" s="48"/>
-      <c r="H5" s="48"/>
-      <c r="I5" s="48"/>
-      <c r="J5" s="48"/>
-      <c r="K5" s="48"/>
-      <c r="L5" s="48"/>
-      <c r="M5" s="48"/>
-      <c r="N5" s="48"/>
-      <c r="O5" s="48"/>
-      <c r="P5" s="48"/>
+      <c r="D5" s="52"/>
+      <c r="E5" s="52"/>
+      <c r="F5" s="52"/>
+      <c r="G5" s="52"/>
+      <c r="H5" s="52"/>
+      <c r="I5" s="52"/>
+      <c r="J5" s="52"/>
+      <c r="K5" s="52"/>
+      <c r="L5" s="52"/>
+      <c r="M5" s="52"/>
+      <c r="N5" s="52"/>
+      <c r="O5" s="52"/>
+      <c r="P5" s="52"/>
     </row>
     <row r="6" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="30" t="s">
@@ -3402,67 +3413,67 @@
       <c r="C6" s="31">
         <v>43101</v>
       </c>
-      <c r="D6" s="48"/>
-      <c r="E6" s="48"/>
-      <c r="F6" s="48"/>
-      <c r="G6" s="48"/>
-      <c r="H6" s="48"/>
-      <c r="I6" s="48"/>
-      <c r="J6" s="48"/>
-      <c r="K6" s="48"/>
-      <c r="L6" s="48"/>
-      <c r="M6" s="48"/>
-      <c r="N6" s="48"/>
-      <c r="O6" s="48"/>
-      <c r="P6" s="48"/>
+      <c r="D6" s="52"/>
+      <c r="E6" s="52"/>
+      <c r="F6" s="52"/>
+      <c r="G6" s="52"/>
+      <c r="H6" s="52"/>
+      <c r="I6" s="52"/>
+      <c r="J6" s="52"/>
+      <c r="K6" s="52"/>
+      <c r="L6" s="52"/>
+      <c r="M6" s="52"/>
+      <c r="N6" s="52"/>
+      <c r="O6" s="52"/>
+      <c r="P6" s="52"/>
     </row>
     <row r="7" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="30" t="s">
         <v>9</v>
       </c>
-      <c r="B7" s="49" t="s">
+      <c r="B7" s="53" t="s">
         <v>18</v>
       </c>
-      <c r="C7" s="49" t="s">
+      <c r="C7" s="53" t="s">
         <v>18</v>
       </c>
-      <c r="D7" s="48"/>
-      <c r="E7" s="48"/>
-      <c r="F7" s="48"/>
-      <c r="G7" s="48"/>
-      <c r="H7" s="50"/>
-      <c r="I7" s="50"/>
-      <c r="J7" s="48"/>
-      <c r="K7" s="48"/>
-      <c r="L7" s="48"/>
-      <c r="M7" s="48"/>
-      <c r="N7" s="48"/>
-      <c r="O7" s="48"/>
-      <c r="P7" s="48"/>
+      <c r="D7" s="52"/>
+      <c r="E7" s="52"/>
+      <c r="F7" s="52"/>
+      <c r="G7" s="52"/>
+      <c r="H7" s="54"/>
+      <c r="I7" s="54"/>
+      <c r="J7" s="52"/>
+      <c r="K7" s="52"/>
+      <c r="L7" s="52"/>
+      <c r="M7" s="52"/>
+      <c r="N7" s="52"/>
+      <c r="O7" s="52"/>
+      <c r="P7" s="52"/>
     </row>
     <row r="8" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="30" t="s">
         <v>10</v>
       </c>
-      <c r="B8" s="51" t="s">
+      <c r="B8" s="55" t="s">
         <v>67</v>
       </c>
-      <c r="C8" s="49" t="s">
+      <c r="C8" s="53" t="s">
         <v>18</v>
       </c>
-      <c r="D8" s="48"/>
-      <c r="E8" s="48"/>
-      <c r="F8" s="48"/>
-      <c r="G8" s="48"/>
-      <c r="H8" s="48"/>
-      <c r="I8" s="48"/>
-      <c r="J8" s="48"/>
-      <c r="K8" s="48"/>
-      <c r="L8" s="48"/>
-      <c r="M8" s="48"/>
-      <c r="N8" s="48"/>
-      <c r="O8" s="48"/>
-      <c r="P8" s="48"/>
+      <c r="D8" s="52"/>
+      <c r="E8" s="52"/>
+      <c r="F8" s="52"/>
+      <c r="G8" s="52"/>
+      <c r="H8" s="52"/>
+      <c r="I8" s="52"/>
+      <c r="J8" s="52"/>
+      <c r="K8" s="52"/>
+      <c r="L8" s="52"/>
+      <c r="M8" s="52"/>
+      <c r="N8" s="52"/>
+      <c r="O8" s="52"/>
+      <c r="P8" s="52"/>
     </row>
     <row r="9" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="30" t="s">
@@ -3474,19 +3485,19 @@
       <c r="C9" s="31" t="s">
         <v>20</v>
       </c>
-      <c r="D9" s="48"/>
-      <c r="E9" s="48"/>
-      <c r="F9" s="48"/>
-      <c r="G9" s="48"/>
-      <c r="H9" s="48"/>
-      <c r="I9" s="48"/>
-      <c r="J9" s="48"/>
-      <c r="K9" s="48"/>
-      <c r="L9" s="48"/>
-      <c r="M9" s="48"/>
-      <c r="N9" s="48"/>
-      <c r="O9" s="52"/>
-      <c r="P9" s="53"/>
+      <c r="D9" s="52"/>
+      <c r="E9" s="52"/>
+      <c r="F9" s="52"/>
+      <c r="G9" s="52"/>
+      <c r="H9" s="52"/>
+      <c r="I9" s="52"/>
+      <c r="J9" s="52"/>
+      <c r="K9" s="52"/>
+      <c r="L9" s="52"/>
+      <c r="M9" s="52"/>
+      <c r="N9" s="52"/>
+      <c r="O9" s="56"/>
+      <c r="P9" s="57"/>
     </row>
     <row r="10" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="30" t="s">
@@ -3494,43 +3505,43 @@
       </c>
       <c r="B10" s="31"/>
       <c r="C10" s="31"/>
-      <c r="D10" s="48"/>
-      <c r="E10" s="48"/>
-      <c r="F10" s="48"/>
-      <c r="G10" s="48"/>
-      <c r="H10" s="48"/>
-      <c r="I10" s="48"/>
-      <c r="J10" s="48"/>
-      <c r="K10" s="48"/>
-      <c r="L10" s="48"/>
-      <c r="M10" s="48"/>
-      <c r="N10" s="48"/>
-      <c r="O10" s="48"/>
-      <c r="P10" s="48"/>
+      <c r="D10" s="52"/>
+      <c r="E10" s="52"/>
+      <c r="F10" s="52"/>
+      <c r="G10" s="52"/>
+      <c r="H10" s="52"/>
+      <c r="I10" s="52"/>
+      <c r="J10" s="52"/>
+      <c r="K10" s="52"/>
+      <c r="L10" s="52"/>
+      <c r="M10" s="52"/>
+      <c r="N10" s="52"/>
+      <c r="O10" s="52"/>
+      <c r="P10" s="52"/>
     </row>
     <row r="11" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="30" t="s">
         <v>14</v>
       </c>
-      <c r="B11" s="49" t="s">
+      <c r="B11" s="53" t="s">
         <v>18</v>
       </c>
-      <c r="C11" s="49" t="s">
+      <c r="C11" s="53" t="s">
         <v>18</v>
       </c>
-      <c r="D11" s="48"/>
-      <c r="E11" s="48"/>
-      <c r="F11" s="48"/>
-      <c r="G11" s="48"/>
-      <c r="H11" s="48"/>
-      <c r="I11" s="48"/>
-      <c r="J11" s="48"/>
-      <c r="K11" s="48"/>
-      <c r="L11" s="48"/>
-      <c r="M11" s="48"/>
-      <c r="N11" s="48"/>
-      <c r="O11" s="48"/>
-      <c r="P11" s="48"/>
+      <c r="D11" s="52"/>
+      <c r="E11" s="52"/>
+      <c r="F11" s="52"/>
+      <c r="G11" s="52"/>
+      <c r="H11" s="52"/>
+      <c r="I11" s="52"/>
+      <c r="J11" s="52"/>
+      <c r="K11" s="52"/>
+      <c r="L11" s="52"/>
+      <c r="M11" s="52"/>
+      <c r="N11" s="52"/>
+      <c r="O11" s="52"/>
+      <c r="P11" s="52"/>
     </row>
     <row r="12" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="30" t="s">
@@ -3538,43 +3549,43 @@
       </c>
       <c r="B12" s="31"/>
       <c r="C12" s="31"/>
-      <c r="D12" s="48"/>
-      <c r="E12" s="48"/>
-      <c r="F12" s="48"/>
-      <c r="G12" s="48"/>
-      <c r="H12" s="48"/>
-      <c r="I12" s="48"/>
-      <c r="J12" s="48"/>
-      <c r="K12" s="48"/>
-      <c r="L12" s="48"/>
-      <c r="M12" s="48"/>
-      <c r="N12" s="48"/>
-      <c r="O12" s="48"/>
-      <c r="P12" s="48"/>
+      <c r="D12" s="52"/>
+      <c r="E12" s="52"/>
+      <c r="F12" s="52"/>
+      <c r="G12" s="52"/>
+      <c r="H12" s="52"/>
+      <c r="I12" s="52"/>
+      <c r="J12" s="52"/>
+      <c r="K12" s="52"/>
+      <c r="L12" s="52"/>
+      <c r="M12" s="52"/>
+      <c r="N12" s="52"/>
+      <c r="O12" s="52"/>
+      <c r="P12" s="52"/>
     </row>
     <row r="13" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="30" t="s">
         <v>17</v>
       </c>
-      <c r="B13" s="51" t="s">
+      <c r="B13" s="55" t="s">
         <v>67</v>
       </c>
-      <c r="C13" s="51" t="s">
+      <c r="C13" s="55" t="s">
         <v>67</v>
       </c>
-      <c r="D13" s="48"/>
-      <c r="E13" s="48"/>
-      <c r="F13" s="48"/>
-      <c r="G13" s="48"/>
-      <c r="H13" s="48"/>
-      <c r="I13" s="48"/>
-      <c r="J13" s="48"/>
-      <c r="K13" s="48"/>
-      <c r="L13" s="48"/>
-      <c r="M13" s="48"/>
-      <c r="N13" s="48"/>
-      <c r="O13" s="48"/>
-      <c r="P13" s="48"/>
+      <c r="D13" s="52"/>
+      <c r="E13" s="52"/>
+      <c r="F13" s="52"/>
+      <c r="G13" s="52"/>
+      <c r="H13" s="52"/>
+      <c r="I13" s="52"/>
+      <c r="J13" s="52"/>
+      <c r="K13" s="52"/>
+      <c r="L13" s="52"/>
+      <c r="M13" s="52"/>
+      <c r="N13" s="52"/>
+      <c r="O13" s="52"/>
+      <c r="P13" s="52"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3604,24 +3615,27 @@
   <sheetData>
     <row r="1" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="29"/>
-      <c r="B1" s="40" t="s">
+      <c r="B1" s="42" t="s">
         <v>54</v>
       </c>
+      <c r="C1" s="43"/>
+      <c r="D1" s="44"/>
+      <c r="E1" s="43"/>
     </row>
     <row r="2" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="30" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="41" t="s">
+      <c r="B2" s="45" t="s">
         <v>55</v>
       </c>
-      <c r="C2" s="41" t="s">
+      <c r="C2" s="45" t="s">
         <v>56</v>
       </c>
-      <c r="D2" s="42" t="s">
+      <c r="D2" s="46" t="s">
         <v>57</v>
       </c>
-      <c r="E2" s="41" t="s">
+      <c r="E2" s="45" t="s">
         <v>58</v>
       </c>
     </row>
@@ -3629,16 +3643,16 @@
       <c r="A3" s="30" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="43">
+      <c r="B3" s="47">
         <v>48.717812000000002</v>
       </c>
-      <c r="C3" s="43">
+      <c r="C3" s="47">
         <v>48.717812000000002</v>
       </c>
-      <c r="D3" s="43">
+      <c r="D3" s="47">
         <v>48.717812000000002</v>
       </c>
-      <c r="E3" s="43">
+      <c r="E3" s="47">
         <v>48.717812000000002</v>
       </c>
     </row>
@@ -3646,16 +3660,16 @@
       <c r="A4" s="30" t="s">
         <v>41</v>
       </c>
-      <c r="B4" s="43">
+      <c r="B4" s="47">
         <v>31.323521</v>
       </c>
-      <c r="C4" s="43">
+      <c r="C4" s="47">
         <v>31.323521</v>
       </c>
-      <c r="D4" s="43">
+      <c r="D4" s="47">
         <v>31.323521</v>
       </c>
-      <c r="E4" s="43">
+      <c r="E4" s="47">
         <v>31.323521</v>
       </c>
     </row>
@@ -3680,16 +3694,16 @@
       <c r="A6" s="30" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="43" t="s">
+      <c r="B6" s="47" t="s">
         <v>59</v>
       </c>
-      <c r="C6" s="43" t="s">
+      <c r="C6" s="47" t="s">
         <v>59</v>
       </c>
-      <c r="D6" s="44" t="s">
+      <c r="D6" s="48" t="s">
         <v>60</v>
       </c>
-      <c r="E6" s="43" t="s">
+      <c r="E6" s="47" t="s">
         <v>60</v>
       </c>
     </row>
@@ -3697,16 +3711,16 @@
       <c r="A7" s="30" t="s">
         <v>9</v>
       </c>
-      <c r="B7" s="43" t="s">
+      <c r="B7" s="47" t="s">
         <v>61</v>
       </c>
-      <c r="C7" s="43" t="s">
+      <c r="C7" s="47" t="s">
         <v>61</v>
       </c>
-      <c r="D7" s="44" t="s">
+      <c r="D7" s="48" t="s">
         <v>62</v>
       </c>
-      <c r="E7" s="43" t="s">
+      <c r="E7" s="47" t="s">
         <v>62</v>
       </c>
     </row>
@@ -3714,16 +3728,16 @@
       <c r="A8" s="30" t="s">
         <v>10</v>
       </c>
-      <c r="B8" s="43" t="s">
+      <c r="B8" s="47" t="s">
         <v>63</v>
       </c>
-      <c r="C8" s="43" t="s">
+      <c r="C8" s="47" t="s">
         <v>63</v>
       </c>
-      <c r="D8" s="44" t="s">
+      <c r="D8" s="48" t="s">
         <v>63</v>
       </c>
-      <c r="E8" s="43" t="s">
+      <c r="E8" s="47" t="s">
         <v>63</v>
       </c>
     </row>
@@ -3731,16 +3745,16 @@
       <c r="A9" s="30" t="s">
         <v>12</v>
       </c>
-      <c r="B9" s="44">
+      <c r="B9" s="48">
         <v>50</v>
       </c>
-      <c r="C9" s="44">
+      <c r="C9" s="48">
         <v>50</v>
       </c>
-      <c r="D9" s="44">
+      <c r="D9" s="48">
         <v>50</v>
       </c>
-      <c r="E9" s="44">
+      <c r="E9" s="48">
         <v>50</v>
       </c>
     </row>
@@ -3748,16 +3762,16 @@
       <c r="A10" s="30" t="s">
         <v>13</v>
       </c>
-      <c r="B10" s="44">
+      <c r="B10" s="48">
         <v>44</v>
       </c>
-      <c r="C10" s="44">
+      <c r="C10" s="48">
         <v>44</v>
       </c>
-      <c r="D10" s="44">
+      <c r="D10" s="48">
         <v>44</v>
       </c>
-      <c r="E10" s="44">
+      <c r="E10" s="48">
         <v>44</v>
       </c>
     </row>
@@ -3765,16 +3779,16 @@
       <c r="A11" s="30" t="s">
         <v>14</v>
       </c>
-      <c r="B11" s="43" t="s">
+      <c r="B11" s="47" t="s">
         <v>44</v>
       </c>
-      <c r="C11" s="43" t="s">
+      <c r="C11" s="47" t="s">
         <v>44</v>
       </c>
-      <c r="D11" s="44" t="s">
+      <c r="D11" s="48" t="s">
         <v>44</v>
       </c>
-      <c r="E11" s="43" t="s">
+      <c r="E11" s="47" t="s">
         <v>44</v>
       </c>
     </row>
@@ -3782,16 +3796,16 @@
       <c r="A12" s="30" t="s">
         <v>16</v>
       </c>
-      <c r="B12" s="43">
+      <c r="B12" s="47">
         <v>15.8</v>
       </c>
-      <c r="C12" s="43">
+      <c r="C12" s="47">
         <v>14.7</v>
       </c>
-      <c r="D12" s="44">
+      <c r="D12" s="48">
         <v>6</v>
       </c>
-      <c r="E12" s="43">
+      <c r="E12" s="47">
         <v>5.8</v>
       </c>
     </row>
@@ -3799,16 +3813,16 @@
       <c r="A13" s="30" t="s">
         <v>17</v>
       </c>
-      <c r="B13" s="43" t="s">
+      <c r="B13" s="47" t="s">
         <v>64</v>
       </c>
-      <c r="C13" s="43" t="s">
+      <c r="C13" s="47" t="s">
         <v>64</v>
       </c>
-      <c r="D13" s="44" t="s">
+      <c r="D13" s="48" t="s">
         <v>64</v>
       </c>
-      <c r="E13" s="43" t="s">
+      <c r="E13" s="47" t="s">
         <v>64</v>
       </c>
     </row>
@@ -3829,8 +3843,8 @@
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="49.5546875" style="19" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.109375" style="39" bestFit="1" customWidth="1"/>
-    <col min="3" max="10" width="13.5546875" style="39" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.109375" style="41" bestFit="1" customWidth="1"/>
+    <col min="3" max="10" width="13.5546875" style="41" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -4311,8 +4325,30 @@
         <v>45</v>
       </c>
     </row>
-    <row r="17" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="18" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="17" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="39"/>
+      <c r="B17" s="40"/>
+      <c r="C17" s="40"/>
+      <c r="D17" s="40"/>
+      <c r="E17" s="40"/>
+      <c r="F17" s="40"/>
+      <c r="G17" s="40"/>
+      <c r="H17" s="40"/>
+      <c r="I17" s="40"/>
+      <c r="J17" s="40"/>
+    </row>
+    <row r="18" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="39"/>
+      <c r="B18" s="40"/>
+      <c r="C18" s="40"/>
+      <c r="D18" s="40"/>
+      <c r="E18" s="40"/>
+      <c r="F18" s="40"/>
+      <c r="G18" s="40"/>
+      <c r="H18" s="40"/>
+      <c r="I18" s="40"/>
+      <c r="J18" s="40"/>
+    </row>
     <row r="19" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="30" t="s">
         <v>12</v>

</xml_diff>

<commit_message>
Load excel compatibility + precip data
</commit_message>
<xml_diff>
--- a/heliostrome/jip_project/results/Factors to run simulation.xlsx
+++ b/heliostrome/jip_project/results/Factors to run simulation.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gaeta\Desktop\TU Delft\JIP\Github\heliostrome\heliostrome\jip_project\results\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://tud365-my.sharepoint.com/personal/sparijs_tudelft_nl/Documents/Documents/helios/heliostrome/heliostrome/jip_project/results/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A98C91F8-B721-4382-941D-A6B13FD4C840}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="4" documentId="13_ncr:1_{A98C91F8-B721-4382-941D-A6B13FD4C840}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{272AE8E0-57FE-4E03-8C09-B0E9DA8D17E6}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="1" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="All Case Studies (compatability" sheetId="1" r:id="rId1"/>
@@ -1207,6 +1207,10 @@
 </styleSheet>
 </file>
 
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -1502,16 +1506,16 @@
       <selection pane="topRight"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.6640625" style="19" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.44140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="21.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.7109375" style="19" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="17" style="19" bestFit="1" customWidth="1"/>
-    <col min="5" max="7" width="13.5546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="7" width="13.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="39"/>
       <c r="B1" s="52" t="s">
         <v>133</v>
@@ -1532,7 +1536,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="52" t="s">
         <v>138</v>
       </c>
@@ -1543,7 +1547,7 @@
       <c r="F2" s="94"/>
       <c r="G2" s="95"/>
     </row>
-    <row r="3" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="52" t="s">
         <v>139</v>
       </c>
@@ -1554,7 +1558,7 @@
       <c r="F3" s="93"/>
       <c r="G3" s="93"/>
     </row>
-    <row r="4" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="52" t="s">
         <v>140</v>
       </c>
@@ -1565,7 +1569,7 @@
       <c r="F4" s="93"/>
       <c r="G4" s="94"/>
     </row>
-    <row r="5" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="52" t="s">
         <v>141</v>
       </c>
@@ -1576,7 +1580,7 @@
       <c r="F5" s="95"/>
       <c r="G5" s="93"/>
     </row>
-    <row r="6" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="52" t="s">
         <v>142</v>
       </c>
@@ -1587,7 +1591,7 @@
       <c r="F6" s="93"/>
       <c r="G6" s="94"/>
     </row>
-    <row r="7" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="52" t="s">
         <v>143</v>
       </c>
@@ -1598,7 +1602,7 @@
       <c r="F7" s="93"/>
       <c r="G7" s="93"/>
     </row>
-    <row r="8" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="52" t="s">
         <v>144</v>
       </c>
@@ -1609,7 +1613,7 @@
       <c r="F8" s="94"/>
       <c r="G8" s="94"/>
     </row>
-    <row r="9" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="52" t="s">
         <v>145</v>
       </c>
@@ -1620,7 +1624,7 @@
       <c r="F9" s="93"/>
       <c r="G9" s="94"/>
     </row>
-    <row r="10" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="52" t="s">
         <v>146</v>
       </c>
@@ -1631,7 +1635,7 @@
       <c r="F10" s="93"/>
       <c r="G10" s="93"/>
     </row>
-    <row r="11" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="52" t="s">
         <v>147</v>
       </c>
@@ -1642,19 +1646,19 @@
       <c r="F11" s="95"/>
       <c r="G11" s="93"/>
     </row>
-    <row r="12" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="52" t="s">
         <v>148</v>
       </c>
       <c r="D12" s="54"/>
     </row>
-    <row r="13" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="52" t="s">
         <v>149</v>
       </c>
       <c r="D13" s="54"/>
     </row>
-    <row r="14" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="52" t="s">
         <v>150</v>
       </c>
@@ -1672,20 +1676,20 @@
   </sheetPr>
   <dimension ref="A1:Q31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+    <sheetView topLeftCell="A11" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection pane="topRight" activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="46.88671875" style="19" bestFit="1" customWidth="1"/>
-    <col min="2" max="15" width="24.33203125" style="90" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="46.85546875" style="19" bestFit="1" customWidth="1"/>
+    <col min="2" max="15" width="24.28515625" style="90" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="24" style="91" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="22.33203125" style="91" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="22.28515625" style="91" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:17" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="58"/>
       <c r="B1" s="59" t="s">
         <v>54</v>
@@ -1706,7 +1710,7 @@
       <c r="P1" s="44"/>
       <c r="Q1" s="40"/>
     </row>
-    <row r="2" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="30" t="s">
         <v>1</v>
       </c>
@@ -1759,7 +1763,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="3" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="64" t="s">
         <v>5</v>
       </c>
@@ -1812,7 +1816,7 @@
         <v>90.37</v>
       </c>
     </row>
-    <row r="4" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="64" t="s">
         <v>41</v>
       </c>
@@ -1865,7 +1869,7 @@
         <v>22.7</v>
       </c>
     </row>
-    <row r="5" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="64" t="s">
         <v>7</v>
       </c>
@@ -1918,7 +1922,7 @@
         <v>40179</v>
       </c>
     </row>
-    <row r="6" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="64" t="s">
         <v>8</v>
       </c>
@@ -1971,7 +1975,7 @@
         <v>41639</v>
       </c>
     </row>
-    <row r="7" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="64" t="s">
         <v>9</v>
       </c>
@@ -2024,7 +2028,7 @@
         <v>38387</v>
       </c>
     </row>
-    <row r="8" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="64" t="s">
         <v>10</v>
       </c>
@@ -2077,7 +2081,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="9" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="64" t="s">
         <v>12</v>
       </c>
@@ -2130,7 +2134,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="10" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="64" t="s">
         <v>13</v>
       </c>
@@ -2183,7 +2187,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="11" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="64" t="s">
         <v>14</v>
       </c>
@@ -2236,7 +2240,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="12" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="64" t="s">
         <v>16</v>
       </c>
@@ -2289,7 +2293,7 @@
         <v>3.4</v>
       </c>
     </row>
-    <row r="13" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="64" t="s">
         <v>17</v>
       </c>
@@ -2342,7 +2346,7 @@
         <v>1252</v>
       </c>
     </row>
-    <row r="14" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="51" t="s">
         <v>86</v>
       </c>
@@ -2395,7 +2399,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:17" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:17" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="77" t="s">
         <v>87</v>
       </c>
@@ -2448,7 +2452,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="16" spans="1:17" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:17" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="77" t="s">
         <v>88</v>
       </c>
@@ -2501,7 +2505,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="17" spans="1:17" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:17" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="77" t="s">
         <v>89</v>
       </c>
@@ -2554,7 +2558,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="18" spans="1:17" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:17" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="77" t="s">
         <v>90</v>
       </c>
@@ -2607,7 +2611,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:17" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:17" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="77" t="s">
         <v>91</v>
       </c>
@@ -2660,7 +2664,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="20" spans="1:17" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:17" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="77" t="s">
         <v>93</v>
       </c>
@@ -2713,7 +2717,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="21" spans="1:17" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:17" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="77" t="s">
         <v>95</v>
       </c>
@@ -2766,7 +2770,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="22" spans="1:17" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:17" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="77" t="s">
         <v>96</v>
       </c>
@@ -2819,7 +2823,7 @@
         <v>537.5</v>
       </c>
     </row>
-    <row r="23" spans="1:17" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:17" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="77" t="s">
         <v>97</v>
       </c>
@@ -2872,7 +2876,7 @@
         <v>3.7999999999999999E-2</v>
       </c>
     </row>
-    <row r="24" spans="1:17" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:17" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="77" t="s">
         <v>98</v>
       </c>
@@ -2925,7 +2929,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="25" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="39"/>
       <c r="B25" s="40"/>
       <c r="C25" s="44"/>
@@ -2944,7 +2948,7 @@
       <c r="P25" s="44"/>
       <c r="Q25" s="40"/>
     </row>
-    <row r="26" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="30" t="s">
         <v>7</v>
       </c>
@@ -2997,7 +3001,7 @@
         <v>40544</v>
       </c>
     </row>
-    <row r="27" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="64" t="s">
         <v>8</v>
       </c>
@@ -3050,7 +3054,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="28" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="64" t="s">
         <v>12</v>
       </c>
@@ -3103,7 +3107,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="29" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="64" t="s">
         <v>13</v>
       </c>
@@ -3154,7 +3158,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="30" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="64" t="s">
         <v>9</v>
       </c>
@@ -3207,7 +3211,7 @@
         <v>38444</v>
       </c>
     </row>
-    <row r="31" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="87" t="s">
         <v>12</v>
       </c>
@@ -3277,17 +3281,17 @@
       <selection pane="topRight"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="46.88671875" style="19" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="30.109375" style="41" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="28.88671875" style="41" bestFit="1" customWidth="1"/>
-    <col min="4" max="14" width="24.33203125" style="19" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="46.85546875" style="19" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="30.140625" style="41" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="28.85546875" style="41" bestFit="1" customWidth="1"/>
+    <col min="4" max="14" width="24.28515625" style="19" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="24" style="19" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="13.5546875" style="19" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="13.5703125" style="19" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="29"/>
       <c r="B1" s="49" t="s">
         <v>54</v>
@@ -3307,7 +3311,7 @@
       <c r="O1" s="39"/>
       <c r="P1" s="39"/>
     </row>
-    <row r="2" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="30" t="s">
         <v>1</v>
       </c>
@@ -3331,7 +3335,7 @@
       <c r="O2" s="51"/>
       <c r="P2" s="51"/>
     </row>
-    <row r="3" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="30" t="s">
         <v>5</v>
       </c>
@@ -3355,7 +3359,7 @@
       <c r="O3" s="52"/>
       <c r="P3" s="52"/>
     </row>
-    <row r="4" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="30" t="s">
         <v>41</v>
       </c>
@@ -3379,7 +3383,7 @@
       <c r="O4" s="52"/>
       <c r="P4" s="52"/>
     </row>
-    <row r="5" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="30" t="s">
         <v>7</v>
       </c>
@@ -3403,7 +3407,7 @@
       <c r="O5" s="52"/>
       <c r="P5" s="52"/>
     </row>
-    <row r="6" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="30" t="s">
         <v>8</v>
       </c>
@@ -3427,7 +3431,7 @@
       <c r="O6" s="52"/>
       <c r="P6" s="52"/>
     </row>
-    <row r="7" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="30" t="s">
         <v>9</v>
       </c>
@@ -3451,7 +3455,7 @@
       <c r="O7" s="52"/>
       <c r="P7" s="52"/>
     </row>
-    <row r="8" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="30" t="s">
         <v>10</v>
       </c>
@@ -3475,7 +3479,7 @@
       <c r="O8" s="52"/>
       <c r="P8" s="52"/>
     </row>
-    <row r="9" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="30" t="s">
         <v>12</v>
       </c>
@@ -3499,7 +3503,7 @@
       <c r="O9" s="56"/>
       <c r="P9" s="57"/>
     </row>
-    <row r="10" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="30" t="s">
         <v>13</v>
       </c>
@@ -3519,7 +3523,7 @@
       <c r="O10" s="52"/>
       <c r="P10" s="52"/>
     </row>
-    <row r="11" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="30" t="s">
         <v>14</v>
       </c>
@@ -3543,7 +3547,7 @@
       <c r="O11" s="52"/>
       <c r="P11" s="52"/>
     </row>
-    <row r="12" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="30" t="s">
         <v>16</v>
       </c>
@@ -3563,7 +3567,7 @@
       <c r="O12" s="52"/>
       <c r="P12" s="52"/>
     </row>
-    <row r="13" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="30" t="s">
         <v>17</v>
       </c>
@@ -3604,16 +3608,16 @@
       <selection pane="topRight"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="46.88671875" style="19" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="24.33203125" style="20" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="24.44140625" style="20" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="25.109375" style="21" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="26.109375" style="20" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="46.85546875" style="19" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.28515625" style="20" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="24.42578125" style="20" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="25.140625" style="21" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="26.140625" style="20" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="29"/>
       <c r="B1" s="42" t="s">
         <v>54</v>
@@ -3622,7 +3626,7 @@
       <c r="D1" s="44"/>
       <c r="E1" s="43"/>
     </row>
-    <row r="2" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="30" t="s">
         <v>1</v>
       </c>
@@ -3639,7 +3643,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="30" t="s">
         <v>5</v>
       </c>
@@ -3656,7 +3660,7 @@
         <v>48.717812000000002</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="30" t="s">
         <v>41</v>
       </c>
@@ -3673,7 +3677,7 @@
         <v>31.323521</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="30" t="s">
         <v>7</v>
       </c>
@@ -3690,7 +3694,7 @@
         <v>37987</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="30" t="s">
         <v>8</v>
       </c>
@@ -3707,7 +3711,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="30" t="s">
         <v>9</v>
       </c>
@@ -3724,7 +3728,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="30" t="s">
         <v>10</v>
       </c>
@@ -3741,7 +3745,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="30" t="s">
         <v>12</v>
       </c>
@@ -3758,7 +3762,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="30" t="s">
         <v>13</v>
       </c>
@@ -3775,7 +3779,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="30" t="s">
         <v>14</v>
       </c>
@@ -3792,7 +3796,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="12" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="30" t="s">
         <v>16</v>
       </c>
@@ -3809,7 +3813,7 @@
         <v>5.8</v>
       </c>
     </row>
-    <row r="13" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="30" t="s">
         <v>17</v>
       </c>
@@ -3838,16 +3842,18 @@
   </sheetPr>
   <dimension ref="A1:J22"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="N6" sqref="N6"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="49.5546875" style="19" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.109375" style="41" bestFit="1" customWidth="1"/>
-    <col min="3" max="10" width="13.5546875" style="41" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="49.5703125" style="19" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.140625" style="41" bestFit="1" customWidth="1"/>
+    <col min="3" max="10" width="13.5703125" style="41" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="97" t="s">
         <v>33</v>
       </c>
@@ -3861,7 +3867,7 @@
       <c r="I1" s="98"/>
       <c r="J1" s="98"/>
     </row>
-    <row r="2" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="30" t="s">
         <v>1</v>
       </c>
@@ -3893,7 +3899,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="30" t="s">
         <v>5</v>
       </c>
@@ -3925,7 +3931,7 @@
         <v>-7.61111</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="30" t="s">
         <v>41</v>
       </c>
@@ -3957,12 +3963,12 @@
         <v>31.66667</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="30" t="s">
         <v>7</v>
       </c>
       <c r="B5" s="31">
-        <v>38353</v>
+        <v>38718</v>
       </c>
       <c r="C5" s="31">
         <v>38353</v>
@@ -3971,57 +3977,57 @@
         <v>38353</v>
       </c>
       <c r="E5" s="31">
-        <v>38353</v>
+        <v>38718</v>
       </c>
       <c r="F5" s="31">
-        <v>38353</v>
+        <v>38718</v>
       </c>
       <c r="G5" s="31">
-        <v>38353</v>
+        <v>38718</v>
       </c>
       <c r="H5" s="31">
-        <v>38353</v>
+        <v>38718</v>
       </c>
       <c r="I5" s="31">
-        <v>38353</v>
+        <v>38718</v>
       </c>
       <c r="J5" s="31">
-        <v>38353</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+        <v>38718</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="30" t="s">
         <v>8</v>
       </c>
       <c r="B6" s="31">
-        <v>42369</v>
+        <v>40543</v>
       </c>
       <c r="C6" s="31">
-        <v>42004</v>
+        <v>40178</v>
       </c>
       <c r="D6" s="31">
-        <v>42004</v>
+        <v>40178</v>
       </c>
       <c r="E6" s="31">
-        <v>42369</v>
+        <v>40543</v>
       </c>
       <c r="F6" s="31">
-        <v>42369</v>
+        <v>40543</v>
       </c>
       <c r="G6" s="31">
-        <v>42369</v>
+        <v>40543</v>
       </c>
       <c r="H6" s="31">
-        <v>42369</v>
+        <v>40543</v>
       </c>
       <c r="I6" s="31">
-        <v>42369</v>
+        <v>40543</v>
       </c>
       <c r="J6" s="31">
-        <v>42369</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+        <v>40543</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="30" t="s">
         <v>9</v>
       </c>
@@ -4053,7 +4059,7 @@
         <v>37979</v>
       </c>
     </row>
-    <row r="8" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="30" t="s">
         <v>10</v>
       </c>
@@ -4085,7 +4091,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="9" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="30" t="s">
         <v>12</v>
       </c>
@@ -4117,7 +4123,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="30" t="s">
         <v>13</v>
       </c>
@@ -4133,7 +4139,7 @@
       <c r="I10" s="100"/>
       <c r="J10" s="101"/>
     </row>
-    <row r="11" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="30" t="s">
         <v>14</v>
       </c>
@@ -4165,7 +4171,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="12" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="30" t="s">
         <v>16</v>
       </c>
@@ -4197,7 +4203,7 @@
         <v>2.25</v>
       </c>
     </row>
-    <row r="13" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="30" t="s">
         <v>17</v>
       </c>
@@ -4229,7 +4235,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="14" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="30" t="s">
         <v>45</v>
       </c>
@@ -4261,7 +4267,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="15" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="30" t="s">
         <v>46</v>
       </c>
@@ -4293,7 +4299,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="16" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="30" t="s">
         <v>47</v>
       </c>
@@ -4325,7 +4331,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="17" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="39"/>
       <c r="B17" s="40"/>
       <c r="C17" s="40"/>
@@ -4337,7 +4343,7 @@
       <c r="I17" s="40"/>
       <c r="J17" s="40"/>
     </row>
-    <row r="18" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="39"/>
       <c r="B18" s="40"/>
       <c r="C18" s="40"/>
@@ -4349,7 +4355,7 @@
       <c r="I18" s="40"/>
       <c r="J18" s="40"/>
     </row>
-    <row r="19" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="30" t="s">
         <v>12</v>
       </c>
@@ -4381,7 +4387,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="20" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="30" t="s">
         <v>13</v>
       </c>
@@ -4397,7 +4403,7 @@
       <c r="I20" s="100"/>
       <c r="J20" s="101"/>
     </row>
-    <row r="21" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="30" t="s">
         <v>16</v>
       </c>
@@ -4429,7 +4435,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="22" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="30" t="s">
         <v>8</v>
       </c>
@@ -4478,19 +4484,21 @@
   </sheetPr>
   <dimension ref="A1:G17"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3:G4"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="47.109375" style="19" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.88671875" style="20" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="31.33203125" style="21" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="31.33203125" style="20" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="46.44140625" style="20" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.5546875" style="20" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="47.140625" style="19" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.85546875" style="20" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="31.28515625" style="21" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="31.28515625" style="20" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="46.42578125" style="20" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.5703125" style="20" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
       <c r="B1" s="22" t="s">
         <v>21</v>
@@ -4501,7 +4509,7 @@
       <c r="F1" s="22"/>
       <c r="G1" s="24"/>
     </row>
-    <row r="2" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
@@ -4524,53 +4532,53 @@
         <v>27</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>5</v>
       </c>
       <c r="B3" s="5">
-        <v>119.19</v>
+        <v>114</v>
       </c>
       <c r="C3" s="5">
-        <v>119.19</v>
+        <v>114</v>
       </c>
       <c r="D3" s="5">
-        <v>119.19</v>
+        <v>114</v>
       </c>
       <c r="E3" s="5">
-        <v>119.19</v>
+        <v>114</v>
       </c>
       <c r="F3" s="5">
-        <v>119.19</v>
+        <v>114</v>
       </c>
       <c r="G3" s="5">
-        <v>119.19</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>6</v>
       </c>
       <c r="B4" s="5">
-        <v>42.57</v>
+        <v>40</v>
       </c>
       <c r="C4" s="5">
-        <v>42.57</v>
+        <v>40</v>
       </c>
       <c r="D4" s="5">
-        <v>42.57</v>
+        <v>40</v>
       </c>
       <c r="E4" s="5">
-        <v>42.57</v>
+        <v>40</v>
       </c>
       <c r="F4" s="5">
-        <v>42.57</v>
+        <v>40</v>
       </c>
       <c r="G4" s="5">
-        <v>42.57</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>7</v>
       </c>
@@ -4593,7 +4601,7 @@
         <v>42109</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>8</v>
       </c>
@@ -4616,7 +4624,7 @@
         <v>42658</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>9</v>
       </c>
@@ -4639,7 +4647,7 @@
         <v>42491</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>10</v>
       </c>
@@ -4662,7 +4670,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>12</v>
       </c>
@@ -4685,7 +4693,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>13</v>
       </c>
@@ -4708,7 +4716,7 @@
         <v>30.01</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>14</v>
       </c>
@@ -4731,7 +4739,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>16</v>
       </c>
@@ -4754,7 +4762,7 @@
         <v>9.4</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>17</v>
       </c>
@@ -4765,7 +4773,7 @@
       <c r="F13" s="3"/>
       <c r="G13" s="3"/>
     </row>
-    <row r="14" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="25" t="s">
         <v>30</v>
       </c>
@@ -4788,7 +4796,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="26"/>
       <c r="B15" s="27"/>
       <c r="C15" s="28"/>
@@ -4797,7 +4805,7 @@
       <c r="F15" s="27"/>
       <c r="G15" s="27"/>
     </row>
-    <row r="16" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="1"/>
       <c r="B16" s="22"/>
       <c r="C16" s="23"/>
@@ -4806,7 +4814,7 @@
       <c r="F16" s="22"/>
       <c r="G16" s="22"/>
     </row>
-    <row r="17" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>12</v>
       </c>
@@ -4843,18 +4851,18 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="47.109375" style="19" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.88671875" style="20" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="31.33203125" style="21" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="31.33203125" style="20" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="46.44140625" style="20" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="46.44140625" style="21" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.5546875" style="20" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="47.140625" style="19" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.85546875" style="20" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="31.28515625" style="21" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="31.28515625" style="20" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="46.42578125" style="20" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="46.42578125" style="21" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.5703125" style="20" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="39.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
       <c r="B1" s="102" t="s">
         <v>0</v>
@@ -4865,7 +4873,7 @@
       <c r="F1" s="103"/>
       <c r="G1" s="104"/>
     </row>
-    <row r="2" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
@@ -4888,7 +4896,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>5</v>
       </c>
@@ -4911,7 +4919,7 @@
         <v>50.55</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>6</v>
       </c>
@@ -4934,7 +4942,7 @@
         <v>32.18</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>7</v>
       </c>
@@ -4957,7 +4965,7 @@
         <v>41640</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>8</v>
       </c>
@@ -4980,7 +4988,7 @@
         <v>42004</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>9</v>
       </c>
@@ -5003,7 +5011,7 @@
         <v>41805</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>10</v>
       </c>
@@ -5026,7 +5034,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>12</v>
       </c>
@@ -5049,7 +5057,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>13</v>
       </c>
@@ -5072,7 +5080,7 @@
         <v>24.61</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>14</v>
       </c>
@@ -5095,7 +5103,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>16</v>
       </c>
@@ -5118,7 +5126,7 @@
         <v>6.84</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="10" t="s">
         <v>17</v>
       </c>
@@ -5141,7 +5149,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="13" t="s">
         <v>19</v>
       </c>
@@ -5164,7 +5172,7 @@
         <v>7.95</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="16"/>
       <c r="B15" s="17"/>
       <c r="C15" s="18"/>
@@ -5173,7 +5181,7 @@
       <c r="F15" s="17"/>
       <c r="G15" s="17"/>
     </row>
-    <row r="16" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>12</v>
       </c>

</xml_diff>

<commit_message>
Factors to run simulation updated
</commit_message>
<xml_diff>
--- a/heliostrome/jip_project/results/Factors to run simulation.xlsx
+++ b/heliostrome/jip_project/results/Factors to run simulation.xlsx
@@ -415,13 +415,13 @@
     <t>Length of pipes</t>
   </si>
   <si>
-    <t>39 m</t>
-  </si>
-  <si>
-    <t>213 m</t>
-  </si>
-  <si>
-    <t>70 m</t>
+    <t>66 m</t>
+  </si>
+  <si>
+    <t>253 m</t>
+  </si>
+  <si>
+    <t>90 m</t>
   </si>
   <si>
     <t>Lowering the cost - MIT</t>

</xml_diff>

<commit_message>
factors to run simulation & case study comp update
</commit_message>
<xml_diff>
--- a/heliostrome/jip_project/results/Factors to run simulation.xlsx
+++ b/heliostrome/jip_project/results/Factors to run simulation.xlsx
@@ -4,23 +4,24 @@
   <fileVersion rupBuild="9303" lowestEdited="5" lastEdited="5" appName="xl"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="1"/>
+    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet r:id="rId1" sheetId="1" name="All Case Studies (compatability"/>
     <sheet r:id="rId2" sheetId="2" name="Bangladesh Case Study"/>
-    <sheet r:id="rId3" sheetId="3" name="Morocco Case Study"/>
-    <sheet r:id="rId4" sheetId="4" name="Ahvaz Iran Case Study"/>
-    <sheet r:id="rId5" sheetId="5" name="Morocco Wheat Case Study"/>
-    <sheet r:id="rId6" sheetId="6" name="Northeast China Case Study"/>
-    <sheet r:id="rId7" sheetId="7" name="Iran Potato Case Study"/>
+    <sheet r:id="rId3" sheetId="3" name="Case study pump"/>
+    <sheet r:id="rId4" sheetId="4" name="Morocco Case Study"/>
+    <sheet r:id="rId5" sheetId="5" name="Ahvaz Iran Case Study"/>
+    <sheet r:id="rId6" sheetId="6" name="Morocco Wheat Case Study"/>
+    <sheet r:id="rId7" sheetId="7" name="Northeast China Case Study"/>
+    <sheet r:id="rId8" sheetId="8" name="Iran Potato Case Study"/>
   </sheets>
   <calcPr fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="418" uniqueCount="156">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="593" uniqueCount="157">
   <si>
     <t>Evaluation of AquaCrop for potato yield and biomass
 simulation under different water amounts in drip and
@@ -229,12 +230,78 @@
     <t>See comment</t>
   </si>
   <si>
+    <t>Summer Tomato - Drip (Gazipur)</t>
+  </si>
+  <si>
+    <t>FC</t>
+  </si>
+  <si>
+    <t>Tomato</t>
+  </si>
+  <si>
+    <t>Mulch</t>
+  </si>
+  <si>
+    <t>Maximum Flow rate (L/min)</t>
+  </si>
+  <si>
+    <t>Average Flow Rate (L/min)</t>
+  </si>
+  <si>
+    <t>Modules Per String</t>
+  </si>
+  <si>
+    <t>String in Parralel</t>
+  </si>
+  <si>
+    <t>PV Module Name</t>
+  </si>
+  <si>
+    <t>Trina Solar TSM-260PA05A</t>
+  </si>
+  <si>
+    <t>Pump Name</t>
+  </si>
+  <si>
+    <t>Lorentz_ps2_1800</t>
+  </si>
+  <si>
+    <t>SCB_10_150_180_BL</t>
+  </si>
+  <si>
+    <t>SCB_10_200_180_BL</t>
+  </si>
+  <si>
+    <t>SCB_10_220_180_BL</t>
+  </si>
+  <si>
+    <t>Static Head (m)</t>
+  </si>
+  <si>
+    <t>Total Length of Pipes (m)</t>
+  </si>
+  <si>
+    <t>Diameter of Pipes (m)</t>
+  </si>
+  <si>
+    <t>Material of Pipes</t>
+  </si>
+  <si>
+    <t>plastic</t>
+  </si>
+  <si>
+    <t>Drip -Below 35%</t>
+  </si>
+  <si>
+    <t>26/06/2013</t>
+  </si>
+  <si>
+    <t>Area of Field</t>
+  </si>
+  <si>
     <t>Summer Tomato - Furrow (Gazipur)</t>
   </si>
   <si>
-    <t>Summer Tomato - Drip (Gazipur)</t>
-  </si>
-  <si>
     <t>Winter Tomato - Drip (Gazipur)</t>
   </si>
   <si>
@@ -268,12 +335,6 @@
     <t>Rice (Barisal)</t>
   </si>
   <si>
-    <t>FC</t>
-  </si>
-  <si>
-    <t>Tomato</t>
-  </si>
-  <si>
     <t>PaddyRice</t>
   </si>
   <si>
@@ -283,60 +344,12 @@
     <t>141-460</t>
   </si>
   <si>
-    <t>Mulch</t>
-  </si>
-  <si>
-    <t>Maximum Flow rate (L/min)</t>
-  </si>
-  <si>
-    <t>Average Flow Rate (L/min)</t>
-  </si>
-  <si>
-    <t>Modules Per String</t>
-  </si>
-  <si>
-    <t>String in Parralel</t>
-  </si>
-  <si>
-    <t>PV Module Name</t>
-  </si>
-  <si>
-    <t>Trina Solar TSM-260PA05A</t>
-  </si>
-  <si>
-    <t>Pump Name</t>
-  </si>
-  <si>
     <t>Lorentz_ps1200</t>
   </si>
   <si>
-    <t>SCB_10_150_180_BL</t>
-  </si>
-  <si>
-    <t>SCB_10_200_180_BL</t>
-  </si>
-  <si>
-    <t>SCB_10_220_180_BL</t>
-  </si>
-  <si>
     <t>SCB_10_265_180_BL</t>
   </si>
   <si>
-    <t>Static Head (m)</t>
-  </si>
-  <si>
-    <t>Total Length of Pipes (m)</t>
-  </si>
-  <si>
-    <t>Diameter of Pipes (m)</t>
-  </si>
-  <si>
-    <t>Material of Pipes</t>
-  </si>
-  <si>
-    <t>plastic</t>
-  </si>
-  <si>
     <t>31/08/2012</t>
   </si>
   <si>
@@ -364,9 +377,6 @@
     <t>Furrow -Below 35%</t>
   </si>
   <si>
-    <t>Drip -Below 35%</t>
-  </si>
-  <si>
     <t>Drip -Below 33%</t>
   </si>
   <si>
@@ -394,9 +404,6 @@
     <t>SAT or 41% WC</t>
   </si>
   <si>
-    <t>26/06/2013</t>
-  </si>
-  <si>
     <t>26/06/2014</t>
   </si>
   <si>
@@ -434,9 +441,6 @@
   </si>
   <si>
     <t>26/06/2026</t>
-  </si>
-  <si>
-    <t>Area of Field</t>
   </si>
   <si>
     <t>Lowering the cost - MIT</t>
@@ -1097,9 +1101,6 @@
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="17" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="17" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf xfId="0" numFmtId="0" borderId="21" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1109,24 +1110,57 @@
     <xf xfId="0" numFmtId="14" applyNumberFormat="1" borderId="22" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="14" applyNumberFormat="1" borderId="9" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf xfId="0" numFmtId="14" applyNumberFormat="1" borderId="11" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="14" applyNumberFormat="1" borderId="11" applyBorder="1" fontId="1" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="22" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="22" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="22" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="13" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="14" applyBorder="1" fontId="7" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="14" applyBorder="1" fontId="5" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="165" applyNumberFormat="1" borderId="14" applyBorder="1" fontId="5" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="166" applyNumberFormat="1" borderId="14" applyBorder="1" fontId="5" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="164" applyNumberFormat="1" borderId="17" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="164" applyNumberFormat="1" borderId="22" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="19" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="18" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="17" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="14" applyNumberFormat="1" borderId="9" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="14" applyNumberFormat="1" borderId="11" applyBorder="1" fontId="1" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="22" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="20" applyBorder="1" fontId="1" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -1136,28 +1170,7 @@
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="17" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="13" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="14" applyBorder="1" fontId="7" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="14" applyBorder="1" fontId="5" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="14" applyBorder="1" fontId="5" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf xfId="0" numFmtId="165" applyNumberFormat="1" borderId="14" applyBorder="1" fontId="5" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf xfId="0" numFmtId="166" applyNumberFormat="1" borderId="14" applyBorder="1" fontId="5" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf xfId="0" numFmtId="164" applyNumberFormat="1" borderId="17" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf xfId="0" numFmtId="164" applyNumberFormat="1" borderId="22" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="20" applyBorder="1" fontId="1" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
@@ -1169,16 +1182,7 @@
     <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="17" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="19" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="18" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="19" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
@@ -1527,27 +1531,27 @@
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
       <c r="A1" s="45"/>
       <c r="B1" s="58" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="C1" s="58" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="D1" s="100" t="s">
         <v>54</v>
       </c>
       <c r="E1" s="58" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="F1" s="58" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="G1" s="100" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75">
       <c r="A2" s="58" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="B2" s="101"/>
       <c r="C2" s="101"/>
@@ -1558,7 +1562,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18.75">
       <c r="A3" s="58" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="B3" s="101"/>
       <c r="C3" s="102"/>
@@ -1569,7 +1573,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18.75">
       <c r="A4" s="58" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="B4" s="102"/>
       <c r="C4" s="104"/>
@@ -1580,7 +1584,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18.75">
       <c r="A5" s="58" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="B5" s="102"/>
       <c r="C5" s="103"/>
@@ -1591,7 +1595,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18.75">
       <c r="A6" s="58" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="B6" s="102"/>
       <c r="C6" s="103"/>
@@ -1602,7 +1606,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="18.75">
       <c r="A7" s="58" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="B7" s="101"/>
       <c r="C7" s="101"/>
@@ -1613,7 +1617,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="18.75">
       <c r="A8" s="58" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="B8" s="101"/>
       <c r="C8" s="102"/>
@@ -1624,7 +1628,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="18.75">
       <c r="A9" s="58" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="B9" s="102"/>
       <c r="C9" s="102"/>
@@ -1635,7 +1639,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="18.75">
       <c r="A10" s="58" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="B10" s="101"/>
       <c r="C10" s="101"/>
@@ -1646,7 +1650,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="18.75">
       <c r="A11" s="58" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="B11" s="101"/>
       <c r="C11" s="102"/>
@@ -1657,7 +1661,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="18.75">
       <c r="A12" s="58" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="B12" s="105"/>
       <c r="C12" s="105"/>
@@ -1668,7 +1672,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="18.75">
       <c r="A13" s="58" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="B13" s="105"/>
       <c r="C13" s="105"/>
@@ -1679,7 +1683,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="18.75">
       <c r="A14" s="58" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="B14" s="105"/>
       <c r="C14" s="105"/>
@@ -1700,27 +1704,27 @@
   </sheetPr>
   <dimension ref="A1:Q31"/>
   <sheetViews>
-    <sheetView workbookViewId="0" tabSelected="1">
+    <sheetView workbookViewId="0">
       <pane state="frozen" activePane="topRight" topLeftCell="B1" ySplit="0" xSplit="1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" style="22" width="46.86214285714286" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="98" width="24.290714285714284" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="98" width="24.290714285714284" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="98" width="24.290714285714284" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="98" width="24.290714285714284" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="98" width="24.290714285714284" customWidth="1" bestFit="1"/>
-    <col min="7" max="7" style="98" width="24.290714285714284" customWidth="1" bestFit="1"/>
-    <col min="8" max="8" style="98" width="24.290714285714284" customWidth="1" bestFit="1"/>
-    <col min="9" max="9" style="98" width="24.290714285714284" customWidth="1" bestFit="1"/>
-    <col min="10" max="10" style="98" width="24.290714285714284" customWidth="1" bestFit="1"/>
-    <col min="11" max="11" style="98" width="24.290714285714284" customWidth="1" bestFit="1"/>
-    <col min="12" max="12" style="98" width="24.290714285714284" customWidth="1" bestFit="1"/>
-    <col min="13" max="13" style="98" width="24.290714285714284" customWidth="1" bestFit="1"/>
-    <col min="14" max="14" style="98" width="24.290714285714284" customWidth="1" bestFit="1"/>
-    <col min="15" max="15" style="98" width="24.290714285714284" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="86" width="24.290714285714284" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="86" width="24.290714285714284" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="86" width="24.290714285714284" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="86" width="24.290714285714284" customWidth="1" bestFit="1"/>
+    <col min="6" max="6" style="86" width="24.290714285714284" customWidth="1" bestFit="1"/>
+    <col min="7" max="7" style="86" width="24.290714285714284" customWidth="1" bestFit="1"/>
+    <col min="8" max="8" style="86" width="24.290714285714284" customWidth="1" bestFit="1"/>
+    <col min="9" max="9" style="86" width="24.290714285714284" customWidth="1" bestFit="1"/>
+    <col min="10" max="10" style="86" width="24.290714285714284" customWidth="1" bestFit="1"/>
+    <col min="11" max="11" style="86" width="24.290714285714284" customWidth="1" bestFit="1"/>
+    <col min="12" max="12" style="86" width="24.290714285714284" customWidth="1" bestFit="1"/>
+    <col min="13" max="13" style="86" width="24.290714285714284" customWidth="1" bestFit="1"/>
+    <col min="14" max="14" style="86" width="24.290714285714284" customWidth="1" bestFit="1"/>
+    <col min="15" max="15" style="86" width="24.290714285714284" customWidth="1" bestFit="1"/>
     <col min="16" max="16" style="99" width="24.005" customWidth="1" bestFit="1"/>
     <col min="17" max="17" style="99" width="13.576428571428572" customWidth="1" bestFit="1"/>
   </cols>
@@ -1751,342 +1755,342 @@
         <v>1</v>
       </c>
       <c r="B2" s="70" t="s">
+        <v>91</v>
+      </c>
+      <c r="C2" s="70" t="s">
         <v>68</v>
       </c>
-      <c r="C2" s="70" t="s">
-        <v>69</v>
-      </c>
       <c r="D2" s="70" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E2" s="70" t="s">
-        <v>70</v>
+        <v>92</v>
       </c>
       <c r="F2" s="70" t="s">
-        <v>71</v>
+        <v>93</v>
       </c>
       <c r="G2" s="70" t="s">
-        <v>70</v>
+        <v>92</v>
       </c>
       <c r="H2" s="70" t="s">
-        <v>71</v>
+        <v>93</v>
       </c>
       <c r="I2" s="70" t="s">
-        <v>72</v>
+        <v>94</v>
       </c>
       <c r="J2" s="70" t="s">
-        <v>73</v>
+        <v>95</v>
       </c>
       <c r="K2" s="70" t="s">
-        <v>74</v>
+        <v>96</v>
       </c>
       <c r="L2" s="70" t="s">
-        <v>75</v>
+        <v>97</v>
       </c>
       <c r="M2" s="70" t="s">
-        <v>76</v>
+        <v>98</v>
       </c>
       <c r="N2" s="70" t="s">
-        <v>77</v>
+        <v>99</v>
       </c>
       <c r="O2" s="70" t="s">
-        <v>78</v>
-      </c>
-      <c r="P2" s="71" t="s">
-        <v>79</v>
-      </c>
-      <c r="Q2" s="71" t="s">
-        <v>80</v>
+        <v>100</v>
+      </c>
+      <c r="P2" s="87" t="s">
+        <v>101</v>
+      </c>
+      <c r="Q2" s="87" t="s">
+        <v>102</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18.75">
-      <c r="A3" s="72" t="s">
+      <c r="A3" s="71" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="73">
+      <c r="B3" s="72">
         <v>90.41</v>
       </c>
-      <c r="C3" s="73">
+      <c r="C3" s="72">
         <v>90.41</v>
       </c>
-      <c r="D3" s="73">
+      <c r="D3" s="72">
         <v>90.41</v>
       </c>
-      <c r="E3" s="73">
+      <c r="E3" s="72">
         <v>90.41</v>
       </c>
-      <c r="F3" s="73">
+      <c r="F3" s="72">
         <v>90.41</v>
       </c>
-      <c r="G3" s="73">
+      <c r="G3" s="72">
         <v>90.41</v>
       </c>
-      <c r="H3" s="73">
+      <c r="H3" s="72">
         <v>90.41</v>
       </c>
-      <c r="I3" s="73">
+      <c r="I3" s="72">
         <v>89.94</v>
       </c>
-      <c r="J3" s="73">
+      <c r="J3" s="72">
         <v>89.94</v>
       </c>
-      <c r="K3" s="73">
+      <c r="K3" s="72">
         <v>89.94</v>
       </c>
-      <c r="L3" s="73">
+      <c r="L3" s="72">
         <v>89.94</v>
       </c>
-      <c r="M3" s="73">
+      <c r="M3" s="72">
         <v>89.94</v>
       </c>
-      <c r="N3" s="73">
+      <c r="N3" s="72">
         <v>89.94</v>
       </c>
-      <c r="O3" s="73">
+      <c r="O3" s="72">
         <v>90.41</v>
       </c>
-      <c r="P3" s="73">
+      <c r="P3" s="72">
         <v>89.42</v>
       </c>
-      <c r="Q3" s="73">
+      <c r="Q3" s="72">
         <v>90.37</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18.75">
-      <c r="A4" s="72" t="s">
+      <c r="A4" s="71" t="s">
         <v>41</v>
       </c>
-      <c r="B4" s="73">
+      <c r="B4" s="72">
         <v>24.1</v>
       </c>
-      <c r="C4" s="73">
+      <c r="C4" s="72">
         <v>24.1</v>
       </c>
-      <c r="D4" s="73">
+      <c r="D4" s="72">
         <v>24.1</v>
       </c>
-      <c r="E4" s="73">
+      <c r="E4" s="72">
         <v>24.1</v>
       </c>
-      <c r="F4" s="73">
+      <c r="F4" s="72">
         <v>24.1</v>
       </c>
-      <c r="G4" s="73">
+      <c r="G4" s="72">
         <v>24.1</v>
       </c>
-      <c r="H4" s="73">
+      <c r="H4" s="72">
         <v>24.1</v>
       </c>
-      <c r="I4" s="73">
+      <c r="I4" s="72">
         <v>24.92</v>
       </c>
-      <c r="J4" s="73">
+      <c r="J4" s="72">
         <v>24.92</v>
       </c>
-      <c r="K4" s="73">
+      <c r="K4" s="72">
         <v>24.92</v>
       </c>
-      <c r="L4" s="73">
+      <c r="L4" s="72">
         <v>24.92</v>
       </c>
-      <c r="M4" s="73">
+      <c r="M4" s="72">
         <v>24.92</v>
       </c>
-      <c r="N4" s="73">
+      <c r="N4" s="72">
         <v>24.92</v>
       </c>
-      <c r="O4" s="73">
+      <c r="O4" s="72">
         <v>24.1</v>
       </c>
-      <c r="P4" s="73">
+      <c r="P4" s="72">
         <v>23.49</v>
       </c>
-      <c r="Q4" s="73">
+      <c r="Q4" s="72">
         <v>22.7</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18.75">
-      <c r="A5" s="72" t="s">
+      <c r="A5" s="71" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="74">
+      <c r="B5" s="73">
         <v>40179</v>
       </c>
-      <c r="C5" s="74">
+      <c r="C5" s="73">
         <v>40179</v>
       </c>
-      <c r="D5" s="74">
+      <c r="D5" s="73">
         <v>40179</v>
       </c>
-      <c r="E5" s="74">
+      <c r="E5" s="73">
         <v>40179</v>
       </c>
-      <c r="F5" s="74">
+      <c r="F5" s="73">
         <v>40179</v>
       </c>
-      <c r="G5" s="74">
+      <c r="G5" s="73">
         <v>40179</v>
       </c>
-      <c r="H5" s="74">
+      <c r="H5" s="73">
         <v>40179</v>
       </c>
-      <c r="I5" s="74">
+      <c r="I5" s="73">
         <v>40179</v>
       </c>
-      <c r="J5" s="74">
+      <c r="J5" s="73">
         <v>40179</v>
       </c>
-      <c r="K5" s="74">
+      <c r="K5" s="73">
         <v>40179</v>
       </c>
-      <c r="L5" s="74">
+      <c r="L5" s="73">
         <v>40179</v>
       </c>
-      <c r="M5" s="74">
+      <c r="M5" s="73">
         <v>40179</v>
       </c>
-      <c r="N5" s="74">
+      <c r="N5" s="73">
         <v>40179</v>
       </c>
-      <c r="O5" s="74">
+      <c r="O5" s="73">
         <v>40179</v>
       </c>
-      <c r="P5" s="74">
+      <c r="P5" s="73">
         <v>40179</v>
       </c>
-      <c r="Q5" s="74">
+      <c r="Q5" s="73">
         <v>40179</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18.75">
-      <c r="A6" s="72" t="s">
+      <c r="A6" s="71" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="74">
+      <c r="B6" s="73">
         <v>41639</v>
       </c>
-      <c r="C6" s="74">
+      <c r="C6" s="73">
         <v>41639</v>
       </c>
-      <c r="D6" s="74">
+      <c r="D6" s="73">
         <v>41639</v>
       </c>
-      <c r="E6" s="74">
+      <c r="E6" s="73">
         <v>41639</v>
       </c>
-      <c r="F6" s="74">
+      <c r="F6" s="73">
         <v>41639</v>
       </c>
-      <c r="G6" s="74">
+      <c r="G6" s="73">
         <v>41639</v>
       </c>
-      <c r="H6" s="74">
+      <c r="H6" s="73">
         <v>41639</v>
       </c>
-      <c r="I6" s="74">
+      <c r="I6" s="73">
         <v>41639</v>
       </c>
-      <c r="J6" s="74">
+      <c r="J6" s="73">
         <v>41639</v>
       </c>
-      <c r="K6" s="74">
+      <c r="K6" s="73">
         <v>41639</v>
       </c>
-      <c r="L6" s="74">
+      <c r="L6" s="73">
         <v>41639</v>
       </c>
-      <c r="M6" s="74">
+      <c r="M6" s="73">
         <v>41639</v>
       </c>
-      <c r="N6" s="74">
+      <c r="N6" s="73">
         <v>41639</v>
       </c>
-      <c r="O6" s="74">
+      <c r="O6" s="73">
         <v>41639</v>
       </c>
-      <c r="P6" s="74">
+      <c r="P6" s="73">
         <v>41639</v>
       </c>
-      <c r="Q6" s="74">
+      <c r="Q6" s="73">
         <v>41639</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="18.75">
-      <c r="A7" s="72" t="s">
+      <c r="A7" s="71" t="s">
         <v>9</v>
       </c>
-      <c r="B7" s="75">
+      <c r="B7" s="88">
         <v>41086</v>
       </c>
-      <c r="C7" s="76">
+      <c r="C7" s="74">
         <v>41086</v>
       </c>
-      <c r="D7" s="76">
+      <c r="D7" s="74">
         <v>41086</v>
       </c>
-      <c r="E7" s="76">
+      <c r="E7" s="74">
         <v>40881</v>
       </c>
-      <c r="F7" s="76">
+      <c r="F7" s="74">
         <v>40881</v>
       </c>
-      <c r="G7" s="76">
+      <c r="G7" s="74">
         <v>40881</v>
       </c>
-      <c r="H7" s="76">
+      <c r="H7" s="74">
         <v>40881</v>
       </c>
-      <c r="I7" s="77">
+      <c r="I7" s="89">
         <v>40486</v>
       </c>
-      <c r="J7" s="77">
+      <c r="J7" s="89">
         <v>40486</v>
       </c>
-      <c r="K7" s="76">
+      <c r="K7" s="74">
         <v>41230</v>
       </c>
-      <c r="L7" s="76">
+      <c r="L7" s="74">
         <v>41230</v>
       </c>
-      <c r="M7" s="76">
+      <c r="M7" s="74">
         <v>40462</v>
       </c>
-      <c r="N7" s="76">
+      <c r="N7" s="74">
         <v>40462</v>
       </c>
-      <c r="O7" s="76">
+      <c r="O7" s="74">
         <v>38679</v>
       </c>
-      <c r="P7" s="76">
+      <c r="P7" s="74">
         <v>38381</v>
       </c>
-      <c r="Q7" s="76">
+      <c r="Q7" s="74">
         <v>38387</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="18.75">
-      <c r="A8" s="72" t="s">
+      <c r="A8" s="71" t="s">
         <v>10</v>
       </c>
-      <c r="B8" s="78" t="s">
+      <c r="B8" s="75" t="s">
         <v>42</v>
       </c>
-      <c r="C8" s="78" t="s">
+      <c r="C8" s="75" t="s">
         <v>42</v>
       </c>
-      <c r="D8" s="78" t="s">
+      <c r="D8" s="75" t="s">
         <v>42</v>
       </c>
-      <c r="E8" s="78" t="s">
+      <c r="E8" s="75" t="s">
         <v>42</v>
       </c>
-      <c r="F8" s="78" t="s">
+      <c r="F8" s="75" t="s">
         <v>42</v>
       </c>
-      <c r="G8" s="78" t="s">
+      <c r="G8" s="75" t="s">
         <v>42</v>
       </c>
-      <c r="H8" s="78" t="s">
+      <c r="H8" s="75" t="s">
         <v>42</v>
       </c>
       <c r="I8" s="41" t="s">
@@ -2095,1242 +2099,1242 @@
       <c r="J8" s="41" t="s">
         <v>28</v>
       </c>
-      <c r="K8" s="78" t="s">
+      <c r="K8" s="75" t="s">
         <v>28</v>
       </c>
-      <c r="L8" s="78" t="s">
+      <c r="L8" s="75" t="s">
         <v>28</v>
       </c>
-      <c r="M8" s="78" t="s">
+      <c r="M8" s="75" t="s">
         <v>28</v>
       </c>
-      <c r="N8" s="78" t="s">
+      <c r="N8" s="75" t="s">
         <v>28</v>
       </c>
-      <c r="O8" s="78" t="s">
+      <c r="O8" s="75" t="s">
         <v>42</v>
       </c>
-      <c r="P8" s="79" t="s">
+      <c r="P8" s="90" t="s">
         <v>42</v>
       </c>
-      <c r="Q8" s="79" t="s">
+      <c r="Q8" s="90" t="s">
         <v>28</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="18.75">
-      <c r="A9" s="72" t="s">
+      <c r="A9" s="71" t="s">
         <v>12</v>
       </c>
-      <c r="B9" s="80">
+      <c r="B9" s="76">
         <v>60</v>
       </c>
-      <c r="C9" s="80">
+      <c r="C9" s="76">
         <v>60</v>
       </c>
-      <c r="D9" s="80">
+      <c r="D9" s="76">
         <v>60</v>
       </c>
-      <c r="E9" s="80">
+      <c r="E9" s="76">
         <v>60</v>
       </c>
-      <c r="F9" s="80">
+      <c r="F9" s="76">
         <v>60</v>
       </c>
-      <c r="G9" s="80">
+      <c r="G9" s="76">
         <v>60</v>
       </c>
-      <c r="H9" s="80">
+      <c r="H9" s="76">
         <v>60</v>
       </c>
-      <c r="I9" s="80">
+      <c r="I9" s="76">
         <v>60</v>
       </c>
-      <c r="J9" s="80">
+      <c r="J9" s="76">
         <v>60</v>
       </c>
-      <c r="K9" s="80">
+      <c r="K9" s="76">
         <v>60</v>
       </c>
-      <c r="L9" s="80">
+      <c r="L9" s="76">
         <v>60</v>
       </c>
-      <c r="M9" s="80">
+      <c r="M9" s="76">
         <v>60</v>
       </c>
-      <c r="N9" s="80">
+      <c r="N9" s="76">
         <v>60</v>
       </c>
-      <c r="O9" s="80">
+      <c r="O9" s="76">
         <v>100</v>
       </c>
-      <c r="P9" s="81">
+      <c r="P9" s="91">
         <v>100</v>
       </c>
-      <c r="Q9" s="82">
+      <c r="Q9" s="92">
         <v>100</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="18.75">
-      <c r="A10" s="72" t="s">
+      <c r="A10" s="71" t="s">
         <v>13</v>
       </c>
-      <c r="B10" s="80" t="s">
-        <v>81</v>
-      </c>
-      <c r="C10" s="80" t="s">
-        <v>81</v>
-      </c>
-      <c r="D10" s="80" t="s">
-        <v>81</v>
-      </c>
-      <c r="E10" s="80" t="s">
-        <v>81</v>
-      </c>
-      <c r="F10" s="80" t="s">
-        <v>81</v>
-      </c>
-      <c r="G10" s="80" t="s">
-        <v>81</v>
-      </c>
-      <c r="H10" s="80" t="s">
-        <v>81</v>
-      </c>
-      <c r="I10" s="80" t="s">
-        <v>81</v>
-      </c>
-      <c r="J10" s="80" t="s">
-        <v>81</v>
-      </c>
-      <c r="K10" s="80" t="s">
-        <v>81</v>
-      </c>
-      <c r="L10" s="80" t="s">
-        <v>81</v>
-      </c>
-      <c r="M10" s="80" t="s">
-        <v>81</v>
-      </c>
-      <c r="N10" s="80" t="s">
-        <v>81</v>
-      </c>
-      <c r="O10" s="80">
+      <c r="B10" s="76" t="s">
+        <v>69</v>
+      </c>
+      <c r="C10" s="76" t="s">
+        <v>69</v>
+      </c>
+      <c r="D10" s="76" t="s">
+        <v>69</v>
+      </c>
+      <c r="E10" s="76" t="s">
+        <v>69</v>
+      </c>
+      <c r="F10" s="76" t="s">
+        <v>69</v>
+      </c>
+      <c r="G10" s="76" t="s">
+        <v>69</v>
+      </c>
+      <c r="H10" s="76" t="s">
+        <v>69</v>
+      </c>
+      <c r="I10" s="76" t="s">
+        <v>69</v>
+      </c>
+      <c r="J10" s="76" t="s">
+        <v>69</v>
+      </c>
+      <c r="K10" s="76" t="s">
+        <v>69</v>
+      </c>
+      <c r="L10" s="76" t="s">
+        <v>69</v>
+      </c>
+      <c r="M10" s="76" t="s">
+        <v>69</v>
+      </c>
+      <c r="N10" s="76" t="s">
+        <v>69</v>
+      </c>
+      <c r="O10" s="76">
         <v>26</v>
       </c>
-      <c r="P10" s="83">
+      <c r="P10" s="93">
         <v>50</v>
       </c>
-      <c r="Q10" s="80">
+      <c r="Q10" s="76">
         <v>41</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="18.75">
-      <c r="A11" s="72" t="s">
+      <c r="A11" s="71" t="s">
         <v>14</v>
       </c>
-      <c r="B11" s="78" t="s">
-        <v>82</v>
-      </c>
-      <c r="C11" s="78" t="s">
-        <v>82</v>
-      </c>
-      <c r="D11" s="78" t="s">
-        <v>82</v>
-      </c>
-      <c r="E11" s="78" t="s">
-        <v>82</v>
-      </c>
-      <c r="F11" s="78" t="s">
-        <v>82</v>
-      </c>
-      <c r="G11" s="78" t="s">
-        <v>82</v>
-      </c>
-      <c r="H11" s="78" t="s">
-        <v>82</v>
-      </c>
-      <c r="I11" s="78" t="s">
-        <v>82</v>
-      </c>
-      <c r="J11" s="78" t="s">
-        <v>82</v>
-      </c>
-      <c r="K11" s="78" t="s">
-        <v>82</v>
-      </c>
-      <c r="L11" s="78" t="s">
-        <v>82</v>
-      </c>
-      <c r="M11" s="78" t="s">
-        <v>82</v>
-      </c>
-      <c r="N11" s="78" t="s">
-        <v>82</v>
-      </c>
-      <c r="O11" s="78" t="s">
+      <c r="B11" s="75" t="s">
+        <v>70</v>
+      </c>
+      <c r="C11" s="75" t="s">
+        <v>70</v>
+      </c>
+      <c r="D11" s="75" t="s">
+        <v>70</v>
+      </c>
+      <c r="E11" s="75" t="s">
+        <v>70</v>
+      </c>
+      <c r="F11" s="75" t="s">
+        <v>70</v>
+      </c>
+      <c r="G11" s="75" t="s">
+        <v>70</v>
+      </c>
+      <c r="H11" s="75" t="s">
+        <v>70</v>
+      </c>
+      <c r="I11" s="75" t="s">
+        <v>70</v>
+      </c>
+      <c r="J11" s="75" t="s">
+        <v>70</v>
+      </c>
+      <c r="K11" s="75" t="s">
+        <v>70</v>
+      </c>
+      <c r="L11" s="75" t="s">
+        <v>70</v>
+      </c>
+      <c r="M11" s="75" t="s">
+        <v>70</v>
+      </c>
+      <c r="N11" s="75" t="s">
+        <v>70</v>
+      </c>
+      <c r="O11" s="75" t="s">
         <v>44</v>
       </c>
-      <c r="P11" s="79" t="s">
-        <v>83</v>
-      </c>
-      <c r="Q11" s="79" t="s">
-        <v>83</v>
+      <c r="P11" s="90" t="s">
+        <v>103</v>
+      </c>
+      <c r="Q11" s="90" t="s">
+        <v>103</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="18.75">
-      <c r="A12" s="72" t="s">
+      <c r="A12" s="71" t="s">
         <v>16</v>
       </c>
-      <c r="B12" s="73">
+      <c r="B12" s="72">
         <v>31.86</v>
       </c>
-      <c r="C12" s="73">
+      <c r="C12" s="72">
         <v>33.73</v>
       </c>
-      <c r="D12" s="73">
+      <c r="D12" s="72">
         <v>35.28</v>
       </c>
-      <c r="E12" s="73">
+      <c r="E12" s="72">
         <v>62.95</v>
       </c>
-      <c r="F12" s="73">
+      <c r="F12" s="72">
         <v>53.52</v>
       </c>
-      <c r="G12" s="73">
+      <c r="G12" s="72">
         <v>39.92</v>
       </c>
-      <c r="H12" s="73">
+      <c r="H12" s="72">
         <v>30.53</v>
       </c>
-      <c r="I12" s="73">
+      <c r="I12" s="72">
         <v>35.64</v>
       </c>
-      <c r="J12" s="73">
+      <c r="J12" s="72">
         <v>33.83</v>
       </c>
-      <c r="K12" s="73">
+      <c r="K12" s="72">
         <v>27.29</v>
       </c>
-      <c r="L12" s="73">
+      <c r="L12" s="72">
         <v>25.82</v>
       </c>
-      <c r="M12" s="73">
+      <c r="M12" s="72">
         <v>35.18</v>
       </c>
-      <c r="N12" s="73">
+      <c r="N12" s="72">
         <v>32.66</v>
       </c>
-      <c r="O12" s="80">
+      <c r="O12" s="76">
         <v>3</v>
       </c>
-      <c r="P12" s="73">
+      <c r="P12" s="72">
         <v>2.5</v>
       </c>
-      <c r="Q12" s="73">
+      <c r="Q12" s="72">
         <v>3.4</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="18.75">
-      <c r="A13" s="72" t="s">
+      <c r="A13" s="71" t="s">
         <v>17</v>
       </c>
-      <c r="B13" s="80">
+      <c r="B13" s="76">
         <v>429</v>
       </c>
-      <c r="C13" s="80">
+      <c r="C13" s="76">
         <v>225</v>
       </c>
-      <c r="D13" s="80">
+      <c r="D13" s="76">
         <v>212</v>
       </c>
-      <c r="E13" s="80">
+      <c r="E13" s="76">
         <v>254</v>
       </c>
-      <c r="F13" s="80">
+      <c r="F13" s="76">
         <v>590</v>
       </c>
-      <c r="G13" s="80">
+      <c r="G13" s="76">
         <v>335</v>
       </c>
-      <c r="H13" s="80">
+      <c r="H13" s="76">
         <v>610</v>
       </c>
-      <c r="I13" s="80">
+      <c r="I13" s="76">
         <v>249</v>
       </c>
-      <c r="J13" s="80">
+      <c r="J13" s="76">
         <v>568</v>
       </c>
-      <c r="K13" s="80">
+      <c r="K13" s="76">
         <v>228</v>
       </c>
-      <c r="L13" s="80">
+      <c r="L13" s="76">
         <v>453</v>
       </c>
-      <c r="M13" s="78" t="s">
-        <v>84</v>
-      </c>
-      <c r="N13" s="78" t="s">
-        <v>85</v>
-      </c>
-      <c r="O13" s="80">
+      <c r="M13" s="75" t="s">
+        <v>104</v>
+      </c>
+      <c r="N13" s="75" t="s">
+        <v>105</v>
+      </c>
+      <c r="O13" s="76">
         <v>430</v>
       </c>
-      <c r="P13" s="80">
+      <c r="P13" s="76">
         <v>1324</v>
       </c>
-      <c r="Q13" s="80">
+      <c r="Q13" s="76">
         <v>1252</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="18.75">
       <c r="A14" s="57" t="s">
+        <v>71</v>
+      </c>
+      <c r="B14" s="77" t="b">
+        <v>0</v>
+      </c>
+      <c r="C14" s="77" t="b">
+        <v>0</v>
+      </c>
+      <c r="D14" s="77" t="b">
+        <v>0</v>
+      </c>
+      <c r="E14" s="77" t="b">
+        <v>0</v>
+      </c>
+      <c r="F14" s="77" t="b">
+        <v>0</v>
+      </c>
+      <c r="G14" s="77" t="b">
+        <v>0</v>
+      </c>
+      <c r="H14" s="77" t="b">
+        <v>0</v>
+      </c>
+      <c r="I14" s="77" t="b">
+        <v>0</v>
+      </c>
+      <c r="J14" s="77" t="b">
+        <v>0</v>
+      </c>
+      <c r="K14" s="77" t="b">
+        <v>0</v>
+      </c>
+      <c r="L14" s="77" t="b">
+        <v>0</v>
+      </c>
+      <c r="M14" s="77" t="b">
+        <v>0</v>
+      </c>
+      <c r="N14" s="77" t="b">
+        <v>0</v>
+      </c>
+      <c r="O14" s="77" t="b">
+        <v>0</v>
+      </c>
+      <c r="P14" s="77" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q14" s="77" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="18.75">
+      <c r="A15" s="78" t="s">
+        <v>72</v>
+      </c>
+      <c r="B15" s="79">
+        <v>111</v>
+      </c>
+      <c r="C15" s="79">
+        <v>111</v>
+      </c>
+      <c r="D15" s="79">
+        <v>111</v>
+      </c>
+      <c r="E15" s="79">
+        <v>111</v>
+      </c>
+      <c r="F15" s="79">
+        <v>111</v>
+      </c>
+      <c r="G15" s="79">
+        <v>111</v>
+      </c>
+      <c r="H15" s="79">
+        <v>111</v>
+      </c>
+      <c r="I15" s="79">
+        <v>112</v>
+      </c>
+      <c r="J15" s="79">
+        <v>112</v>
+      </c>
+      <c r="K15" s="79">
+        <v>112</v>
+      </c>
+      <c r="L15" s="79">
+        <v>112</v>
+      </c>
+      <c r="M15" s="79">
+        <v>111</v>
+      </c>
+      <c r="N15" s="79">
+        <v>111</v>
+      </c>
+      <c r="O15" s="79">
+        <v>111</v>
+      </c>
+      <c r="P15" s="79">
+        <v>169</v>
+      </c>
+      <c r="Q15" s="79">
+        <v>240</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="19.5">
+      <c r="A16" s="78" t="s">
+        <v>73</v>
+      </c>
+      <c r="B16" s="79">
+        <v>61.24</v>
+      </c>
+      <c r="C16" s="79">
+        <v>61.24</v>
+      </c>
+      <c r="D16" s="79">
+        <v>61.24</v>
+      </c>
+      <c r="E16" s="79">
+        <v>61.24</v>
+      </c>
+      <c r="F16" s="79">
+        <v>61.24</v>
+      </c>
+      <c r="G16" s="94">
+        <v>61.24</v>
+      </c>
+      <c r="H16" s="94">
+        <v>61.24</v>
+      </c>
+      <c r="I16" s="79">
+        <v>74</v>
+      </c>
+      <c r="J16" s="79">
+        <v>74</v>
+      </c>
+      <c r="K16" s="79">
+        <v>74</v>
+      </c>
+      <c r="L16" s="79">
+        <v>74</v>
+      </c>
+      <c r="M16" s="94">
+        <v>61.24</v>
+      </c>
+      <c r="N16" s="94">
+        <v>61.24</v>
+      </c>
+      <c r="O16" s="94">
+        <v>61.24</v>
+      </c>
+      <c r="P16" s="79">
+        <v>110</v>
+      </c>
+      <c r="Q16" s="79">
+        <v>164</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="19.5">
+      <c r="A17" s="78" t="s">
+        <v>74</v>
+      </c>
+      <c r="B17" s="79">
+        <v>4</v>
+      </c>
+      <c r="C17" s="79">
+        <v>4</v>
+      </c>
+      <c r="D17" s="79">
+        <v>4</v>
+      </c>
+      <c r="E17" s="79">
+        <v>4</v>
+      </c>
+      <c r="F17" s="79">
+        <v>4</v>
+      </c>
+      <c r="G17" s="79">
+        <v>4</v>
+      </c>
+      <c r="H17" s="79">
+        <v>4</v>
+      </c>
+      <c r="I17" s="79">
+        <v>4</v>
+      </c>
+      <c r="J17" s="79">
+        <v>4</v>
+      </c>
+      <c r="K17" s="79">
+        <v>4</v>
+      </c>
+      <c r="L17" s="79">
+        <v>4</v>
+      </c>
+      <c r="M17" s="79">
+        <v>4</v>
+      </c>
+      <c r="N17" s="79">
+        <v>4</v>
+      </c>
+      <c r="O17" s="79">
+        <v>4</v>
+      </c>
+      <c r="P17" s="79">
+        <v>4</v>
+      </c>
+      <c r="Q17" s="79">
+        <v>4</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="19.5">
+      <c r="A18" s="78" t="s">
+        <v>75</v>
+      </c>
+      <c r="B18" s="79">
+        <v>1</v>
+      </c>
+      <c r="C18" s="79">
+        <v>1</v>
+      </c>
+      <c r="D18" s="79">
+        <v>1</v>
+      </c>
+      <c r="E18" s="79">
+        <v>1</v>
+      </c>
+      <c r="F18" s="79">
+        <v>1</v>
+      </c>
+      <c r="G18" s="79">
+        <v>1</v>
+      </c>
+      <c r="H18" s="79">
+        <v>1</v>
+      </c>
+      <c r="I18" s="79">
+        <v>1</v>
+      </c>
+      <c r="J18" s="79">
+        <v>1</v>
+      </c>
+      <c r="K18" s="79">
+        <v>1</v>
+      </c>
+      <c r="L18" s="79">
+        <v>1</v>
+      </c>
+      <c r="M18" s="79">
+        <v>1</v>
+      </c>
+      <c r="N18" s="79">
+        <v>1</v>
+      </c>
+      <c r="O18" s="79">
+        <v>1</v>
+      </c>
+      <c r="P18" s="79">
+        <v>1</v>
+      </c>
+      <c r="Q18" s="79">
+        <v>1</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="19.5">
+      <c r="A19" s="78" t="s">
+        <v>76</v>
+      </c>
+      <c r="B19" s="79" t="s">
+        <v>77</v>
+      </c>
+      <c r="C19" s="79" t="s">
+        <v>77</v>
+      </c>
+      <c r="D19" s="79" t="s">
+        <v>77</v>
+      </c>
+      <c r="E19" s="79" t="s">
+        <v>77</v>
+      </c>
+      <c r="F19" s="79" t="s">
+        <v>77</v>
+      </c>
+      <c r="G19" s="79" t="s">
+        <v>77</v>
+      </c>
+      <c r="H19" s="79" t="s">
+        <v>77</v>
+      </c>
+      <c r="I19" s="79" t="s">
+        <v>77</v>
+      </c>
+      <c r="J19" s="79" t="s">
+        <v>77</v>
+      </c>
+      <c r="K19" s="79" t="s">
+        <v>77</v>
+      </c>
+      <c r="L19" s="79" t="s">
+        <v>77</v>
+      </c>
+      <c r="M19" s="79" t="s">
+        <v>77</v>
+      </c>
+      <c r="N19" s="79" t="s">
+        <v>77</v>
+      </c>
+      <c r="O19" s="79" t="s">
+        <v>77</v>
+      </c>
+      <c r="P19" s="94" t="s">
+        <v>77</v>
+      </c>
+      <c r="Q19" s="94" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="19.5">
+      <c r="A20" s="78" t="s">
+        <v>78</v>
+      </c>
+      <c r="B20" s="79" t="s">
+        <v>106</v>
+      </c>
+      <c r="C20" s="79" t="s">
+        <v>80</v>
+      </c>
+      <c r="D20" s="79" t="s">
+        <v>80</v>
+      </c>
+      <c r="E20" s="79" t="s">
+        <v>81</v>
+      </c>
+      <c r="F20" s="79" t="s">
+        <v>82</v>
+      </c>
+      <c r="G20" s="79" t="s">
+        <v>107</v>
+      </c>
+      <c r="H20" s="79" t="s">
+        <v>106</v>
+      </c>
+      <c r="I20" s="79" t="s">
+        <v>106</v>
+      </c>
+      <c r="J20" s="79" t="s">
+        <v>106</v>
+      </c>
+      <c r="K20" s="79" t="s">
+        <v>106</v>
+      </c>
+      <c r="L20" s="79" t="s">
+        <v>106</v>
+      </c>
+      <c r="M20" s="79" t="s">
+        <v>106</v>
+      </c>
+      <c r="N20" s="79" t="s">
+        <v>106</v>
+      </c>
+      <c r="O20" s="79" t="s">
+        <v>106</v>
+      </c>
+      <c r="P20" s="94" t="s">
+        <v>106</v>
+      </c>
+      <c r="Q20" s="94" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="19.5">
+      <c r="A21" s="78" t="s">
+        <v>83</v>
+      </c>
+      <c r="B21" s="80">
+        <v>33.5</v>
+      </c>
+      <c r="C21" s="80">
+        <v>33.5</v>
+      </c>
+      <c r="D21" s="80">
+        <v>33.5</v>
+      </c>
+      <c r="E21" s="80">
+        <v>33.5</v>
+      </c>
+      <c r="F21" s="80">
+        <v>33.5</v>
+      </c>
+      <c r="G21" s="80">
+        <v>33.5</v>
+      </c>
+      <c r="H21" s="80">
+        <v>33.5</v>
+      </c>
+      <c r="I21" s="79">
+        <v>24</v>
+      </c>
+      <c r="J21" s="79">
+        <v>24</v>
+      </c>
+      <c r="K21" s="79">
+        <v>24</v>
+      </c>
+      <c r="L21" s="79">
+        <v>24</v>
+      </c>
+      <c r="M21" s="94">
+        <v>33.5</v>
+      </c>
+      <c r="N21" s="94">
+        <v>33.5</v>
+      </c>
+      <c r="O21" s="94">
+        <v>33.5</v>
+      </c>
+      <c r="P21" s="79">
+        <v>24</v>
+      </c>
+      <c r="Q21" s="79">
+        <v>8</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="19.5">
+      <c r="A22" s="78" t="s">
+        <v>84</v>
+      </c>
+      <c r="B22" s="79">
+        <v>66</v>
+      </c>
+      <c r="C22" s="79">
+        <v>66</v>
+      </c>
+      <c r="D22" s="79">
+        <v>66</v>
+      </c>
+      <c r="E22" s="79">
+        <v>253</v>
+      </c>
+      <c r="F22" s="79">
+        <v>0</v>
+      </c>
+      <c r="G22" s="79">
+        <v>253</v>
+      </c>
+      <c r="H22" s="79">
+        <v>0</v>
+      </c>
+      <c r="I22" s="79">
+        <v>130</v>
+      </c>
+      <c r="J22" s="79">
+        <v>0</v>
+      </c>
+      <c r="K22" s="79">
+        <v>90</v>
+      </c>
+      <c r="L22" s="79">
+        <v>0</v>
+      </c>
+      <c r="M22" s="79">
+        <v>93</v>
+      </c>
+      <c r="N22" s="79">
+        <v>0</v>
+      </c>
+      <c r="O22" s="79">
+        <v>1250</v>
+      </c>
+      <c r="P22" s="79">
+        <v>426.5</v>
+      </c>
+      <c r="Q22" s="79">
+        <v>537.5</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="19.5">
+      <c r="A23" s="78" t="s">
+        <v>85</v>
+      </c>
+      <c r="B23" s="81">
+        <v>0.038</v>
+      </c>
+      <c r="C23" s="81">
+        <v>0.038</v>
+      </c>
+      <c r="D23" s="81">
+        <v>0.038</v>
+      </c>
+      <c r="E23" s="81">
+        <v>0.038</v>
+      </c>
+      <c r="F23" s="81">
+        <v>0.038</v>
+      </c>
+      <c r="G23" s="81">
+        <v>0.038</v>
+      </c>
+      <c r="H23" s="81">
+        <v>0.038</v>
+      </c>
+      <c r="I23" s="81">
+        <v>0.038</v>
+      </c>
+      <c r="J23" s="81">
+        <v>0.038</v>
+      </c>
+      <c r="K23" s="81">
+        <v>0.038</v>
+      </c>
+      <c r="L23" s="81">
+        <v>0.038</v>
+      </c>
+      <c r="M23" s="81">
+        <v>0.038</v>
+      </c>
+      <c r="N23" s="81">
+        <v>0.038</v>
+      </c>
+      <c r="O23" s="81">
+        <v>0.038</v>
+      </c>
+      <c r="P23" s="81">
+        <v>0.038</v>
+      </c>
+      <c r="Q23" s="81">
+        <v>0.038</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="19.5">
+      <c r="A24" s="78" t="s">
         <v>86</v>
       </c>
-      <c r="B14" s="84" t="b">
-        <v>0</v>
-      </c>
-      <c r="C14" s="84" t="b">
-        <v>0</v>
-      </c>
-      <c r="D14" s="84" t="b">
-        <v>0</v>
-      </c>
-      <c r="E14" s="84" t="b">
-        <v>0</v>
-      </c>
-      <c r="F14" s="84" t="b">
-        <v>0</v>
-      </c>
-      <c r="G14" s="84" t="b">
-        <v>0</v>
-      </c>
-      <c r="H14" s="84" t="b">
-        <v>0</v>
-      </c>
-      <c r="I14" s="84" t="b">
-        <v>0</v>
-      </c>
-      <c r="J14" s="84" t="b">
-        <v>0</v>
-      </c>
-      <c r="K14" s="84" t="b">
-        <v>0</v>
-      </c>
-      <c r="L14" s="84" t="b">
-        <v>0</v>
-      </c>
-      <c r="M14" s="84" t="b">
-        <v>0</v>
-      </c>
-      <c r="N14" s="84" t="b">
-        <v>0</v>
-      </c>
-      <c r="O14" s="84" t="b">
-        <v>0</v>
-      </c>
-      <c r="P14" s="84" t="b">
-        <v>0</v>
-      </c>
-      <c r="Q14" s="84" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="18.75">
-      <c r="A15" s="85" t="s">
+      <c r="B24" s="79" t="s">
         <v>87</v>
       </c>
-      <c r="B15" s="86">
-        <v>111</v>
-      </c>
-      <c r="C15" s="86">
-        <v>111</v>
-      </c>
-      <c r="D15" s="86">
-        <v>111</v>
-      </c>
-      <c r="E15" s="86">
-        <v>111</v>
-      </c>
-      <c r="F15" s="86">
-        <v>111</v>
-      </c>
-      <c r="G15" s="86">
-        <v>111</v>
-      </c>
-      <c r="H15" s="86">
-        <v>111</v>
-      </c>
-      <c r="I15" s="86">
-        <v>112</v>
-      </c>
-      <c r="J15" s="86">
-        <v>112</v>
-      </c>
-      <c r="K15" s="86">
-        <v>112</v>
-      </c>
-      <c r="L15" s="86">
-        <v>112</v>
-      </c>
-      <c r="M15" s="86">
-        <v>111</v>
-      </c>
-      <c r="N15" s="86">
-        <v>111</v>
-      </c>
-      <c r="O15" s="86">
-        <v>111</v>
-      </c>
-      <c r="P15" s="86">
-        <v>169</v>
-      </c>
-      <c r="Q15" s="86">
-        <v>240</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="19.5">
-      <c r="A16" s="85" t="s">
-        <v>88</v>
-      </c>
-      <c r="B16" s="86">
-        <v>61.24</v>
-      </c>
-      <c r="C16" s="86">
-        <v>61.24</v>
-      </c>
-      <c r="D16" s="86">
-        <v>61.24</v>
-      </c>
-      <c r="E16" s="86">
-        <v>61.24</v>
-      </c>
-      <c r="F16" s="86">
-        <v>61.24</v>
-      </c>
-      <c r="G16" s="87">
-        <v>61.24</v>
-      </c>
-      <c r="H16" s="87">
-        <v>61.24</v>
-      </c>
-      <c r="I16" s="86">
-        <v>74</v>
-      </c>
-      <c r="J16" s="86">
-        <v>74</v>
-      </c>
-      <c r="K16" s="86">
-        <v>74</v>
-      </c>
-      <c r="L16" s="86">
-        <v>74</v>
-      </c>
-      <c r="M16" s="87">
-        <v>61.24</v>
-      </c>
-      <c r="N16" s="87">
-        <v>61.24</v>
-      </c>
-      <c r="O16" s="87">
-        <v>61.24</v>
-      </c>
-      <c r="P16" s="86">
-        <v>110</v>
-      </c>
-      <c r="Q16" s="86">
-        <v>164</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="19.5">
-      <c r="A17" s="85" t="s">
-        <v>89</v>
-      </c>
-      <c r="B17" s="86">
-        <v>4</v>
-      </c>
-      <c r="C17" s="86">
-        <v>4</v>
-      </c>
-      <c r="D17" s="86">
-        <v>4</v>
-      </c>
-      <c r="E17" s="86">
-        <v>4</v>
-      </c>
-      <c r="F17" s="86">
-        <v>4</v>
-      </c>
-      <c r="G17" s="86">
-        <v>4</v>
-      </c>
-      <c r="H17" s="86">
-        <v>4</v>
-      </c>
-      <c r="I17" s="86">
-        <v>4</v>
-      </c>
-      <c r="J17" s="86">
-        <v>4</v>
-      </c>
-      <c r="K17" s="86">
-        <v>4</v>
-      </c>
-      <c r="L17" s="86">
-        <v>4</v>
-      </c>
-      <c r="M17" s="86">
-        <v>4</v>
-      </c>
-      <c r="N17" s="86">
-        <v>4</v>
-      </c>
-      <c r="O17" s="86">
-        <v>4</v>
-      </c>
-      <c r="P17" s="86">
-        <v>4</v>
-      </c>
-      <c r="Q17" s="86">
-        <v>4</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="19.5">
-      <c r="A18" s="85" t="s">
-        <v>90</v>
-      </c>
-      <c r="B18" s="86">
-        <v>1</v>
-      </c>
-      <c r="C18" s="86">
-        <v>1</v>
-      </c>
-      <c r="D18" s="86">
-        <v>1</v>
-      </c>
-      <c r="E18" s="86">
-        <v>1</v>
-      </c>
-      <c r="F18" s="86">
-        <v>1</v>
-      </c>
-      <c r="G18" s="86">
-        <v>1</v>
-      </c>
-      <c r="H18" s="86">
-        <v>1</v>
-      </c>
-      <c r="I18" s="86">
-        <v>1</v>
-      </c>
-      <c r="J18" s="86">
-        <v>1</v>
-      </c>
-      <c r="K18" s="86">
-        <v>1</v>
-      </c>
-      <c r="L18" s="86">
-        <v>1</v>
-      </c>
-      <c r="M18" s="86">
-        <v>1</v>
-      </c>
-      <c r="N18" s="86">
-        <v>1</v>
-      </c>
-      <c r="O18" s="86">
-        <v>1</v>
-      </c>
-      <c r="P18" s="86">
-        <v>1</v>
-      </c>
-      <c r="Q18" s="86">
-        <v>1</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="19.5">
-      <c r="A19" s="85" t="s">
-        <v>91</v>
-      </c>
-      <c r="B19" s="86" t="s">
-        <v>92</v>
-      </c>
-      <c r="C19" s="86" t="s">
-        <v>92</v>
-      </c>
-      <c r="D19" s="86" t="s">
-        <v>92</v>
-      </c>
-      <c r="E19" s="86" t="s">
-        <v>92</v>
-      </c>
-      <c r="F19" s="86" t="s">
-        <v>92</v>
-      </c>
-      <c r="G19" s="86" t="s">
-        <v>92</v>
-      </c>
-      <c r="H19" s="86" t="s">
-        <v>92</v>
-      </c>
-      <c r="I19" s="86" t="s">
-        <v>92</v>
-      </c>
-      <c r="J19" s="86" t="s">
-        <v>92</v>
-      </c>
-      <c r="K19" s="86" t="s">
-        <v>92</v>
-      </c>
-      <c r="L19" s="86" t="s">
-        <v>92</v>
-      </c>
-      <c r="M19" s="86" t="s">
-        <v>92</v>
-      </c>
-      <c r="N19" s="86" t="s">
-        <v>92</v>
-      </c>
-      <c r="O19" s="86" t="s">
-        <v>92</v>
-      </c>
-      <c r="P19" s="87" t="s">
-        <v>92</v>
-      </c>
-      <c r="Q19" s="87" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="19.5">
-      <c r="A20" s="85" t="s">
-        <v>93</v>
-      </c>
-      <c r="B20" s="86" t="s">
-        <v>94</v>
-      </c>
-      <c r="C20" s="86" t="s">
-        <v>95</v>
-      </c>
-      <c r="D20" s="86" t="s">
-        <v>95</v>
-      </c>
-      <c r="E20" s="86" t="s">
-        <v>96</v>
-      </c>
-      <c r="F20" s="86" t="s">
-        <v>97</v>
-      </c>
-      <c r="G20" s="86" t="s">
-        <v>98</v>
-      </c>
-      <c r="H20" s="86" t="s">
-        <v>94</v>
-      </c>
-      <c r="I20" s="86" t="s">
-        <v>94</v>
-      </c>
-      <c r="J20" s="86" t="s">
-        <v>94</v>
-      </c>
-      <c r="K20" s="86" t="s">
-        <v>94</v>
-      </c>
-      <c r="L20" s="86" t="s">
-        <v>94</v>
-      </c>
-      <c r="M20" s="86" t="s">
-        <v>94</v>
-      </c>
-      <c r="N20" s="86" t="s">
-        <v>94</v>
-      </c>
-      <c r="O20" s="86" t="s">
-        <v>94</v>
-      </c>
-      <c r="P20" s="87" t="s">
-        <v>94</v>
-      </c>
-      <c r="Q20" s="87" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="19.5">
-      <c r="A21" s="85" t="s">
-        <v>99</v>
-      </c>
-      <c r="B21" s="88">
-        <v>33.5</v>
-      </c>
-      <c r="C21" s="88">
-        <v>33.5</v>
-      </c>
-      <c r="D21" s="88">
-        <v>33.5</v>
-      </c>
-      <c r="E21" s="88">
-        <v>33.5</v>
-      </c>
-      <c r="F21" s="88">
-        <v>33.5</v>
-      </c>
-      <c r="G21" s="88">
-        <v>33.5</v>
-      </c>
-      <c r="H21" s="88">
-        <v>33.5</v>
-      </c>
-      <c r="I21" s="86">
-        <v>24</v>
-      </c>
-      <c r="J21" s="86">
-        <v>24</v>
-      </c>
-      <c r="K21" s="86">
-        <v>24</v>
-      </c>
-      <c r="L21" s="86">
-        <v>24</v>
-      </c>
-      <c r="M21" s="87">
-        <v>33.5</v>
-      </c>
-      <c r="N21" s="87">
-        <v>33.5</v>
-      </c>
-      <c r="O21" s="87">
-        <v>33.5</v>
-      </c>
-      <c r="P21" s="86">
-        <v>24</v>
-      </c>
-      <c r="Q21" s="86">
-        <v>8</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="19.5">
-      <c r="A22" s="85" t="s">
-        <v>100</v>
-      </c>
-      <c r="B22" s="86">
-        <v>66</v>
-      </c>
-      <c r="C22" s="86">
-        <v>66</v>
-      </c>
-      <c r="D22" s="86">
-        <v>66</v>
-      </c>
-      <c r="E22" s="86">
-        <v>253</v>
-      </c>
-      <c r="F22" s="86">
-        <v>0</v>
-      </c>
-      <c r="G22" s="86">
-        <v>253</v>
-      </c>
-      <c r="H22" s="86">
-        <v>0</v>
-      </c>
-      <c r="I22" s="86">
-        <v>130</v>
-      </c>
-      <c r="J22" s="86">
-        <v>0</v>
-      </c>
-      <c r="K22" s="86">
-        <v>90</v>
-      </c>
-      <c r="L22" s="86">
-        <v>0</v>
-      </c>
-      <c r="M22" s="86">
-        <v>93</v>
-      </c>
-      <c r="N22" s="86">
-        <v>0</v>
-      </c>
-      <c r="O22" s="86">
-        <v>1250</v>
-      </c>
-      <c r="P22" s="86">
-        <v>426.5</v>
-      </c>
-      <c r="Q22" s="86">
-        <v>537.5</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="19.5">
-      <c r="A23" s="85" t="s">
-        <v>101</v>
-      </c>
-      <c r="B23" s="89">
-        <v>0.038</v>
-      </c>
-      <c r="C23" s="89">
-        <v>0.038</v>
-      </c>
-      <c r="D23" s="89">
-        <v>0.038</v>
-      </c>
-      <c r="E23" s="89">
-        <v>0.038</v>
-      </c>
-      <c r="F23" s="89">
-        <v>0.038</v>
-      </c>
-      <c r="G23" s="89">
-        <v>0.038</v>
-      </c>
-      <c r="H23" s="89">
-        <v>0.038</v>
-      </c>
-      <c r="I23" s="89">
-        <v>0.038</v>
-      </c>
-      <c r="J23" s="89">
-        <v>0.038</v>
-      </c>
-      <c r="K23" s="89">
-        <v>0.038</v>
-      </c>
-      <c r="L23" s="89">
-        <v>0.038</v>
-      </c>
-      <c r="M23" s="89">
-        <v>0.038</v>
-      </c>
-      <c r="N23" s="89">
-        <v>0.038</v>
-      </c>
-      <c r="O23" s="89">
-        <v>0.038</v>
-      </c>
-      <c r="P23" s="89">
-        <v>0.038</v>
-      </c>
-      <c r="Q23" s="89">
-        <v>0.038</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="20.25">
-      <c r="A24" s="85" t="s">
-        <v>102</v>
-      </c>
-      <c r="B24" s="86" t="s">
-        <v>103</v>
-      </c>
-      <c r="C24" s="86" t="s">
-        <v>103</v>
-      </c>
-      <c r="D24" s="86" t="s">
-        <v>103</v>
-      </c>
-      <c r="E24" s="86" t="s">
-        <v>103</v>
-      </c>
-      <c r="F24" s="86" t="s">
-        <v>103</v>
-      </c>
-      <c r="G24" s="86" t="s">
-        <v>103</v>
-      </c>
-      <c r="H24" s="86" t="s">
-        <v>103</v>
-      </c>
-      <c r="I24" s="86" t="s">
-        <v>103</v>
-      </c>
-      <c r="J24" s="86" t="s">
-        <v>103</v>
-      </c>
-      <c r="K24" s="86" t="s">
-        <v>103</v>
-      </c>
-      <c r="L24" s="86" t="s">
-        <v>103</v>
-      </c>
-      <c r="M24" s="86" t="s">
-        <v>103</v>
-      </c>
-      <c r="N24" s="86" t="s">
-        <v>103</v>
-      </c>
-      <c r="O24" s="86" t="s">
-        <v>103</v>
-      </c>
-      <c r="P24" s="87" t="s">
-        <v>103</v>
-      </c>
-      <c r="Q24" s="87" t="s">
-        <v>103</v>
+      <c r="C24" s="79" t="s">
+        <v>87</v>
+      </c>
+      <c r="D24" s="79" t="s">
+        <v>87</v>
+      </c>
+      <c r="E24" s="79" t="s">
+        <v>87</v>
+      </c>
+      <c r="F24" s="79" t="s">
+        <v>87</v>
+      </c>
+      <c r="G24" s="79" t="s">
+        <v>87</v>
+      </c>
+      <c r="H24" s="79" t="s">
+        <v>87</v>
+      </c>
+      <c r="I24" s="79" t="s">
+        <v>87</v>
+      </c>
+      <c r="J24" s="79" t="s">
+        <v>87</v>
+      </c>
+      <c r="K24" s="79" t="s">
+        <v>87</v>
+      </c>
+      <c r="L24" s="79" t="s">
+        <v>87</v>
+      </c>
+      <c r="M24" s="79" t="s">
+        <v>87</v>
+      </c>
+      <c r="N24" s="79" t="s">
+        <v>87</v>
+      </c>
+      <c r="O24" s="79" t="s">
+        <v>87</v>
+      </c>
+      <c r="P24" s="94" t="s">
+        <v>87</v>
+      </c>
+      <c r="Q24" s="94" t="s">
+        <v>87</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="18.75">
       <c r="A25" s="34" t="s">
         <v>7</v>
       </c>
-      <c r="B25" s="90">
+      <c r="B25" s="82">
         <v>40548</v>
       </c>
-      <c r="C25" s="90">
+      <c r="C25" s="82">
         <v>40548</v>
       </c>
       <c r="D25" s="41" t="s">
-        <v>104</v>
-      </c>
-      <c r="E25" s="90">
+        <v>108</v>
+      </c>
+      <c r="E25" s="82">
         <v>40553</v>
       </c>
-      <c r="F25" s="90">
+      <c r="F25" s="82">
         <v>40553</v>
       </c>
-      <c r="G25" s="90">
+      <c r="G25" s="82">
         <v>40918</v>
       </c>
-      <c r="H25" s="90">
+      <c r="H25" s="82">
         <v>40918</v>
       </c>
       <c r="I25" s="41" t="s">
-        <v>105</v>
+        <v>109</v>
       </c>
       <c r="J25" s="41" t="s">
-        <v>105</v>
-      </c>
-      <c r="K25" s="90">
+        <v>109</v>
+      </c>
+      <c r="K25" s="82">
         <v>40544</v>
       </c>
-      <c r="L25" s="90">
+      <c r="L25" s="82">
         <v>40544</v>
       </c>
-      <c r="M25" s="90">
+      <c r="M25" s="82">
         <v>40179</v>
       </c>
-      <c r="N25" s="90">
+      <c r="N25" s="82">
         <v>40179</v>
       </c>
-      <c r="O25" s="90">
+      <c r="O25" s="82">
         <v>40544</v>
       </c>
-      <c r="P25" s="90">
+      <c r="P25" s="82">
         <v>40544</v>
       </c>
-      <c r="Q25" s="90">
+      <c r="Q25" s="82">
         <v>40544</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="26" customHeight="1" ht="18.75">
-      <c r="A26" s="72" t="s">
+      <c r="A26" s="71" t="s">
         <v>8</v>
       </c>
-      <c r="B26" s="91">
+      <c r="B26" s="83">
         <v>40913</v>
       </c>
-      <c r="C26" s="91">
+      <c r="C26" s="83">
         <v>40913</v>
       </c>
-      <c r="D26" s="78" t="s">
-        <v>106</v>
-      </c>
-      <c r="E26" s="78" t="s">
-        <v>107</v>
-      </c>
-      <c r="F26" s="78" t="s">
-        <v>107</v>
-      </c>
-      <c r="G26" s="78" t="s">
-        <v>108</v>
-      </c>
-      <c r="H26" s="78" t="s">
-        <v>108</v>
-      </c>
-      <c r="I26" s="78" t="s">
-        <v>109</v>
-      </c>
-      <c r="J26" s="78" t="s">
-        <v>109</v>
-      </c>
-      <c r="K26" s="78" t="s">
+      <c r="D26" s="75" t="s">
         <v>110</v>
       </c>
-      <c r="L26" s="78" t="s">
-        <v>110</v>
-      </c>
-      <c r="M26" s="78" t="s">
+      <c r="E26" s="75" t="s">
         <v>111</v>
       </c>
-      <c r="N26" s="78" t="s">
+      <c r="F26" s="75" t="s">
         <v>111</v>
       </c>
-      <c r="O26" s="78" t="s">
-        <v>111</v>
-      </c>
-      <c r="P26" s="79" t="s">
-        <v>111</v>
-      </c>
-      <c r="Q26" s="79" t="s">
-        <v>111</v>
+      <c r="G26" s="75" t="s">
+        <v>112</v>
+      </c>
+      <c r="H26" s="75" t="s">
+        <v>112</v>
+      </c>
+      <c r="I26" s="75" t="s">
+        <v>113</v>
+      </c>
+      <c r="J26" s="75" t="s">
+        <v>113</v>
+      </c>
+      <c r="K26" s="75" t="s">
+        <v>114</v>
+      </c>
+      <c r="L26" s="75" t="s">
+        <v>114</v>
+      </c>
+      <c r="M26" s="75" t="s">
+        <v>115</v>
+      </c>
+      <c r="N26" s="75" t="s">
+        <v>115</v>
+      </c>
+      <c r="O26" s="75" t="s">
+        <v>115</v>
+      </c>
+      <c r="P26" s="90" t="s">
+        <v>115</v>
+      </c>
+      <c r="Q26" s="90" t="s">
+        <v>115</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="27" customHeight="1" ht="18.75">
-      <c r="A27" s="72" t="s">
+      <c r="A27" s="71" t="s">
         <v>12</v>
       </c>
-      <c r="B27" s="78" t="s">
-        <v>112</v>
-      </c>
-      <c r="C27" s="78" t="s">
-        <v>113</v>
-      </c>
-      <c r="D27" s="78" t="s">
-        <v>113</v>
-      </c>
-      <c r="E27" s="78" t="s">
-        <v>113</v>
-      </c>
-      <c r="F27" s="78" t="s">
-        <v>112</v>
-      </c>
-      <c r="G27" s="78" t="s">
-        <v>113</v>
-      </c>
-      <c r="H27" s="78" t="s">
-        <v>112</v>
-      </c>
-      <c r="I27" s="78" t="s">
-        <v>114</v>
-      </c>
-      <c r="J27" s="78" t="s">
-        <v>115</v>
-      </c>
-      <c r="K27" s="78" t="s">
+      <c r="B27" s="75" t="s">
         <v>116</v>
       </c>
-      <c r="L27" s="78" t="s">
+      <c r="C27" s="75" t="s">
+        <v>88</v>
+      </c>
+      <c r="D27" s="75" t="s">
+        <v>88</v>
+      </c>
+      <c r="E27" s="75" t="s">
+        <v>88</v>
+      </c>
+      <c r="F27" s="75" t="s">
+        <v>116</v>
+      </c>
+      <c r="G27" s="75" t="s">
+        <v>88</v>
+      </c>
+      <c r="H27" s="75" t="s">
+        <v>116</v>
+      </c>
+      <c r="I27" s="75" t="s">
         <v>117</v>
       </c>
-      <c r="M27" s="78" t="s">
+      <c r="J27" s="75" t="s">
         <v>118</v>
       </c>
-      <c r="N27" s="78" t="s">
+      <c r="K27" s="75" t="s">
         <v>119</v>
       </c>
-      <c r="O27" s="78" t="s">
+      <c r="L27" s="75" t="s">
         <v>120</v>
       </c>
-      <c r="P27" s="92">
+      <c r="M27" s="75" t="s">
+        <v>121</v>
+      </c>
+      <c r="N27" s="75" t="s">
+        <v>122</v>
+      </c>
+      <c r="O27" s="75" t="s">
+        <v>123</v>
+      </c>
+      <c r="P27" s="95">
         <v>100</v>
       </c>
-      <c r="Q27" s="93">
+      <c r="Q27" s="96">
         <v>100</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="28" customHeight="1" ht="18.75">
-      <c r="A28" s="72" t="s">
+      <c r="A28" s="71" t="s">
         <v>13</v>
       </c>
-      <c r="B28" s="80">
+      <c r="B28" s="76">
         <v>26</v>
       </c>
-      <c r="C28" s="80">
+      <c r="C28" s="76">
         <v>26</v>
       </c>
-      <c r="D28" s="80">
+      <c r="D28" s="76">
         <v>26</v>
       </c>
-      <c r="E28" s="80">
+      <c r="E28" s="76">
         <v>26</v>
       </c>
-      <c r="F28" s="80">
+      <c r="F28" s="76">
         <v>26</v>
       </c>
-      <c r="G28" s="80">
+      <c r="G28" s="76">
         <v>26</v>
       </c>
-      <c r="H28" s="80">
+      <c r="H28" s="76">
         <v>26</v>
       </c>
-      <c r="I28" s="78" t="s">
+      <c r="I28" s="75" t="s">
         <v>18</v>
       </c>
-      <c r="J28" s="78" t="s">
+      <c r="J28" s="75" t="s">
         <v>18</v>
       </c>
-      <c r="K28" s="91"/>
-      <c r="L28" s="78" t="s">
+      <c r="K28" s="83"/>
+      <c r="L28" s="75" t="s">
         <v>18</v>
       </c>
-      <c r="M28" s="78" t="s">
+      <c r="M28" s="75" t="s">
         <v>18</v>
       </c>
-      <c r="N28" s="78" t="s">
+      <c r="N28" s="75" t="s">
         <v>18</v>
       </c>
-      <c r="O28" s="78" t="s">
+      <c r="O28" s="75" t="s">
         <v>18</v>
       </c>
-      <c r="P28" s="94" t="s">
-        <v>121</v>
-      </c>
-      <c r="Q28" s="79" t="s">
-        <v>122</v>
+      <c r="P28" s="97" t="s">
+        <v>124</v>
+      </c>
+      <c r="Q28" s="90" t="s">
+        <v>125</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="29" customHeight="1" ht="18.75">
-      <c r="A29" s="72" t="s">
+      <c r="A29" s="71" t="s">
         <v>9</v>
       </c>
-      <c r="B29" s="74">
+      <c r="B29" s="73">
         <v>41086</v>
       </c>
-      <c r="C29" s="78" t="s">
-        <v>123</v>
-      </c>
-      <c r="D29" s="78" t="s">
-        <v>124</v>
-      </c>
-      <c r="E29" s="78" t="s">
-        <v>125</v>
-      </c>
-      <c r="F29" s="78" t="s">
+      <c r="C29" s="75" t="s">
+        <v>89</v>
+      </c>
+      <c r="D29" s="75" t="s">
         <v>126</v>
       </c>
-      <c r="G29" s="78" t="s">
+      <c r="E29" s="75" t="s">
         <v>127</v>
       </c>
-      <c r="H29" s="78" t="s">
+      <c r="F29" s="75" t="s">
         <v>128</v>
       </c>
-      <c r="I29" s="78" t="s">
+      <c r="G29" s="75" t="s">
         <v>129</v>
       </c>
-      <c r="J29" s="78" t="s">
+      <c r="H29" s="75" t="s">
         <v>130</v>
       </c>
-      <c r="K29" s="78" t="s">
+      <c r="I29" s="75" t="s">
         <v>131</v>
       </c>
-      <c r="L29" s="78" t="s">
+      <c r="J29" s="75" t="s">
         <v>132</v>
       </c>
-      <c r="M29" s="78" t="s">
+      <c r="K29" s="75" t="s">
         <v>133</v>
       </c>
-      <c r="N29" s="78" t="s">
+      <c r="L29" s="75" t="s">
         <v>134</v>
       </c>
-      <c r="O29" s="78" t="s">
+      <c r="M29" s="75" t="s">
         <v>135</v>
       </c>
-      <c r="P29" s="79" t="s">
+      <c r="N29" s="75" t="s">
         <v>136</v>
       </c>
-      <c r="Q29" s="74">
+      <c r="O29" s="75" t="s">
+        <v>137</v>
+      </c>
+      <c r="P29" s="90" t="s">
+        <v>138</v>
+      </c>
+      <c r="Q29" s="73">
         <v>38444</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="30" customHeight="1" ht="18.75">
-      <c r="A30" s="95" t="s">
+      <c r="A30" s="84" t="s">
         <v>12</v>
       </c>
-      <c r="B30" s="96">
+      <c r="B30" s="85">
         <v>35</v>
       </c>
-      <c r="C30" s="96">
+      <c r="C30" s="85">
         <v>35</v>
       </c>
-      <c r="D30" s="96">
+      <c r="D30" s="85">
         <v>35</v>
       </c>
-      <c r="E30" s="96">
+      <c r="E30" s="85">
         <v>35</v>
       </c>
-      <c r="F30" s="96">
+      <c r="F30" s="85">
         <v>35</v>
       </c>
-      <c r="G30" s="96">
+      <c r="G30" s="85">
         <v>35</v>
       </c>
-      <c r="H30" s="96">
+      <c r="H30" s="85">
         <v>35</v>
       </c>
-      <c r="I30" s="96">
+      <c r="I30" s="85">
         <v>80</v>
       </c>
-      <c r="J30" s="96">
+      <c r="J30" s="85">
         <v>33</v>
       </c>
-      <c r="K30" s="96">
+      <c r="K30" s="85">
         <v>30</v>
       </c>
-      <c r="L30" s="96">
+      <c r="L30" s="85">
         <v>30</v>
       </c>
-      <c r="M30" s="96">
+      <c r="M30" s="85">
         <v>32</v>
       </c>
-      <c r="N30" s="96">
+      <c r="N30" s="85">
         <v>32</v>
       </c>
-      <c r="O30" s="96">
+      <c r="O30" s="85">
         <v>100</v>
       </c>
-      <c r="P30" s="81">
+      <c r="P30" s="91">
         <v>100</v>
       </c>
-      <c r="Q30" s="97">
+      <c r="Q30" s="98">
         <v>100</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="31" customHeight="1" ht="18.75">
-      <c r="A31" s="95" t="s">
-        <v>137</v>
-      </c>
-      <c r="B31" s="96">
+      <c r="A31" s="84" t="s">
+        <v>90</v>
+      </c>
+      <c r="B31" s="85">
         <v>324</v>
       </c>
-      <c r="C31" s="96">
+      <c r="C31" s="85">
         <v>324</v>
       </c>
-      <c r="D31" s="96">
+      <c r="D31" s="85">
         <v>324</v>
       </c>
-      <c r="E31" s="96">
+      <c r="E31" s="85">
         <v>520</v>
       </c>
-      <c r="F31" s="96">
+      <c r="F31" s="85">
         <v>520</v>
       </c>
-      <c r="G31" s="96">
+      <c r="G31" s="85">
         <v>520</v>
       </c>
-      <c r="H31" s="96">
+      <c r="H31" s="85">
         <v>520</v>
       </c>
-      <c r="I31" s="96">
+      <c r="I31" s="85">
         <v>300</v>
       </c>
-      <c r="J31" s="96">
+      <c r="J31" s="85">
         <v>300</v>
       </c>
-      <c r="K31" s="96">
+      <c r="K31" s="85">
         <v>200</v>
       </c>
-      <c r="L31" s="96">
+      <c r="L31" s="85">
         <v>200</v>
       </c>
-      <c r="M31" s="96">
+      <c r="M31" s="85">
         <v>520</v>
       </c>
-      <c r="N31" s="96">
+      <c r="N31" s="85">
         <v>520</v>
       </c>
-      <c r="O31" s="96">
+      <c r="O31" s="85">
         <v>496</v>
       </c>
-      <c r="P31" s="81">
+      <c r="P31" s="91">
         <v>91</v>
       </c>
-      <c r="Q31" s="97">
+      <c r="Q31" s="98">
         <v>218.75</v>
       </c>
     </row>
@@ -3340,6 +3344,1654 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <outlinePr summaryBelow="0"/>
+  </sheetPr>
+  <dimension ref="A1:Q31"/>
+  <sheetViews>
+    <sheetView workbookViewId="0" tabSelected="1">
+      <pane state="frozen" activePane="topRight" topLeftCell="B1" ySplit="0" xSplit="1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" style="22" width="46.86214285714286" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="86" width="24.290714285714284" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="86" width="24.290714285714284" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="86" width="24.290714285714284" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="86" width="24.290714285714284" customWidth="1" bestFit="1"/>
+    <col min="6" max="6" style="86" width="24.290714285714284" customWidth="1" bestFit="1"/>
+    <col min="7" max="7" style="86" width="24.290714285714284" customWidth="1" bestFit="1"/>
+    <col min="8" max="8" style="86" width="24.290714285714284" customWidth="1" bestFit="1"/>
+    <col min="9" max="9" style="86" width="24.290714285714284" customWidth="1" bestFit="1"/>
+    <col min="10" max="10" style="86" width="24.290714285714284" customWidth="1" bestFit="1"/>
+    <col min="11" max="11" style="86" width="24.290714285714284" customWidth="1" bestFit="1"/>
+    <col min="12" max="12" style="86" width="24.290714285714284" customWidth="1" bestFit="1"/>
+    <col min="13" max="13" style="86" width="30.14785714285714" customWidth="1" bestFit="1"/>
+    <col min="14" max="14" style="86" width="30.14785714285714" customWidth="1" bestFit="1"/>
+    <col min="15" max="15" style="86" width="30.14785714285714" customWidth="1" bestFit="1"/>
+    <col min="16" max="16" style="86" width="30.14785714285714" customWidth="1" bestFit="1"/>
+    <col min="17" max="17" style="86" width="30.14785714285714" customWidth="1" bestFit="1"/>
+  </cols>
+  <sheetData>
+    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="20.25">
+      <c r="A1" s="64"/>
+      <c r="B1" s="65" t="s">
+        <v>54</v>
+      </c>
+      <c r="C1" s="65"/>
+      <c r="D1" s="65"/>
+      <c r="E1" s="65"/>
+      <c r="F1" s="65"/>
+      <c r="G1" s="65"/>
+      <c r="H1" s="65"/>
+      <c r="I1" s="65"/>
+      <c r="J1" s="65"/>
+      <c r="K1" s="66"/>
+      <c r="L1" s="67"/>
+      <c r="M1" s="67"/>
+      <c r="N1" s="67"/>
+      <c r="O1" s="67"/>
+      <c r="P1" s="68"/>
+      <c r="Q1" s="69"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75">
+      <c r="A2" s="34" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="70" t="s">
+        <v>68</v>
+      </c>
+      <c r="C2" s="70" t="s">
+        <v>68</v>
+      </c>
+      <c r="D2" s="70" t="s">
+        <v>68</v>
+      </c>
+      <c r="E2" s="70" t="s">
+        <v>68</v>
+      </c>
+      <c r="F2" s="70" t="s">
+        <v>68</v>
+      </c>
+      <c r="G2" s="70" t="s">
+        <v>68</v>
+      </c>
+      <c r="H2" s="70" t="s">
+        <v>68</v>
+      </c>
+      <c r="I2" s="70" t="s">
+        <v>68</v>
+      </c>
+      <c r="J2" s="70" t="s">
+        <v>68</v>
+      </c>
+      <c r="K2" s="70" t="s">
+        <v>68</v>
+      </c>
+      <c r="L2" s="70" t="s">
+        <v>68</v>
+      </c>
+      <c r="M2" s="70" t="s">
+        <v>68</v>
+      </c>
+      <c r="N2" s="70" t="s">
+        <v>68</v>
+      </c>
+      <c r="O2" s="70" t="s">
+        <v>68</v>
+      </c>
+      <c r="P2" s="70" t="s">
+        <v>68</v>
+      </c>
+      <c r="Q2" s="70" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18.75">
+      <c r="A3" s="71" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="72">
+        <v>90.41</v>
+      </c>
+      <c r="C3" s="72">
+        <v>90.41</v>
+      </c>
+      <c r="D3" s="72">
+        <v>90.41</v>
+      </c>
+      <c r="E3" s="72">
+        <v>90.41</v>
+      </c>
+      <c r="F3" s="72">
+        <v>90.41</v>
+      </c>
+      <c r="G3" s="72">
+        <v>90.41</v>
+      </c>
+      <c r="H3" s="72">
+        <v>90.41</v>
+      </c>
+      <c r="I3" s="72">
+        <v>90.41</v>
+      </c>
+      <c r="J3" s="72">
+        <v>90.41</v>
+      </c>
+      <c r="K3" s="72">
+        <v>90.41</v>
+      </c>
+      <c r="L3" s="72">
+        <v>90.41</v>
+      </c>
+      <c r="M3" s="72">
+        <v>90.41</v>
+      </c>
+      <c r="N3" s="72">
+        <v>90.41</v>
+      </c>
+      <c r="O3" s="72">
+        <v>90.41</v>
+      </c>
+      <c r="P3" s="72">
+        <v>90.41</v>
+      </c>
+      <c r="Q3" s="72">
+        <v>90.41</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18.75">
+      <c r="A4" s="71" t="s">
+        <v>41</v>
+      </c>
+      <c r="B4" s="72">
+        <v>24.1</v>
+      </c>
+      <c r="C4" s="72">
+        <v>24.1</v>
+      </c>
+      <c r="D4" s="72">
+        <v>24.1</v>
+      </c>
+      <c r="E4" s="72">
+        <v>24.1</v>
+      </c>
+      <c r="F4" s="72">
+        <v>24.1</v>
+      </c>
+      <c r="G4" s="72">
+        <v>24.1</v>
+      </c>
+      <c r="H4" s="72">
+        <v>24.1</v>
+      </c>
+      <c r="I4" s="72">
+        <v>24.1</v>
+      </c>
+      <c r="J4" s="72">
+        <v>24.1</v>
+      </c>
+      <c r="K4" s="72">
+        <v>24.1</v>
+      </c>
+      <c r="L4" s="72">
+        <v>24.1</v>
+      </c>
+      <c r="M4" s="72">
+        <v>24.1</v>
+      </c>
+      <c r="N4" s="72">
+        <v>24.1</v>
+      </c>
+      <c r="O4" s="72">
+        <v>24.1</v>
+      </c>
+      <c r="P4" s="72">
+        <v>24.1</v>
+      </c>
+      <c r="Q4" s="72">
+        <v>24.1</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18.75">
+      <c r="A5" s="71" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" s="73">
+        <v>40179</v>
+      </c>
+      <c r="C5" s="73">
+        <v>40179</v>
+      </c>
+      <c r="D5" s="73">
+        <v>40179</v>
+      </c>
+      <c r="E5" s="73">
+        <v>40179</v>
+      </c>
+      <c r="F5" s="73">
+        <v>40179</v>
+      </c>
+      <c r="G5" s="73">
+        <v>40179</v>
+      </c>
+      <c r="H5" s="73">
+        <v>40179</v>
+      </c>
+      <c r="I5" s="73">
+        <v>40179</v>
+      </c>
+      <c r="J5" s="73">
+        <v>40179</v>
+      </c>
+      <c r="K5" s="73">
+        <v>40179</v>
+      </c>
+      <c r="L5" s="73">
+        <v>40179</v>
+      </c>
+      <c r="M5" s="73">
+        <v>40179</v>
+      </c>
+      <c r="N5" s="73">
+        <v>40179</v>
+      </c>
+      <c r="O5" s="73">
+        <v>40179</v>
+      </c>
+      <c r="P5" s="73">
+        <v>40179</v>
+      </c>
+      <c r="Q5" s="73">
+        <v>40179</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18.75">
+      <c r="A6" s="71" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" s="73">
+        <v>41639</v>
+      </c>
+      <c r="C6" s="73">
+        <v>41639</v>
+      </c>
+      <c r="D6" s="73">
+        <v>41639</v>
+      </c>
+      <c r="E6" s="73">
+        <v>41639</v>
+      </c>
+      <c r="F6" s="73">
+        <v>41639</v>
+      </c>
+      <c r="G6" s="73">
+        <v>41639</v>
+      </c>
+      <c r="H6" s="73">
+        <v>41639</v>
+      </c>
+      <c r="I6" s="73">
+        <v>41639</v>
+      </c>
+      <c r="J6" s="73">
+        <v>41639</v>
+      </c>
+      <c r="K6" s="73">
+        <v>41639</v>
+      </c>
+      <c r="L6" s="73">
+        <v>41639</v>
+      </c>
+      <c r="M6" s="73">
+        <v>41639</v>
+      </c>
+      <c r="N6" s="73">
+        <v>41639</v>
+      </c>
+      <c r="O6" s="73">
+        <v>41639</v>
+      </c>
+      <c r="P6" s="73">
+        <v>41639</v>
+      </c>
+      <c r="Q6" s="73">
+        <v>41639</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="18.75">
+      <c r="A7" s="71" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7" s="74">
+        <v>41086</v>
+      </c>
+      <c r="C7" s="74">
+        <v>41086</v>
+      </c>
+      <c r="D7" s="74">
+        <v>41086</v>
+      </c>
+      <c r="E7" s="74">
+        <v>41086</v>
+      </c>
+      <c r="F7" s="74">
+        <v>41086</v>
+      </c>
+      <c r="G7" s="74">
+        <v>41086</v>
+      </c>
+      <c r="H7" s="74">
+        <v>41086</v>
+      </c>
+      <c r="I7" s="74">
+        <v>41086</v>
+      </c>
+      <c r="J7" s="74">
+        <v>41086</v>
+      </c>
+      <c r="K7" s="74">
+        <v>41086</v>
+      </c>
+      <c r="L7" s="74">
+        <v>41086</v>
+      </c>
+      <c r="M7" s="74">
+        <v>41086</v>
+      </c>
+      <c r="N7" s="74">
+        <v>41086</v>
+      </c>
+      <c r="O7" s="74">
+        <v>41086</v>
+      </c>
+      <c r="P7" s="74">
+        <v>41086</v>
+      </c>
+      <c r="Q7" s="74">
+        <v>41086</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="18.75">
+      <c r="A8" s="71" t="s">
+        <v>10</v>
+      </c>
+      <c r="B8" s="75" t="s">
+        <v>42</v>
+      </c>
+      <c r="C8" s="75" t="s">
+        <v>42</v>
+      </c>
+      <c r="D8" s="75" t="s">
+        <v>42</v>
+      </c>
+      <c r="E8" s="75" t="s">
+        <v>42</v>
+      </c>
+      <c r="F8" s="75" t="s">
+        <v>42</v>
+      </c>
+      <c r="G8" s="75" t="s">
+        <v>42</v>
+      </c>
+      <c r="H8" s="75" t="s">
+        <v>42</v>
+      </c>
+      <c r="I8" s="75" t="s">
+        <v>42</v>
+      </c>
+      <c r="J8" s="75" t="s">
+        <v>42</v>
+      </c>
+      <c r="K8" s="75" t="s">
+        <v>42</v>
+      </c>
+      <c r="L8" s="75" t="s">
+        <v>42</v>
+      </c>
+      <c r="M8" s="75" t="s">
+        <v>42</v>
+      </c>
+      <c r="N8" s="75" t="s">
+        <v>42</v>
+      </c>
+      <c r="O8" s="75" t="s">
+        <v>42</v>
+      </c>
+      <c r="P8" s="75" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q8" s="75" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="18.75">
+      <c r="A9" s="71" t="s">
+        <v>12</v>
+      </c>
+      <c r="B9" s="76">
+        <v>60</v>
+      </c>
+      <c r="C9" s="76">
+        <v>60</v>
+      </c>
+      <c r="D9" s="76">
+        <v>60</v>
+      </c>
+      <c r="E9" s="76">
+        <v>60</v>
+      </c>
+      <c r="F9" s="76">
+        <v>60</v>
+      </c>
+      <c r="G9" s="76">
+        <v>60</v>
+      </c>
+      <c r="H9" s="76">
+        <v>60</v>
+      </c>
+      <c r="I9" s="76">
+        <v>60</v>
+      </c>
+      <c r="J9" s="76">
+        <v>60</v>
+      </c>
+      <c r="K9" s="76">
+        <v>60</v>
+      </c>
+      <c r="L9" s="76">
+        <v>60</v>
+      </c>
+      <c r="M9" s="76">
+        <v>60</v>
+      </c>
+      <c r="N9" s="76">
+        <v>60</v>
+      </c>
+      <c r="O9" s="76">
+        <v>60</v>
+      </c>
+      <c r="P9" s="76">
+        <v>60</v>
+      </c>
+      <c r="Q9" s="76">
+        <v>60</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="18.75">
+      <c r="A10" s="71" t="s">
+        <v>13</v>
+      </c>
+      <c r="B10" s="76" t="s">
+        <v>69</v>
+      </c>
+      <c r="C10" s="76" t="s">
+        <v>69</v>
+      </c>
+      <c r="D10" s="76" t="s">
+        <v>69</v>
+      </c>
+      <c r="E10" s="76" t="s">
+        <v>69</v>
+      </c>
+      <c r="F10" s="76" t="s">
+        <v>69</v>
+      </c>
+      <c r="G10" s="76" t="s">
+        <v>69</v>
+      </c>
+      <c r="H10" s="76" t="s">
+        <v>69</v>
+      </c>
+      <c r="I10" s="76" t="s">
+        <v>69</v>
+      </c>
+      <c r="J10" s="76" t="s">
+        <v>69</v>
+      </c>
+      <c r="K10" s="76" t="s">
+        <v>69</v>
+      </c>
+      <c r="L10" s="76" t="s">
+        <v>69</v>
+      </c>
+      <c r="M10" s="76" t="s">
+        <v>69</v>
+      </c>
+      <c r="N10" s="76" t="s">
+        <v>69</v>
+      </c>
+      <c r="O10" s="76" t="s">
+        <v>69</v>
+      </c>
+      <c r="P10" s="76" t="s">
+        <v>69</v>
+      </c>
+      <c r="Q10" s="76" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="18.75">
+      <c r="A11" s="71" t="s">
+        <v>14</v>
+      </c>
+      <c r="B11" s="75" t="s">
+        <v>70</v>
+      </c>
+      <c r="C11" s="75" t="s">
+        <v>70</v>
+      </c>
+      <c r="D11" s="75" t="s">
+        <v>70</v>
+      </c>
+      <c r="E11" s="75" t="s">
+        <v>70</v>
+      </c>
+      <c r="F11" s="75" t="s">
+        <v>70</v>
+      </c>
+      <c r="G11" s="75" t="s">
+        <v>70</v>
+      </c>
+      <c r="H11" s="75" t="s">
+        <v>70</v>
+      </c>
+      <c r="I11" s="75" t="s">
+        <v>70</v>
+      </c>
+      <c r="J11" s="75" t="s">
+        <v>70</v>
+      </c>
+      <c r="K11" s="75" t="s">
+        <v>70</v>
+      </c>
+      <c r="L11" s="75" t="s">
+        <v>70</v>
+      </c>
+      <c r="M11" s="75" t="s">
+        <v>70</v>
+      </c>
+      <c r="N11" s="75" t="s">
+        <v>70</v>
+      </c>
+      <c r="O11" s="75" t="s">
+        <v>70</v>
+      </c>
+      <c r="P11" s="75" t="s">
+        <v>70</v>
+      </c>
+      <c r="Q11" s="75" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="18.75">
+      <c r="A12" s="71" t="s">
+        <v>16</v>
+      </c>
+      <c r="B12" s="72">
+        <v>33.73</v>
+      </c>
+      <c r="C12" s="72">
+        <v>33.73</v>
+      </c>
+      <c r="D12" s="72">
+        <v>33.73</v>
+      </c>
+      <c r="E12" s="72">
+        <v>33.73</v>
+      </c>
+      <c r="F12" s="72">
+        <v>33.73</v>
+      </c>
+      <c r="G12" s="72">
+        <v>33.73</v>
+      </c>
+      <c r="H12" s="72">
+        <v>33.73</v>
+      </c>
+      <c r="I12" s="72">
+        <v>33.73</v>
+      </c>
+      <c r="J12" s="72">
+        <v>33.73</v>
+      </c>
+      <c r="K12" s="72">
+        <v>33.73</v>
+      </c>
+      <c r="L12" s="72">
+        <v>33.73</v>
+      </c>
+      <c r="M12" s="72">
+        <v>33.73</v>
+      </c>
+      <c r="N12" s="72">
+        <v>33.73</v>
+      </c>
+      <c r="O12" s="72">
+        <v>33.73</v>
+      </c>
+      <c r="P12" s="72">
+        <v>33.73</v>
+      </c>
+      <c r="Q12" s="72">
+        <v>33.73</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="18.75">
+      <c r="A13" s="71" t="s">
+        <v>17</v>
+      </c>
+      <c r="B13" s="76">
+        <v>225</v>
+      </c>
+      <c r="C13" s="76">
+        <v>225</v>
+      </c>
+      <c r="D13" s="76">
+        <v>225</v>
+      </c>
+      <c r="E13" s="76">
+        <v>225</v>
+      </c>
+      <c r="F13" s="76">
+        <v>225</v>
+      </c>
+      <c r="G13" s="76">
+        <v>225</v>
+      </c>
+      <c r="H13" s="76">
+        <v>225</v>
+      </c>
+      <c r="I13" s="76">
+        <v>225</v>
+      </c>
+      <c r="J13" s="76">
+        <v>225</v>
+      </c>
+      <c r="K13" s="76">
+        <v>225</v>
+      </c>
+      <c r="L13" s="76">
+        <v>225</v>
+      </c>
+      <c r="M13" s="76">
+        <v>225</v>
+      </c>
+      <c r="N13" s="76">
+        <v>225</v>
+      </c>
+      <c r="O13" s="76">
+        <v>225</v>
+      </c>
+      <c r="P13" s="76">
+        <v>225</v>
+      </c>
+      <c r="Q13" s="76">
+        <v>225</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="18.75">
+      <c r="A14" s="57" t="s">
+        <v>71</v>
+      </c>
+      <c r="B14" s="77" t="b">
+        <v>0</v>
+      </c>
+      <c r="C14" s="77" t="b">
+        <v>0</v>
+      </c>
+      <c r="D14" s="77" t="b">
+        <v>0</v>
+      </c>
+      <c r="E14" s="77" t="b">
+        <v>0</v>
+      </c>
+      <c r="F14" s="77" t="b">
+        <v>0</v>
+      </c>
+      <c r="G14" s="77" t="b">
+        <v>0</v>
+      </c>
+      <c r="H14" s="77" t="b">
+        <v>0</v>
+      </c>
+      <c r="I14" s="77" t="b">
+        <v>0</v>
+      </c>
+      <c r="J14" s="77" t="b">
+        <v>0</v>
+      </c>
+      <c r="K14" s="77" t="b">
+        <v>0</v>
+      </c>
+      <c r="L14" s="77" t="b">
+        <v>0</v>
+      </c>
+      <c r="M14" s="77" t="b">
+        <v>0</v>
+      </c>
+      <c r="N14" s="77" t="b">
+        <v>0</v>
+      </c>
+      <c r="O14" s="77" t="b">
+        <v>0</v>
+      </c>
+      <c r="P14" s="77" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q14" s="77" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="18.75">
+      <c r="A15" s="78" t="s">
+        <v>72</v>
+      </c>
+      <c r="B15" s="79">
+        <v>111</v>
+      </c>
+      <c r="C15" s="79">
+        <v>111</v>
+      </c>
+      <c r="D15" s="79">
+        <v>111</v>
+      </c>
+      <c r="E15" s="79">
+        <v>111</v>
+      </c>
+      <c r="F15" s="79">
+        <v>111</v>
+      </c>
+      <c r="G15" s="79">
+        <v>111</v>
+      </c>
+      <c r="H15" s="79">
+        <v>111</v>
+      </c>
+      <c r="I15" s="79">
+        <v>111</v>
+      </c>
+      <c r="J15" s="79">
+        <v>111</v>
+      </c>
+      <c r="K15" s="79">
+        <v>111</v>
+      </c>
+      <c r="L15" s="79">
+        <v>111</v>
+      </c>
+      <c r="M15" s="79">
+        <v>111</v>
+      </c>
+      <c r="N15" s="79">
+        <v>111</v>
+      </c>
+      <c r="O15" s="79">
+        <v>111</v>
+      </c>
+      <c r="P15" s="79">
+        <v>111</v>
+      </c>
+      <c r="Q15" s="79">
+        <v>111</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="19.5">
+      <c r="A16" s="78" t="s">
+        <v>73</v>
+      </c>
+      <c r="B16" s="79">
+        <v>61.24</v>
+      </c>
+      <c r="C16" s="79">
+        <v>61.24</v>
+      </c>
+      <c r="D16" s="79">
+        <v>61.24</v>
+      </c>
+      <c r="E16" s="79">
+        <v>61.24</v>
+      </c>
+      <c r="F16" s="79">
+        <v>61.24</v>
+      </c>
+      <c r="G16" s="79">
+        <v>61.24</v>
+      </c>
+      <c r="H16" s="79">
+        <v>61.24</v>
+      </c>
+      <c r="I16" s="79">
+        <v>61.24</v>
+      </c>
+      <c r="J16" s="79">
+        <v>61.24</v>
+      </c>
+      <c r="K16" s="79">
+        <v>61.24</v>
+      </c>
+      <c r="L16" s="79">
+        <v>61.24</v>
+      </c>
+      <c r="M16" s="79">
+        <v>61.24</v>
+      </c>
+      <c r="N16" s="79">
+        <v>61.24</v>
+      </c>
+      <c r="O16" s="79">
+        <v>61.24</v>
+      </c>
+      <c r="P16" s="79">
+        <v>61.24</v>
+      </c>
+      <c r="Q16" s="79">
+        <v>61.24</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="19.5">
+      <c r="A17" s="78" t="s">
+        <v>74</v>
+      </c>
+      <c r="B17" s="79">
+        <v>3</v>
+      </c>
+      <c r="C17" s="79">
+        <v>4</v>
+      </c>
+      <c r="D17" s="79">
+        <v>5</v>
+      </c>
+      <c r="E17" s="79">
+        <v>6</v>
+      </c>
+      <c r="F17" s="79">
+        <v>7</v>
+      </c>
+      <c r="G17" s="79">
+        <v>4</v>
+      </c>
+      <c r="H17" s="79">
+        <v>5</v>
+      </c>
+      <c r="I17" s="79">
+        <v>6</v>
+      </c>
+      <c r="J17" s="79">
+        <v>3</v>
+      </c>
+      <c r="K17" s="79">
+        <v>4</v>
+      </c>
+      <c r="L17" s="79">
+        <v>5</v>
+      </c>
+      <c r="M17" s="79">
+        <v>6</v>
+      </c>
+      <c r="N17" s="79">
+        <v>3</v>
+      </c>
+      <c r="O17" s="79">
+        <v>4</v>
+      </c>
+      <c r="P17" s="79">
+        <v>5</v>
+      </c>
+      <c r="Q17" s="79">
+        <v>6</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="19.5">
+      <c r="A18" s="78" t="s">
+        <v>75</v>
+      </c>
+      <c r="B18" s="79">
+        <v>2</v>
+      </c>
+      <c r="C18" s="79">
+        <v>2</v>
+      </c>
+      <c r="D18" s="79">
+        <v>2</v>
+      </c>
+      <c r="E18" s="79">
+        <v>2</v>
+      </c>
+      <c r="F18" s="79">
+        <v>2</v>
+      </c>
+      <c r="G18" s="79">
+        <v>1</v>
+      </c>
+      <c r="H18" s="79">
+        <v>1</v>
+      </c>
+      <c r="I18" s="79">
+        <v>1</v>
+      </c>
+      <c r="J18" s="79">
+        <v>1</v>
+      </c>
+      <c r="K18" s="79">
+        <v>1</v>
+      </c>
+      <c r="L18" s="79">
+        <v>1</v>
+      </c>
+      <c r="M18" s="79">
+        <v>1</v>
+      </c>
+      <c r="N18" s="79">
+        <v>1</v>
+      </c>
+      <c r="O18" s="79">
+        <v>1</v>
+      </c>
+      <c r="P18" s="79">
+        <v>1</v>
+      </c>
+      <c r="Q18" s="79">
+        <v>1</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="19.5">
+      <c r="A19" s="78" t="s">
+        <v>76</v>
+      </c>
+      <c r="B19" s="79" t="s">
+        <v>77</v>
+      </c>
+      <c r="C19" s="79" t="s">
+        <v>77</v>
+      </c>
+      <c r="D19" s="79" t="s">
+        <v>77</v>
+      </c>
+      <c r="E19" s="79" t="s">
+        <v>77</v>
+      </c>
+      <c r="F19" s="79" t="s">
+        <v>77</v>
+      </c>
+      <c r="G19" s="79" t="s">
+        <v>77</v>
+      </c>
+      <c r="H19" s="79" t="s">
+        <v>77</v>
+      </c>
+      <c r="I19" s="79" t="s">
+        <v>77</v>
+      </c>
+      <c r="J19" s="79" t="s">
+        <v>77</v>
+      </c>
+      <c r="K19" s="79" t="s">
+        <v>77</v>
+      </c>
+      <c r="L19" s="79" t="s">
+        <v>77</v>
+      </c>
+      <c r="M19" s="79" t="s">
+        <v>77</v>
+      </c>
+      <c r="N19" s="79" t="s">
+        <v>77</v>
+      </c>
+      <c r="O19" s="79" t="s">
+        <v>77</v>
+      </c>
+      <c r="P19" s="79" t="s">
+        <v>77</v>
+      </c>
+      <c r="Q19" s="79" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="19.5">
+      <c r="A20" s="78" t="s">
+        <v>78</v>
+      </c>
+      <c r="B20" s="79" t="s">
+        <v>79</v>
+      </c>
+      <c r="C20" s="79" t="s">
+        <v>79</v>
+      </c>
+      <c r="D20" s="79" t="s">
+        <v>79</v>
+      </c>
+      <c r="E20" s="79" t="s">
+        <v>79</v>
+      </c>
+      <c r="F20" s="79" t="s">
+        <v>79</v>
+      </c>
+      <c r="G20" s="79" t="s">
+        <v>80</v>
+      </c>
+      <c r="H20" s="79" t="s">
+        <v>80</v>
+      </c>
+      <c r="I20" s="79" t="s">
+        <v>80</v>
+      </c>
+      <c r="J20" s="79" t="s">
+        <v>81</v>
+      </c>
+      <c r="K20" s="79" t="s">
+        <v>81</v>
+      </c>
+      <c r="L20" s="79" t="s">
+        <v>81</v>
+      </c>
+      <c r="M20" s="79" t="s">
+        <v>81</v>
+      </c>
+      <c r="N20" s="79" t="s">
+        <v>82</v>
+      </c>
+      <c r="O20" s="79" t="s">
+        <v>82</v>
+      </c>
+      <c r="P20" s="79" t="s">
+        <v>82</v>
+      </c>
+      <c r="Q20" s="79" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="19.5">
+      <c r="A21" s="78" t="s">
+        <v>83</v>
+      </c>
+      <c r="B21" s="80">
+        <v>33.5</v>
+      </c>
+      <c r="C21" s="80">
+        <v>33.5</v>
+      </c>
+      <c r="D21" s="80">
+        <v>33.5</v>
+      </c>
+      <c r="E21" s="80">
+        <v>33.5</v>
+      </c>
+      <c r="F21" s="80">
+        <v>33.5</v>
+      </c>
+      <c r="G21" s="80">
+        <v>33.5</v>
+      </c>
+      <c r="H21" s="80">
+        <v>33.5</v>
+      </c>
+      <c r="I21" s="80">
+        <v>33.5</v>
+      </c>
+      <c r="J21" s="80">
+        <v>33.5</v>
+      </c>
+      <c r="K21" s="80">
+        <v>33.5</v>
+      </c>
+      <c r="L21" s="80">
+        <v>33.5</v>
+      </c>
+      <c r="M21" s="80">
+        <v>33.5</v>
+      </c>
+      <c r="N21" s="80">
+        <v>33.5</v>
+      </c>
+      <c r="O21" s="80">
+        <v>33.5</v>
+      </c>
+      <c r="P21" s="80">
+        <v>33.5</v>
+      </c>
+      <c r="Q21" s="80">
+        <v>33.5</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="19.5">
+      <c r="A22" s="78" t="s">
+        <v>84</v>
+      </c>
+      <c r="B22" s="79">
+        <v>66</v>
+      </c>
+      <c r="C22" s="79">
+        <v>66</v>
+      </c>
+      <c r="D22" s="79">
+        <v>66</v>
+      </c>
+      <c r="E22" s="79">
+        <v>66</v>
+      </c>
+      <c r="F22" s="79">
+        <v>66</v>
+      </c>
+      <c r="G22" s="79">
+        <v>66</v>
+      </c>
+      <c r="H22" s="79">
+        <v>66</v>
+      </c>
+      <c r="I22" s="79">
+        <v>66</v>
+      </c>
+      <c r="J22" s="79">
+        <v>66</v>
+      </c>
+      <c r="K22" s="79">
+        <v>66</v>
+      </c>
+      <c r="L22" s="79">
+        <v>66</v>
+      </c>
+      <c r="M22" s="79">
+        <v>66</v>
+      </c>
+      <c r="N22" s="79">
+        <v>66</v>
+      </c>
+      <c r="O22" s="79">
+        <v>66</v>
+      </c>
+      <c r="P22" s="79">
+        <v>66</v>
+      </c>
+      <c r="Q22" s="79">
+        <v>66</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="19.5">
+      <c r="A23" s="78" t="s">
+        <v>85</v>
+      </c>
+      <c r="B23" s="81">
+        <v>0.038</v>
+      </c>
+      <c r="C23" s="81">
+        <v>0.038</v>
+      </c>
+      <c r="D23" s="81">
+        <v>0.038</v>
+      </c>
+      <c r="E23" s="81">
+        <v>0.038</v>
+      </c>
+      <c r="F23" s="81">
+        <v>0.038</v>
+      </c>
+      <c r="G23" s="81">
+        <v>0.038</v>
+      </c>
+      <c r="H23" s="81">
+        <v>0.038</v>
+      </c>
+      <c r="I23" s="81">
+        <v>0.038</v>
+      </c>
+      <c r="J23" s="81">
+        <v>0.038</v>
+      </c>
+      <c r="K23" s="81">
+        <v>0.038</v>
+      </c>
+      <c r="L23" s="81">
+        <v>0.038</v>
+      </c>
+      <c r="M23" s="81">
+        <v>0.038</v>
+      </c>
+      <c r="N23" s="81">
+        <v>0.038</v>
+      </c>
+      <c r="O23" s="81">
+        <v>0.038</v>
+      </c>
+      <c r="P23" s="81">
+        <v>0.038</v>
+      </c>
+      <c r="Q23" s="81">
+        <v>0.038</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="20.25">
+      <c r="A24" s="78" t="s">
+        <v>86</v>
+      </c>
+      <c r="B24" s="79" t="s">
+        <v>87</v>
+      </c>
+      <c r="C24" s="79" t="s">
+        <v>87</v>
+      </c>
+      <c r="D24" s="79" t="s">
+        <v>87</v>
+      </c>
+      <c r="E24" s="79" t="s">
+        <v>87</v>
+      </c>
+      <c r="F24" s="79" t="s">
+        <v>87</v>
+      </c>
+      <c r="G24" s="79" t="s">
+        <v>87</v>
+      </c>
+      <c r="H24" s="79" t="s">
+        <v>87</v>
+      </c>
+      <c r="I24" s="79" t="s">
+        <v>87</v>
+      </c>
+      <c r="J24" s="79" t="s">
+        <v>87</v>
+      </c>
+      <c r="K24" s="79" t="s">
+        <v>87</v>
+      </c>
+      <c r="L24" s="79" t="s">
+        <v>87</v>
+      </c>
+      <c r="M24" s="79" t="s">
+        <v>87</v>
+      </c>
+      <c r="N24" s="79" t="s">
+        <v>87</v>
+      </c>
+      <c r="O24" s="79" t="s">
+        <v>87</v>
+      </c>
+      <c r="P24" s="79" t="s">
+        <v>87</v>
+      </c>
+      <c r="Q24" s="79" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="18.75">
+      <c r="A25" s="34" t="s">
+        <v>7</v>
+      </c>
+      <c r="B25" s="82">
+        <v>40548</v>
+      </c>
+      <c r="C25" s="82">
+        <v>40548</v>
+      </c>
+      <c r="D25" s="82">
+        <v>40548</v>
+      </c>
+      <c r="E25" s="82">
+        <v>40548</v>
+      </c>
+      <c r="F25" s="82">
+        <v>40548</v>
+      </c>
+      <c r="G25" s="82">
+        <v>40548</v>
+      </c>
+      <c r="H25" s="82">
+        <v>40548</v>
+      </c>
+      <c r="I25" s="82">
+        <v>40548</v>
+      </c>
+      <c r="J25" s="82">
+        <v>40548</v>
+      </c>
+      <c r="K25" s="82">
+        <v>40548</v>
+      </c>
+      <c r="L25" s="82">
+        <v>40548</v>
+      </c>
+      <c r="M25" s="82">
+        <v>40548</v>
+      </c>
+      <c r="N25" s="82">
+        <v>40548</v>
+      </c>
+      <c r="O25" s="82">
+        <v>40548</v>
+      </c>
+      <c r="P25" s="82">
+        <v>40548</v>
+      </c>
+      <c r="Q25" s="82">
+        <v>40548</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="26" customHeight="1" ht="18.75">
+      <c r="A26" s="71" t="s">
+        <v>8</v>
+      </c>
+      <c r="B26" s="83">
+        <v>40913</v>
+      </c>
+      <c r="C26" s="83">
+        <v>40913</v>
+      </c>
+      <c r="D26" s="83">
+        <v>40913</v>
+      </c>
+      <c r="E26" s="83">
+        <v>40913</v>
+      </c>
+      <c r="F26" s="83">
+        <v>40913</v>
+      </c>
+      <c r="G26" s="83">
+        <v>40913</v>
+      </c>
+      <c r="H26" s="83">
+        <v>40913</v>
+      </c>
+      <c r="I26" s="83">
+        <v>40913</v>
+      </c>
+      <c r="J26" s="83">
+        <v>40913</v>
+      </c>
+      <c r="K26" s="83">
+        <v>40913</v>
+      </c>
+      <c r="L26" s="83">
+        <v>40913</v>
+      </c>
+      <c r="M26" s="83">
+        <v>40913</v>
+      </c>
+      <c r="N26" s="83">
+        <v>40913</v>
+      </c>
+      <c r="O26" s="83">
+        <v>40913</v>
+      </c>
+      <c r="P26" s="83">
+        <v>40913</v>
+      </c>
+      <c r="Q26" s="83">
+        <v>40913</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="27" customHeight="1" ht="18.75">
+      <c r="A27" s="71" t="s">
+        <v>12</v>
+      </c>
+      <c r="B27" s="75" t="s">
+        <v>88</v>
+      </c>
+      <c r="C27" s="75" t="s">
+        <v>88</v>
+      </c>
+      <c r="D27" s="75" t="s">
+        <v>88</v>
+      </c>
+      <c r="E27" s="75" t="s">
+        <v>88</v>
+      </c>
+      <c r="F27" s="75" t="s">
+        <v>88</v>
+      </c>
+      <c r="G27" s="75" t="s">
+        <v>88</v>
+      </c>
+      <c r="H27" s="75" t="s">
+        <v>88</v>
+      </c>
+      <c r="I27" s="75" t="s">
+        <v>88</v>
+      </c>
+      <c r="J27" s="75" t="s">
+        <v>88</v>
+      </c>
+      <c r="K27" s="75" t="s">
+        <v>88</v>
+      </c>
+      <c r="L27" s="75" t="s">
+        <v>88</v>
+      </c>
+      <c r="M27" s="75" t="s">
+        <v>88</v>
+      </c>
+      <c r="N27" s="75" t="s">
+        <v>88</v>
+      </c>
+      <c r="O27" s="75" t="s">
+        <v>88</v>
+      </c>
+      <c r="P27" s="75" t="s">
+        <v>88</v>
+      </c>
+      <c r="Q27" s="75" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="28" customHeight="1" ht="18.75">
+      <c r="A28" s="71" t="s">
+        <v>13</v>
+      </c>
+      <c r="B28" s="76">
+        <v>26</v>
+      </c>
+      <c r="C28" s="76">
+        <v>26</v>
+      </c>
+      <c r="D28" s="76">
+        <v>26</v>
+      </c>
+      <c r="E28" s="76">
+        <v>26</v>
+      </c>
+      <c r="F28" s="76">
+        <v>26</v>
+      </c>
+      <c r="G28" s="76">
+        <v>26</v>
+      </c>
+      <c r="H28" s="76">
+        <v>26</v>
+      </c>
+      <c r="I28" s="76">
+        <v>26</v>
+      </c>
+      <c r="J28" s="76">
+        <v>26</v>
+      </c>
+      <c r="K28" s="76">
+        <v>26</v>
+      </c>
+      <c r="L28" s="76">
+        <v>26</v>
+      </c>
+      <c r="M28" s="76">
+        <v>26</v>
+      </c>
+      <c r="N28" s="76">
+        <v>26</v>
+      </c>
+      <c r="O28" s="76">
+        <v>26</v>
+      </c>
+      <c r="P28" s="76">
+        <v>26</v>
+      </c>
+      <c r="Q28" s="76">
+        <v>26</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="29" customHeight="1" ht="18.75">
+      <c r="A29" s="71" t="s">
+        <v>9</v>
+      </c>
+      <c r="B29" s="75" t="s">
+        <v>89</v>
+      </c>
+      <c r="C29" s="75" t="s">
+        <v>89</v>
+      </c>
+      <c r="D29" s="75" t="s">
+        <v>89</v>
+      </c>
+      <c r="E29" s="75" t="s">
+        <v>89</v>
+      </c>
+      <c r="F29" s="75" t="s">
+        <v>89</v>
+      </c>
+      <c r="G29" s="75" t="s">
+        <v>89</v>
+      </c>
+      <c r="H29" s="75" t="s">
+        <v>89</v>
+      </c>
+      <c r="I29" s="75" t="s">
+        <v>89</v>
+      </c>
+      <c r="J29" s="75" t="s">
+        <v>89</v>
+      </c>
+      <c r="K29" s="75" t="s">
+        <v>89</v>
+      </c>
+      <c r="L29" s="75" t="s">
+        <v>89</v>
+      </c>
+      <c r="M29" s="75" t="s">
+        <v>89</v>
+      </c>
+      <c r="N29" s="75" t="s">
+        <v>89</v>
+      </c>
+      <c r="O29" s="75" t="s">
+        <v>89</v>
+      </c>
+      <c r="P29" s="75" t="s">
+        <v>89</v>
+      </c>
+      <c r="Q29" s="75" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="30" customHeight="1" ht="18.75">
+      <c r="A30" s="84" t="s">
+        <v>12</v>
+      </c>
+      <c r="B30" s="85">
+        <v>35</v>
+      </c>
+      <c r="C30" s="85">
+        <v>35</v>
+      </c>
+      <c r="D30" s="85">
+        <v>35</v>
+      </c>
+      <c r="E30" s="85">
+        <v>35</v>
+      </c>
+      <c r="F30" s="85">
+        <v>35</v>
+      </c>
+      <c r="G30" s="85">
+        <v>35</v>
+      </c>
+      <c r="H30" s="85">
+        <v>35</v>
+      </c>
+      <c r="I30" s="85">
+        <v>35</v>
+      </c>
+      <c r="J30" s="85">
+        <v>35</v>
+      </c>
+      <c r="K30" s="85">
+        <v>35</v>
+      </c>
+      <c r="L30" s="85">
+        <v>35</v>
+      </c>
+      <c r="M30" s="85">
+        <v>35</v>
+      </c>
+      <c r="N30" s="85">
+        <v>35</v>
+      </c>
+      <c r="O30" s="85">
+        <v>35</v>
+      </c>
+      <c r="P30" s="85">
+        <v>35</v>
+      </c>
+      <c r="Q30" s="85">
+        <v>35</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="31" customHeight="1" ht="18.75">
+      <c r="A31" s="84" t="s">
+        <v>90</v>
+      </c>
+      <c r="B31" s="85">
+        <v>324</v>
+      </c>
+      <c r="C31" s="85">
+        <v>324</v>
+      </c>
+      <c r="D31" s="85">
+        <v>324</v>
+      </c>
+      <c r="E31" s="85">
+        <v>324</v>
+      </c>
+      <c r="F31" s="85">
+        <v>324</v>
+      </c>
+      <c r="G31" s="85">
+        <v>324</v>
+      </c>
+      <c r="H31" s="85">
+        <v>324</v>
+      </c>
+      <c r="I31" s="85">
+        <v>324</v>
+      </c>
+      <c r="J31" s="85">
+        <v>324</v>
+      </c>
+      <c r="K31" s="85">
+        <v>324</v>
+      </c>
+      <c r="L31" s="85">
+        <v>324</v>
+      </c>
+      <c r="M31" s="85">
+        <v>324</v>
+      </c>
+      <c r="N31" s="85">
+        <v>324</v>
+      </c>
+      <c r="O31" s="85">
+        <v>324</v>
+      </c>
+      <c r="P31" s="85">
+        <v>324</v>
+      </c>
+      <c r="Q31" s="85">
+        <v>324</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
@@ -3675,7 +5327,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
@@ -3913,7 +5565,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
@@ -4560,7 +6212,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
@@ -4924,7 +6576,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <outlinePr summaryBelow="0"/>

</xml_diff>

<commit_message>
graph for pumping potential of various pumps
</commit_message>
<xml_diff>
--- a/heliostrome/jip_project/results/Factors to run simulation.xlsx
+++ b/heliostrome/jip_project/results/Factors to run simulation.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="593" uniqueCount="157">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="593" uniqueCount="156">
   <si>
     <t>Evaluation of AquaCrop for potato yield and biomass
 simulation under different water amounts in drip and
@@ -261,9 +261,6 @@
   </si>
   <si>
     <t>Pump Name</t>
-  </si>
-  <si>
-    <t>Lorentz_ps2_1800</t>
   </si>
   <si>
     <t>SCB_10_150_180_BL</t>
@@ -506,7 +503,7 @@
     <numFmt numFmtId="165" formatCode="#,##0.0"/>
     <numFmt numFmtId="166" formatCode="#,##0.000"/>
   </numFmts>
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -550,6 +547,12 @@
       <sz val="10"/>
       <color rgb="FF333333"/>
       <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
       <family val="2"/>
     </font>
     <font>
@@ -1023,10 +1026,10 @@
     <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="14" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf xfId="0" numFmtId="14" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="13" applyBorder="1" fontId="7" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="14" applyNumberFormat="1" borderId="13" applyBorder="1" fontId="7" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf xfId="0" numFmtId="14" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
@@ -1035,10 +1038,10 @@
     <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="13" applyBorder="1" fontId="4" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="13" applyBorder="1" fontId="7" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="13" applyBorder="1" fontId="7" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="14" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
@@ -1122,7 +1125,7 @@
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="13" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="14" applyBorder="1" fontId="7" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="14" applyBorder="1" fontId="8" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="14" applyBorder="1" fontId="5" applyFont="1" fillId="0" applyAlignment="1">
@@ -1200,7 +1203,7 @@
     <xf xfId="0" numFmtId="0" borderId="20" applyBorder="1" fontId="1" applyFont="1" fillId="4" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="20" applyBorder="1" fontId="8" applyFont="1" fillId="6" applyFill="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="20" applyBorder="1" fontId="9" applyFont="1" fillId="6" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
@@ -1531,27 +1534,27 @@
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
       <c r="A1" s="45"/>
       <c r="B1" s="58" t="s">
+        <v>138</v>
+      </c>
+      <c r="C1" s="58" t="s">
         <v>139</v>
-      </c>
-      <c r="C1" s="58" t="s">
-        <v>140</v>
       </c>
       <c r="D1" s="100" t="s">
         <v>54</v>
       </c>
       <c r="E1" s="58" t="s">
+        <v>140</v>
+      </c>
+      <c r="F1" s="58" t="s">
         <v>141</v>
       </c>
-      <c r="F1" s="58" t="s">
+      <c r="G1" s="100" t="s">
         <v>142</v>
-      </c>
-      <c r="G1" s="100" t="s">
-        <v>143</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75">
       <c r="A2" s="58" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B2" s="101"/>
       <c r="C2" s="101"/>
@@ -1562,7 +1565,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18.75">
       <c r="A3" s="58" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B3" s="101"/>
       <c r="C3" s="102"/>
@@ -1573,7 +1576,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18.75">
       <c r="A4" s="58" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B4" s="102"/>
       <c r="C4" s="104"/>
@@ -1584,7 +1587,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18.75">
       <c r="A5" s="58" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B5" s="102"/>
       <c r="C5" s="103"/>
@@ -1595,7 +1598,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18.75">
       <c r="A6" s="58" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B6" s="102"/>
       <c r="C6" s="103"/>
@@ -1606,7 +1609,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="18.75">
       <c r="A7" s="58" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B7" s="101"/>
       <c r="C7" s="101"/>
@@ -1617,7 +1620,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="18.75">
       <c r="A8" s="58" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B8" s="101"/>
       <c r="C8" s="102"/>
@@ -1628,7 +1631,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="18.75">
       <c r="A9" s="58" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B9" s="102"/>
       <c r="C9" s="102"/>
@@ -1639,7 +1642,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="18.75">
       <c r="A10" s="58" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B10" s="101"/>
       <c r="C10" s="101"/>
@@ -1650,7 +1653,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="18.75">
       <c r="A11" s="58" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B11" s="101"/>
       <c r="C11" s="102"/>
@@ -1661,7 +1664,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="18.75">
       <c r="A12" s="58" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B12" s="105"/>
       <c r="C12" s="105"/>
@@ -1672,7 +1675,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="18.75">
       <c r="A13" s="58" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B13" s="105"/>
       <c r="C13" s="105"/>
@@ -1683,7 +1686,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="18.75">
       <c r="A14" s="58" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B14" s="105"/>
       <c r="C14" s="105"/>
@@ -1755,7 +1758,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="70" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C2" s="70" t="s">
         <v>68</v>
@@ -1764,43 +1767,43 @@
         <v>68</v>
       </c>
       <c r="E2" s="70" t="s">
+        <v>91</v>
+      </c>
+      <c r="F2" s="70" t="s">
         <v>92</v>
       </c>
-      <c r="F2" s="70" t="s">
+      <c r="G2" s="70" t="s">
+        <v>91</v>
+      </c>
+      <c r="H2" s="70" t="s">
+        <v>92</v>
+      </c>
+      <c r="I2" s="70" t="s">
         <v>93</v>
       </c>
-      <c r="G2" s="70" t="s">
-        <v>92</v>
-      </c>
-      <c r="H2" s="70" t="s">
-        <v>93</v>
-      </c>
-      <c r="I2" s="70" t="s">
+      <c r="J2" s="70" t="s">
         <v>94</v>
       </c>
-      <c r="J2" s="70" t="s">
+      <c r="K2" s="70" t="s">
         <v>95</v>
       </c>
-      <c r="K2" s="70" t="s">
+      <c r="L2" s="70" t="s">
         <v>96</v>
       </c>
-      <c r="L2" s="70" t="s">
+      <c r="M2" s="70" t="s">
         <v>97</v>
       </c>
-      <c r="M2" s="70" t="s">
+      <c r="N2" s="70" t="s">
         <v>98</v>
       </c>
-      <c r="N2" s="70" t="s">
+      <c r="O2" s="70" t="s">
         <v>99</v>
       </c>
-      <c r="O2" s="70" t="s">
+      <c r="P2" s="87" t="s">
         <v>100</v>
       </c>
-      <c r="P2" s="87" t="s">
+      <c r="Q2" s="87" t="s">
         <v>101</v>
-      </c>
-      <c r="Q2" s="87" t="s">
-        <v>102</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18.75">
@@ -2274,10 +2277,10 @@
         <v>44</v>
       </c>
       <c r="P11" s="90" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="Q11" s="90" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="18.75">
@@ -2371,10 +2374,10 @@
         <v>453</v>
       </c>
       <c r="M13" s="75" t="s">
+        <v>103</v>
+      </c>
+      <c r="N13" s="75" t="s">
         <v>104</v>
-      </c>
-      <c r="N13" s="75" t="s">
-        <v>105</v>
       </c>
       <c r="O13" s="76">
         <v>430</v>
@@ -2709,57 +2712,57 @@
         <v>78</v>
       </c>
       <c r="B20" s="79" t="s">
+        <v>105</v>
+      </c>
+      <c r="C20" s="79" t="s">
+        <v>79</v>
+      </c>
+      <c r="D20" s="79" t="s">
+        <v>79</v>
+      </c>
+      <c r="E20" s="79" t="s">
+        <v>80</v>
+      </c>
+      <c r="F20" s="79" t="s">
+        <v>81</v>
+      </c>
+      <c r="G20" s="79" t="s">
         <v>106</v>
       </c>
-      <c r="C20" s="79" t="s">
-        <v>80</v>
-      </c>
-      <c r="D20" s="79" t="s">
-        <v>80</v>
-      </c>
-      <c r="E20" s="79" t="s">
-        <v>81</v>
-      </c>
-      <c r="F20" s="79" t="s">
-        <v>82</v>
-      </c>
-      <c r="G20" s="79" t="s">
-        <v>107</v>
-      </c>
       <c r="H20" s="79" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="I20" s="79" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="J20" s="79" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="K20" s="79" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="L20" s="79" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="M20" s="79" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="N20" s="79" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="O20" s="79" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="P20" s="94" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="Q20" s="94" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="19.5">
       <c r="A21" s="78" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B21" s="80">
         <v>33.5</v>
@@ -2812,7 +2815,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="19.5">
       <c r="A22" s="78" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B22" s="79">
         <v>66</v>
@@ -2865,7 +2868,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="19.5">
       <c r="A23" s="78" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B23" s="81">
         <v>0.038</v>
@@ -2918,55 +2921,55 @@
     </row>
     <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="19.5">
       <c r="A24" s="78" t="s">
+        <v>85</v>
+      </c>
+      <c r="B24" s="79" t="s">
         <v>86</v>
       </c>
-      <c r="B24" s="79" t="s">
-        <v>87</v>
-      </c>
       <c r="C24" s="79" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D24" s="79" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E24" s="79" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="F24" s="79" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="G24" s="79" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="H24" s="79" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="I24" s="79" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="J24" s="79" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="K24" s="79" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="L24" s="79" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="M24" s="79" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="N24" s="79" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="O24" s="79" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="P24" s="94" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="Q24" s="94" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="18.75">
@@ -2980,7 +2983,7 @@
         <v>40548</v>
       </c>
       <c r="D25" s="41" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E25" s="82">
         <v>40553</v>
@@ -2995,10 +2998,10 @@
         <v>40918</v>
       </c>
       <c r="I25" s="41" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="J25" s="41" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="K25" s="82">
         <v>40544</v>
@@ -3033,46 +3036,46 @@
         <v>40913</v>
       </c>
       <c r="D26" s="75" t="s">
+        <v>109</v>
+      </c>
+      <c r="E26" s="75" t="s">
         <v>110</v>
       </c>
-      <c r="E26" s="75" t="s">
+      <c r="F26" s="75" t="s">
+        <v>110</v>
+      </c>
+      <c r="G26" s="75" t="s">
         <v>111</v>
       </c>
-      <c r="F26" s="75" t="s">
+      <c r="H26" s="75" t="s">
         <v>111</v>
       </c>
-      <c r="G26" s="75" t="s">
+      <c r="I26" s="75" t="s">
         <v>112</v>
       </c>
-      <c r="H26" s="75" t="s">
+      <c r="J26" s="75" t="s">
         <v>112</v>
       </c>
-      <c r="I26" s="75" t="s">
+      <c r="K26" s="75" t="s">
         <v>113</v>
       </c>
-      <c r="J26" s="75" t="s">
+      <c r="L26" s="75" t="s">
         <v>113</v>
       </c>
-      <c r="K26" s="75" t="s">
+      <c r="M26" s="75" t="s">
         <v>114</v>
       </c>
-      <c r="L26" s="75" t="s">
+      <c r="N26" s="75" t="s">
         <v>114</v>
       </c>
-      <c r="M26" s="75" t="s">
-        <v>115</v>
-      </c>
-      <c r="N26" s="75" t="s">
-        <v>115</v>
-      </c>
       <c r="O26" s="75" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="P26" s="90" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="Q26" s="90" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="27" customHeight="1" ht="18.75">
@@ -3080,46 +3083,46 @@
         <v>12</v>
       </c>
       <c r="B27" s="75" t="s">
+        <v>115</v>
+      </c>
+      <c r="C27" s="75" t="s">
+        <v>87</v>
+      </c>
+      <c r="D27" s="75" t="s">
+        <v>87</v>
+      </c>
+      <c r="E27" s="75" t="s">
+        <v>87</v>
+      </c>
+      <c r="F27" s="75" t="s">
+        <v>115</v>
+      </c>
+      <c r="G27" s="75" t="s">
+        <v>87</v>
+      </c>
+      <c r="H27" s="75" t="s">
+        <v>115</v>
+      </c>
+      <c r="I27" s="75" t="s">
         <v>116</v>
       </c>
-      <c r="C27" s="75" t="s">
-        <v>88</v>
-      </c>
-      <c r="D27" s="75" t="s">
-        <v>88</v>
-      </c>
-      <c r="E27" s="75" t="s">
-        <v>88</v>
-      </c>
-      <c r="F27" s="75" t="s">
-        <v>116</v>
-      </c>
-      <c r="G27" s="75" t="s">
-        <v>88</v>
-      </c>
-      <c r="H27" s="75" t="s">
-        <v>116</v>
-      </c>
-      <c r="I27" s="75" t="s">
+      <c r="J27" s="75" t="s">
         <v>117</v>
       </c>
-      <c r="J27" s="75" t="s">
+      <c r="K27" s="75" t="s">
         <v>118</v>
       </c>
-      <c r="K27" s="75" t="s">
+      <c r="L27" s="75" t="s">
         <v>119</v>
       </c>
-      <c r="L27" s="75" t="s">
+      <c r="M27" s="75" t="s">
         <v>120</v>
       </c>
-      <c r="M27" s="75" t="s">
+      <c r="N27" s="75" t="s">
         <v>121</v>
       </c>
-      <c r="N27" s="75" t="s">
+      <c r="O27" s="75" t="s">
         <v>122</v>
-      </c>
-      <c r="O27" s="75" t="s">
-        <v>123</v>
       </c>
       <c r="P27" s="95">
         <v>100</v>
@@ -3173,10 +3176,10 @@
         <v>18</v>
       </c>
       <c r="P28" s="97" t="s">
+        <v>123</v>
+      </c>
+      <c r="Q28" s="90" t="s">
         <v>124</v>
-      </c>
-      <c r="Q28" s="90" t="s">
-        <v>125</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="29" customHeight="1" ht="18.75">
@@ -3187,46 +3190,46 @@
         <v>41086</v>
       </c>
       <c r="C29" s="75" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D29" s="75" t="s">
+        <v>125</v>
+      </c>
+      <c r="E29" s="75" t="s">
         <v>126</v>
       </c>
-      <c r="E29" s="75" t="s">
+      <c r="F29" s="75" t="s">
         <v>127</v>
       </c>
-      <c r="F29" s="75" t="s">
+      <c r="G29" s="75" t="s">
         <v>128</v>
       </c>
-      <c r="G29" s="75" t="s">
+      <c r="H29" s="75" t="s">
         <v>129</v>
       </c>
-      <c r="H29" s="75" t="s">
+      <c r="I29" s="75" t="s">
         <v>130</v>
       </c>
-      <c r="I29" s="75" t="s">
+      <c r="J29" s="75" t="s">
         <v>131</v>
       </c>
-      <c r="J29" s="75" t="s">
+      <c r="K29" s="75" t="s">
         <v>132</v>
       </c>
-      <c r="K29" s="75" t="s">
+      <c r="L29" s="75" t="s">
         <v>133</v>
       </c>
-      <c r="L29" s="75" t="s">
+      <c r="M29" s="75" t="s">
         <v>134</v>
       </c>
-      <c r="M29" s="75" t="s">
+      <c r="N29" s="75" t="s">
         <v>135</v>
       </c>
-      <c r="N29" s="75" t="s">
+      <c r="O29" s="75" t="s">
         <v>136</v>
       </c>
-      <c r="O29" s="75" t="s">
+      <c r="P29" s="90" t="s">
         <v>137</v>
-      </c>
-      <c r="P29" s="90" t="s">
-        <v>138</v>
       </c>
       <c r="Q29" s="73">
         <v>38444</v>
@@ -3287,7 +3290,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="31" customHeight="1" ht="18.75">
       <c r="A31" s="84" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B31" s="85">
         <v>324</v>
@@ -4085,7 +4088,7 @@
         <v>0</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="19.5">
       <c r="A15" s="78" t="s">
         <v>72</v>
       </c>
@@ -4196,31 +4199,31 @@
         <v>74</v>
       </c>
       <c r="B17" s="79">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C17" s="79">
+        <v>5</v>
+      </c>
+      <c r="D17" s="79">
+        <v>6</v>
+      </c>
+      <c r="E17" s="79">
         <v>4</v>
       </c>
-      <c r="D17" s="79">
+      <c r="F17" s="79">
         <v>5</v>
       </c>
-      <c r="E17" s="79">
+      <c r="G17" s="79">
         <v>6</v>
       </c>
-      <c r="F17" s="79">
-        <v>7</v>
-      </c>
-      <c r="G17" s="79">
+      <c r="H17" s="79">
         <v>4</v>
       </c>
-      <c r="H17" s="79">
+      <c r="I17" s="79">
         <v>5</v>
       </c>
-      <c r="I17" s="79">
+      <c r="J17" s="79">
         <v>6</v>
-      </c>
-      <c r="J17" s="79">
-        <v>3</v>
       </c>
       <c r="K17" s="79">
         <v>4</v>
@@ -4249,19 +4252,19 @@
         <v>75</v>
       </c>
       <c r="B18" s="79">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C18" s="79">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D18" s="79">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E18" s="79">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F18" s="79">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G18" s="79">
         <v>1</v>
@@ -4364,48 +4367,48 @@
         <v>79</v>
       </c>
       <c r="E20" s="79" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="F20" s="79" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="G20" s="79" t="s">
         <v>80</v>
       </c>
       <c r="H20" s="79" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="I20" s="79" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="J20" s="79" t="s">
         <v>81</v>
       </c>
       <c r="K20" s="79" t="s">
+        <v>80</v>
+      </c>
+      <c r="L20" s="79" t="s">
+        <v>80</v>
+      </c>
+      <c r="M20" s="79" t="s">
+        <v>80</v>
+      </c>
+      <c r="N20" s="79" t="s">
         <v>81</v>
       </c>
-      <c r="L20" s="79" t="s">
+      <c r="O20" s="79" t="s">
         <v>81</v>
       </c>
-      <c r="M20" s="79" t="s">
+      <c r="P20" s="79" t="s">
         <v>81</v>
       </c>
-      <c r="N20" s="79" t="s">
-        <v>82</v>
-      </c>
-      <c r="O20" s="79" t="s">
-        <v>82</v>
-      </c>
-      <c r="P20" s="79" t="s">
-        <v>82</v>
-      </c>
       <c r="Q20" s="79" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="19.5">
       <c r="A21" s="78" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B21" s="80">
         <v>33.5</v>
@@ -4458,7 +4461,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="19.5">
       <c r="A22" s="78" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B22" s="79">
         <v>66</v>
@@ -4511,7 +4514,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="19.5">
       <c r="A23" s="78" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B23" s="81">
         <v>0.038</v>
@@ -4562,57 +4565,57 @@
         <v>0.038</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="20.25">
+    <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="19.5">
       <c r="A24" s="78" t="s">
+        <v>85</v>
+      </c>
+      <c r="B24" s="79" t="s">
         <v>86</v>
       </c>
-      <c r="B24" s="79" t="s">
-        <v>87</v>
-      </c>
       <c r="C24" s="79" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D24" s="79" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E24" s="79" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="F24" s="79" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="G24" s="79" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="H24" s="79" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="I24" s="79" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="J24" s="79" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="K24" s="79" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="L24" s="79" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="M24" s="79" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="N24" s="79" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="O24" s="79" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="P24" s="79" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="Q24" s="79" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="18.75">
@@ -4726,52 +4729,52 @@
         <v>12</v>
       </c>
       <c r="B27" s="75" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C27" s="75" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D27" s="75" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E27" s="75" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="F27" s="75" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G27" s="75" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="H27" s="75" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="I27" s="75" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="J27" s="75" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="K27" s="75" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="L27" s="75" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="M27" s="75" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="N27" s="75" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="O27" s="75" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="P27" s="75" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="Q27" s="75" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="28" customHeight="1" ht="18.75">
@@ -4832,52 +4835,52 @@
         <v>9</v>
       </c>
       <c r="B29" s="75" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C29" s="75" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D29" s="75" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E29" s="75" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="F29" s="75" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="G29" s="75" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="H29" s="75" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="I29" s="75" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="J29" s="75" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="K29" s="75" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="L29" s="75" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="M29" s="75" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="N29" s="75" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="O29" s="75" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="P29" s="75" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="Q29" s="75" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="30" customHeight="1" ht="18.75">
@@ -4935,7 +4938,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="31" customHeight="1" ht="18.75">
       <c r="A31" s="84" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B31" s="85">
         <v>324</v>

</xml_diff>

<commit_message>
added a new tab for submersible pumps and need to run it
</commit_message>
<xml_diff>
--- a/heliostrome/jip_project/results/Factors to run simulation.xlsx
+++ b/heliostrome/jip_project/results/Factors to run simulation.xlsx
@@ -1,34 +1,35 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Shubham\OneDrive\Documents\heliostrome\heliostrome\jip_project\results\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gaeta\Desktop\TU Delft\JIP\Github\heliostrome\heliostrome\jip_project\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FCF499B-8EC8-4239-8838-B7E4D0C93C25}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B9DEE96-CADD-4FAD-BF35-F21791197EC5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="All Case Studies (compatability" sheetId="1" r:id="rId1"/>
     <sheet name="Bangladesh Case Study" sheetId="2" r:id="rId2"/>
     <sheet name="Bangladesh Case Study Drip" sheetId="9" r:id="rId3"/>
     <sheet name="Case study pump" sheetId="3" r:id="rId4"/>
-    <sheet name="Morocco Case Study" sheetId="4" r:id="rId5"/>
-    <sheet name="Ahvaz Iran Case Study" sheetId="5" r:id="rId6"/>
-    <sheet name="Morocco Wheat Case Study" sheetId="6" r:id="rId7"/>
-    <sheet name="Northeast China Case Study" sheetId="7" r:id="rId8"/>
-    <sheet name="Iran Potato Case Study" sheetId="8" r:id="rId9"/>
+    <sheet name="Case study pump 2" sheetId="10" r:id="rId5"/>
+    <sheet name="Morocco Case Study" sheetId="4" r:id="rId6"/>
+    <sheet name="Ahvaz Iran Case Study" sheetId="5" r:id="rId7"/>
+    <sheet name="Morocco Wheat Case Study" sheetId="6" r:id="rId8"/>
+    <sheet name="Northeast China Case Study" sheetId="7" r:id="rId9"/>
+    <sheet name="Iran Potato Case Study" sheetId="8" r:id="rId10"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="714" uniqueCount="161">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="905" uniqueCount="166">
   <si>
     <t>Evaluation of AquaCrop for potato yield and biomass
 simulation under different water amounts in drip and
@@ -514,6 +515,21 @@
   </si>
   <si>
     <t>Solar Pump System for Green Agriculture</t>
+  </si>
+  <si>
+    <t>SCS_7_210_60_BL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SCS_8_410_120_BL </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SCS_8_500_180_BL </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SCS_10_165_60_BL </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SCS_10_210_120Y_BL </t>
   </si>
 </sst>
 </file>
@@ -1709,6 +1725,376 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
+  <sheetPr>
+    <outlinePr summaryBelow="0"/>
+  </sheetPr>
+  <dimension ref="A1:G16"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="47.109375" style="19" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.88671875" style="20" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="31.33203125" style="21" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="31.33203125" style="20" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="46.44140625" style="20" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="46.44140625" style="21" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.5546875" style="20" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" ht="39.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="1"/>
+      <c r="B1" s="106" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="107"/>
+      <c r="D1" s="107"/>
+      <c r="E1" s="107"/>
+      <c r="F1" s="107"/>
+      <c r="G1" s="108"/>
+    </row>
+    <row r="2" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="5">
+        <v>50.55</v>
+      </c>
+      <c r="C3" s="5">
+        <v>50.55</v>
+      </c>
+      <c r="D3" s="5">
+        <v>50.55</v>
+      </c>
+      <c r="E3" s="5">
+        <v>50.55</v>
+      </c>
+      <c r="F3" s="5">
+        <v>50.55</v>
+      </c>
+      <c r="G3" s="5">
+        <v>50.55</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="5">
+        <v>32.18</v>
+      </c>
+      <c r="C4" s="5">
+        <v>32.18</v>
+      </c>
+      <c r="D4" s="5">
+        <v>32.18</v>
+      </c>
+      <c r="E4" s="5">
+        <v>32.18</v>
+      </c>
+      <c r="F4" s="5">
+        <v>32.18</v>
+      </c>
+      <c r="G4" s="5">
+        <v>32.18</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" s="6">
+        <v>41275</v>
+      </c>
+      <c r="C5" s="6">
+        <v>41275</v>
+      </c>
+      <c r="D5" s="6">
+        <v>41275</v>
+      </c>
+      <c r="E5" s="6">
+        <v>41640</v>
+      </c>
+      <c r="F5" s="6">
+        <v>41640</v>
+      </c>
+      <c r="G5" s="6">
+        <v>41640</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" s="6">
+        <v>41639</v>
+      </c>
+      <c r="C6" s="6">
+        <v>41639</v>
+      </c>
+      <c r="D6" s="6">
+        <v>41639</v>
+      </c>
+      <c r="E6" s="6">
+        <v>42004</v>
+      </c>
+      <c r="F6" s="6">
+        <v>42004</v>
+      </c>
+      <c r="G6" s="6">
+        <v>42004</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7" s="7">
+        <v>41440</v>
+      </c>
+      <c r="C7" s="7">
+        <v>41440</v>
+      </c>
+      <c r="D7" s="7">
+        <v>41440</v>
+      </c>
+      <c r="E7" s="6">
+        <v>41805</v>
+      </c>
+      <c r="F7" s="6">
+        <v>41805</v>
+      </c>
+      <c r="G7" s="6">
+        <v>41805</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B8" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="C8" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="D8" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="E8" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="F8" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="G8" s="8" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B9" s="4">
+        <v>100</v>
+      </c>
+      <c r="C9" s="4">
+        <v>100</v>
+      </c>
+      <c r="D9" s="4">
+        <v>100</v>
+      </c>
+      <c r="E9" s="4">
+        <v>100</v>
+      </c>
+      <c r="F9" s="4">
+        <v>100</v>
+      </c>
+      <c r="G9" s="4">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B10" s="8">
+        <v>24.61</v>
+      </c>
+      <c r="C10" s="8">
+        <v>24.61</v>
+      </c>
+      <c r="D10" s="8">
+        <v>24.61</v>
+      </c>
+      <c r="E10" s="8">
+        <v>24.61</v>
+      </c>
+      <c r="F10" s="8">
+        <v>24.61</v>
+      </c>
+      <c r="G10" s="8">
+        <v>24.61</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="F11" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G11" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B12" s="3">
+        <v>12.15</v>
+      </c>
+      <c r="C12" s="4">
+        <v>10.210000000000001</v>
+      </c>
+      <c r="D12" s="3">
+        <v>6.84</v>
+      </c>
+      <c r="E12" s="3">
+        <v>12.15</v>
+      </c>
+      <c r="F12" s="4">
+        <v>10.210000000000001</v>
+      </c>
+      <c r="G12" s="3">
+        <v>6.84</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="B13" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="C13" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="D13" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="E13" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="F13" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="G13" s="11" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="B14" s="14">
+        <v>11.5</v>
+      </c>
+      <c r="C14" s="15">
+        <v>9.24</v>
+      </c>
+      <c r="D14" s="14">
+        <v>7.95</v>
+      </c>
+      <c r="E14" s="14">
+        <v>11.5</v>
+      </c>
+      <c r="F14" s="15">
+        <v>9.24</v>
+      </c>
+      <c r="G14" s="14">
+        <v>7.95</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="16"/>
+      <c r="B15" s="17"/>
+      <c r="C15" s="18"/>
+      <c r="D15" s="17"/>
+      <c r="E15" s="17"/>
+      <c r="F15" s="17"/>
+      <c r="G15" s="17"/>
+    </row>
+    <row r="16" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="E16" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="F16" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="G16" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B1:G1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
@@ -3354,7 +3740,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D10AA0B3-E901-44DB-9B66-2C103393184F}">
   <dimension ref="A1:H31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
@@ -5798,6 +6184,1641 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{366C6A32-9B44-4F4D-A840-F9EA6B49929D}">
+  <sheetPr>
+    <outlinePr summaryBelow="0"/>
+  </sheetPr>
+  <dimension ref="A1:Q31"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="D17" sqref="D17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="46.88671875" style="19" bestFit="1" customWidth="1"/>
+    <col min="2" max="12" width="24.33203125" style="80" bestFit="1" customWidth="1"/>
+    <col min="13" max="17" width="30.109375" style="80" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:17" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="61"/>
+      <c r="B1" s="62" t="s">
+        <v>54</v>
+      </c>
+      <c r="C1" s="62"/>
+      <c r="D1" s="62"/>
+      <c r="E1" s="62"/>
+      <c r="F1" s="62"/>
+      <c r="G1" s="62"/>
+      <c r="H1" s="62"/>
+      <c r="I1" s="62"/>
+      <c r="J1" s="62"/>
+      <c r="K1" s="63"/>
+      <c r="L1" s="64"/>
+      <c r="M1" s="64"/>
+      <c r="N1" s="64"/>
+      <c r="O1" s="64"/>
+      <c r="P1" s="47"/>
+      <c r="Q1" s="30"/>
+    </row>
+    <row r="2" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="35" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="65" t="s">
+        <v>68</v>
+      </c>
+      <c r="C2" s="65" t="s">
+        <v>68</v>
+      </c>
+      <c r="D2" s="65" t="s">
+        <v>68</v>
+      </c>
+      <c r="E2" s="65" t="s">
+        <v>68</v>
+      </c>
+      <c r="F2" s="65" t="s">
+        <v>68</v>
+      </c>
+      <c r="G2" s="65" t="s">
+        <v>68</v>
+      </c>
+      <c r="H2" s="65" t="s">
+        <v>68</v>
+      </c>
+      <c r="I2" s="65" t="s">
+        <v>68</v>
+      </c>
+      <c r="J2" s="65" t="s">
+        <v>68</v>
+      </c>
+      <c r="K2" s="65" t="s">
+        <v>68</v>
+      </c>
+      <c r="L2" s="65" t="s">
+        <v>68</v>
+      </c>
+      <c r="M2" s="65" t="s">
+        <v>68</v>
+      </c>
+      <c r="N2" s="65" t="s">
+        <v>68</v>
+      </c>
+      <c r="O2" s="65" t="s">
+        <v>68</v>
+      </c>
+      <c r="P2" s="65" t="s">
+        <v>68</v>
+      </c>
+      <c r="Q2" s="65" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="66" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="67">
+        <v>90.41</v>
+      </c>
+      <c r="C3" s="67">
+        <v>90.41</v>
+      </c>
+      <c r="D3" s="67">
+        <v>90.41</v>
+      </c>
+      <c r="E3" s="67">
+        <v>90.41</v>
+      </c>
+      <c r="F3" s="67">
+        <v>90.41</v>
+      </c>
+      <c r="G3" s="67">
+        <v>90.41</v>
+      </c>
+      <c r="H3" s="67">
+        <v>90.41</v>
+      </c>
+      <c r="I3" s="67">
+        <v>90.41</v>
+      </c>
+      <c r="J3" s="67">
+        <v>90.41</v>
+      </c>
+      <c r="K3" s="67">
+        <v>90.41</v>
+      </c>
+      <c r="L3" s="67">
+        <v>90.41</v>
+      </c>
+      <c r="M3" s="67">
+        <v>90.41</v>
+      </c>
+      <c r="N3" s="67">
+        <v>90.41</v>
+      </c>
+      <c r="O3" s="67">
+        <v>90.41</v>
+      </c>
+      <c r="P3" s="67">
+        <v>90.41</v>
+      </c>
+      <c r="Q3" s="67">
+        <v>90.41</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="66" t="s">
+        <v>41</v>
+      </c>
+      <c r="B4" s="67">
+        <v>24.1</v>
+      </c>
+      <c r="C4" s="67">
+        <v>24.1</v>
+      </c>
+      <c r="D4" s="67">
+        <v>24.1</v>
+      </c>
+      <c r="E4" s="67">
+        <v>24.1</v>
+      </c>
+      <c r="F4" s="67">
+        <v>24.1</v>
+      </c>
+      <c r="G4" s="67">
+        <v>24.1</v>
+      </c>
+      <c r="H4" s="67">
+        <v>24.1</v>
+      </c>
+      <c r="I4" s="67">
+        <v>24.1</v>
+      </c>
+      <c r="J4" s="67">
+        <v>24.1</v>
+      </c>
+      <c r="K4" s="67">
+        <v>24.1</v>
+      </c>
+      <c r="L4" s="67">
+        <v>24.1</v>
+      </c>
+      <c r="M4" s="67">
+        <v>24.1</v>
+      </c>
+      <c r="N4" s="67">
+        <v>24.1</v>
+      </c>
+      <c r="O4" s="67">
+        <v>24.1</v>
+      </c>
+      <c r="P4" s="67">
+        <v>24.1</v>
+      </c>
+      <c r="Q4" s="67">
+        <v>24.1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="66" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" s="68">
+        <v>38353</v>
+      </c>
+      <c r="C5" s="68">
+        <v>38353</v>
+      </c>
+      <c r="D5" s="68">
+        <v>38353</v>
+      </c>
+      <c r="E5" s="68">
+        <v>38353</v>
+      </c>
+      <c r="F5" s="68">
+        <v>38353</v>
+      </c>
+      <c r="G5" s="68">
+        <v>38353</v>
+      </c>
+      <c r="H5" s="68">
+        <v>38353</v>
+      </c>
+      <c r="I5" s="68">
+        <v>38353</v>
+      </c>
+      <c r="J5" s="68">
+        <v>38353</v>
+      </c>
+      <c r="K5" s="68">
+        <v>38353</v>
+      </c>
+      <c r="L5" s="68">
+        <v>38353</v>
+      </c>
+      <c r="M5" s="68">
+        <v>38353</v>
+      </c>
+      <c r="N5" s="68">
+        <v>38353</v>
+      </c>
+      <c r="O5" s="68">
+        <v>38353</v>
+      </c>
+      <c r="P5" s="68">
+        <v>38353</v>
+      </c>
+      <c r="Q5" s="68">
+        <v>38353</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="66" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" s="68">
+        <v>42735</v>
+      </c>
+      <c r="C6" s="68">
+        <v>42735</v>
+      </c>
+      <c r="D6" s="68">
+        <v>42735</v>
+      </c>
+      <c r="E6" s="68">
+        <v>42735</v>
+      </c>
+      <c r="F6" s="68">
+        <v>42735</v>
+      </c>
+      <c r="G6" s="68">
+        <v>42735</v>
+      </c>
+      <c r="H6" s="68">
+        <v>42735</v>
+      </c>
+      <c r="I6" s="68">
+        <v>42735</v>
+      </c>
+      <c r="J6" s="68">
+        <v>42735</v>
+      </c>
+      <c r="K6" s="68">
+        <v>42735</v>
+      </c>
+      <c r="L6" s="68">
+        <v>42735</v>
+      </c>
+      <c r="M6" s="68">
+        <v>42735</v>
+      </c>
+      <c r="N6" s="68">
+        <v>42735</v>
+      </c>
+      <c r="O6" s="68">
+        <v>42735</v>
+      </c>
+      <c r="P6" s="68">
+        <v>42735</v>
+      </c>
+      <c r="Q6" s="68">
+        <v>42735</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="66" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7" s="69">
+        <v>38529</v>
+      </c>
+      <c r="C7" s="69">
+        <v>38529</v>
+      </c>
+      <c r="D7" s="69">
+        <v>38529</v>
+      </c>
+      <c r="E7" s="69">
+        <v>38529</v>
+      </c>
+      <c r="F7" s="69">
+        <v>38529</v>
+      </c>
+      <c r="G7" s="69">
+        <v>38529</v>
+      </c>
+      <c r="H7" s="69">
+        <v>38529</v>
+      </c>
+      <c r="I7" s="69">
+        <v>38529</v>
+      </c>
+      <c r="J7" s="69">
+        <v>38529</v>
+      </c>
+      <c r="K7" s="69">
+        <v>38529</v>
+      </c>
+      <c r="L7" s="69">
+        <v>38529</v>
+      </c>
+      <c r="M7" s="69">
+        <v>38529</v>
+      </c>
+      <c r="N7" s="69">
+        <v>38529</v>
+      </c>
+      <c r="O7" s="69">
+        <v>38529</v>
+      </c>
+      <c r="P7" s="69">
+        <v>38529</v>
+      </c>
+      <c r="Q7" s="69">
+        <v>38529</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="66" t="s">
+        <v>10</v>
+      </c>
+      <c r="B8" s="70" t="s">
+        <v>42</v>
+      </c>
+      <c r="C8" s="70" t="s">
+        <v>42</v>
+      </c>
+      <c r="D8" s="70" t="s">
+        <v>42</v>
+      </c>
+      <c r="E8" s="70" t="s">
+        <v>42</v>
+      </c>
+      <c r="F8" s="70" t="s">
+        <v>42</v>
+      </c>
+      <c r="G8" s="70" t="s">
+        <v>42</v>
+      </c>
+      <c r="H8" s="70" t="s">
+        <v>42</v>
+      </c>
+      <c r="I8" s="70" t="s">
+        <v>42</v>
+      </c>
+      <c r="J8" s="70" t="s">
+        <v>42</v>
+      </c>
+      <c r="K8" s="70" t="s">
+        <v>42</v>
+      </c>
+      <c r="L8" s="70" t="s">
+        <v>42</v>
+      </c>
+      <c r="M8" s="70" t="s">
+        <v>42</v>
+      </c>
+      <c r="N8" s="70" t="s">
+        <v>42</v>
+      </c>
+      <c r="O8" s="70" t="s">
+        <v>42</v>
+      </c>
+      <c r="P8" s="70" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q8" s="70" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="66" t="s">
+        <v>12</v>
+      </c>
+      <c r="B9" s="71">
+        <v>35</v>
+      </c>
+      <c r="C9" s="71">
+        <v>35</v>
+      </c>
+      <c r="D9" s="71">
+        <v>35</v>
+      </c>
+      <c r="E9" s="71">
+        <v>35</v>
+      </c>
+      <c r="F9" s="71">
+        <v>35</v>
+      </c>
+      <c r="G9" s="71">
+        <v>35</v>
+      </c>
+      <c r="H9" s="71">
+        <v>35</v>
+      </c>
+      <c r="I9" s="71">
+        <v>35</v>
+      </c>
+      <c r="J9" s="71">
+        <v>35</v>
+      </c>
+      <c r="K9" s="71">
+        <v>35</v>
+      </c>
+      <c r="L9" s="71">
+        <v>35</v>
+      </c>
+      <c r="M9" s="71">
+        <v>35</v>
+      </c>
+      <c r="N9" s="71">
+        <v>35</v>
+      </c>
+      <c r="O9" s="71">
+        <v>35</v>
+      </c>
+      <c r="P9" s="71">
+        <v>35</v>
+      </c>
+      <c r="Q9" s="71">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="66" t="s">
+        <v>13</v>
+      </c>
+      <c r="B10" s="71" t="s">
+        <v>69</v>
+      </c>
+      <c r="C10" s="71" t="s">
+        <v>69</v>
+      </c>
+      <c r="D10" s="71" t="s">
+        <v>69</v>
+      </c>
+      <c r="E10" s="71" t="s">
+        <v>69</v>
+      </c>
+      <c r="F10" s="71" t="s">
+        <v>69</v>
+      </c>
+      <c r="G10" s="71" t="s">
+        <v>69</v>
+      </c>
+      <c r="H10" s="71" t="s">
+        <v>69</v>
+      </c>
+      <c r="I10" s="71" t="s">
+        <v>69</v>
+      </c>
+      <c r="J10" s="71" t="s">
+        <v>69</v>
+      </c>
+      <c r="K10" s="71" t="s">
+        <v>69</v>
+      </c>
+      <c r="L10" s="71" t="s">
+        <v>69</v>
+      </c>
+      <c r="M10" s="71" t="s">
+        <v>69</v>
+      </c>
+      <c r="N10" s="71" t="s">
+        <v>69</v>
+      </c>
+      <c r="O10" s="71" t="s">
+        <v>69</v>
+      </c>
+      <c r="P10" s="71" t="s">
+        <v>69</v>
+      </c>
+      <c r="Q10" s="71" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="66" t="s">
+        <v>14</v>
+      </c>
+      <c r="B11" s="70" t="s">
+        <v>70</v>
+      </c>
+      <c r="C11" s="70" t="s">
+        <v>70</v>
+      </c>
+      <c r="D11" s="70" t="s">
+        <v>70</v>
+      </c>
+      <c r="E11" s="70" t="s">
+        <v>70</v>
+      </c>
+      <c r="F11" s="70" t="s">
+        <v>70</v>
+      </c>
+      <c r="G11" s="70" t="s">
+        <v>70</v>
+      </c>
+      <c r="H11" s="70" t="s">
+        <v>70</v>
+      </c>
+      <c r="I11" s="70" t="s">
+        <v>70</v>
+      </c>
+      <c r="J11" s="70" t="s">
+        <v>70</v>
+      </c>
+      <c r="K11" s="70" t="s">
+        <v>70</v>
+      </c>
+      <c r="L11" s="70" t="s">
+        <v>70</v>
+      </c>
+      <c r="M11" s="70" t="s">
+        <v>70</v>
+      </c>
+      <c r="N11" s="70" t="s">
+        <v>70</v>
+      </c>
+      <c r="O11" s="70" t="s">
+        <v>70</v>
+      </c>
+      <c r="P11" s="70" t="s">
+        <v>70</v>
+      </c>
+      <c r="Q11" s="70" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="66" t="s">
+        <v>16</v>
+      </c>
+      <c r="B12" s="67">
+        <v>33.729999999999997</v>
+      </c>
+      <c r="C12" s="67">
+        <v>33.729999999999997</v>
+      </c>
+      <c r="D12" s="67">
+        <v>33.729999999999997</v>
+      </c>
+      <c r="E12" s="67">
+        <v>33.729999999999997</v>
+      </c>
+      <c r="F12" s="67">
+        <v>33.729999999999997</v>
+      </c>
+      <c r="G12" s="67">
+        <v>33.729999999999997</v>
+      </c>
+      <c r="H12" s="67">
+        <v>33.729999999999997</v>
+      </c>
+      <c r="I12" s="67">
+        <v>33.729999999999997</v>
+      </c>
+      <c r="J12" s="67">
+        <v>33.729999999999997</v>
+      </c>
+      <c r="K12" s="67">
+        <v>33.729999999999997</v>
+      </c>
+      <c r="L12" s="67">
+        <v>33.729999999999997</v>
+      </c>
+      <c r="M12" s="67">
+        <v>33.729999999999997</v>
+      </c>
+      <c r="N12" s="67">
+        <v>33.729999999999997</v>
+      </c>
+      <c r="O12" s="67">
+        <v>33.729999999999997</v>
+      </c>
+      <c r="P12" s="67">
+        <v>33.729999999999997</v>
+      </c>
+      <c r="Q12" s="67">
+        <v>33.729999999999997</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="66" t="s">
+        <v>17</v>
+      </c>
+      <c r="B13" s="71">
+        <v>225</v>
+      </c>
+      <c r="C13" s="71">
+        <v>225</v>
+      </c>
+      <c r="D13" s="71">
+        <v>225</v>
+      </c>
+      <c r="E13" s="71">
+        <v>225</v>
+      </c>
+      <c r="F13" s="71">
+        <v>225</v>
+      </c>
+      <c r="G13" s="71">
+        <v>225</v>
+      </c>
+      <c r="H13" s="71">
+        <v>225</v>
+      </c>
+      <c r="I13" s="71">
+        <v>225</v>
+      </c>
+      <c r="J13" s="71">
+        <v>225</v>
+      </c>
+      <c r="K13" s="71">
+        <v>225</v>
+      </c>
+      <c r="L13" s="71">
+        <v>225</v>
+      </c>
+      <c r="M13" s="71">
+        <v>225</v>
+      </c>
+      <c r="N13" s="71">
+        <v>225</v>
+      </c>
+      <c r="O13" s="71">
+        <v>225</v>
+      </c>
+      <c r="P13" s="71">
+        <v>225</v>
+      </c>
+      <c r="Q13" s="71">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="54" t="s">
+        <v>71</v>
+      </c>
+      <c r="B14" s="72" t="b">
+        <v>0</v>
+      </c>
+      <c r="C14" s="72" t="b">
+        <v>0</v>
+      </c>
+      <c r="D14" s="72" t="b">
+        <v>0</v>
+      </c>
+      <c r="E14" s="72" t="b">
+        <v>0</v>
+      </c>
+      <c r="F14" s="72" t="b">
+        <v>0</v>
+      </c>
+      <c r="G14" s="72" t="b">
+        <v>0</v>
+      </c>
+      <c r="H14" s="72" t="b">
+        <v>0</v>
+      </c>
+      <c r="I14" s="72" t="b">
+        <v>0</v>
+      </c>
+      <c r="J14" s="72" t="b">
+        <v>0</v>
+      </c>
+      <c r="K14" s="72" t="b">
+        <v>0</v>
+      </c>
+      <c r="L14" s="72" t="b">
+        <v>0</v>
+      </c>
+      <c r="M14" s="72" t="b">
+        <v>0</v>
+      </c>
+      <c r="N14" s="72" t="b">
+        <v>0</v>
+      </c>
+      <c r="O14" s="72" t="b">
+        <v>0</v>
+      </c>
+      <c r="P14" s="72" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q14" s="72" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="73" t="s">
+        <v>72</v>
+      </c>
+      <c r="B15" s="74">
+        <v>111</v>
+      </c>
+      <c r="C15" s="74">
+        <v>111</v>
+      </c>
+      <c r="D15" s="74">
+        <v>111</v>
+      </c>
+      <c r="E15" s="74">
+        <v>111</v>
+      </c>
+      <c r="F15" s="74">
+        <v>111</v>
+      </c>
+      <c r="G15" s="74">
+        <v>111</v>
+      </c>
+      <c r="H15" s="74">
+        <v>111</v>
+      </c>
+      <c r="I15" s="74">
+        <v>111</v>
+      </c>
+      <c r="J15" s="74">
+        <v>111</v>
+      </c>
+      <c r="K15" s="74">
+        <v>111</v>
+      </c>
+      <c r="L15" s="74">
+        <v>111</v>
+      </c>
+      <c r="M15" s="74">
+        <v>111</v>
+      </c>
+      <c r="N15" s="74">
+        <v>111</v>
+      </c>
+      <c r="O15" s="74">
+        <v>111</v>
+      </c>
+      <c r="P15" s="74">
+        <v>111</v>
+      </c>
+      <c r="Q15" s="74">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="73" t="s">
+        <v>73</v>
+      </c>
+      <c r="B16" s="74">
+        <v>61.24</v>
+      </c>
+      <c r="C16" s="74">
+        <v>61.24</v>
+      </c>
+      <c r="D16" s="74">
+        <v>61.24</v>
+      </c>
+      <c r="E16" s="74">
+        <v>61.24</v>
+      </c>
+      <c r="F16" s="74">
+        <v>61.24</v>
+      </c>
+      <c r="G16" s="74">
+        <v>61.24</v>
+      </c>
+      <c r="H16" s="74">
+        <v>61.24</v>
+      </c>
+      <c r="I16" s="74">
+        <v>61.24</v>
+      </c>
+      <c r="J16" s="74">
+        <v>61.24</v>
+      </c>
+      <c r="K16" s="74">
+        <v>61.24</v>
+      </c>
+      <c r="L16" s="74">
+        <v>61.24</v>
+      </c>
+      <c r="M16" s="74">
+        <v>61.24</v>
+      </c>
+      <c r="N16" s="74">
+        <v>61.24</v>
+      </c>
+      <c r="O16" s="74">
+        <v>61.24</v>
+      </c>
+      <c r="P16" s="74">
+        <v>61.24</v>
+      </c>
+      <c r="Q16" s="74">
+        <v>61.24</v>
+      </c>
+    </row>
+    <row r="17" spans="1:17" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="73" t="s">
+        <v>74</v>
+      </c>
+      <c r="B17" s="74">
+        <v>2</v>
+      </c>
+      <c r="C17" s="74">
+        <v>3</v>
+      </c>
+      <c r="D17" s="74">
+        <v>4</v>
+      </c>
+      <c r="E17" s="74">
+        <v>3</v>
+      </c>
+      <c r="F17" s="74">
+        <v>4</v>
+      </c>
+      <c r="G17" s="74">
+        <v>5</v>
+      </c>
+      <c r="H17" s="74">
+        <v>4</v>
+      </c>
+      <c r="I17" s="74">
+        <v>5</v>
+      </c>
+      <c r="J17" s="74">
+        <v>6</v>
+      </c>
+      <c r="K17" s="74">
+        <v>3</v>
+      </c>
+      <c r="L17" s="74">
+        <v>4</v>
+      </c>
+      <c r="M17" s="74">
+        <v>5</v>
+      </c>
+      <c r="N17" s="74">
+        <v>3</v>
+      </c>
+      <c r="O17" s="74">
+        <v>4</v>
+      </c>
+      <c r="P17" s="74">
+        <v>5</v>
+      </c>
+      <c r="Q17" s="74">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="18" spans="1:17" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="73" t="s">
+        <v>75</v>
+      </c>
+      <c r="B18" s="74">
+        <v>1</v>
+      </c>
+      <c r="C18" s="74">
+        <v>1</v>
+      </c>
+      <c r="D18" s="74">
+        <v>1</v>
+      </c>
+      <c r="E18" s="74">
+        <v>1</v>
+      </c>
+      <c r="F18" s="74">
+        <v>1</v>
+      </c>
+      <c r="G18" s="74">
+        <v>1</v>
+      </c>
+      <c r="H18" s="74">
+        <v>1</v>
+      </c>
+      <c r="I18" s="74">
+        <v>1</v>
+      </c>
+      <c r="J18" s="74">
+        <v>1</v>
+      </c>
+      <c r="K18" s="74">
+        <v>1</v>
+      </c>
+      <c r="L18" s="74">
+        <v>1</v>
+      </c>
+      <c r="M18" s="74">
+        <v>1</v>
+      </c>
+      <c r="N18" s="74">
+        <v>1</v>
+      </c>
+      <c r="O18" s="74">
+        <v>1</v>
+      </c>
+      <c r="P18" s="74">
+        <v>1</v>
+      </c>
+      <c r="Q18" s="74">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:17" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="73" t="s">
+        <v>76</v>
+      </c>
+      <c r="B19" s="74" t="s">
+        <v>77</v>
+      </c>
+      <c r="C19" s="74" t="s">
+        <v>77</v>
+      </c>
+      <c r="D19" s="74" t="s">
+        <v>77</v>
+      </c>
+      <c r="E19" s="74" t="s">
+        <v>77</v>
+      </c>
+      <c r="F19" s="74" t="s">
+        <v>77</v>
+      </c>
+      <c r="G19" s="74" t="s">
+        <v>77</v>
+      </c>
+      <c r="H19" s="74" t="s">
+        <v>77</v>
+      </c>
+      <c r="I19" s="74" t="s">
+        <v>77</v>
+      </c>
+      <c r="J19" s="74" t="s">
+        <v>77</v>
+      </c>
+      <c r="K19" s="74" t="s">
+        <v>77</v>
+      </c>
+      <c r="L19" s="74" t="s">
+        <v>77</v>
+      </c>
+      <c r="M19" s="74" t="s">
+        <v>77</v>
+      </c>
+      <c r="N19" s="74" t="s">
+        <v>77</v>
+      </c>
+      <c r="O19" s="74" t="s">
+        <v>77</v>
+      </c>
+      <c r="P19" s="74" t="s">
+        <v>77</v>
+      </c>
+      <c r="Q19" s="74" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="20" spans="1:17" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="73" t="s">
+        <v>78</v>
+      </c>
+      <c r="B20" s="74" t="s">
+        <v>161</v>
+      </c>
+      <c r="C20" s="74" t="s">
+        <v>161</v>
+      </c>
+      <c r="D20" s="74" t="s">
+        <v>161</v>
+      </c>
+      <c r="E20" s="74" t="s">
+        <v>162</v>
+      </c>
+      <c r="F20" s="74" t="s">
+        <v>162</v>
+      </c>
+      <c r="G20" s="74" t="s">
+        <v>162</v>
+      </c>
+      <c r="H20" s="74" t="s">
+        <v>163</v>
+      </c>
+      <c r="I20" s="74" t="s">
+        <v>163</v>
+      </c>
+      <c r="J20" s="74" t="s">
+        <v>163</v>
+      </c>
+      <c r="K20" s="74" t="s">
+        <v>164</v>
+      </c>
+      <c r="L20" s="74" t="s">
+        <v>164</v>
+      </c>
+      <c r="M20" s="74" t="s">
+        <v>164</v>
+      </c>
+      <c r="N20" s="74" t="s">
+        <v>165</v>
+      </c>
+      <c r="O20" s="74" t="s">
+        <v>165</v>
+      </c>
+      <c r="P20" s="74" t="s">
+        <v>165</v>
+      </c>
+      <c r="Q20" s="74" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="21" spans="1:17" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="73" t="s">
+        <v>82</v>
+      </c>
+      <c r="B21" s="75">
+        <v>33.5</v>
+      </c>
+      <c r="C21" s="75">
+        <v>33.5</v>
+      </c>
+      <c r="D21" s="75">
+        <v>33.5</v>
+      </c>
+      <c r="E21" s="75">
+        <v>33.5</v>
+      </c>
+      <c r="F21" s="75">
+        <v>33.5</v>
+      </c>
+      <c r="G21" s="75">
+        <v>33.5</v>
+      </c>
+      <c r="H21" s="75">
+        <v>33.5</v>
+      </c>
+      <c r="I21" s="75">
+        <v>33.5</v>
+      </c>
+      <c r="J21" s="75">
+        <v>33.5</v>
+      </c>
+      <c r="K21" s="75">
+        <v>33.5</v>
+      </c>
+      <c r="L21" s="75">
+        <v>33.5</v>
+      </c>
+      <c r="M21" s="75">
+        <v>33.5</v>
+      </c>
+      <c r="N21" s="75">
+        <v>33.5</v>
+      </c>
+      <c r="O21" s="75">
+        <v>33.5</v>
+      </c>
+      <c r="P21" s="75">
+        <v>33.5</v>
+      </c>
+      <c r="Q21" s="75">
+        <v>33.5</v>
+      </c>
+    </row>
+    <row r="22" spans="1:17" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="73" t="s">
+        <v>83</v>
+      </c>
+      <c r="B22" s="74">
+        <v>66</v>
+      </c>
+      <c r="C22" s="74">
+        <v>66</v>
+      </c>
+      <c r="D22" s="74">
+        <v>66</v>
+      </c>
+      <c r="E22" s="74">
+        <v>66</v>
+      </c>
+      <c r="F22" s="74">
+        <v>66</v>
+      </c>
+      <c r="G22" s="74">
+        <v>66</v>
+      </c>
+      <c r="H22" s="74">
+        <v>66</v>
+      </c>
+      <c r="I22" s="74">
+        <v>66</v>
+      </c>
+      <c r="J22" s="74">
+        <v>66</v>
+      </c>
+      <c r="K22" s="74">
+        <v>66</v>
+      </c>
+      <c r="L22" s="74">
+        <v>66</v>
+      </c>
+      <c r="M22" s="74">
+        <v>66</v>
+      </c>
+      <c r="N22" s="74">
+        <v>66</v>
+      </c>
+      <c r="O22" s="74">
+        <v>66</v>
+      </c>
+      <c r="P22" s="74">
+        <v>66</v>
+      </c>
+      <c r="Q22" s="74">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="23" spans="1:17" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="73" t="s">
+        <v>84</v>
+      </c>
+      <c r="B23" s="76">
+        <v>3.7999999999999999E-2</v>
+      </c>
+      <c r="C23" s="76">
+        <v>3.7999999999999999E-2</v>
+      </c>
+      <c r="D23" s="76">
+        <v>3.7999999999999999E-2</v>
+      </c>
+      <c r="E23" s="76">
+        <v>3.7999999999999999E-2</v>
+      </c>
+      <c r="F23" s="76">
+        <v>3.7999999999999999E-2</v>
+      </c>
+      <c r="G23" s="76">
+        <v>3.7999999999999999E-2</v>
+      </c>
+      <c r="H23" s="76">
+        <v>3.7999999999999999E-2</v>
+      </c>
+      <c r="I23" s="76">
+        <v>3.7999999999999999E-2</v>
+      </c>
+      <c r="J23" s="76">
+        <v>3.7999999999999999E-2</v>
+      </c>
+      <c r="K23" s="76">
+        <v>3.7999999999999999E-2</v>
+      </c>
+      <c r="L23" s="76">
+        <v>3.7999999999999999E-2</v>
+      </c>
+      <c r="M23" s="76">
+        <v>3.7999999999999999E-2</v>
+      </c>
+      <c r="N23" s="76">
+        <v>3.7999999999999999E-2</v>
+      </c>
+      <c r="O23" s="76">
+        <v>3.7999999999999999E-2</v>
+      </c>
+      <c r="P23" s="76">
+        <v>3.7999999999999999E-2</v>
+      </c>
+      <c r="Q23" s="76">
+        <v>3.7999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:17" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="73" t="s">
+        <v>85</v>
+      </c>
+      <c r="B24" s="74" t="s">
+        <v>86</v>
+      </c>
+      <c r="C24" s="74" t="s">
+        <v>86</v>
+      </c>
+      <c r="D24" s="74" t="s">
+        <v>86</v>
+      </c>
+      <c r="E24" s="74" t="s">
+        <v>86</v>
+      </c>
+      <c r="F24" s="74" t="s">
+        <v>86</v>
+      </c>
+      <c r="G24" s="74" t="s">
+        <v>86</v>
+      </c>
+      <c r="H24" s="74" t="s">
+        <v>86</v>
+      </c>
+      <c r="I24" s="74" t="s">
+        <v>86</v>
+      </c>
+      <c r="J24" s="74" t="s">
+        <v>86</v>
+      </c>
+      <c r="K24" s="74" t="s">
+        <v>86</v>
+      </c>
+      <c r="L24" s="74" t="s">
+        <v>86</v>
+      </c>
+      <c r="M24" s="74" t="s">
+        <v>86</v>
+      </c>
+      <c r="N24" s="74" t="s">
+        <v>86</v>
+      </c>
+      <c r="O24" s="74" t="s">
+        <v>86</v>
+      </c>
+      <c r="P24" s="74" t="s">
+        <v>86</v>
+      </c>
+      <c r="Q24" s="74" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="25" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="35" t="s">
+        <v>7</v>
+      </c>
+      <c r="B25" s="77">
+        <v>41275</v>
+      </c>
+      <c r="C25" s="77">
+        <v>41275</v>
+      </c>
+      <c r="D25" s="77">
+        <v>41275</v>
+      </c>
+      <c r="E25" s="77">
+        <v>41275</v>
+      </c>
+      <c r="F25" s="77">
+        <v>41275</v>
+      </c>
+      <c r="G25" s="77">
+        <v>41275</v>
+      </c>
+      <c r="H25" s="77">
+        <v>41275</v>
+      </c>
+      <c r="I25" s="77">
+        <v>41275</v>
+      </c>
+      <c r="J25" s="77">
+        <v>41275</v>
+      </c>
+      <c r="K25" s="77">
+        <v>41275</v>
+      </c>
+      <c r="L25" s="77">
+        <v>41275</v>
+      </c>
+      <c r="M25" s="77">
+        <v>41275</v>
+      </c>
+      <c r="N25" s="77">
+        <v>41275</v>
+      </c>
+      <c r="O25" s="77">
+        <v>41275</v>
+      </c>
+      <c r="P25" s="77">
+        <v>41275</v>
+      </c>
+      <c r="Q25" s="77">
+        <v>41275</v>
+      </c>
+    </row>
+    <row r="26" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="66" t="s">
+        <v>8</v>
+      </c>
+      <c r="B26" s="70" t="s">
+        <v>87</v>
+      </c>
+      <c r="C26" s="70" t="s">
+        <v>87</v>
+      </c>
+      <c r="D26" s="70" t="s">
+        <v>87</v>
+      </c>
+      <c r="E26" s="70" t="s">
+        <v>87</v>
+      </c>
+      <c r="F26" s="70" t="s">
+        <v>87</v>
+      </c>
+      <c r="G26" s="70" t="s">
+        <v>87</v>
+      </c>
+      <c r="H26" s="70" t="s">
+        <v>87</v>
+      </c>
+      <c r="I26" s="70" t="s">
+        <v>87</v>
+      </c>
+      <c r="J26" s="70" t="s">
+        <v>87</v>
+      </c>
+      <c r="K26" s="70" t="s">
+        <v>87</v>
+      </c>
+      <c r="L26" s="70" t="s">
+        <v>87</v>
+      </c>
+      <c r="M26" s="70" t="s">
+        <v>87</v>
+      </c>
+      <c r="N26" s="70" t="s">
+        <v>87</v>
+      </c>
+      <c r="O26" s="70" t="s">
+        <v>87</v>
+      </c>
+      <c r="P26" s="70" t="s">
+        <v>87</v>
+      </c>
+      <c r="Q26" s="70" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="27" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="66" t="s">
+        <v>12</v>
+      </c>
+      <c r="B27" s="70" t="s">
+        <v>88</v>
+      </c>
+      <c r="C27" s="70" t="s">
+        <v>88</v>
+      </c>
+      <c r="D27" s="70" t="s">
+        <v>88</v>
+      </c>
+      <c r="E27" s="70" t="s">
+        <v>88</v>
+      </c>
+      <c r="F27" s="70" t="s">
+        <v>88</v>
+      </c>
+      <c r="G27" s="70" t="s">
+        <v>88</v>
+      </c>
+      <c r="H27" s="70" t="s">
+        <v>88</v>
+      </c>
+      <c r="I27" s="70" t="s">
+        <v>88</v>
+      </c>
+      <c r="J27" s="70" t="s">
+        <v>88</v>
+      </c>
+      <c r="K27" s="70" t="s">
+        <v>88</v>
+      </c>
+      <c r="L27" s="70" t="s">
+        <v>88</v>
+      </c>
+      <c r="M27" s="70" t="s">
+        <v>88</v>
+      </c>
+      <c r="N27" s="70" t="s">
+        <v>88</v>
+      </c>
+      <c r="O27" s="70" t="s">
+        <v>88</v>
+      </c>
+      <c r="P27" s="70" t="s">
+        <v>88</v>
+      </c>
+      <c r="Q27" s="70" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="28" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="66" t="s">
+        <v>13</v>
+      </c>
+      <c r="B28" s="71">
+        <v>26</v>
+      </c>
+      <c r="C28" s="71">
+        <v>26</v>
+      </c>
+      <c r="D28" s="71">
+        <v>26</v>
+      </c>
+      <c r="E28" s="71">
+        <v>26</v>
+      </c>
+      <c r="F28" s="71">
+        <v>26</v>
+      </c>
+      <c r="G28" s="71">
+        <v>26</v>
+      </c>
+      <c r="H28" s="71">
+        <v>26</v>
+      </c>
+      <c r="I28" s="71">
+        <v>26</v>
+      </c>
+      <c r="J28" s="71">
+        <v>26</v>
+      </c>
+      <c r="K28" s="71">
+        <v>26</v>
+      </c>
+      <c r="L28" s="71">
+        <v>26</v>
+      </c>
+      <c r="M28" s="71">
+        <v>26</v>
+      </c>
+      <c r="N28" s="71">
+        <v>26</v>
+      </c>
+      <c r="O28" s="71">
+        <v>26</v>
+      </c>
+      <c r="P28" s="71">
+        <v>26</v>
+      </c>
+      <c r="Q28" s="71">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="29" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="66" t="s">
+        <v>9</v>
+      </c>
+      <c r="B29" s="70" t="s">
+        <v>89</v>
+      </c>
+      <c r="C29" s="70" t="s">
+        <v>89</v>
+      </c>
+      <c r="D29" s="70" t="s">
+        <v>89</v>
+      </c>
+      <c r="E29" s="70" t="s">
+        <v>89</v>
+      </c>
+      <c r="F29" s="70" t="s">
+        <v>89</v>
+      </c>
+      <c r="G29" s="70" t="s">
+        <v>89</v>
+      </c>
+      <c r="H29" s="70" t="s">
+        <v>89</v>
+      </c>
+      <c r="I29" s="70" t="s">
+        <v>89</v>
+      </c>
+      <c r="J29" s="70" t="s">
+        <v>89</v>
+      </c>
+      <c r="K29" s="70" t="s">
+        <v>89</v>
+      </c>
+      <c r="L29" s="70" t="s">
+        <v>89</v>
+      </c>
+      <c r="M29" s="70" t="s">
+        <v>89</v>
+      </c>
+      <c r="N29" s="70" t="s">
+        <v>89</v>
+      </c>
+      <c r="O29" s="70" t="s">
+        <v>89</v>
+      </c>
+      <c r="P29" s="70" t="s">
+        <v>89</v>
+      </c>
+      <c r="Q29" s="70" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="30" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="78" t="s">
+        <v>12</v>
+      </c>
+      <c r="B30" s="79">
+        <v>35</v>
+      </c>
+      <c r="C30" s="79">
+        <v>35</v>
+      </c>
+      <c r="D30" s="79">
+        <v>35</v>
+      </c>
+      <c r="E30" s="79">
+        <v>35</v>
+      </c>
+      <c r="F30" s="79">
+        <v>35</v>
+      </c>
+      <c r="G30" s="79">
+        <v>35</v>
+      </c>
+      <c r="H30" s="79">
+        <v>35</v>
+      </c>
+      <c r="I30" s="79">
+        <v>35</v>
+      </c>
+      <c r="J30" s="79">
+        <v>35</v>
+      </c>
+      <c r="K30" s="79">
+        <v>35</v>
+      </c>
+      <c r="L30" s="79">
+        <v>35</v>
+      </c>
+      <c r="M30" s="79">
+        <v>35</v>
+      </c>
+      <c r="N30" s="79">
+        <v>35</v>
+      </c>
+      <c r="O30" s="79">
+        <v>35</v>
+      </c>
+      <c r="P30" s="79">
+        <v>35</v>
+      </c>
+      <c r="Q30" s="79">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="31" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="78" t="s">
+        <v>90</v>
+      </c>
+      <c r="B31" s="79">
+        <v>2500</v>
+      </c>
+      <c r="C31" s="79">
+        <v>2500</v>
+      </c>
+      <c r="D31" s="79">
+        <v>2500</v>
+      </c>
+      <c r="E31" s="79">
+        <v>2500</v>
+      </c>
+      <c r="F31" s="79">
+        <v>2500</v>
+      </c>
+      <c r="G31" s="79">
+        <v>2500</v>
+      </c>
+      <c r="H31" s="79">
+        <v>2500</v>
+      </c>
+      <c r="I31" s="79">
+        <v>2500</v>
+      </c>
+      <c r="J31" s="79">
+        <v>2500</v>
+      </c>
+      <c r="K31" s="79">
+        <v>2500</v>
+      </c>
+      <c r="L31" s="79">
+        <v>2500</v>
+      </c>
+      <c r="M31" s="79">
+        <v>2500</v>
+      </c>
+      <c r="N31" s="79">
+        <v>2500</v>
+      </c>
+      <c r="O31" s="79">
+        <v>2500</v>
+      </c>
+      <c r="P31" s="79">
+        <v>2500</v>
+      </c>
+      <c r="Q31" s="79">
+        <v>2500</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
@@ -6124,7 +8145,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
@@ -6363,7 +8384,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
@@ -7003,7 +9024,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
@@ -7743,374 +9764,4 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
-  <sheetPr>
-    <outlinePr summaryBelow="0"/>
-  </sheetPr>
-  <dimension ref="A1:G16"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="47.109375" style="19" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.88671875" style="20" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="31.33203125" style="21" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="31.33203125" style="20" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="46.44140625" style="20" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="46.44140625" style="21" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.5546875" style="20" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:7" ht="39.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="1"/>
-      <c r="B1" s="106" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="107"/>
-      <c r="D1" s="107"/>
-      <c r="E1" s="107"/>
-      <c r="F1" s="107"/>
-      <c r="G1" s="108"/>
-    </row>
-    <row r="2" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="F2" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="G2" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B3" s="5">
-        <v>50.55</v>
-      </c>
-      <c r="C3" s="5">
-        <v>50.55</v>
-      </c>
-      <c r="D3" s="5">
-        <v>50.55</v>
-      </c>
-      <c r="E3" s="5">
-        <v>50.55</v>
-      </c>
-      <c r="F3" s="5">
-        <v>50.55</v>
-      </c>
-      <c r="G3" s="5">
-        <v>50.55</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" s="5">
-        <v>32.18</v>
-      </c>
-      <c r="C4" s="5">
-        <v>32.18</v>
-      </c>
-      <c r="D4" s="5">
-        <v>32.18</v>
-      </c>
-      <c r="E4" s="5">
-        <v>32.18</v>
-      </c>
-      <c r="F4" s="5">
-        <v>32.18</v>
-      </c>
-      <c r="G4" s="5">
-        <v>32.18</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B5" s="6">
-        <v>41275</v>
-      </c>
-      <c r="C5" s="6">
-        <v>41275</v>
-      </c>
-      <c r="D5" s="6">
-        <v>41275</v>
-      </c>
-      <c r="E5" s="6">
-        <v>41640</v>
-      </c>
-      <c r="F5" s="6">
-        <v>41640</v>
-      </c>
-      <c r="G5" s="6">
-        <v>41640</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B6" s="6">
-        <v>41639</v>
-      </c>
-      <c r="C6" s="6">
-        <v>41639</v>
-      </c>
-      <c r="D6" s="6">
-        <v>41639</v>
-      </c>
-      <c r="E6" s="6">
-        <v>42004</v>
-      </c>
-      <c r="F6" s="6">
-        <v>42004</v>
-      </c>
-      <c r="G6" s="6">
-        <v>42004</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B7" s="7">
-        <v>41440</v>
-      </c>
-      <c r="C7" s="7">
-        <v>41440</v>
-      </c>
-      <c r="D7" s="7">
-        <v>41440</v>
-      </c>
-      <c r="E7" s="6">
-        <v>41805</v>
-      </c>
-      <c r="F7" s="6">
-        <v>41805</v>
-      </c>
-      <c r="G7" s="6">
-        <v>41805</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B8" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="C8" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="D8" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="E8" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="F8" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="G8" s="8" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B9" s="4">
-        <v>100</v>
-      </c>
-      <c r="C9" s="4">
-        <v>100</v>
-      </c>
-      <c r="D9" s="4">
-        <v>100</v>
-      </c>
-      <c r="E9" s="4">
-        <v>100</v>
-      </c>
-      <c r="F9" s="4">
-        <v>100</v>
-      </c>
-      <c r="G9" s="4">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B10" s="8">
-        <v>24.61</v>
-      </c>
-      <c r="C10" s="8">
-        <v>24.61</v>
-      </c>
-      <c r="D10" s="8">
-        <v>24.61</v>
-      </c>
-      <c r="E10" s="8">
-        <v>24.61</v>
-      </c>
-      <c r="F10" s="8">
-        <v>24.61</v>
-      </c>
-      <c r="G10" s="8">
-        <v>24.61</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="B11" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="C11" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="D11" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="E11" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="F11" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="G11" s="3" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="B12" s="3">
-        <v>12.15</v>
-      </c>
-      <c r="C12" s="4">
-        <v>10.210000000000001</v>
-      </c>
-      <c r="D12" s="3">
-        <v>6.84</v>
-      </c>
-      <c r="E12" s="3">
-        <v>12.15</v>
-      </c>
-      <c r="F12" s="4">
-        <v>10.210000000000001</v>
-      </c>
-      <c r="G12" s="3">
-        <v>6.84</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="B13" s="11" t="s">
-        <v>18</v>
-      </c>
-      <c r="C13" s="12" t="s">
-        <v>18</v>
-      </c>
-      <c r="D13" s="11" t="s">
-        <v>18</v>
-      </c>
-      <c r="E13" s="11" t="s">
-        <v>18</v>
-      </c>
-      <c r="F13" s="12" t="s">
-        <v>18</v>
-      </c>
-      <c r="G13" s="11" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="13" t="s">
-        <v>19</v>
-      </c>
-      <c r="B14" s="14">
-        <v>11.5</v>
-      </c>
-      <c r="C14" s="15">
-        <v>9.24</v>
-      </c>
-      <c r="D14" s="14">
-        <v>7.95</v>
-      </c>
-      <c r="E14" s="14">
-        <v>11.5</v>
-      </c>
-      <c r="F14" s="15">
-        <v>9.24</v>
-      </c>
-      <c r="G14" s="14">
-        <v>7.95</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="16"/>
-      <c r="B15" s="17"/>
-      <c r="C15" s="18"/>
-      <c r="D15" s="17"/>
-      <c r="E15" s="17"/>
-      <c r="F15" s="17"/>
-      <c r="G15" s="17"/>
-    </row>
-    <row r="16" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B16" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="C16" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="D16" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="E16" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="F16" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="G16" s="3" t="s">
-        <v>20</v>
-      </c>
-    </row>
-  </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="B1:G1"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
morocco wheat updates 10 years sim
</commit_message>
<xml_diff>
--- a/heliostrome/jip_project/results/Factors to run simulation.xlsx
+++ b/heliostrome/jip_project/results/Factors to run simulation.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://tud365-my.sharepoint.com/personal/sparijs_tudelft_nl/Documents/Documents/helios/heliostrome/heliostrome/jip_project/results/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2" documentId="13_ncr:1_{B4D4FD77-2C4B-4739-8C69-6565BFD02EFF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A27D3F77-02AF-4A88-82C4-AE50345F1A5A}"/>
+  <xr:revisionPtr revIDLastSave="13" documentId="13_ncr:1_{B4D4FD77-2C4B-4739-8C69-6565BFD02EFF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D62B7968-87B9-45F8-B899-E8BDE0BF6DD5}"/>
   <bookViews>
     <workbookView xWindow="3930" yWindow="2805" windowWidth="21600" windowHeight="11295" firstSheet="3" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1270,6 +1270,10 @@
 </styleSheet>
 </file>
 
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -8396,7 +8400,7 @@
   <dimension ref="A1:J22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8553,31 +8557,31 @@
         <v>8</v>
       </c>
       <c r="B6" s="36">
-        <v>40543</v>
+        <v>42369</v>
       </c>
       <c r="C6" s="36">
-        <v>40178</v>
+        <v>42004</v>
       </c>
       <c r="D6" s="36">
-        <v>40178</v>
+        <v>42004</v>
       </c>
       <c r="E6" s="36">
-        <v>40543</v>
+        <v>42369</v>
       </c>
       <c r="F6" s="36">
-        <v>40543</v>
+        <v>42369</v>
       </c>
       <c r="G6" s="36">
-        <v>40543</v>
+        <v>42369</v>
       </c>
       <c r="H6" s="36">
-        <v>40543</v>
+        <v>42369</v>
       </c>
       <c r="I6" s="36">
-        <v>40543</v>
+        <v>42369</v>
       </c>
       <c r="J6" s="36">
-        <v>40543</v>
+        <v>42369</v>
       </c>
     </row>
     <row r="7" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Final panel sizing for 5 pumps
</commit_message>
<xml_diff>
--- a/heliostrome/jip_project/results/Factors to run simulation.xlsx
+++ b/heliostrome/jip_project/results/Factors to run simulation.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://tud365-my.sharepoint.com/personal/sparijs_tudelft_nl/Documents/Documents/helios/heliostrome/heliostrome/jip_project/results/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Shubham\OneDrive\Documents\heliostrome\heliostrome\jip_project\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2" documentId="13_ncr:1_{B4D4FD77-2C4B-4739-8C69-6565BFD02EFF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A27D3F77-02AF-4A88-82C4-AE50345F1A5A}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF2093B9-EB69-4C6D-B962-51940B900009}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3930" yWindow="2805" windowWidth="21600" windowHeight="11295" firstSheet="3" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="3" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="All Case Studies (compatability" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="905" uniqueCount="167">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="925" uniqueCount="167">
   <si>
     <t>Evaluation of AquaCrop for potato yield and biomass
 simulation under different water amounts in drip and
@@ -1565,16 +1565,16 @@
       <selection pane="topRight"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="14.7109375" style="19" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="21.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.6640625" style="19" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21.44140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="17" style="19" bestFit="1" customWidth="1"/>
-    <col min="5" max="7" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="7" width="13.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="44"/>
       <c r="B1" s="55" t="s">
         <v>149</v>
@@ -1595,7 +1595,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="55" t="s">
         <v>154</v>
       </c>
@@ -1606,7 +1606,7 @@
       <c r="F2" s="98"/>
       <c r="G2" s="99"/>
     </row>
-    <row r="3" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="55" t="s">
         <v>155</v>
       </c>
@@ -1617,7 +1617,7 @@
       <c r="F3" s="97"/>
       <c r="G3" s="97"/>
     </row>
-    <row r="4" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="55" t="s">
         <v>156</v>
       </c>
@@ -1628,7 +1628,7 @@
       <c r="F4" s="97"/>
       <c r="G4" s="98"/>
     </row>
-    <row r="5" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="55" t="s">
         <v>157</v>
       </c>
@@ -1639,7 +1639,7 @@
       <c r="F5" s="99"/>
       <c r="G5" s="97"/>
     </row>
-    <row r="6" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="55" t="s">
         <v>158</v>
       </c>
@@ -1650,7 +1650,7 @@
       <c r="F6" s="97"/>
       <c r="G6" s="98"/>
     </row>
-    <row r="7" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="55" t="s">
         <v>159</v>
       </c>
@@ -1661,7 +1661,7 @@
       <c r="F7" s="97"/>
       <c r="G7" s="97"/>
     </row>
-    <row r="8" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="55" t="s">
         <v>160</v>
       </c>
@@ -1672,7 +1672,7 @@
       <c r="F8" s="98"/>
       <c r="G8" s="98"/>
     </row>
-    <row r="9" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="55" t="s">
         <v>161</v>
       </c>
@@ -1683,7 +1683,7 @@
       <c r="F9" s="97"/>
       <c r="G9" s="98"/>
     </row>
-    <row r="10" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="55" t="s">
         <v>162</v>
       </c>
@@ -1694,7 +1694,7 @@
       <c r="F10" s="97"/>
       <c r="G10" s="97"/>
     </row>
-    <row r="11" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="55" t="s">
         <v>163</v>
       </c>
@@ -1705,19 +1705,19 @@
       <c r="F11" s="99"/>
       <c r="G11" s="97"/>
     </row>
-    <row r="12" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="55" t="s">
         <v>164</v>
       </c>
       <c r="D12" s="57"/>
     </row>
-    <row r="13" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="55" t="s">
         <v>165</v>
       </c>
       <c r="D13" s="57"/>
     </row>
-    <row r="14" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="55" t="s">
         <v>166</v>
       </c>
@@ -1737,18 +1737,18 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="47.140625" style="19" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.85546875" style="20" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="31.28515625" style="21" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="31.28515625" style="20" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="46.42578125" style="20" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="46.42578125" style="21" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.5703125" style="20" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="47.109375" style="19" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.88671875" style="20" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="31.33203125" style="21" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="31.33203125" style="20" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="46.44140625" style="20" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="46.44140625" style="21" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.5546875" style="20" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" ht="39.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1"/>
       <c r="B1" s="106" t="s">
         <v>0</v>
@@ -1759,7 +1759,7 @@
       <c r="F1" s="107"/>
       <c r="G1" s="108"/>
     </row>
-    <row r="2" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
@@ -1782,7 +1782,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>5</v>
       </c>
@@ -1805,7 +1805,7 @@
         <v>50.55</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>6</v>
       </c>
@@ -1828,7 +1828,7 @@
         <v>32.18</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>7</v>
       </c>
@@ -1851,7 +1851,7 @@
         <v>41640</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>8</v>
       </c>
@@ -1874,7 +1874,7 @@
         <v>42004</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>9</v>
       </c>
@@ -1897,7 +1897,7 @@
         <v>41805</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>10</v>
       </c>
@@ -1920,7 +1920,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>12</v>
       </c>
@@ -1943,7 +1943,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>13</v>
       </c>
@@ -1966,7 +1966,7 @@
         <v>24.61</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>14</v>
       </c>
@@ -1989,7 +1989,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
         <v>16</v>
       </c>
@@ -2012,7 +2012,7 @@
         <v>6.84</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="10" t="s">
         <v>17</v>
       </c>
@@ -2035,7 +2035,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="13" t="s">
         <v>19</v>
       </c>
@@ -2058,7 +2058,7 @@
         <v>7.95</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="16"/>
       <c r="B15" s="17"/>
       <c r="C15" s="18"/>
@@ -2067,7 +2067,7 @@
       <c r="F15" s="17"/>
       <c r="G15" s="17"/>
     </row>
-    <row r="16" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
         <v>12</v>
       </c>
@@ -2110,22 +2110,22 @@
       <selection pane="topRight"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="46.85546875" style="19" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="27.140625" style="80" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="38.85546875" style="80" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="35.140625" style="80" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="46.88671875" style="19" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="27.109375" style="80" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="38.88671875" style="80" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="35.109375" style="80" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="40" style="80" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="36.85546875" style="80" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="35.28515625" style="80" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="30.140625" style="80" bestFit="1" customWidth="1"/>
-    <col min="9" max="15" width="24.28515625" style="80" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="36.88671875" style="80" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="35.33203125" style="80" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="30.109375" style="80" bestFit="1" customWidth="1"/>
+    <col min="9" max="15" width="24.33203125" style="80" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="24" style="33" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="13.5703125" style="33" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="13.5546875" style="33" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="61"/>
       <c r="B1" s="62" t="s">
         <v>54</v>
@@ -2146,7 +2146,7 @@
       <c r="P1" s="47"/>
       <c r="Q1" s="30"/>
     </row>
-    <row r="2" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="35" t="s">
         <v>1</v>
       </c>
@@ -2199,7 +2199,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="3" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="66" t="s">
         <v>5</v>
       </c>
@@ -2252,7 +2252,7 @@
         <v>90.37</v>
       </c>
     </row>
-    <row r="4" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="66" t="s">
         <v>41</v>
       </c>
@@ -2305,7 +2305,7 @@
         <v>22.7</v>
       </c>
     </row>
-    <row r="5" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="66" t="s">
         <v>7</v>
       </c>
@@ -2358,7 +2358,7 @@
         <v>40179</v>
       </c>
     </row>
-    <row r="6" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="66" t="s">
         <v>8</v>
       </c>
@@ -2411,7 +2411,7 @@
         <v>41639</v>
       </c>
     </row>
-    <row r="7" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="66" t="s">
         <v>9</v>
       </c>
@@ -2464,7 +2464,7 @@
         <v>38387</v>
       </c>
     </row>
-    <row r="8" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="66" t="s">
         <v>10</v>
       </c>
@@ -2517,7 +2517,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="9" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="66" t="s">
         <v>12</v>
       </c>
@@ -2570,7 +2570,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="10" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="66" t="s">
         <v>13</v>
       </c>
@@ -2623,7 +2623,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="11" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="66" t="s">
         <v>14</v>
       </c>
@@ -2676,7 +2676,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="12" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="66" t="s">
         <v>16</v>
       </c>
@@ -2729,7 +2729,7 @@
         <v>3.4</v>
       </c>
     </row>
-    <row r="13" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="66" t="s">
         <v>17</v>
       </c>
@@ -2782,7 +2782,7 @@
         <v>1252</v>
       </c>
     </row>
-    <row r="14" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="54" t="s">
         <v>71</v>
       </c>
@@ -2835,7 +2835,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:17" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:17" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="73" t="s">
         <v>72</v>
       </c>
@@ -2888,7 +2888,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="16" spans="1:17" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:17" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="73" t="s">
         <v>73</v>
       </c>
@@ -2941,7 +2941,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="17" spans="1:17" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:17" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="73" t="s">
         <v>74</v>
       </c>
@@ -2994,7 +2994,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="18" spans="1:17" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:17" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="73" t="s">
         <v>75</v>
       </c>
@@ -3047,7 +3047,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:17" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:17" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="73" t="s">
         <v>76</v>
       </c>
@@ -3100,7 +3100,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="20" spans="1:17" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:17" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="73" t="s">
         <v>78</v>
       </c>
@@ -3153,7 +3153,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="21" spans="1:17" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:17" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="73" t="s">
         <v>85</v>
       </c>
@@ -3206,7 +3206,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="22" spans="1:17" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:17" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="73" t="s">
         <v>86</v>
       </c>
@@ -3259,7 +3259,7 @@
         <v>537.5</v>
       </c>
     </row>
-    <row r="23" spans="1:17" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:17" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="73" t="s">
         <v>87</v>
       </c>
@@ -3312,7 +3312,7 @@
         <v>3.7999999999999999E-2</v>
       </c>
     </row>
-    <row r="24" spans="1:17" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:17" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="73" t="s">
         <v>88</v>
       </c>
@@ -3365,7 +3365,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="25" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="35" t="s">
         <v>7</v>
       </c>
@@ -3418,7 +3418,7 @@
         <v>40544</v>
       </c>
     </row>
-    <row r="26" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="66" t="s">
         <v>8</v>
       </c>
@@ -3471,7 +3471,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="27" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="66" t="s">
         <v>12</v>
       </c>
@@ -3524,7 +3524,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="28" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="66" t="s">
         <v>13</v>
       </c>
@@ -3575,7 +3575,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="29" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" s="66" t="s">
         <v>9</v>
       </c>
@@ -3628,7 +3628,7 @@
         <v>38444</v>
       </c>
     </row>
-    <row r="30" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30" s="78" t="s">
         <v>12</v>
       </c>
@@ -3681,7 +3681,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="31" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" s="78" t="s">
         <v>93</v>
       </c>
@@ -3748,16 +3748,16 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="53.5703125" style="19" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="35.7109375" style="80" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="32.7109375" style="80" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="29.85546875" style="80" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="22.85546875" style="80" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="53.5546875" style="19" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="35.6640625" style="80" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="32.6640625" style="80" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="29.88671875" style="80" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="22.88671875" style="80" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="61"/>
       <c r="B1" s="62" t="s">
         <v>97</v>
@@ -3769,7 +3769,7 @@
       <c r="G1" s="63"/>
       <c r="H1" s="64"/>
     </row>
-    <row r="2" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="35" t="s">
         <v>1</v>
       </c>
@@ -3795,7 +3795,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="66" t="s">
         <v>5</v>
       </c>
@@ -3821,7 +3821,7 @@
         <v>89.94</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="66" t="s">
         <v>41</v>
       </c>
@@ -3847,7 +3847,7 @@
         <v>24.92</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="66" t="s">
         <v>7</v>
       </c>
@@ -3873,7 +3873,7 @@
         <v>40179</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="66" t="s">
         <v>8</v>
       </c>
@@ -3899,7 +3899,7 @@
         <v>41639</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="66" t="s">
         <v>9</v>
       </c>
@@ -3925,7 +3925,7 @@
         <v>40462</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="66" t="s">
         <v>10</v>
       </c>
@@ -3951,7 +3951,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="66" t="s">
         <v>12</v>
       </c>
@@ -3977,7 +3977,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="10" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="66" t="s">
         <v>13</v>
       </c>
@@ -4003,7 +4003,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="66" t="s">
         <v>14</v>
       </c>
@@ -4029,7 +4029,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="12" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="66" t="s">
         <v>16</v>
       </c>
@@ -4055,7 +4055,7 @@
         <v>35.18</v>
       </c>
     </row>
-    <row r="13" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="66" t="s">
         <v>17</v>
       </c>
@@ -4081,7 +4081,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="14" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="54" t="s">
         <v>71</v>
       </c>
@@ -4107,7 +4107,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:8" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="73" t="s">
         <v>72</v>
       </c>
@@ -4133,7 +4133,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="16" spans="1:8" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="73" t="s">
         <v>73</v>
       </c>
@@ -4159,7 +4159,7 @@
         <v>61.24</v>
       </c>
     </row>
-    <row r="17" spans="1:8" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="73" t="s">
         <v>74</v>
       </c>
@@ -4185,7 +4185,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="18" spans="1:8" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="73" t="s">
         <v>75</v>
       </c>
@@ -4211,7 +4211,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:8" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="73" t="s">
         <v>76</v>
       </c>
@@ -4237,7 +4237,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="20" spans="1:8" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="73" t="s">
         <v>78</v>
       </c>
@@ -4263,7 +4263,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="21" spans="1:8" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="73" t="s">
         <v>85</v>
       </c>
@@ -4289,7 +4289,7 @@
         <v>33.5</v>
       </c>
     </row>
-    <row r="22" spans="1:8" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="73" t="s">
         <v>86</v>
       </c>
@@ -4315,7 +4315,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="23" spans="1:8" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="73" t="s">
         <v>87</v>
       </c>
@@ -4341,7 +4341,7 @@
         <v>3.7999999999999999E-2</v>
       </c>
     </row>
-    <row r="24" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="73" t="s">
         <v>88</v>
       </c>
@@ -4367,7 +4367,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="25" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="35" t="s">
         <v>7</v>
       </c>
@@ -4393,7 +4393,7 @@
         <v>40179</v>
       </c>
     </row>
-    <row r="26" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="66" t="s">
         <v>8</v>
       </c>
@@ -4419,7 +4419,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="27" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="66" t="s">
         <v>12</v>
       </c>
@@ -4445,7 +4445,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="28" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="66" t="s">
         <v>13</v>
       </c>
@@ -4469,7 +4469,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="29" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" s="66" t="s">
         <v>9</v>
       </c>
@@ -4495,7 +4495,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="30" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30" s="78" t="s">
         <v>12</v>
       </c>
@@ -4521,7 +4521,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="31" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" s="78" t="s">
         <v>93</v>
       </c>
@@ -4564,14 +4564,14 @@
       <selection pane="topRight"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="46.85546875" style="19" bestFit="1" customWidth="1"/>
-    <col min="2" max="12" width="24.28515625" style="80" bestFit="1" customWidth="1"/>
-    <col min="13" max="17" width="30.140625" style="80" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="46.88671875" style="19" bestFit="1" customWidth="1"/>
+    <col min="2" max="12" width="24.33203125" style="80" bestFit="1" customWidth="1"/>
+    <col min="13" max="17" width="30.109375" style="80" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="61"/>
       <c r="B1" s="62" t="s">
         <v>54</v>
@@ -4592,7 +4592,7 @@
       <c r="P1" s="47"/>
       <c r="Q1" s="30"/>
     </row>
-    <row r="2" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="35" t="s">
         <v>1</v>
       </c>
@@ -4645,7 +4645,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="3" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="66" t="s">
         <v>5</v>
       </c>
@@ -4698,7 +4698,7 @@
         <v>90.41</v>
       </c>
     </row>
-    <row r="4" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="66" t="s">
         <v>41</v>
       </c>
@@ -4751,7 +4751,7 @@
         <v>24.1</v>
       </c>
     </row>
-    <row r="5" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="66" t="s">
         <v>7</v>
       </c>
@@ -4804,7 +4804,7 @@
         <v>38353</v>
       </c>
     </row>
-    <row r="6" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="66" t="s">
         <v>8</v>
       </c>
@@ -4857,7 +4857,7 @@
         <v>42735</v>
       </c>
     </row>
-    <row r="7" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="66" t="s">
         <v>9</v>
       </c>
@@ -4910,7 +4910,7 @@
         <v>38529</v>
       </c>
     </row>
-    <row r="8" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="66" t="s">
         <v>10</v>
       </c>
@@ -4963,7 +4963,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="9" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="66" t="s">
         <v>12</v>
       </c>
@@ -5016,7 +5016,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="10" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="66" t="s">
         <v>13</v>
       </c>
@@ -5069,7 +5069,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="11" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="66" t="s">
         <v>14</v>
       </c>
@@ -5122,7 +5122,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="12" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="66" t="s">
         <v>16</v>
       </c>
@@ -5175,7 +5175,7 @@
         <v>33.729999999999997</v>
       </c>
     </row>
-    <row r="13" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="66" t="s">
         <v>17</v>
       </c>
@@ -5228,7 +5228,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="14" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="54" t="s">
         <v>71</v>
       </c>
@@ -5281,7 +5281,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:17" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:17" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="73" t="s">
         <v>72</v>
       </c>
@@ -5334,7 +5334,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="16" spans="1:17" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:17" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="73" t="s">
         <v>73</v>
       </c>
@@ -5387,7 +5387,7 @@
         <v>61.24</v>
       </c>
     </row>
-    <row r="17" spans="1:17" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:17" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="73" t="s">
         <v>74</v>
       </c>
@@ -5440,7 +5440,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="18" spans="1:17" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:17" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="73" t="s">
         <v>75</v>
       </c>
@@ -5493,7 +5493,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:17" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:17" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="73" t="s">
         <v>76</v>
       </c>
@@ -5546,7 +5546,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="20" spans="1:17" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:17" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="73" t="s">
         <v>78</v>
       </c>
@@ -5599,7 +5599,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="21" spans="1:17" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:17" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="73" t="s">
         <v>85</v>
       </c>
@@ -5652,7 +5652,7 @@
         <v>33.5</v>
       </c>
     </row>
-    <row r="22" spans="1:17" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:17" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="73" t="s">
         <v>86</v>
       </c>
@@ -5705,7 +5705,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="23" spans="1:17" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:17" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="73" t="s">
         <v>87</v>
       </c>
@@ -5758,7 +5758,7 @@
         <v>3.7999999999999999E-2</v>
       </c>
     </row>
-    <row r="24" spans="1:17" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:17" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="73" t="s">
         <v>88</v>
       </c>
@@ -5811,7 +5811,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="25" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="35" t="s">
         <v>7</v>
       </c>
@@ -5864,7 +5864,7 @@
         <v>41275</v>
       </c>
     </row>
-    <row r="26" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="66" t="s">
         <v>8</v>
       </c>
@@ -5917,7 +5917,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="27" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="66" t="s">
         <v>12</v>
       </c>
@@ -5970,7 +5970,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="28" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="66" t="s">
         <v>13</v>
       </c>
@@ -6023,7 +6023,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="29" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" s="66" t="s">
         <v>9</v>
       </c>
@@ -6076,7 +6076,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="30" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30" s="78" t="s">
         <v>12</v>
       </c>
@@ -6129,7 +6129,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="31" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" s="78" t="s">
         <v>93</v>
       </c>
@@ -6192,21 +6192,22 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:Q31"/>
+  <dimension ref="A1:S31"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="O1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="S18" sqref="S18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="46.85546875" style="19" bestFit="1" customWidth="1"/>
-    <col min="2" max="12" width="24.28515625" style="80" bestFit="1" customWidth="1"/>
-    <col min="13" max="17" width="30.140625" style="80" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="46.88671875" style="19" bestFit="1" customWidth="1"/>
+    <col min="2" max="12" width="24.33203125" style="80" bestFit="1" customWidth="1"/>
+    <col min="13" max="17" width="30.109375" style="80" bestFit="1" customWidth="1"/>
+    <col min="18" max="19" width="30.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:19" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="61"/>
       <c r="B1" s="62" t="s">
         <v>54</v>
@@ -6227,7 +6228,7 @@
       <c r="P1" s="47"/>
       <c r="Q1" s="30"/>
     </row>
-    <row r="2" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:19" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="35" t="s">
         <v>1</v>
       </c>
@@ -6279,8 +6280,14 @@
       <c r="Q2" s="65" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="3" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="R2" s="65" t="s">
+        <v>68</v>
+      </c>
+      <c r="S2" s="65" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="66" t="s">
         <v>5</v>
       </c>
@@ -6332,8 +6339,14 @@
       <c r="Q3" s="67">
         <v>90.41</v>
       </c>
-    </row>
-    <row r="4" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="R3" s="67">
+        <v>90.41</v>
+      </c>
+      <c r="S3" s="67">
+        <v>90.41</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="66" t="s">
         <v>41</v>
       </c>
@@ -6385,8 +6398,14 @@
       <c r="Q4" s="67">
         <v>24.1</v>
       </c>
-    </row>
-    <row r="5" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="R4" s="67">
+        <v>24.1</v>
+      </c>
+      <c r="S4" s="67">
+        <v>24.1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="66" t="s">
         <v>7</v>
       </c>
@@ -6438,8 +6457,14 @@
       <c r="Q5" s="68">
         <v>38353</v>
       </c>
-    </row>
-    <row r="6" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="R5" s="68">
+        <v>38353</v>
+      </c>
+      <c r="S5" s="68">
+        <v>38353</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="66" t="s">
         <v>8</v>
       </c>
@@ -6491,8 +6516,14 @@
       <c r="Q6" s="68">
         <v>42735</v>
       </c>
-    </row>
-    <row r="7" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="R6" s="68">
+        <v>42735</v>
+      </c>
+      <c r="S6" s="68">
+        <v>42735</v>
+      </c>
+    </row>
+    <row r="7" spans="1:19" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="66" t="s">
         <v>9</v>
       </c>
@@ -6544,8 +6575,14 @@
       <c r="Q7" s="69">
         <v>38529</v>
       </c>
-    </row>
-    <row r="8" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="R7" s="69">
+        <v>38529</v>
+      </c>
+      <c r="S7" s="69">
+        <v>38529</v>
+      </c>
+    </row>
+    <row r="8" spans="1:19" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="66" t="s">
         <v>10</v>
       </c>
@@ -6597,8 +6634,14 @@
       <c r="Q8" s="70" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="9" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="R8" s="70" t="s">
+        <v>42</v>
+      </c>
+      <c r="S8" s="70" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="9" spans="1:19" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="66" t="s">
         <v>12</v>
       </c>
@@ -6650,8 +6693,14 @@
       <c r="Q9" s="71">
         <v>35</v>
       </c>
-    </row>
-    <row r="10" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="R9" s="71">
+        <v>35</v>
+      </c>
+      <c r="S9" s="71">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="10" spans="1:19" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="66" t="s">
         <v>13</v>
       </c>
@@ -6703,8 +6752,14 @@
       <c r="Q10" s="71" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="11" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="R10" s="71" t="s">
+        <v>69</v>
+      </c>
+      <c r="S10" s="71" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="11" spans="1:19" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="66" t="s">
         <v>14</v>
       </c>
@@ -6756,8 +6811,14 @@
       <c r="Q11" s="70" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="12" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="R11" s="70" t="s">
+        <v>70</v>
+      </c>
+      <c r="S11" s="70" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="12" spans="1:19" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="66" t="s">
         <v>16</v>
       </c>
@@ -6809,8 +6870,14 @@
       <c r="Q12" s="67">
         <v>33.729999999999997</v>
       </c>
-    </row>
-    <row r="13" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="R12" s="67">
+        <v>33.729999999999997</v>
+      </c>
+      <c r="S12" s="67">
+        <v>33.729999999999997</v>
+      </c>
+    </row>
+    <row r="13" spans="1:19" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="66" t="s">
         <v>17</v>
       </c>
@@ -6862,8 +6929,14 @@
       <c r="Q13" s="71">
         <v>225</v>
       </c>
-    </row>
-    <row r="14" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="R13" s="71">
+        <v>225</v>
+      </c>
+      <c r="S13" s="71">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="14" spans="1:19" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="54" t="s">
         <v>71</v>
       </c>
@@ -6915,8 +6988,14 @@
       <c r="Q14" s="72" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="15" spans="1:17" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="R14" s="72" t="b">
+        <v>0</v>
+      </c>
+      <c r="S14" s="72" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:19" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="73" t="s">
         <v>72</v>
       </c>
@@ -6968,8 +7047,14 @@
       <c r="Q15" s="74">
         <v>111</v>
       </c>
-    </row>
-    <row r="16" spans="1:17" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="R15" s="74">
+        <v>111</v>
+      </c>
+      <c r="S15" s="74">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="16" spans="1:19" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="73" t="s">
         <v>73</v>
       </c>
@@ -7021,8 +7106,14 @@
       <c r="Q16" s="74">
         <v>61.24</v>
       </c>
-    </row>
-    <row r="17" spans="1:17" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="R16" s="74">
+        <v>61.24</v>
+      </c>
+      <c r="S16" s="74">
+        <v>61.24</v>
+      </c>
+    </row>
+    <row r="17" spans="1:19" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="73" t="s">
         <v>74</v>
       </c>
@@ -7074,8 +7165,14 @@
       <c r="Q17" s="74">
         <v>6</v>
       </c>
-    </row>
-    <row r="18" spans="1:17" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="R17" s="74">
+        <v>2</v>
+      </c>
+      <c r="S17" s="74">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:19" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="73" t="s">
         <v>75</v>
       </c>
@@ -7127,8 +7224,14 @@
       <c r="Q18" s="74">
         <v>1</v>
       </c>
-    </row>
-    <row r="19" spans="1:17" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="R18" s="74">
+        <v>2</v>
+      </c>
+      <c r="S18" s="74">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:19" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="73" t="s">
         <v>76</v>
       </c>
@@ -7180,8 +7283,14 @@
       <c r="Q19" s="74" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="20" spans="1:17" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="R19" s="74" t="s">
+        <v>77</v>
+      </c>
+      <c r="S19" s="74" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="20" spans="1:19" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="73" t="s">
         <v>78</v>
       </c>
@@ -7233,8 +7342,14 @@
       <c r="Q20" s="74" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="21" spans="1:17" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="R20" s="74" t="s">
+        <v>84</v>
+      </c>
+      <c r="S20" s="74" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="21" spans="1:19" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="73" t="s">
         <v>85</v>
       </c>
@@ -7286,8 +7401,14 @@
       <c r="Q21" s="75">
         <v>33.5</v>
       </c>
-    </row>
-    <row r="22" spans="1:17" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="R21" s="75">
+        <v>33.5</v>
+      </c>
+      <c r="S21" s="75">
+        <v>33.5</v>
+      </c>
+    </row>
+    <row r="22" spans="1:19" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="73" t="s">
         <v>86</v>
       </c>
@@ -7339,8 +7460,14 @@
       <c r="Q22" s="74">
         <v>66</v>
       </c>
-    </row>
-    <row r="23" spans="1:17" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="R22" s="74">
+        <v>66</v>
+      </c>
+      <c r="S22" s="74">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="23" spans="1:19" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="73" t="s">
         <v>87</v>
       </c>
@@ -7392,8 +7519,14 @@
       <c r="Q23" s="76">
         <v>3.7999999999999999E-2</v>
       </c>
-    </row>
-    <row r="24" spans="1:17" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="R23" s="76">
+        <v>3.7999999999999999E-2</v>
+      </c>
+      <c r="S23" s="76">
+        <v>3.7999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:19" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="73" t="s">
         <v>88</v>
       </c>
@@ -7445,8 +7578,14 @@
       <c r="Q24" s="74" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="25" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="R24" s="74" t="s">
+        <v>89</v>
+      </c>
+      <c r="S24" s="74" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="25" spans="1:19" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="35" t="s">
         <v>7</v>
       </c>
@@ -7498,8 +7637,14 @@
       <c r="Q25" s="77">
         <v>41275</v>
       </c>
-    </row>
-    <row r="26" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="R25" s="77">
+        <v>41275</v>
+      </c>
+      <c r="S25" s="77">
+        <v>41275</v>
+      </c>
+    </row>
+    <row r="26" spans="1:19" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="66" t="s">
         <v>8</v>
       </c>
@@ -7551,8 +7696,14 @@
       <c r="Q26" s="70" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="27" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="R26" s="70" t="s">
+        <v>90</v>
+      </c>
+      <c r="S26" s="70" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="27" spans="1:19" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="66" t="s">
         <v>12</v>
       </c>
@@ -7604,8 +7755,14 @@
       <c r="Q27" s="70" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="28" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="R27" s="70" t="s">
+        <v>91</v>
+      </c>
+      <c r="S27" s="70" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="28" spans="1:19" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="66" t="s">
         <v>13</v>
       </c>
@@ -7657,8 +7814,14 @@
       <c r="Q28" s="71">
         <v>26</v>
       </c>
-    </row>
-    <row r="29" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="R28" s="71">
+        <v>26</v>
+      </c>
+      <c r="S28" s="71">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="29" spans="1:19" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" s="66" t="s">
         <v>9</v>
       </c>
@@ -7710,8 +7873,14 @@
       <c r="Q29" s="70" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="30" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="R29" s="70" t="s">
+        <v>92</v>
+      </c>
+      <c r="S29" s="70" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="30" spans="1:19" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30" s="78" t="s">
         <v>12</v>
       </c>
@@ -7763,8 +7932,14 @@
       <c r="Q30" s="79">
         <v>35</v>
       </c>
-    </row>
-    <row r="31" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="R30" s="79">
+        <v>35</v>
+      </c>
+      <c r="S30" s="79">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="31" spans="1:19" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" s="78" t="s">
         <v>93</v>
       </c>
@@ -7814,6 +7989,12 @@
         <v>10000</v>
       </c>
       <c r="Q31" s="79">
+        <v>10000</v>
+      </c>
+      <c r="R31" s="79">
+        <v>10000</v>
+      </c>
+      <c r="S31" s="79">
         <v>10000</v>
       </c>
     </row>
@@ -7834,17 +8015,17 @@
       <selection pane="topRight"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="46.85546875" style="19" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="30.140625" style="32" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="28.85546875" style="32" bestFit="1" customWidth="1"/>
-    <col min="4" max="14" width="24.28515625" style="19" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="46.88671875" style="19" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="30.109375" style="32" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="28.88671875" style="32" bestFit="1" customWidth="1"/>
+    <col min="4" max="14" width="24.33203125" style="19" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="24" style="19" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="13.5703125" style="19" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="13.5546875" style="19" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="34"/>
       <c r="B1" s="52" t="s">
         <v>54</v>
@@ -7864,7 +8045,7 @@
       <c r="O1" s="44"/>
       <c r="P1" s="44"/>
     </row>
-    <row r="2" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="35" t="s">
         <v>1</v>
       </c>
@@ -7888,7 +8069,7 @@
       <c r="O2" s="54"/>
       <c r="P2" s="54"/>
     </row>
-    <row r="3" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="35" t="s">
         <v>5</v>
       </c>
@@ -7912,7 +8093,7 @@
       <c r="O3" s="55"/>
       <c r="P3" s="55"/>
     </row>
-    <row r="4" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="35" t="s">
         <v>41</v>
       </c>
@@ -7936,7 +8117,7 @@
       <c r="O4" s="55"/>
       <c r="P4" s="55"/>
     </row>
-    <row r="5" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="35" t="s">
         <v>7</v>
       </c>
@@ -7960,7 +8141,7 @@
       <c r="O5" s="55"/>
       <c r="P5" s="55"/>
     </row>
-    <row r="6" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="35" t="s">
         <v>8</v>
       </c>
@@ -7984,7 +8165,7 @@
       <c r="O6" s="55"/>
       <c r="P6" s="55"/>
     </row>
-    <row r="7" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="35" t="s">
         <v>9</v>
       </c>
@@ -8008,7 +8189,7 @@
       <c r="O7" s="55"/>
       <c r="P7" s="55"/>
     </row>
-    <row r="8" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="35" t="s">
         <v>10</v>
       </c>
@@ -8032,7 +8213,7 @@
       <c r="O8" s="55"/>
       <c r="P8" s="55"/>
     </row>
-    <row r="9" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="35" t="s">
         <v>12</v>
       </c>
@@ -8056,7 +8237,7 @@
       <c r="O9" s="59"/>
       <c r="P9" s="60"/>
     </row>
-    <row r="10" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="35" t="s">
         <v>13</v>
       </c>
@@ -8076,7 +8257,7 @@
       <c r="O10" s="55"/>
       <c r="P10" s="55"/>
     </row>
-    <row r="11" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="35" t="s">
         <v>14</v>
       </c>
@@ -8100,7 +8281,7 @@
       <c r="O11" s="55"/>
       <c r="P11" s="55"/>
     </row>
-    <row r="12" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="35" t="s">
         <v>16</v>
       </c>
@@ -8120,7 +8301,7 @@
       <c r="O12" s="55"/>
       <c r="P12" s="55"/>
     </row>
-    <row r="13" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="35" t="s">
         <v>17</v>
       </c>
@@ -8161,16 +8342,16 @@
       <selection pane="topRight"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="46.85546875" style="19" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="24.28515625" style="20" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="24.42578125" style="20" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="25.140625" style="21" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="26.140625" style="20" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="46.88671875" style="19" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.33203125" style="20" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="24.44140625" style="20" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="25.109375" style="21" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="26.109375" style="20" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="34"/>
       <c r="B1" s="45" t="s">
         <v>54</v>
@@ -8179,7 +8360,7 @@
       <c r="D1" s="47"/>
       <c r="E1" s="46"/>
     </row>
-    <row r="2" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="35" t="s">
         <v>1</v>
       </c>
@@ -8196,7 +8377,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="35" t="s">
         <v>5</v>
       </c>
@@ -8213,7 +8394,7 @@
         <v>48.717812000000002</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="35" t="s">
         <v>41</v>
       </c>
@@ -8230,7 +8411,7 @@
         <v>31.323521</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="35" t="s">
         <v>7</v>
       </c>
@@ -8247,7 +8428,7 @@
         <v>37987</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="35" t="s">
         <v>8</v>
       </c>
@@ -8264,7 +8445,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="35" t="s">
         <v>9</v>
       </c>
@@ -8281,7 +8462,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="35" t="s">
         <v>10</v>
       </c>
@@ -8298,7 +8479,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="35" t="s">
         <v>12</v>
       </c>
@@ -8315,7 +8496,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="35" t="s">
         <v>13</v>
       </c>
@@ -8332,7 +8513,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="35" t="s">
         <v>14</v>
       </c>
@@ -8349,7 +8530,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="12" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="35" t="s">
         <v>16</v>
       </c>
@@ -8366,7 +8547,7 @@
         <v>5.8</v>
       </c>
     </row>
-    <row r="13" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="35" t="s">
         <v>17</v>
       </c>
@@ -8395,18 +8576,18 @@
   </sheetPr>
   <dimension ref="A1:J22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="49.5703125" style="19" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.140625" style="32" bestFit="1" customWidth="1"/>
-    <col min="3" max="10" width="13.5703125" style="32" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="49.5546875" style="19" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.109375" style="32" bestFit="1" customWidth="1"/>
+    <col min="3" max="10" width="13.5546875" style="32" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="101" t="s">
         <v>33</v>
       </c>
@@ -8420,7 +8601,7 @@
       <c r="I1" s="102"/>
       <c r="J1" s="102"/>
     </row>
-    <row r="2" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="35" t="s">
         <v>1</v>
       </c>
@@ -8452,7 +8633,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="35" t="s">
         <v>5</v>
       </c>
@@ -8484,7 +8665,7 @@
         <v>-7.5958300000000003</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="35" t="s">
         <v>41</v>
       </c>
@@ -8516,7 +8697,7 @@
         <v>31.68056</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="35" t="s">
         <v>7</v>
       </c>
@@ -8548,7 +8729,7 @@
         <v>38718</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="35" t="s">
         <v>8</v>
       </c>
@@ -8580,7 +8761,7 @@
         <v>40543</v>
       </c>
     </row>
-    <row r="7" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="35" t="s">
         <v>9</v>
       </c>
@@ -8612,7 +8793,7 @@
         <v>37979</v>
       </c>
     </row>
-    <row r="8" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="35" t="s">
         <v>10</v>
       </c>
@@ -8644,7 +8825,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="9" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="35" t="s">
         <v>12</v>
       </c>
@@ -8676,7 +8857,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="35" t="s">
         <v>13</v>
       </c>
@@ -8692,7 +8873,7 @@
       <c r="I10" s="104"/>
       <c r="J10" s="105"/>
     </row>
-    <row r="11" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="35" t="s">
         <v>14</v>
       </c>
@@ -8724,7 +8905,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="12" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="35" t="s">
         <v>16</v>
       </c>
@@ -8756,7 +8937,7 @@
         <v>2.25</v>
       </c>
     </row>
-    <row r="13" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="35" t="s">
         <v>17</v>
       </c>
@@ -8788,7 +8969,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="14" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="35" t="s">
         <v>45</v>
       </c>
@@ -8820,7 +9001,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="15" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="35" t="s">
         <v>46</v>
       </c>
@@ -8852,7 +9033,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="16" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="35" t="s">
         <v>47</v>
       </c>
@@ -8884,7 +9065,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="17" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="44"/>
       <c r="B17" s="30"/>
       <c r="C17" s="30"/>
@@ -8896,7 +9077,7 @@
       <c r="I17" s="30"/>
       <c r="J17" s="30"/>
     </row>
-    <row r="18" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="44"/>
       <c r="B18" s="30"/>
       <c r="C18" s="30"/>
@@ -8908,7 +9089,7 @@
       <c r="I18" s="30"/>
       <c r="J18" s="30"/>
     </row>
-    <row r="19" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="35" t="s">
         <v>12</v>
       </c>
@@ -8940,7 +9121,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="20" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="35" t="s">
         <v>13</v>
       </c>
@@ -8956,7 +9137,7 @@
       <c r="I20" s="104"/>
       <c r="J20" s="105"/>
     </row>
-    <row r="21" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="35" t="s">
         <v>16</v>
       </c>
@@ -8988,7 +9169,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="22" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="35" t="s">
         <v>8</v>
       </c>
@@ -9039,16 +9220,16 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="47.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.85546875" style="32" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="31.28515625" style="32" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="46.42578125" style="32" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.5703125" style="33" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="47.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.88671875" style="32" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="31.33203125" style="32" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="46.44140625" style="32" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.5546875" style="33" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1"/>
       <c r="B1" s="22" t="s">
         <v>21</v>
@@ -9059,7 +9240,7 @@
       <c r="F1" s="24"/>
       <c r="G1" s="25"/>
     </row>
-    <row r="2" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
@@ -9082,7 +9263,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>5</v>
       </c>
@@ -9105,7 +9286,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>6</v>
       </c>
@@ -9128,7 +9309,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>7</v>
       </c>
@@ -9151,7 +9332,7 @@
         <v>41275</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>8</v>
       </c>
@@ -9174,7 +9355,7 @@
         <v>42735</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>9</v>
       </c>
@@ -9197,7 +9378,7 @@
         <v>42491</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>10</v>
       </c>
@@ -9220,7 +9401,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>12</v>
       </c>
@@ -9243,7 +9424,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>13</v>
       </c>
@@ -9266,7 +9447,7 @@
         <v>30.01</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>14</v>
       </c>
@@ -9289,7 +9470,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
         <v>16</v>
       </c>
@@ -9312,7 +9493,7 @@
         <v>9.4</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
         <v>17</v>
       </c>
@@ -9323,7 +9504,7 @@
       <c r="F13" s="3"/>
       <c r="G13" s="3"/>
     </row>
-    <row r="14" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="26" t="s">
         <v>30</v>
       </c>
@@ -9346,7 +9527,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="27"/>
       <c r="B15" s="28"/>
       <c r="C15" s="29"/>
@@ -9355,7 +9536,7 @@
       <c r="F15" s="28"/>
       <c r="G15" s="28"/>
     </row>
-    <row r="16" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="1"/>
       <c r="B16" s="24"/>
       <c r="C16" s="23"/>
@@ -9364,7 +9545,7 @@
       <c r="F16" s="24"/>
       <c r="G16" s="24"/>
     </row>
-    <row r="17" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
         <v>12</v>
       </c>
@@ -9387,7 +9568,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="18" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B18" s="30"/>
       <c r="C18" s="30"/>
       <c r="D18" s="30"/>
@@ -9395,7 +9576,7 @@
       <c r="F18" s="30"/>
       <c r="G18" s="31"/>
     </row>
-    <row r="19" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B19" s="30"/>
       <c r="C19" s="30"/>
       <c r="D19" s="30"/>
@@ -9403,7 +9584,7 @@
       <c r="F19" s="30"/>
       <c r="G19" s="31"/>
     </row>
-    <row r="20" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B20" s="30"/>
       <c r="C20" s="30"/>
       <c r="D20" s="30"/>
@@ -9411,7 +9592,7 @@
       <c r="F20" s="30"/>
       <c r="G20" s="31"/>
     </row>
-    <row r="21" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B21" s="30"/>
       <c r="C21" s="30"/>
       <c r="D21" s="30"/>
@@ -9419,7 +9600,7 @@
       <c r="F21" s="30"/>
       <c r="G21" s="31"/>
     </row>
-    <row r="22" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B22" s="30"/>
       <c r="C22" s="30"/>
       <c r="D22" s="30"/>
@@ -9427,7 +9608,7 @@
       <c r="F22" s="30"/>
       <c r="G22" s="31"/>
     </row>
-    <row r="23" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B23" s="30"/>
       <c r="C23" s="30"/>
       <c r="D23" s="30"/>
@@ -9435,7 +9616,7 @@
       <c r="F23" s="30"/>
       <c r="G23" s="31"/>
     </row>
-    <row r="24" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B24" s="30"/>
       <c r="C24" s="30"/>
       <c r="D24" s="30"/>
@@ -9443,7 +9624,7 @@
       <c r="F24" s="30"/>
       <c r="G24" s="31"/>
     </row>
-    <row r="25" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B25" s="30"/>
       <c r="C25" s="30"/>
       <c r="D25" s="30"/>
@@ -9451,7 +9632,7 @@
       <c r="F25" s="30"/>
       <c r="G25" s="31"/>
     </row>
-    <row r="26" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B26" s="30"/>
       <c r="C26" s="30"/>
       <c r="D26" s="30"/>
@@ -9459,7 +9640,7 @@
       <c r="F26" s="30"/>
       <c r="G26" s="31"/>
     </row>
-    <row r="27" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B27" s="30"/>
       <c r="C27" s="30"/>
       <c r="D27" s="30"/>
@@ -9467,7 +9648,7 @@
       <c r="F27" s="30"/>
       <c r="G27" s="31"/>
     </row>
-    <row r="28" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B28" s="30"/>
       <c r="C28" s="30"/>
       <c r="D28" s="30"/>
@@ -9475,7 +9656,7 @@
       <c r="F28" s="30"/>
       <c r="G28" s="31"/>
     </row>
-    <row r="29" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B29" s="30"/>
       <c r="C29" s="30"/>
       <c r="D29" s="30"/>
@@ -9483,7 +9664,7 @@
       <c r="F29" s="30"/>
       <c r="G29" s="31"/>
     </row>
-    <row r="30" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B30" s="30"/>
       <c r="C30" s="30"/>
       <c r="D30" s="30"/>
@@ -9491,7 +9672,7 @@
       <c r="F30" s="30"/>
       <c r="G30" s="31"/>
     </row>
-    <row r="31" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B31" s="30"/>
       <c r="C31" s="30"/>
       <c r="D31" s="30"/>
@@ -9499,7 +9680,7 @@
       <c r="F31" s="30"/>
       <c r="G31" s="31"/>
     </row>
-    <row r="32" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B32" s="30"/>
       <c r="C32" s="30"/>
       <c r="D32" s="30"/>
@@ -9507,7 +9688,7 @@
       <c r="F32" s="30"/>
       <c r="G32" s="31"/>
     </row>
-    <row r="33" spans="2:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B33" s="30"/>
       <c r="C33" s="30"/>
       <c r="D33" s="30"/>
@@ -9515,7 +9696,7 @@
       <c r="F33" s="30"/>
       <c r="G33" s="31"/>
     </row>
-    <row r="34" spans="2:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B34" s="30"/>
       <c r="C34" s="30"/>
       <c r="D34" s="30"/>
@@ -9523,7 +9704,7 @@
       <c r="F34" s="30"/>
       <c r="G34" s="31"/>
     </row>
-    <row r="35" spans="2:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B35" s="30"/>
       <c r="C35" s="30"/>
       <c r="D35" s="30"/>
@@ -9531,7 +9712,7 @@
       <c r="F35" s="30"/>
       <c r="G35" s="31"/>
     </row>
-    <row r="36" spans="2:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B36" s="30"/>
       <c r="C36" s="30"/>
       <c r="D36" s="30"/>
@@ -9539,7 +9720,7 @@
       <c r="F36" s="30"/>
       <c r="G36" s="31"/>
     </row>
-    <row r="37" spans="2:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B37" s="30"/>
       <c r="C37" s="30"/>
       <c r="D37" s="30"/>
@@ -9547,7 +9728,7 @@
       <c r="F37" s="30"/>
       <c r="G37" s="31"/>
     </row>
-    <row r="38" spans="2:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B38" s="30"/>
       <c r="C38" s="30"/>
       <c r="D38" s="30"/>
@@ -9555,7 +9736,7 @@
       <c r="F38" s="30"/>
       <c r="G38" s="31"/>
     </row>
-    <row r="39" spans="2:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B39" s="30"/>
       <c r="C39" s="30"/>
       <c r="D39" s="30"/>
@@ -9563,7 +9744,7 @@
       <c r="F39" s="30"/>
       <c r="G39" s="31"/>
     </row>
-    <row r="40" spans="2:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B40" s="30"/>
       <c r="C40" s="30"/>
       <c r="D40" s="30"/>
@@ -9571,7 +9752,7 @@
       <c r="F40" s="30"/>
       <c r="G40" s="31"/>
     </row>
-    <row r="41" spans="2:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B41" s="30"/>
       <c r="C41" s="30"/>
       <c r="D41" s="30"/>
@@ -9579,7 +9760,7 @@
       <c r="F41" s="30"/>
       <c r="G41" s="31"/>
     </row>
-    <row r="42" spans="2:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B42" s="30"/>
       <c r="C42" s="30"/>
       <c r="D42" s="30"/>
@@ -9587,7 +9768,7 @@
       <c r="F42" s="30"/>
       <c r="G42" s="31"/>
     </row>
-    <row r="43" spans="2:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B43" s="30"/>
       <c r="C43" s="30"/>
       <c r="D43" s="30"/>
@@ -9595,7 +9776,7 @@
       <c r="F43" s="30"/>
       <c r="G43" s="31"/>
     </row>
-    <row r="44" spans="2:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B44" s="30"/>
       <c r="C44" s="30"/>
       <c r="D44" s="30"/>
@@ -9603,7 +9784,7 @@
       <c r="F44" s="30"/>
       <c r="G44" s="31"/>
     </row>
-    <row r="45" spans="2:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B45" s="30"/>
       <c r="C45" s="30"/>
       <c r="D45" s="30"/>
@@ -9611,7 +9792,7 @@
       <c r="F45" s="30"/>
       <c r="G45" s="31"/>
     </row>
-    <row r="46" spans="2:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B46" s="30"/>
       <c r="C46" s="30"/>
       <c r="D46" s="30"/>
@@ -9619,7 +9800,7 @@
       <c r="F46" s="30"/>
       <c r="G46" s="31"/>
     </row>
-    <row r="47" spans="2:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="2:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B47" s="30"/>
       <c r="C47" s="30"/>
       <c r="D47" s="30"/>
@@ -9627,7 +9808,7 @@
       <c r="F47" s="30"/>
       <c r="G47" s="31"/>
     </row>
-    <row r="48" spans="2:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="2:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B48" s="30"/>
       <c r="C48" s="30"/>
       <c r="D48" s="30"/>
@@ -9635,7 +9816,7 @@
       <c r="F48" s="30"/>
       <c r="G48" s="31"/>
     </row>
-    <row r="49" spans="2:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="2:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B49" s="30"/>
       <c r="C49" s="30"/>
       <c r="D49" s="30"/>
@@ -9643,7 +9824,7 @@
       <c r="F49" s="30"/>
       <c r="G49" s="31"/>
     </row>
-    <row r="50" spans="2:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="2:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B50" s="30"/>
       <c r="C50" s="30"/>
       <c r="D50" s="30"/>
@@ -9651,7 +9832,7 @@
       <c r="F50" s="30"/>
       <c r="G50" s="31"/>
     </row>
-    <row r="51" spans="2:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="2:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B51" s="30"/>
       <c r="C51" s="30"/>
       <c r="D51" s="30"/>
@@ -9659,7 +9840,7 @@
       <c r="F51" s="30"/>
       <c r="G51" s="31"/>
     </row>
-    <row r="52" spans="2:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="2:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B52" s="30"/>
       <c r="C52" s="30"/>
       <c r="D52" s="30"/>
@@ -9667,7 +9848,7 @@
       <c r="F52" s="30"/>
       <c r="G52" s="31"/>
     </row>
-    <row r="53" spans="2:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="2:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B53" s="30"/>
       <c r="C53" s="30"/>
       <c r="D53" s="30"/>
@@ -9675,7 +9856,7 @@
       <c r="F53" s="30"/>
       <c r="G53" s="31"/>
     </row>
-    <row r="54" spans="2:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="2:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B54" s="30"/>
       <c r="C54" s="30"/>
       <c r="D54" s="30"/>
@@ -9683,7 +9864,7 @@
       <c r="F54" s="30"/>
       <c r="G54" s="31"/>
     </row>
-    <row r="55" spans="2:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="2:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B55" s="30"/>
       <c r="C55" s="30"/>
       <c r="D55" s="30"/>
@@ -9691,7 +9872,7 @@
       <c r="F55" s="30"/>
       <c r="G55" s="31"/>
     </row>
-    <row r="56" spans="2:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="2:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B56" s="30"/>
       <c r="C56" s="30"/>
       <c r="D56" s="30"/>
@@ -9699,7 +9880,7 @@
       <c r="F56" s="30"/>
       <c r="G56" s="31"/>
     </row>
-    <row r="57" spans="2:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="2:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B57" s="30"/>
       <c r="C57" s="30"/>
       <c r="D57" s="30"/>
@@ -9707,7 +9888,7 @@
       <c r="F57" s="30"/>
       <c r="G57" s="31"/>
     </row>
-    <row r="58" spans="2:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="2:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B58" s="30"/>
       <c r="C58" s="30"/>
       <c r="D58" s="30"/>
@@ -9715,7 +9896,7 @@
       <c r="F58" s="30"/>
       <c r="G58" s="31"/>
     </row>
-    <row r="59" spans="2:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="2:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B59" s="30"/>
       <c r="C59" s="30"/>
       <c r="D59" s="30"/>
@@ -9723,7 +9904,7 @@
       <c r="F59" s="30"/>
       <c r="G59" s="31"/>
     </row>
-    <row r="60" spans="2:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="2:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B60" s="30"/>
       <c r="C60" s="30"/>
       <c r="D60" s="30"/>
@@ -9731,7 +9912,7 @@
       <c r="F60" s="30"/>
       <c r="G60" s="31"/>
     </row>
-    <row r="61" spans="2:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="2:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B61" s="6">
         <v>41379</v>
       </c>
@@ -9749,7 +9930,7 @@
       </c>
       <c r="G61" s="31"/>
     </row>
-    <row r="62" spans="2:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="2:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B62" s="6">
         <v>41562</v>
       </c>

</xml_diff>